<commit_message>
Excel file changes are done for Reorder Testcase
</commit_message>
<xml_diff>
--- a/src/main/resources/AutomationCatalogue_Batch41_TestData.xlsx
+++ b/src/main/resources/AutomationCatalogue_Batch41_TestData.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AutomationCatalogue\Projects\TestAutomationCatalogue_Batch41\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\triveni\TestAutomationCatalogue_Batch41\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C637A15D-5345-4595-B479-4DB219908DC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{730DFE44-7FDD-4DD6-A342-FDD6C492BBB2}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="OrangeHRM_Login" sheetId="1" r:id="rId1"/>
@@ -19,7 +18,7 @@
     <sheet name="DemoWebshop_ReOrder" sheetId="4" r:id="rId4"/>
     <sheet name="DemoWebshop_CreateAddress" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="67">
   <si>
     <t>S. No</t>
   </si>
@@ -224,12 +223,18 @@
   </si>
   <si>
     <t>OrderNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> DemoWebshop Application ReOrder</t>
+  </si>
+  <si>
+    <t>aarosagarch@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -614,22 +619,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F18C6FE-6D5B-4DA8-AB38-9D02E4FEBF53}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="26" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -646,7 +651,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -663,7 +668,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -680,7 +685,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -697,7 +702,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -714,7 +719,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -731,7 +736,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
@@ -748,7 +753,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
@@ -765,7 +770,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
@@ -782,7 +787,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
@@ -799,7 +804,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
@@ -818,37 +823,37 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{49644686-807E-4BDD-B3FC-AFC45775B9C8}"/>
-    <hyperlink ref="E3:E11" r:id="rId2" display="Admin@123" xr:uid="{3A88243C-5576-4973-BB74-92823AFD61E7}"/>
+    <hyperlink ref="E2" r:id="rId1"/>
+    <hyperlink ref="E3:E11" r:id="rId2" display="Admin@123"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{681D0824-3508-4439-9388-79D31E041950}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="30" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="38" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -892,7 +897,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -933,7 +938,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -968,7 +973,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -1003,7 +1008,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -1035,7 +1040,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -1055,7 +1060,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
@@ -1081,7 +1086,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
@@ -1101,7 +1106,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
@@ -1118,7 +1123,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
@@ -1135,7 +1140,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
@@ -1155,41 +1160,41 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{A2E61A8E-512C-4665-AAAD-DF0376542DCC}"/>
-    <hyperlink ref="E3" r:id="rId2" xr:uid="{09C4D3C9-2535-4875-8C96-3B33D195A97B}"/>
-    <hyperlink ref="E4" r:id="rId3" xr:uid="{A509F7A5-5D21-466A-A61C-405412914E86}"/>
-    <hyperlink ref="E5" r:id="rId4" xr:uid="{87E2B86A-BB58-486C-8001-0CC5DA699084}"/>
-    <hyperlink ref="E6" r:id="rId5" xr:uid="{6E56D7DF-1739-42B5-A97F-35AB81072A9F}"/>
-    <hyperlink ref="E7" r:id="rId6" xr:uid="{4695766B-1035-4F53-996B-E914F5B7FB17}"/>
-    <hyperlink ref="E8" r:id="rId7" xr:uid="{7060BCF3-1224-4CEC-BE25-5432A4CAFB60}"/>
-    <hyperlink ref="E9" r:id="rId8" xr:uid="{D5991558-DAA6-4C7B-AF29-B79105796867}"/>
-    <hyperlink ref="E10" r:id="rId9" xr:uid="{53F00551-3A35-4E23-9214-FFC981AE5516}"/>
-    <hyperlink ref="E11" r:id="rId10" xr:uid="{639C3CBD-8CFA-48D3-BFC2-0DC333029FD4}"/>
+    <hyperlink ref="E2" r:id="rId1"/>
+    <hyperlink ref="E3" r:id="rId2"/>
+    <hyperlink ref="E4" r:id="rId3"/>
+    <hyperlink ref="E5" r:id="rId4"/>
+    <hyperlink ref="E6" r:id="rId5"/>
+    <hyperlink ref="E7" r:id="rId6"/>
+    <hyperlink ref="E8" r:id="rId7"/>
+    <hyperlink ref="E9" r:id="rId8"/>
+    <hyperlink ref="E10" r:id="rId9"/>
+    <hyperlink ref="E11" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0039E566-26BE-41C7-B54C-07E46582CC6C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1218,52 +1223,52 @@
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
@@ -1275,23 +1280,23 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C32ADADF-6387-4766-ADFA-377853296F4F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="28" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" customWidth="1"/>
-    <col min="6" max="6" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34" customWidth="1"/>
+    <col min="4" max="4" width="23" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1311,110 +1316,214 @@
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B2" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B3" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B4" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B5" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B6" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B7" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C7" t="s">
+        <v>65</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B8" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C8" t="s">
+        <v>65</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B9" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C9" t="s">
+        <v>65</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B10" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C10" t="s">
+        <v>65</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B11" t="s">
         <v>63</v>
       </c>
+      <c r="C11" t="s">
+        <v>65</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>18</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="D3:D11" r:id="rId2" display="aarosagarch@gmail.com"/>
+    <hyperlink ref="E2" r:id="rId3"/>
+    <hyperlink ref="E3" r:id="rId4"/>
+    <hyperlink ref="E4" r:id="rId5"/>
+    <hyperlink ref="E5" r:id="rId6"/>
+    <hyperlink ref="E6" r:id="rId7"/>
+    <hyperlink ref="E7" r:id="rId8"/>
+    <hyperlink ref="E8" r:id="rId9"/>
+    <hyperlink ref="E9" r:id="rId10"/>
+    <hyperlink ref="E10" r:id="rId11"/>
+    <hyperlink ref="E11" r:id="rId12"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId13"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D76F8C9-C1B2-447E-91D5-FE56BF995D20}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Reorder testcase excel file writing
</commit_message>
<xml_diff>
--- a/src/main/resources/AutomationCatalogue_Batch41_TestData.xlsx
+++ b/src/main/resources/AutomationCatalogue_Batch41_TestData.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\triveni\TestAutomationCatalogue_Batch41\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AutomationCatalogue\Projects\TestAutomationCatalogue_Batch41\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B368D06-9270-4B64-B286-2EA1939A4E50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OrangeHRM_Login" sheetId="1" r:id="rId1"/>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="68">
   <si>
     <t>S. No</t>
   </si>
@@ -229,12 +230,15 @@
   </si>
   <si>
     <t>aarosagarch@gmail.com</t>
+  </si>
+  <si>
+    <t>Order number: 1481373</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -619,22 +623,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="26" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -651,7 +655,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -668,7 +672,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -685,7 +689,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -702,7 +706,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -719,7 +723,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -736,7 +740,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
@@ -753,7 +757,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
@@ -770,7 +774,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
@@ -787,7 +791,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
@@ -804,7 +808,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
@@ -823,37 +827,37 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1"/>
-    <hyperlink ref="E3:E11" r:id="rId2" display="Admin@123"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="E3:E11" r:id="rId2" display="Admin@123" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="30" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="38" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.44140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -897,7 +901,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -938,7 +942,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -973,7 +977,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -1008,7 +1012,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -1040,7 +1044,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -1060,7 +1064,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
@@ -1086,7 +1090,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
@@ -1106,7 +1110,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
@@ -1123,7 +1127,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
@@ -1140,7 +1144,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
@@ -1160,41 +1164,41 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1"/>
-    <hyperlink ref="E3" r:id="rId2"/>
-    <hyperlink ref="E4" r:id="rId3"/>
-    <hyperlink ref="E5" r:id="rId4"/>
-    <hyperlink ref="E6" r:id="rId5"/>
-    <hyperlink ref="E7" r:id="rId6"/>
-    <hyperlink ref="E8" r:id="rId7"/>
-    <hyperlink ref="E9" r:id="rId8"/>
-    <hyperlink ref="E10" r:id="rId9"/>
-    <hyperlink ref="E11" r:id="rId10"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="E4" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="E5" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="E6" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
+    <hyperlink ref="E7" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
+    <hyperlink ref="E8" r:id="rId7" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
+    <hyperlink ref="E9" r:id="rId8" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
+    <hyperlink ref="E10" r:id="rId9" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
+    <hyperlink ref="E11" r:id="rId10" xr:uid="{00000000-0004-0000-0100-000009000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1223,52 +1227,52 @@
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
@@ -1280,23 +1284,23 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="28" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="34" customWidth="1"/>
     <col min="4" max="4" width="23" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" customWidth="1"/>
+    <col min="6" max="6" width="21.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1316,7 +1320,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -1332,8 +1336,11 @@
       <c r="E2" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -1350,7 +1357,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -1367,7 +1374,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -1384,7 +1391,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -1401,7 +1408,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
@@ -1418,7 +1425,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
@@ -1435,7 +1442,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
@@ -1452,7 +1459,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
@@ -1469,7 +1476,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
@@ -1489,18 +1496,18 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-    <hyperlink ref="D3:D11" r:id="rId2" display="aarosagarch@gmail.com"/>
-    <hyperlink ref="E2" r:id="rId3"/>
-    <hyperlink ref="E3" r:id="rId4"/>
-    <hyperlink ref="E4" r:id="rId5"/>
-    <hyperlink ref="E5" r:id="rId6"/>
-    <hyperlink ref="E6" r:id="rId7"/>
-    <hyperlink ref="E7" r:id="rId8"/>
-    <hyperlink ref="E8" r:id="rId9"/>
-    <hyperlink ref="E9" r:id="rId10"/>
-    <hyperlink ref="E10" r:id="rId11"/>
-    <hyperlink ref="E11" r:id="rId12"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="D3:D11" r:id="rId2" display="aarosagarch@gmail.com" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
+    <hyperlink ref="E2" r:id="rId3" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
+    <hyperlink ref="E3" r:id="rId4" xr:uid="{00000000-0004-0000-0300-000003000000}"/>
+    <hyperlink ref="E4" r:id="rId5" xr:uid="{00000000-0004-0000-0300-000004000000}"/>
+    <hyperlink ref="E5" r:id="rId6" xr:uid="{00000000-0004-0000-0300-000005000000}"/>
+    <hyperlink ref="E6" r:id="rId7" xr:uid="{00000000-0004-0000-0300-000006000000}"/>
+    <hyperlink ref="E7" r:id="rId8" xr:uid="{00000000-0004-0000-0300-000007000000}"/>
+    <hyperlink ref="E8" r:id="rId9" xr:uid="{00000000-0004-0000-0300-000008000000}"/>
+    <hyperlink ref="E9" r:id="rId10" xr:uid="{00000000-0004-0000-0300-000009000000}"/>
+    <hyperlink ref="E10" r:id="rId11" xr:uid="{00000000-0004-0000-0300-00000A000000}"/>
+    <hyperlink ref="E11" r:id="rId12" xr:uid="{00000000-0004-0000-0300-00000B000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId13"/>
@@ -1508,22 +1515,22 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
TC_15 DemoWebshop_TotalOrders sheet is added
</commit_message>
<xml_diff>
--- a/src/main/resources/AutomationCatalogue_Batch41_TestData.xlsx
+++ b/src/main/resources/AutomationCatalogue_Batch41_TestData.xlsx
@@ -1,27 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AutomationCatalogue\Projects\TestAutomationCatalogue_Batch41\src\main\resources\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B368D06-9270-4B64-B286-2EA1939A4E50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="15480" windowHeight="11640" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="OrangeHRM_Login" sheetId="1" r:id="rId1"/>
     <sheet name="OrangeHRM_AddEmployee" sheetId="2" r:id="rId2"/>
     <sheet name="OrangeHRM_AddUser" sheetId="3" r:id="rId3"/>
-    <sheet name="DemoWebshop_ReOrder" sheetId="4" r:id="rId4"/>
-    <sheet name="DemoWebshop_CreateAddress" sheetId="5" r:id="rId5"/>
+    <sheet name="DemoWebshop_TotalOrders" sheetId="6" r:id="rId4"/>
+    <sheet name="DemoWebshop_ReOrder" sheetId="4" r:id="rId5"/>
+    <sheet name="DemoWebshop_CreateAddress" sheetId="5" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="124519"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -29,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="70">
   <si>
     <t>S. No</t>
   </si>
@@ -233,13 +228,19 @@
   </si>
   <si>
     <t>Order number: 1481373</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> DemoWebshop Application TotalOrders</t>
+  </si>
+  <si>
+    <t>TC15_DemoWebshop_TotalOrders</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -370,7 +371,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -422,7 +423,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -616,29 +617,29 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="26" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -655,7 +656,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -672,7 +673,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -689,7 +690,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -706,7 +707,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -723,7 +724,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -740,7 +741,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
@@ -757,7 +758,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
@@ -774,7 +775,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
@@ -791,7 +792,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
@@ -808,7 +809,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5">
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
@@ -827,37 +828,37 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="E3:E11" r:id="rId2" display="Admin@123" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="E2" r:id="rId1"/>
+    <hyperlink ref="E3:E11" r:id="rId2" display="Admin@123"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="30" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="38" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -901,7 +902,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -942,7 +943,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -977,7 +978,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -1012,7 +1013,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -1044,7 +1045,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -1064,7 +1065,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
@@ -1090,7 +1091,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
@@ -1110,7 +1111,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
@@ -1127,7 +1128,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
@@ -1144,7 +1145,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14">
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
@@ -1164,41 +1165,41 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="E3" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
-    <hyperlink ref="E4" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
-    <hyperlink ref="E5" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
-    <hyperlink ref="E6" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
-    <hyperlink ref="E7" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
-    <hyperlink ref="E8" r:id="rId7" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
-    <hyperlink ref="E9" r:id="rId8" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
-    <hyperlink ref="E10" r:id="rId9" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
-    <hyperlink ref="E11" r:id="rId10" xr:uid="{00000000-0004-0000-0100-000009000000}"/>
+    <hyperlink ref="E2" r:id="rId1"/>
+    <hyperlink ref="E3" r:id="rId2"/>
+    <hyperlink ref="E4" r:id="rId3"/>
+    <hyperlink ref="E5" r:id="rId4"/>
+    <hyperlink ref="E6" r:id="rId5"/>
+    <hyperlink ref="E7" r:id="rId6"/>
+    <hyperlink ref="E8" r:id="rId7"/>
+    <hyperlink ref="E9" r:id="rId8"/>
+    <hyperlink ref="E10" r:id="rId9"/>
+    <hyperlink ref="E11" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1227,52 +1228,52 @@
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9">
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
@@ -1284,23 +1285,245 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="41.140625" customWidth="1"/>
+    <col min="3" max="3" width="40" customWidth="1"/>
+    <col min="4" max="4" width="24.42578125" customWidth="1"/>
+    <col min="5" max="5" width="19.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C6" t="s">
+        <v>68</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C7" t="s">
+        <v>68</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" t="s">
+        <v>69</v>
+      </c>
+      <c r="C8" t="s">
+        <v>68</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C9" t="s">
+        <v>68</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" t="s">
+        <v>69</v>
+      </c>
+      <c r="C10" t="s">
+        <v>68</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" t="s">
+        <v>69</v>
+      </c>
+      <c r="C11" t="s">
+        <v>68</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="D3:D11" r:id="rId2" display="aarosagarch@gmail.com"/>
+    <hyperlink ref="E2" r:id="rId3"/>
+    <hyperlink ref="E3" r:id="rId4"/>
+    <hyperlink ref="E4" r:id="rId5"/>
+    <hyperlink ref="E5" r:id="rId6"/>
+    <hyperlink ref="E6" r:id="rId7"/>
+    <hyperlink ref="E7" r:id="rId8"/>
+    <hyperlink ref="E8" r:id="rId9"/>
+    <hyperlink ref="E9" r:id="rId10"/>
+    <hyperlink ref="E10" r:id="rId11"/>
+    <hyperlink ref="E11" r:id="rId12"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="28" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="34" customWidth="1"/>
     <col min="4" max="4" width="23" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" customWidth="1"/>
-    <col min="6" max="6" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" customWidth="1"/>
+    <col min="6" max="6" width="21.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1320,7 +1543,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -1340,7 +1563,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -1357,7 +1580,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -1374,7 +1597,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -1391,7 +1614,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -1408,7 +1631,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
@@ -1425,7 +1648,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
@@ -1442,7 +1665,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
@@ -1459,7 +1682,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
@@ -1476,7 +1699,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6">
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
@@ -1496,41 +1719,41 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
-    <hyperlink ref="D3:D11" r:id="rId2" display="aarosagarch@gmail.com" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
-    <hyperlink ref="E2" r:id="rId3" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
-    <hyperlink ref="E3" r:id="rId4" xr:uid="{00000000-0004-0000-0300-000003000000}"/>
-    <hyperlink ref="E4" r:id="rId5" xr:uid="{00000000-0004-0000-0300-000004000000}"/>
-    <hyperlink ref="E5" r:id="rId6" xr:uid="{00000000-0004-0000-0300-000005000000}"/>
-    <hyperlink ref="E6" r:id="rId7" xr:uid="{00000000-0004-0000-0300-000006000000}"/>
-    <hyperlink ref="E7" r:id="rId8" xr:uid="{00000000-0004-0000-0300-000007000000}"/>
-    <hyperlink ref="E8" r:id="rId9" xr:uid="{00000000-0004-0000-0300-000008000000}"/>
-    <hyperlink ref="E9" r:id="rId10" xr:uid="{00000000-0004-0000-0300-000009000000}"/>
-    <hyperlink ref="E10" r:id="rId11" xr:uid="{00000000-0004-0000-0300-00000A000000}"/>
-    <hyperlink ref="E11" r:id="rId12" xr:uid="{00000000-0004-0000-0300-00000B000000}"/>
+    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="D3:D11" r:id="rId2" display="aarosagarch@gmail.com"/>
+    <hyperlink ref="E2" r:id="rId3"/>
+    <hyperlink ref="E3" r:id="rId4"/>
+    <hyperlink ref="E4" r:id="rId5"/>
+    <hyperlink ref="E5" r:id="rId6"/>
+    <hyperlink ref="E6" r:id="rId7"/>
+    <hyperlink ref="E7" r:id="rId8"/>
+    <hyperlink ref="E8" r:id="rId9"/>
+    <hyperlink ref="E9" r:id="rId10"/>
+    <hyperlink ref="E10" r:id="rId11"/>
+    <hyperlink ref="E11" r:id="rId12"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId13"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
TC_15 DemoWebshop_TotalOrders: Written TotalNumberOf Orders and SumOfAllOrder values back to excel file
</commit_message>
<xml_diff>
--- a/src/main/resources/AutomationCatalogue_Batch41_TestData.xlsx
+++ b/src/main/resources/AutomationCatalogue_Batch41_TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="15480" windowHeight="11640" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="15480" windowHeight="11640" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="OrangeHRM_Login" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="74">
   <si>
     <t>S. No</t>
   </si>
@@ -227,19 +227,32 @@
     <t>aarosagarch@gmail.com</t>
   </si>
   <si>
-    <t>Order number: 1481373</t>
-  </si>
-  <si>
     <t xml:space="preserve"> DemoWebshop Application TotalOrders</t>
   </si>
   <si>
     <t>TC15_DemoWebshop_TotalOrders</t>
+  </si>
+  <si>
+    <t>TotalNumberOfOrders</t>
+  </si>
+  <si>
+    <t>Order number: 1481392</t>
+  </si>
+  <si>
+    <t>313</t>
+  </si>
+  <si>
+    <t>SumOfAllOrders</t>
+  </si>
+  <si>
+    <t>47639.6</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="4">
     <font>
       <sz val="11"/>
@@ -617,7 +630,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -633,10 +646,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="26" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="26.0"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="24.42578125"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.7109375"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="11.28515625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -660,13 +673,13 @@
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>15</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>16</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="0">
         <v>17</v>
       </c>
       <c r="E2" s="3" t="s">
@@ -677,13 +690,13 @@
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>15</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>16</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" t="s" s="0">
         <v>19</v>
       </c>
       <c r="E3" s="3" t="s">
@@ -694,13 +707,13 @@
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>15</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" t="s" s="0">
         <v>16</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" t="s" s="0">
         <v>20</v>
       </c>
       <c r="E4" s="3" t="s">
@@ -711,13 +724,13 @@
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" t="s" s="0">
         <v>15</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" t="s" s="0">
         <v>16</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" t="s" s="0">
         <v>21</v>
       </c>
       <c r="E5" s="3" t="s">
@@ -728,13 +741,13 @@
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" t="s" s="0">
         <v>15</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" t="s" s="0">
         <v>16</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" t="s" s="0">
         <v>22</v>
       </c>
       <c r="E6" s="3" t="s">
@@ -745,13 +758,13 @@
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" t="s" s="0">
         <v>15</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" t="s" s="0">
         <v>16</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" t="s" s="0">
         <v>23</v>
       </c>
       <c r="E7" s="3" t="s">
@@ -762,13 +775,13 @@
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" t="s" s="0">
         <v>15</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" t="s" s="0">
         <v>16</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" t="s" s="0">
         <v>24</v>
       </c>
       <c r="E8" s="3" t="s">
@@ -779,13 +792,13 @@
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" t="s" s="0">
         <v>15</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" t="s" s="0">
         <v>16</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" t="s" s="0">
         <v>25</v>
       </c>
       <c r="E9" s="3" t="s">
@@ -796,13 +809,13 @@
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" t="s" s="0">
         <v>15</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" t="s" s="0">
         <v>16</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" t="s" s="0">
         <v>26</v>
       </c>
       <c r="E10" s="3" t="s">
@@ -813,13 +826,13 @@
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" t="s" s="0">
         <v>15</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" t="s" s="0">
         <v>16</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" t="s" s="0">
         <v>27</v>
       </c>
       <c r="E11" s="3" t="s">
@@ -845,17 +858,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="30" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="30.0"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="38.0"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.140625"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="11.28515625"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="9.85546875"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="9.42578125"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="25.42578125"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="13.0"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="10.7109375"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="16.85546875"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="11.28515625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -906,40 +919,40 @@
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>38</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="0">
         <v>17</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" t="s" s="0">
         <v>39</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" t="s" s="0">
         <v>40</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" t="s" s="0">
         <v>58</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" t="s" s="0">
         <v>41</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" t="s" s="0">
         <v>42</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" t="s" s="0">
         <v>43</v>
       </c>
       <c r="L2" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="M2" t="s">
+      <c r="M2" t="s" s="0">
         <v>52</v>
       </c>
     </row>
@@ -947,34 +960,34 @@
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>38</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" t="s" s="0">
         <v>17</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" t="s" s="0">
         <v>56</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" t="s" s="0">
         <v>46</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" t="s" s="0">
         <v>48</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K3" t="s" s="0">
         <v>44</v>
       </c>
       <c r="L3" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="M3" t="s">
+      <c r="M3" t="s" s="0">
         <v>53</v>
       </c>
     </row>
@@ -982,25 +995,25 @@
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" t="s" s="0">
         <v>38</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" t="s" s="0">
         <v>17</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" t="s" s="0">
         <v>57</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" t="s" s="0">
         <v>47</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" t="s" s="0">
         <v>49</v>
       </c>
       <c r="K4" s="2" t="s">
@@ -1009,7 +1022,7 @@
       <c r="L4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="M4" t="s">
+      <c r="M4" t="s" s="0">
         <v>54</v>
       </c>
     </row>
@@ -1017,31 +1030,31 @@
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" t="s" s="0">
         <v>38</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" t="s" s="0">
         <v>17</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" t="s" s="0">
         <v>59</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I5" t="s" s="0">
         <v>41</v>
       </c>
-      <c r="J5" t="s">
+      <c r="J5" t="s" s="0">
         <v>48</v>
       </c>
       <c r="K5" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="M5" t="s">
+      <c r="M5" t="s" s="0">
         <v>55</v>
       </c>
     </row>
@@ -1049,19 +1062,19 @@
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" t="s" s="0">
         <v>38</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" t="s" s="0">
         <v>17</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="M6" t="s">
+      <c r="M6" t="s" s="0">
         <v>53</v>
       </c>
     </row>
@@ -1069,25 +1082,25 @@
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" t="s" s="0">
         <v>38</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" t="s" s="0">
         <v>17</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I7" t="s">
+      <c r="I7" t="s" s="0">
         <v>46</v>
       </c>
-      <c r="J7" t="s">
+      <c r="J7" t="s" s="0">
         <v>42</v>
       </c>
-      <c r="M7" t="s">
+      <c r="M7" t="s" s="0">
         <v>52</v>
       </c>
     </row>
@@ -1095,19 +1108,19 @@
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" t="s" s="0">
         <v>38</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" t="s" s="0">
         <v>17</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="M8" t="s">
+      <c r="M8" t="s" s="0">
         <v>54</v>
       </c>
     </row>
@@ -1115,13 +1128,13 @@
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" t="s" s="0">
         <v>38</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" t="s" s="0">
         <v>17</v>
       </c>
       <c r="E9" s="3" t="s">
@@ -1132,13 +1145,13 @@
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" t="s" s="0">
         <v>38</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" t="s" s="0">
         <v>17</v>
       </c>
       <c r="E10" s="3" t="s">
@@ -1149,13 +1162,13 @@
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" t="s" s="0">
         <v>38</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" t="s" s="0">
         <v>17</v>
       </c>
       <c r="E11" s="3" t="s">
@@ -1190,13 +1203,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="14.28515625"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="19.140625"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.140625"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="9.140625"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="14.85546875"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="18.85546875"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="16.28515625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -1286,21 +1299,23 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="41.140625" customWidth="1"/>
-    <col min="3" max="3" width="40" customWidth="1"/>
-    <col min="4" max="4" width="24.42578125" customWidth="1"/>
-    <col min="5" max="5" width="19.5703125" customWidth="1"/>
+    <col min="2" max="2" customWidth="true" width="41.140625"/>
+    <col min="3" max="3" customWidth="true" width="40.0"/>
+    <col min="4" max="4" customWidth="true" width="24.42578125"/>
+    <col min="5" max="5" customWidth="true" width="19.5703125"/>
+    <col min="6" max="6" customWidth="true" width="22.85546875"/>
+    <col min="7" max="7" customWidth="true" width="20.28515625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1316,34 +1331,46 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
-        <v>69</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="B2" t="s" s="0">
         <v>68</v>
       </c>
+      <c r="C2" t="s" s="0">
+        <v>67</v>
+      </c>
       <c r="D2" s="3" t="s">
         <v>66</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="F2" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="G2" t="s" s="0">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
-        <v>69</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="B3" t="s" s="0">
         <v>68</v>
       </c>
+      <c r="C3" t="s" s="0">
+        <v>67</v>
+      </c>
       <c r="D3" s="3" t="s">
         <v>66</v>
       </c>
@@ -1351,16 +1378,16 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:7">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B4" t="s">
-        <v>69</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="B4" t="s" s="0">
         <v>68</v>
       </c>
+      <c r="C4" t="s" s="0">
+        <v>67</v>
+      </c>
       <c r="D4" s="3" t="s">
         <v>66</v>
       </c>
@@ -1368,16 +1395,16 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:7">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="B5" t="s" s="0">
         <v>68</v>
       </c>
+      <c r="C5" t="s" s="0">
+        <v>67</v>
+      </c>
       <c r="D5" s="3" t="s">
         <v>66</v>
       </c>
@@ -1385,16 +1412,16 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:7">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B6" t="s">
-        <v>69</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="B6" t="s" s="0">
         <v>68</v>
       </c>
+      <c r="C6" t="s" s="0">
+        <v>67</v>
+      </c>
       <c r="D6" s="3" t="s">
         <v>66</v>
       </c>
@@ -1402,16 +1429,16 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:7">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B7" t="s">
-        <v>69</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="B7" t="s" s="0">
         <v>68</v>
       </c>
+      <c r="C7" t="s" s="0">
+        <v>67</v>
+      </c>
       <c r="D7" s="3" t="s">
         <v>66</v>
       </c>
@@ -1419,16 +1446,16 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:7">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B8" t="s">
-        <v>69</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="B8" t="s" s="0">
         <v>68</v>
       </c>
+      <c r="C8" t="s" s="0">
+        <v>67</v>
+      </c>
       <c r="D8" s="3" t="s">
         <v>66</v>
       </c>
@@ -1436,16 +1463,16 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:7">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B9" t="s">
-        <v>69</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="B9" t="s" s="0">
         <v>68</v>
       </c>
+      <c r="C9" t="s" s="0">
+        <v>67</v>
+      </c>
       <c r="D9" s="3" t="s">
         <v>66</v>
       </c>
@@ -1453,16 +1480,16 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:7">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B10" t="s">
-        <v>69</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="B10" t="s" s="0">
         <v>68</v>
       </c>
+      <c r="C10" t="s" s="0">
+        <v>67</v>
+      </c>
       <c r="D10" s="3" t="s">
         <v>66</v>
       </c>
@@ -1470,15 +1497,15 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:7">
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B11" t="s">
-        <v>69</v>
-      </c>
-      <c r="C11" t="s">
+      <c r="B11" t="s" s="0">
         <v>68</v>
+      </c>
+      <c r="C11" t="s" s="0">
+        <v>67</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>66</v>
@@ -1503,6 +1530,7 @@
     <hyperlink ref="E11" r:id="rId12"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId13"/>
 </worksheet>
 </file>
 
@@ -1516,11 +1544,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="28" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34" customWidth="1"/>
-    <col min="4" max="4" width="23" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" customWidth="1"/>
-    <col min="6" max="6" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="28.0"/>
+    <col min="3" max="3" customWidth="true" width="34.0"/>
+    <col min="4" max="4" customWidth="true" width="23.0"/>
+    <col min="5" max="5" customWidth="true" width="11.28515625"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="21.28515625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1547,10 +1575,10 @@
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>63</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>65</v>
       </c>
       <c r="D2" s="3" t="s">
@@ -1559,18 +1587,18 @@
       <c r="E2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F2" t="s">
-        <v>67</v>
+      <c r="F2" t="s" s="0">
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>63</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>65</v>
       </c>
       <c r="D3" s="3" t="s">
@@ -1584,10 +1612,10 @@
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>63</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" t="s" s="0">
         <v>65</v>
       </c>
       <c r="D4" s="3" t="s">
@@ -1601,10 +1629,10 @@
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" t="s" s="0">
         <v>63</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" t="s" s="0">
         <v>65</v>
       </c>
       <c r="D5" s="3" t="s">
@@ -1618,10 +1646,10 @@
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" t="s" s="0">
         <v>63</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" t="s" s="0">
         <v>65</v>
       </c>
       <c r="D6" s="3" t="s">
@@ -1635,10 +1663,10 @@
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" t="s" s="0">
         <v>63</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" t="s" s="0">
         <v>65</v>
       </c>
       <c r="D7" s="3" t="s">
@@ -1652,10 +1680,10 @@
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" t="s" s="0">
         <v>63</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" t="s" s="0">
         <v>65</v>
       </c>
       <c r="D8" s="3" t="s">
@@ -1669,10 +1697,10 @@
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" t="s" s="0">
         <v>63</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" t="s" s="0">
         <v>65</v>
       </c>
       <c r="D9" s="3" t="s">
@@ -1686,10 +1714,10 @@
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" t="s" s="0">
         <v>63</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" t="s" s="0">
         <v>65</v>
       </c>
       <c r="D10" s="3" t="s">
@@ -1703,10 +1731,10 @@
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" t="s" s="0">
         <v>63</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" t="s" s="0">
         <v>65</v>
       </c>
       <c r="D11" s="3" t="s">
@@ -1747,10 +1775,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="14.28515625"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="19.140625"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.140625"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="9.140625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">

</xml_diff>

<commit_message>
Excel file changes are done for ApplyDiscount Testcase
</commit_message>
<xml_diff>
--- a/src/main/resources/AutomationCatalogue_Batch41_TestData.xlsx
+++ b/src/main/resources/AutomationCatalogue_Batch41_TestData.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\triveni\TestAutomationCatalogue_Batch41\src\main\resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="15480" windowHeight="11640" firstSheet="2" activeTab="3"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="15480" windowHeight="11640" firstSheet="3" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="OrangeHRM_Login" sheetId="1" r:id="rId1"/>
@@ -12,11 +17,12 @@
     <sheet name="OrangeHRM_AddUser" sheetId="3" r:id="rId3"/>
     <sheet name="DemoWebshop_TotalOrders" sheetId="6" r:id="rId4"/>
     <sheet name="DemoWebshop_ReOrder" sheetId="4" r:id="rId5"/>
-    <sheet name="DemoWebshop_CreateAddress" sheetId="5" r:id="rId6"/>
+    <sheet name="DemoWebshop_ApplyDiscount" sheetId="7" r:id="rId6"/>
+    <sheet name="DemoWebshop_CreateAddress" sheetId="5" r:id="rId7"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="79">
   <si>
     <t>S. No</t>
   </si>
@@ -246,14 +252,28 @@
   </si>
   <si>
     <t>47639.6</t>
+  </si>
+  <si>
+    <t>TC18_DemoWebshop_ApplyDiscount</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> DemoWebshop Application ApplyDisscount</t>
+  </si>
+  <si>
+    <t>ApplyCoupon</t>
+  </si>
+  <si>
+    <t>AutomationDiscount2</t>
+  </si>
+  <si>
+    <t>Order number: 1482444</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -279,6 +299,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFF00"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -317,12 +345,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -637,22 +666,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="26.0"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="24.42578125"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="10.7109375"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="11.28515625"/>
+    <col min="2" max="2" width="26" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -669,170 +698,170 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s" s="0">
+      <c r="B2" t="s">
         <v>15</v>
       </c>
-      <c r="C2" t="s" s="0">
+      <c r="C2" t="s">
         <v>16</v>
       </c>
-      <c r="D2" t="s" s="0">
+      <c r="D2" t="s">
         <v>17</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s" s="0">
+      <c r="B3" t="s">
         <v>15</v>
       </c>
-      <c r="C3" t="s" s="0">
+      <c r="C3" t="s">
         <v>16</v>
       </c>
-      <c r="D3" t="s" s="0">
+      <c r="D3" t="s">
         <v>19</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B4" t="s" s="0">
+      <c r="B4" t="s">
         <v>15</v>
       </c>
-      <c r="C4" t="s" s="0">
+      <c r="C4" t="s">
         <v>16</v>
       </c>
-      <c r="D4" t="s" s="0">
+      <c r="D4" t="s">
         <v>20</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B5" t="s" s="0">
+      <c r="B5" t="s">
         <v>15</v>
       </c>
-      <c r="C5" t="s" s="0">
+      <c r="C5" t="s">
         <v>16</v>
       </c>
-      <c r="D5" t="s" s="0">
+      <c r="D5" t="s">
         <v>21</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B6" t="s" s="0">
+      <c r="B6" t="s">
         <v>15</v>
       </c>
-      <c r="C6" t="s" s="0">
+      <c r="C6" t="s">
         <v>16</v>
       </c>
-      <c r="D6" t="s" s="0">
+      <c r="D6" t="s">
         <v>22</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B7" t="s" s="0">
+      <c r="B7" t="s">
         <v>15</v>
       </c>
-      <c r="C7" t="s" s="0">
+      <c r="C7" t="s">
         <v>16</v>
       </c>
-      <c r="D7" t="s" s="0">
+      <c r="D7" t="s">
         <v>23</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B8" t="s" s="0">
+      <c r="B8" t="s">
         <v>15</v>
       </c>
-      <c r="C8" t="s" s="0">
+      <c r="C8" t="s">
         <v>16</v>
       </c>
-      <c r="D8" t="s" s="0">
+      <c r="D8" t="s">
         <v>24</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B9" t="s" s="0">
+      <c r="B9" t="s">
         <v>15</v>
       </c>
-      <c r="C9" t="s" s="0">
+      <c r="C9" t="s">
         <v>16</v>
       </c>
-      <c r="D9" t="s" s="0">
+      <c r="D9" t="s">
         <v>25</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B10" t="s" s="0">
+      <c r="B10" t="s">
         <v>15</v>
       </c>
-      <c r="C10" t="s" s="0">
+      <c r="C10" t="s">
         <v>16</v>
       </c>
-      <c r="D10" t="s" s="0">
+      <c r="D10" t="s">
         <v>26</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B11" t="s" s="0">
+      <c r="B11" t="s">
         <v>15</v>
       </c>
-      <c r="C11" t="s" s="0">
+      <c r="C11" t="s">
         <v>16</v>
       </c>
-      <c r="D11" t="s" s="0">
+      <c r="D11" t="s">
         <v>27</v>
       </c>
       <c r="E11" s="3" t="s">
@@ -849,29 +878,29 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="30.0"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="38.0"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="10.140625"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="11.28515625"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="9.85546875"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="9.42578125"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="25.42578125"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="13.0"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="10.7109375"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="16.85546875"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="11.28515625"/>
+    <col min="2" max="2" width="30" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -915,105 +944,105 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s" s="0">
+      <c r="B2" t="s">
         <v>37</v>
       </c>
-      <c r="C2" t="s" s="0">
+      <c r="C2" t="s">
         <v>38</v>
       </c>
-      <c r="D2" t="s" s="0">
+      <c r="D2" t="s">
         <v>17</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F2" t="s" s="0">
+      <c r="F2" t="s">
         <v>39</v>
       </c>
-      <c r="G2" t="s" s="0">
+      <c r="G2" t="s">
         <v>40</v>
       </c>
-      <c r="H2" t="s" s="0">
+      <c r="H2" t="s">
         <v>58</v>
       </c>
-      <c r="I2" t="s" s="0">
+      <c r="I2" t="s">
         <v>41</v>
       </c>
-      <c r="J2" t="s" s="0">
+      <c r="J2" t="s">
         <v>42</v>
       </c>
-      <c r="K2" t="s" s="0">
+      <c r="K2" t="s">
         <v>43</v>
       </c>
       <c r="L2" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="M2" t="s" s="0">
+      <c r="M2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s" s="0">
+      <c r="B3" t="s">
         <v>37</v>
       </c>
-      <c r="C3" t="s" s="0">
+      <c r="C3" t="s">
         <v>38</v>
       </c>
-      <c r="D3" t="s" s="0">
+      <c r="D3" t="s">
         <v>17</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="H3" t="s" s="0">
+      <c r="H3" t="s">
         <v>56</v>
       </c>
-      <c r="I3" t="s" s="0">
+      <c r="I3" t="s">
         <v>46</v>
       </c>
-      <c r="J3" t="s" s="0">
+      <c r="J3" t="s">
         <v>48</v>
       </c>
-      <c r="K3" t="s" s="0">
+      <c r="K3" t="s">
         <v>44</v>
       </c>
       <c r="L3" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="M3" t="s" s="0">
+      <c r="M3" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B4" t="s" s="0">
+      <c r="B4" t="s">
         <v>37</v>
       </c>
-      <c r="C4" t="s" s="0">
+      <c r="C4" t="s">
         <v>38</v>
       </c>
-      <c r="D4" t="s" s="0">
+      <c r="D4" t="s">
         <v>17</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="H4" t="s" s="0">
+      <c r="H4" t="s">
         <v>57</v>
       </c>
-      <c r="I4" t="s" s="0">
+      <c r="I4" t="s">
         <v>47</v>
       </c>
-      <c r="J4" t="s" s="0">
+      <c r="J4" t="s">
         <v>49</v>
       </c>
       <c r="K4" s="2" t="s">
@@ -1022,153 +1051,153 @@
       <c r="L4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="M4" t="s" s="0">
+      <c r="M4" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B5" t="s" s="0">
+      <c r="B5" t="s">
         <v>37</v>
       </c>
-      <c r="C5" t="s" s="0">
+      <c r="C5" t="s">
         <v>38</v>
       </c>
-      <c r="D5" t="s" s="0">
+      <c r="D5" t="s">
         <v>17</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="H5" t="s" s="0">
+      <c r="H5" t="s">
         <v>59</v>
       </c>
-      <c r="I5" t="s" s="0">
+      <c r="I5" t="s">
         <v>41</v>
       </c>
-      <c r="J5" t="s" s="0">
+      <c r="J5" t="s">
         <v>48</v>
       </c>
       <c r="K5" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="M5" t="s" s="0">
+      <c r="M5" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B6" t="s" s="0">
+      <c r="B6" t="s">
         <v>37</v>
       </c>
-      <c r="C6" t="s" s="0">
+      <c r="C6" t="s">
         <v>38</v>
       </c>
-      <c r="D6" t="s" s="0">
+      <c r="D6" t="s">
         <v>17</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="M6" t="s" s="0">
+      <c r="M6" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B7" t="s" s="0">
+      <c r="B7" t="s">
         <v>37</v>
       </c>
-      <c r="C7" t="s" s="0">
+      <c r="C7" t="s">
         <v>38</v>
       </c>
-      <c r="D7" t="s" s="0">
+      <c r="D7" t="s">
         <v>17</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I7" t="s" s="0">
+      <c r="I7" t="s">
         <v>46</v>
       </c>
-      <c r="J7" t="s" s="0">
+      <c r="J7" t="s">
         <v>42</v>
       </c>
-      <c r="M7" t="s" s="0">
+      <c r="M7" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B8" t="s" s="0">
+      <c r="B8" t="s">
         <v>37</v>
       </c>
-      <c r="C8" t="s" s="0">
+      <c r="C8" t="s">
         <v>38</v>
       </c>
-      <c r="D8" t="s" s="0">
+      <c r="D8" t="s">
         <v>17</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="M8" t="s" s="0">
+      <c r="M8" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B9" t="s" s="0">
+      <c r="B9" t="s">
         <v>37</v>
       </c>
-      <c r="C9" t="s" s="0">
+      <c r="C9" t="s">
         <v>38</v>
       </c>
-      <c r="D9" t="s" s="0">
+      <c r="D9" t="s">
         <v>17</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B10" t="s" s="0">
+      <c r="B10" t="s">
         <v>37</v>
       </c>
-      <c r="C10" t="s" s="0">
+      <c r="C10" t="s">
         <v>38</v>
       </c>
-      <c r="D10" t="s" s="0">
+      <c r="D10" t="s">
         <v>17</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B11" t="s" s="0">
+      <c r="B11" t="s">
         <v>37</v>
       </c>
-      <c r="C11" t="s" s="0">
+      <c r="C11" t="s">
         <v>38</v>
       </c>
-      <c r="D11" t="s" s="0">
+      <c r="D11" t="s">
         <v>17</v>
       </c>
       <c r="E11" s="3" t="s">
@@ -1194,25 +1223,25 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="14.28515625"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="19.140625"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="10.140625"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="9.140625"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="14.85546875"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="18.85546875"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="16.28515625"/>
+    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1241,52 +1270,52 @@
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
@@ -1298,24 +1327,24 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="41.140625"/>
-    <col min="3" max="3" customWidth="true" width="40.0"/>
-    <col min="4" max="4" customWidth="true" width="24.42578125"/>
-    <col min="5" max="5" customWidth="true" width="19.5703125"/>
-    <col min="6" max="6" customWidth="true" width="22.85546875"/>
-    <col min="7" max="7" customWidth="true" width="20.28515625"/>
+    <col min="2" max="2" width="41.140625" customWidth="1"/>
+    <col min="3" max="3" width="40" customWidth="1"/>
+    <col min="4" max="4" width="24.42578125" customWidth="1"/>
+    <col min="5" max="5" width="19.5703125" customWidth="1"/>
+    <col min="6" max="6" width="22.85546875" customWidth="1"/>
+    <col min="7" max="7" width="20.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1338,14 +1367,14 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s" s="0">
+      <c r="B2" t="s">
         <v>68</v>
       </c>
-      <c r="C2" t="s" s="0">
+      <c r="C2" t="s">
         <v>67</v>
       </c>
       <c r="D2" s="3" t="s">
@@ -1354,21 +1383,21 @@
       <c r="E2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F2" t="s" s="0">
+      <c r="F2" t="s">
         <v>71</v>
       </c>
-      <c r="G2" t="s" s="0">
+      <c r="G2" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s" s="0">
+      <c r="B3" t="s">
         <v>68</v>
       </c>
-      <c r="C3" t="s" s="0">
+      <c r="C3" t="s">
         <v>67</v>
       </c>
       <c r="D3" s="3" t="s">
@@ -1378,14 +1407,14 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B4" t="s" s="0">
+      <c r="B4" t="s">
         <v>68</v>
       </c>
-      <c r="C4" t="s" s="0">
+      <c r="C4" t="s">
         <v>67</v>
       </c>
       <c r="D4" s="3" t="s">
@@ -1395,14 +1424,14 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B5" t="s" s="0">
+      <c r="B5" t="s">
         <v>68</v>
       </c>
-      <c r="C5" t="s" s="0">
+      <c r="C5" t="s">
         <v>67</v>
       </c>
       <c r="D5" s="3" t="s">
@@ -1412,14 +1441,14 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B6" t="s" s="0">
+      <c r="B6" t="s">
         <v>68</v>
       </c>
-      <c r="C6" t="s" s="0">
+      <c r="C6" t="s">
         <v>67</v>
       </c>
       <c r="D6" s="3" t="s">
@@ -1429,14 +1458,14 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B7" t="s" s="0">
+      <c r="B7" t="s">
         <v>68</v>
       </c>
-      <c r="C7" t="s" s="0">
+      <c r="C7" t="s">
         <v>67</v>
       </c>
       <c r="D7" s="3" t="s">
@@ -1446,14 +1475,14 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B8" t="s" s="0">
+      <c r="B8" t="s">
         <v>68</v>
       </c>
-      <c r="C8" t="s" s="0">
+      <c r="C8" t="s">
         <v>67</v>
       </c>
       <c r="D8" s="3" t="s">
@@ -1463,14 +1492,14 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B9" t="s" s="0">
+      <c r="B9" t="s">
         <v>68</v>
       </c>
-      <c r="C9" t="s" s="0">
+      <c r="C9" t="s">
         <v>67</v>
       </c>
       <c r="D9" s="3" t="s">
@@ -1480,14 +1509,14 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B10" t="s" s="0">
+      <c r="B10" t="s">
         <v>68</v>
       </c>
-      <c r="C10" t="s" s="0">
+      <c r="C10" t="s">
         <v>67</v>
       </c>
       <c r="D10" s="3" t="s">
@@ -1497,14 +1526,14 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B11" t="s" s="0">
+      <c r="B11" t="s">
         <v>68</v>
       </c>
-      <c r="C11" t="s" s="0">
+      <c r="C11" t="s">
         <v>67</v>
       </c>
       <c r="D11" s="3" t="s">
@@ -1535,23 +1564,23 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E11"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="28.0"/>
-    <col min="3" max="3" customWidth="true" width="34.0"/>
-    <col min="4" max="4" customWidth="true" width="23.0"/>
-    <col min="5" max="5" customWidth="true" width="11.28515625"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="21.28515625"/>
+    <col min="2" max="2" width="28" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34" customWidth="1"/>
+    <col min="4" max="4" width="23" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" customWidth="1"/>
+    <col min="6" max="6" width="21.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1571,14 +1600,14 @@
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s" s="0">
+      <c r="B2" t="s">
         <v>63</v>
       </c>
-      <c r="C2" t="s" s="0">
+      <c r="C2" t="s">
         <v>65</v>
       </c>
       <c r="D2" s="3" t="s">
@@ -1587,18 +1616,18 @@
       <c r="E2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F2" t="s" s="0">
+      <c r="F2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s" s="0">
+      <c r="B3" t="s">
         <v>63</v>
       </c>
-      <c r="C3" t="s" s="0">
+      <c r="C3" t="s">
         <v>65</v>
       </c>
       <c r="D3" s="3" t="s">
@@ -1608,14 +1637,14 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B4" t="s" s="0">
+      <c r="B4" t="s">
         <v>63</v>
       </c>
-      <c r="C4" t="s" s="0">
+      <c r="C4" t="s">
         <v>65</v>
       </c>
       <c r="D4" s="3" t="s">
@@ -1625,14 +1654,14 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B5" t="s" s="0">
+      <c r="B5" t="s">
         <v>63</v>
       </c>
-      <c r="C5" t="s" s="0">
+      <c r="C5" t="s">
         <v>65</v>
       </c>
       <c r="D5" s="3" t="s">
@@ -1642,14 +1671,14 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B6" t="s" s="0">
+      <c r="B6" t="s">
         <v>63</v>
       </c>
-      <c r="C6" t="s" s="0">
+      <c r="C6" t="s">
         <v>65</v>
       </c>
       <c r="D6" s="3" t="s">
@@ -1659,14 +1688,14 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B7" t="s" s="0">
+      <c r="B7" t="s">
         <v>63</v>
       </c>
-      <c r="C7" t="s" s="0">
+      <c r="C7" t="s">
         <v>65</v>
       </c>
       <c r="D7" s="3" t="s">
@@ -1676,14 +1705,14 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B8" t="s" s="0">
+      <c r="B8" t="s">
         <v>63</v>
       </c>
-      <c r="C8" t="s" s="0">
+      <c r="C8" t="s">
         <v>65</v>
       </c>
       <c r="D8" s="3" t="s">
@@ -1693,14 +1722,14 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B9" t="s" s="0">
+      <c r="B9" t="s">
         <v>63</v>
       </c>
-      <c r="C9" t="s" s="0">
+      <c r="C9" t="s">
         <v>65</v>
       </c>
       <c r="D9" s="3" t="s">
@@ -1710,14 +1739,14 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B10" t="s" s="0">
+      <c r="B10" t="s">
         <v>63</v>
       </c>
-      <c r="C10" t="s" s="0">
+      <c r="C10" t="s">
         <v>65</v>
       </c>
       <c r="D10" s="3" t="s">
@@ -1727,14 +1756,14 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B11" t="s" s="0">
+      <c r="B11" t="s">
         <v>63</v>
       </c>
-      <c r="C11" t="s" s="0">
+      <c r="C11" t="s">
         <v>65</v>
       </c>
       <c r="D11" s="3" t="s">
@@ -1766,22 +1795,322 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.42578125" customWidth="1"/>
+    <col min="2" max="2" width="34.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.140625" customWidth="1"/>
+    <col min="4" max="4" width="22.7109375" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" customWidth="1"/>
+    <col min="6" max="6" width="21.42578125" customWidth="1"/>
+    <col min="7" max="7" width="21.140625" customWidth="1"/>
+    <col min="8" max="8" width="18.28515625" customWidth="1"/>
+    <col min="9" max="9" width="9.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="1"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" t="s">
+        <v>77</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" t="s">
+        <v>77</v>
+      </c>
+      <c r="G3" s="2"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" t="s">
+        <v>77</v>
+      </c>
+      <c r="G4" s="2"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>74</v>
+      </c>
+      <c r="C5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" t="s">
+        <v>77</v>
+      </c>
+      <c r="G5" s="2"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C6" t="s">
+        <v>75</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" t="s">
+        <v>77</v>
+      </c>
+      <c r="G6" s="2"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>74</v>
+      </c>
+      <c r="C7" t="s">
+        <v>75</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" t="s">
+        <v>77</v>
+      </c>
+      <c r="G7" s="2"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C8" t="s">
+        <v>75</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" t="s">
+        <v>77</v>
+      </c>
+      <c r="G8" s="2"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C9" t="s">
+        <v>75</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" t="s">
+        <v>77</v>
+      </c>
+      <c r="G9" s="2"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" t="s">
+        <v>74</v>
+      </c>
+      <c r="C10" t="s">
+        <v>75</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" t="s">
+        <v>77</v>
+      </c>
+      <c r="G10" s="2"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" t="s">
+        <v>74</v>
+      </c>
+      <c r="C11" t="s">
+        <v>75</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" t="s">
+        <v>77</v>
+      </c>
+      <c r="G11" s="2"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="D3:D11" r:id="rId2" display="aarosagarch@gmail.com"/>
+    <hyperlink ref="E2" r:id="rId3"/>
+    <hyperlink ref="E3" r:id="rId4"/>
+    <hyperlink ref="E4" r:id="rId5"/>
+    <hyperlink ref="E5" r:id="rId6"/>
+    <hyperlink ref="E6" r:id="rId7"/>
+    <hyperlink ref="E7" r:id="rId8"/>
+    <hyperlink ref="E8" r:id="rId9"/>
+    <hyperlink ref="E9" r:id="rId10"/>
+    <hyperlink ref="E10" r:id="rId11"/>
+    <hyperlink ref="E11" r:id="rId12"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="14.28515625"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="19.140625"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="10.140625"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="9.140625"/>
+    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Excel code is added to Edit Employee testcase
</commit_message>
<xml_diff>
--- a/src/main/resources/AutomationCatalogue_Batch41_TestData.xlsx
+++ b/src/main/resources/AutomationCatalogue_Batch41_TestData.xlsx
@@ -1,25 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AutomationCatalogue\Projects\TestAutomationCatalogue_Batch41\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Automation Catalogue\Projects\TestAutomationCatalogue_Batch41\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C637A15D-5345-4595-B479-4DB219908DC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{730DFE44-7FDD-4DD6-A342-FDD6C492BBB2}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="2" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="OrangeHRM_Login" sheetId="1" r:id="rId1"/>
     <sheet name="OrangeHRM_AddEmployee" sheetId="2" r:id="rId2"/>
     <sheet name="OrangeHRM_AddUser" sheetId="3" r:id="rId3"/>
     <sheet name="DemoWebshop_ReOrder" sheetId="4" r:id="rId4"/>
-    <sheet name="DemoWebshop_CreateAddress" sheetId="5" r:id="rId5"/>
+    <sheet name="OrangeHRM_EditEmployee" sheetId="6" r:id="rId5"/>
+    <sheet name="DemoWebshop_CreateAddress" sheetId="5" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="76">
   <si>
     <t>S. No</t>
   </si>
@@ -224,13 +224,46 @@
   </si>
   <si>
     <t>OrderNumber</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Date of Birth</t>
+  </si>
+  <si>
+    <t>Nationality</t>
+  </si>
+  <si>
+    <t>Allergies(Yes/No)</t>
+  </si>
+  <si>
+    <t>Naidu</t>
+  </si>
+  <si>
+    <t>Indian</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Dietary Requirements(1)</t>
+  </si>
+  <si>
+    <t>Dietary Requirements(2)</t>
+  </si>
+  <si>
+    <t>Koshler</t>
+  </si>
+  <si>
+    <t>Vegetarian</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -260,6 +293,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -281,7 +327,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -289,17 +335,56 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -614,22 +699,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F18C6FE-6D5B-4DA8-AB38-9D02E4FEBF53}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="26" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -646,7 +731,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -663,7 +748,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -680,7 +765,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -697,7 +782,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -714,7 +799,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -731,7 +816,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
@@ -748,7 +833,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
@@ -765,7 +850,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
@@ -782,7 +867,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
@@ -799,7 +884,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
@@ -818,37 +903,37 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{49644686-807E-4BDD-B3FC-AFC45775B9C8}"/>
-    <hyperlink ref="E3:E11" r:id="rId2" display="Admin@123" xr:uid="{3A88243C-5576-4973-BB74-92823AFD61E7}"/>
+    <hyperlink ref="E2" r:id="rId1"/>
+    <hyperlink ref="E3:E11" r:id="rId2" display="Admin@123"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{681D0824-3508-4439-9388-79D31E041950}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+      <selection sqref="A1:E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="30" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="38" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -892,7 +977,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -933,7 +1018,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -968,7 +1053,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -1003,7 +1088,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -1035,7 +1120,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -1055,7 +1140,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
@@ -1081,7 +1166,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
@@ -1101,7 +1186,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
@@ -1118,7 +1203,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
@@ -1135,7 +1220,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
@@ -1155,41 +1240,41 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{A2E61A8E-512C-4665-AAAD-DF0376542DCC}"/>
-    <hyperlink ref="E3" r:id="rId2" xr:uid="{09C4D3C9-2535-4875-8C96-3B33D195A97B}"/>
-    <hyperlink ref="E4" r:id="rId3" xr:uid="{A509F7A5-5D21-466A-A61C-405412914E86}"/>
-    <hyperlink ref="E5" r:id="rId4" xr:uid="{87E2B86A-BB58-486C-8001-0CC5DA699084}"/>
-    <hyperlink ref="E6" r:id="rId5" xr:uid="{6E56D7DF-1739-42B5-A97F-35AB81072A9F}"/>
-    <hyperlink ref="E7" r:id="rId6" xr:uid="{4695766B-1035-4F53-996B-E914F5B7FB17}"/>
-    <hyperlink ref="E8" r:id="rId7" xr:uid="{7060BCF3-1224-4CEC-BE25-5432A4CAFB60}"/>
-    <hyperlink ref="E9" r:id="rId8" xr:uid="{D5991558-DAA6-4C7B-AF29-B79105796867}"/>
-    <hyperlink ref="E10" r:id="rId9" xr:uid="{53F00551-3A35-4E23-9214-FFC981AE5516}"/>
-    <hyperlink ref="E11" r:id="rId10" xr:uid="{639C3CBD-8CFA-48D3-BFC2-0DC333029FD4}"/>
+    <hyperlink ref="E2" r:id="rId1"/>
+    <hyperlink ref="E3" r:id="rId2"/>
+    <hyperlink ref="E4" r:id="rId3"/>
+    <hyperlink ref="E5" r:id="rId4"/>
+    <hyperlink ref="E6" r:id="rId5"/>
+    <hyperlink ref="E7" r:id="rId6"/>
+    <hyperlink ref="E8" r:id="rId7"/>
+    <hyperlink ref="E9" r:id="rId8"/>
+    <hyperlink ref="E10" r:id="rId9"/>
+    <hyperlink ref="E11" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0039E566-26BE-41C7-B54C-07E46582CC6C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1218,52 +1303,52 @@
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
@@ -1275,23 +1360,23 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C32ADADF-6387-4766-ADFA-377853296F4F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="28" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" customWidth="1"/>
-    <col min="6" max="6" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1311,7 +1396,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -1319,7 +1404,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -1327,7 +1412,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -1335,7 +1420,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -1343,7 +1428,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -1351,7 +1436,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
@@ -1359,7 +1444,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
@@ -1367,7 +1452,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
@@ -1375,7 +1460,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
@@ -1383,7 +1468,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
@@ -1399,22 +1484,341 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D76F8C9-C1B2-447E-91D5-FE56BF995D20}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="5"/>
+    <col min="2" max="2" width="30.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.7109375" style="5" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="G2" s="12">
+        <v>32896</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="8"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E11" r:id="rId1"/>
+    <hyperlink ref="E10" r:id="rId2"/>
+    <hyperlink ref="E9" r:id="rId3"/>
+    <hyperlink ref="E8" r:id="rId4"/>
+    <hyperlink ref="E7" r:id="rId5"/>
+    <hyperlink ref="E6" r:id="rId6"/>
+    <hyperlink ref="E5" r:id="rId7"/>
+    <hyperlink ref="E4" r:id="rId8"/>
+    <hyperlink ref="E3" r:id="rId9"/>
+    <hyperlink ref="E2" r:id="rId10"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId11"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Changed the project path in edit employee
</commit_message>
<xml_diff>
--- a/src/main/resources/AutomationCatalogue_Batch41_TestData.xlsx
+++ b/src/main/resources/AutomationCatalogue_Batch41_TestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Automation Catalogue\Projects\TestAutomationCatalogue_Batch41\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="91">
   <si>
     <t>S. No</t>
   </si>
@@ -301,6 +301,9 @@
   </si>
   <si>
     <t>Vegetarian</t>
+  </si>
+  <si>
+    <t>23-January-1990</t>
   </si>
 </sst>
 </file>
@@ -432,10 +435,10 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2184,24 +2187,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="13"/>
-    <col min="2" max="2" width="30.85546875" style="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" style="13" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.5703125" style="13" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.85546875" style="13" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17" style="13" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.7109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.7109375" style="13" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="13"/>
+    <col min="1" max="1" width="9.140625" style="12"/>
+    <col min="2" max="2" width="30.85546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.85546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17" style="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.7109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.7109375" style="12" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="12"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -2239,7 +2242,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>5</v>
       </c>
@@ -2258,8 +2261,8 @@
       <c r="F2" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="G2" s="12">
-        <v>32896</v>
+      <c r="G2" s="13" t="s">
+        <v>90</v>
       </c>
       <c r="H2" s="10" t="s">
         <v>86</v>
@@ -2495,6 +2498,7 @@
     <hyperlink ref="E2" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId11"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Utility developments for Login, getTitle and select drop-down
</commit_message>
<xml_diff>
--- a/src/main/resources/AutomationCatalogue_Batch41_TestData.xlsx
+++ b/src/main/resources/AutomationCatalogue_Batch41_TestData.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AutomationCatalogue\Projects\TestAutomationCatalogue_Batch41\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75901A2E-F834-48E0-BC1D-75A4638AA28F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="4" activeTab="6"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="788" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OrangeHRM_Login" sheetId="1" r:id="rId1"/>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="91">
   <si>
     <t>S. No</t>
   </si>
@@ -243,18 +244,9 @@
     <t>TotalNumberOfOrders</t>
   </si>
   <si>
-    <t>Order number: 1481392</t>
-  </si>
-  <si>
-    <t>313</t>
-  </si>
-  <si>
     <t>SumOfAllOrders</t>
   </si>
   <si>
-    <t>47639.6</t>
-  </si>
-  <si>
     <t>TC18_DemoWebshop_ApplyDiscount</t>
   </si>
   <si>
@@ -267,9 +259,6 @@
     <t>AutomationDiscount2</t>
   </si>
   <si>
-    <t>Order number: 1482444</t>
-  </si>
-  <si>
     <t>Last Name</t>
   </si>
   <si>
@@ -301,12 +290,27 @@
   </si>
   <si>
     <t>Vegetarian</t>
+  </si>
+  <si>
+    <t>Order number: 1484075</t>
+  </si>
+  <si>
+    <t>320</t>
+  </si>
+  <si>
+    <t>48205.0</t>
+  </si>
+  <si>
+    <t>Order number: 1484077</t>
+  </si>
+  <si>
+    <t>23-January-1990</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -407,7 +411,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -420,7 +424,7 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
@@ -432,10 +436,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -499,7 +500,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -551,7 +552,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -752,22 +753,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="Q14" sqref="Q14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="26" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -784,7 +785,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -801,7 +802,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -818,7 +819,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -835,7 +836,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -852,7 +853,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -869,7 +870,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
@@ -886,7 +887,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
@@ -903,7 +904,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
@@ -920,7 +921,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
@@ -937,7 +938,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
@@ -956,37 +957,37 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1"/>
-    <hyperlink ref="E3:E11" r:id="rId2" display="Admin@123"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="E3:E11" r:id="rId2" display="Admin@123" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="30" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="38" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.44140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1030,7 +1031,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -1071,7 +1072,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -1106,7 +1107,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -1141,7 +1142,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -1173,7 +1174,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -1193,7 +1194,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
@@ -1219,7 +1220,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
@@ -1239,7 +1240,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
@@ -1256,7 +1257,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
@@ -1273,7 +1274,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
@@ -1293,41 +1294,41 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1"/>
-    <hyperlink ref="E3" r:id="rId2"/>
-    <hyperlink ref="E4" r:id="rId3"/>
-    <hyperlink ref="E5" r:id="rId4"/>
-    <hyperlink ref="E6" r:id="rId5"/>
-    <hyperlink ref="E7" r:id="rId6"/>
-    <hyperlink ref="E8" r:id="rId7"/>
-    <hyperlink ref="E9" r:id="rId8"/>
-    <hyperlink ref="E10" r:id="rId9"/>
-    <hyperlink ref="E11" r:id="rId10"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="E4" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="E5" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="E6" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
+    <hyperlink ref="E7" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
+    <hyperlink ref="E8" r:id="rId7" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
+    <hyperlink ref="E9" r:id="rId8" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
+    <hyperlink ref="E10" r:id="rId9" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
+    <hyperlink ref="E11" r:id="rId10" xr:uid="{00000000-0004-0000-0100-000009000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1356,52 +1357,52 @@
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
@@ -1413,24 +1414,24 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="41.140625" customWidth="1"/>
+    <col min="2" max="2" width="41.109375" customWidth="1"/>
     <col min="3" max="3" width="40" customWidth="1"/>
-    <col min="4" max="4" width="24.42578125" customWidth="1"/>
-    <col min="5" max="5" width="19.5703125" customWidth="1"/>
-    <col min="6" max="6" width="22.85546875" customWidth="1"/>
-    <col min="7" max="7" width="20.28515625" customWidth="1"/>
+    <col min="4" max="4" width="24.44140625" customWidth="1"/>
+    <col min="5" max="5" width="19.5546875" customWidth="1"/>
+    <col min="6" max="6" width="22.88671875" customWidth="1"/>
+    <col min="7" max="7" width="20.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1450,10 +1451,10 @@
         <v>69</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -1470,13 +1471,13 @@
         <v>18</v>
       </c>
       <c r="F2" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="G2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -1493,7 +1494,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -1510,7 +1511,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -1527,7 +1528,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -1544,7 +1545,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
@@ -1561,7 +1562,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
@@ -1578,7 +1579,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
@@ -1595,7 +1596,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
@@ -1612,7 +1613,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
@@ -1631,18 +1632,18 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-    <hyperlink ref="D3:D11" r:id="rId2" display="aarosagarch@gmail.com"/>
-    <hyperlink ref="E2" r:id="rId3"/>
-    <hyperlink ref="E3" r:id="rId4"/>
-    <hyperlink ref="E4" r:id="rId5"/>
-    <hyperlink ref="E5" r:id="rId6"/>
-    <hyperlink ref="E6" r:id="rId7"/>
-    <hyperlink ref="E7" r:id="rId8"/>
-    <hyperlink ref="E8" r:id="rId9"/>
-    <hyperlink ref="E9" r:id="rId10"/>
-    <hyperlink ref="E10" r:id="rId11"/>
-    <hyperlink ref="E11" r:id="rId12"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="D3:D11" r:id="rId2" display="aarosagarch@gmail.com" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
+    <hyperlink ref="E2" r:id="rId3" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
+    <hyperlink ref="E3" r:id="rId4" xr:uid="{00000000-0004-0000-0300-000003000000}"/>
+    <hyperlink ref="E4" r:id="rId5" xr:uid="{00000000-0004-0000-0300-000004000000}"/>
+    <hyperlink ref="E5" r:id="rId6" xr:uid="{00000000-0004-0000-0300-000005000000}"/>
+    <hyperlink ref="E6" r:id="rId7" xr:uid="{00000000-0004-0000-0300-000006000000}"/>
+    <hyperlink ref="E7" r:id="rId8" xr:uid="{00000000-0004-0000-0300-000007000000}"/>
+    <hyperlink ref="E8" r:id="rId9" xr:uid="{00000000-0004-0000-0300-000008000000}"/>
+    <hyperlink ref="E9" r:id="rId10" xr:uid="{00000000-0004-0000-0300-000009000000}"/>
+    <hyperlink ref="E10" r:id="rId11" xr:uid="{00000000-0004-0000-0300-00000A000000}"/>
+    <hyperlink ref="E11" r:id="rId12" xr:uid="{00000000-0004-0000-0300-00000B000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId13"/>
@@ -1650,23 +1651,23 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="28" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="34" customWidth="1"/>
     <col min="4" max="4" width="23" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" customWidth="1"/>
-    <col min="6" max="6" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" customWidth="1"/>
+    <col min="6" max="6" width="21.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1686,7 +1687,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -1703,10 +1704,10 @@
         <v>18</v>
       </c>
       <c r="F2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -1723,7 +1724,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -1740,7 +1741,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -1757,7 +1758,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -1774,7 +1775,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
@@ -1791,7 +1792,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
@@ -1808,7 +1809,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
@@ -1825,7 +1826,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
@@ -1842,7 +1843,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
@@ -1862,18 +1863,18 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-    <hyperlink ref="D3:D11" r:id="rId2" display="aarosagarch@gmail.com"/>
-    <hyperlink ref="E2" r:id="rId3"/>
-    <hyperlink ref="E3" r:id="rId4"/>
-    <hyperlink ref="E4" r:id="rId5"/>
-    <hyperlink ref="E5" r:id="rId6"/>
-    <hyperlink ref="E6" r:id="rId7"/>
-    <hyperlink ref="E7" r:id="rId8"/>
-    <hyperlink ref="E8" r:id="rId9"/>
-    <hyperlink ref="E9" r:id="rId10"/>
-    <hyperlink ref="E10" r:id="rId11"/>
-    <hyperlink ref="E11" r:id="rId12"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
+    <hyperlink ref="D3:D11" r:id="rId2" display="aarosagarch@gmail.com" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
+    <hyperlink ref="E2" r:id="rId3" xr:uid="{00000000-0004-0000-0400-000002000000}"/>
+    <hyperlink ref="E3" r:id="rId4" xr:uid="{00000000-0004-0000-0400-000003000000}"/>
+    <hyperlink ref="E4" r:id="rId5" xr:uid="{00000000-0004-0000-0400-000004000000}"/>
+    <hyperlink ref="E5" r:id="rId6" xr:uid="{00000000-0004-0000-0400-000005000000}"/>
+    <hyperlink ref="E6" r:id="rId7" xr:uid="{00000000-0004-0000-0400-000006000000}"/>
+    <hyperlink ref="E7" r:id="rId8" xr:uid="{00000000-0004-0000-0400-000007000000}"/>
+    <hyperlink ref="E8" r:id="rId9" xr:uid="{00000000-0004-0000-0400-000008000000}"/>
+    <hyperlink ref="E9" r:id="rId10" xr:uid="{00000000-0004-0000-0400-000009000000}"/>
+    <hyperlink ref="E10" r:id="rId11" xr:uid="{00000000-0004-0000-0400-00000A000000}"/>
+    <hyperlink ref="E11" r:id="rId12" xr:uid="{00000000-0004-0000-0400-00000B000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId13"/>
@@ -1881,27 +1882,27 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.42578125" customWidth="1"/>
-    <col min="2" max="2" width="34.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="40.140625" customWidth="1"/>
-    <col min="4" max="4" width="22.7109375" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" customWidth="1"/>
-    <col min="6" max="6" width="21.42578125" customWidth="1"/>
-    <col min="7" max="7" width="21.140625" customWidth="1"/>
-    <col min="8" max="8" width="18.28515625" customWidth="1"/>
-    <col min="9" max="9" width="9.28515625" customWidth="1"/>
+    <col min="1" max="1" width="6.44140625" customWidth="1"/>
+    <col min="2" max="2" width="34.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.109375" customWidth="1"/>
+    <col min="4" max="4" width="22.6640625" customWidth="1"/>
+    <col min="5" max="5" width="12.44140625" customWidth="1"/>
+    <col min="6" max="6" width="21.44140625" customWidth="1"/>
+    <col min="7" max="7" width="21.109375" customWidth="1"/>
+    <col min="8" max="8" width="18.33203125" customWidth="1"/>
+    <col min="9" max="9" width="9.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1918,7 +1919,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>64</v>
@@ -1928,233 +1929,233 @@
       <c r="J1" s="5"/>
       <c r="K1" s="1"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" t="s">
         <v>74</v>
       </c>
-      <c r="C2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F2" t="s">
-        <v>77</v>
-      </c>
       <c r="G2" s="2" t="s">
-        <v>78</v>
+        <v>89</v>
       </c>
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" t="s">
         <v>74</v>
-      </c>
-      <c r="C3" t="s">
-        <v>75</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" t="s">
-        <v>77</v>
       </c>
       <c r="G3" s="2"/>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" t="s">
         <v>74</v>
-      </c>
-      <c r="C4" t="s">
-        <v>75</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" t="s">
-        <v>77</v>
       </c>
       <c r="G4" s="2"/>
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C5" t="s">
+        <v>72</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" t="s">
         <v>74</v>
-      </c>
-      <c r="C5" t="s">
-        <v>75</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F5" t="s">
-        <v>77</v>
       </c>
       <c r="G5" s="2"/>
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C6" t="s">
+        <v>72</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" t="s">
         <v>74</v>
-      </c>
-      <c r="C6" t="s">
-        <v>75</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F6" t="s">
-        <v>77</v>
       </c>
       <c r="G6" s="2"/>
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C7" t="s">
+        <v>72</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" t="s">
         <v>74</v>
-      </c>
-      <c r="C7" t="s">
-        <v>75</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F7" t="s">
-        <v>77</v>
       </c>
       <c r="G7" s="2"/>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B8" t="s">
+        <v>71</v>
+      </c>
+      <c r="C8" t="s">
+        <v>72</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" t="s">
         <v>74</v>
-      </c>
-      <c r="C8" t="s">
-        <v>75</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F8" t="s">
-        <v>77</v>
       </c>
       <c r="G8" s="2"/>
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B9" t="s">
+        <v>71</v>
+      </c>
+      <c r="C9" t="s">
+        <v>72</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" t="s">
         <v>74</v>
-      </c>
-      <c r="C9" t="s">
-        <v>75</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F9" t="s">
-        <v>77</v>
       </c>
       <c r="G9" s="2"/>
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B10" t="s">
+        <v>71</v>
+      </c>
+      <c r="C10" t="s">
+        <v>72</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" t="s">
         <v>74</v>
-      </c>
-      <c r="C10" t="s">
-        <v>75</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F10" t="s">
-        <v>77</v>
       </c>
       <c r="G10" s="2"/>
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B11" t="s">
+        <v>71</v>
+      </c>
+      <c r="C11" t="s">
+        <v>72</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" t="s">
         <v>74</v>
-      </c>
-      <c r="C11" t="s">
-        <v>75</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F11" t="s">
-        <v>77</v>
       </c>
       <c r="G11" s="2"/>
       <c r="J11" s="3"/>
@@ -2162,18 +2163,18 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-    <hyperlink ref="D3:D11" r:id="rId2" display="aarosagarch@gmail.com"/>
-    <hyperlink ref="E2" r:id="rId3"/>
-    <hyperlink ref="E3" r:id="rId4"/>
-    <hyperlink ref="E4" r:id="rId5"/>
-    <hyperlink ref="E5" r:id="rId6"/>
-    <hyperlink ref="E6" r:id="rId7"/>
-    <hyperlink ref="E7" r:id="rId8"/>
-    <hyperlink ref="E8" r:id="rId9"/>
-    <hyperlink ref="E9" r:id="rId10"/>
-    <hyperlink ref="E10" r:id="rId11"/>
-    <hyperlink ref="E11" r:id="rId12"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
+    <hyperlink ref="D3:D11" r:id="rId2" display="aarosagarch@gmail.com" xr:uid="{00000000-0004-0000-0500-000001000000}"/>
+    <hyperlink ref="E2" r:id="rId3" xr:uid="{00000000-0004-0000-0500-000002000000}"/>
+    <hyperlink ref="E3" r:id="rId4" xr:uid="{00000000-0004-0000-0500-000003000000}"/>
+    <hyperlink ref="E4" r:id="rId5" xr:uid="{00000000-0004-0000-0500-000004000000}"/>
+    <hyperlink ref="E5" r:id="rId6" xr:uid="{00000000-0004-0000-0500-000005000000}"/>
+    <hyperlink ref="E6" r:id="rId7" xr:uid="{00000000-0004-0000-0500-000006000000}"/>
+    <hyperlink ref="E7" r:id="rId8" xr:uid="{00000000-0004-0000-0500-000007000000}"/>
+    <hyperlink ref="E8" r:id="rId9" xr:uid="{00000000-0004-0000-0500-000008000000}"/>
+    <hyperlink ref="E9" r:id="rId10" xr:uid="{00000000-0004-0000-0500-000009000000}"/>
+    <hyperlink ref="E10" r:id="rId11" xr:uid="{00000000-0004-0000-0500-00000A000000}"/>
+    <hyperlink ref="E11" r:id="rId12" xr:uid="{00000000-0004-0000-0500-00000B000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -2181,30 +2182,30 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="13"/>
-    <col min="2" max="2" width="30.85546875" style="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" style="13" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.5703125" style="13" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.85546875" style="13" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17" style="13" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.7109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.7109375" style="13" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="13"/>
+    <col min="1" max="1" width="9.109375" style="8"/>
+    <col min="2" max="2" width="30.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.44140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.5546875" style="8" customWidth="1"/>
+    <col min="8" max="8" width="10.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17" style="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.6640625" style="8" customWidth="1"/>
+    <col min="12" max="16384" width="9.109375" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -2221,25 +2222,25 @@
         <v>4</v>
       </c>
       <c r="F1" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="J1" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="K1" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="H1" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>5</v>
       </c>
@@ -2256,25 +2257,25 @@
         <v>18</v>
       </c>
       <c r="F2" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="I2" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="J2" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="K2" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="G2" s="12">
-        <v>32896</v>
-      </c>
-      <c r="H2" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="I2" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="J2" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="K2" s="10" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
         <v>6</v>
       </c>
@@ -2297,7 +2298,7 @@
       <c r="J3" s="10"/>
       <c r="K3" s="10"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
         <v>7</v>
       </c>
@@ -2320,7 +2321,7 @@
       <c r="J4" s="10"/>
       <c r="K4" s="10"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
         <v>8</v>
       </c>
@@ -2343,7 +2344,7 @@
       <c r="J5" s="10"/>
       <c r="K5" s="10"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
         <v>9</v>
       </c>
@@ -2366,7 +2367,7 @@
       <c r="J6" s="10"/>
       <c r="K6" s="10"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
         <v>10</v>
       </c>
@@ -2389,7 +2390,7 @@
       <c r="J7" s="10"/>
       <c r="K7" s="10"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
         <v>11</v>
       </c>
@@ -2412,7 +2413,7 @@
       <c r="J8" s="10"/>
       <c r="K8" s="10"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
         <v>12</v>
       </c>
@@ -2435,7 +2436,7 @@
       <c r="J9" s="10"/>
       <c r="K9" s="10"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
         <v>13</v>
       </c>
@@ -2458,7 +2459,7 @@
       <c r="J10" s="10"/>
       <c r="K10" s="10"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
         <v>14</v>
       </c>
@@ -2483,38 +2484,38 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E11" r:id="rId1"/>
-    <hyperlink ref="E10" r:id="rId2"/>
-    <hyperlink ref="E9" r:id="rId3"/>
-    <hyperlink ref="E8" r:id="rId4"/>
-    <hyperlink ref="E7" r:id="rId5"/>
-    <hyperlink ref="E6" r:id="rId6"/>
-    <hyperlink ref="E5" r:id="rId7"/>
-    <hyperlink ref="E4" r:id="rId8"/>
-    <hyperlink ref="E3" r:id="rId9"/>
-    <hyperlink ref="E2" r:id="rId10"/>
+    <hyperlink ref="E11" r:id="rId1" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
+    <hyperlink ref="E10" r:id="rId2" xr:uid="{00000000-0004-0000-0600-000001000000}"/>
+    <hyperlink ref="E9" r:id="rId3" xr:uid="{00000000-0004-0000-0600-000002000000}"/>
+    <hyperlink ref="E8" r:id="rId4" xr:uid="{00000000-0004-0000-0600-000003000000}"/>
+    <hyperlink ref="E7" r:id="rId5" xr:uid="{00000000-0004-0000-0600-000004000000}"/>
+    <hyperlink ref="E6" r:id="rId6" xr:uid="{00000000-0004-0000-0600-000005000000}"/>
+    <hyperlink ref="E5" r:id="rId7" xr:uid="{00000000-0004-0000-0600-000006000000}"/>
+    <hyperlink ref="E4" r:id="rId8" xr:uid="{00000000-0004-0000-0600-000007000000}"/>
+    <hyperlink ref="E3" r:id="rId9" xr:uid="{00000000-0004-0000-0600-000008000000}"/>
+    <hyperlink ref="E2" r:id="rId10" xr:uid="{00000000-0004-0000-0600-000009000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
changes done in update shopping cart orange hrm goals
</commit_message>
<xml_diff>
--- a/src/main/resources/AutomationCatalogue_Batch41_TestData.xlsx
+++ b/src/main/resources/AutomationCatalogue_Batch41_TestData.xlsx
@@ -9,17 +9,18 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="4" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="706" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="OrangeHRM_Login" sheetId="1" r:id="rId1"/>
-    <sheet name="OrangeHRM_AddEmployee" sheetId="2" r:id="rId2"/>
-    <sheet name="OrangeHRM_AddUser" sheetId="3" r:id="rId3"/>
-    <sheet name="DemoWebshop_TotalOrders" sheetId="6" r:id="rId4"/>
-    <sheet name="DemoWebshop_ReOrder" sheetId="4" r:id="rId5"/>
-    <sheet name="DemoWebshop_ApplyDiscount" sheetId="7" r:id="rId6"/>
-    <sheet name="OrangeHRM_EditEmployee" sheetId="8" r:id="rId7"/>
-    <sheet name="DemoWebshop_CreateAddress" sheetId="5" r:id="rId8"/>
+    <sheet name="DemoWebshop_UpdateShoppingCart" sheetId="9" r:id="rId2"/>
+    <sheet name="OrangeHRM_AddEmployee" sheetId="2" r:id="rId3"/>
+    <sheet name="OrangeHRM_AddUser" sheetId="3" r:id="rId4"/>
+    <sheet name="DemoWebshop_TotalOrders" sheetId="6" r:id="rId5"/>
+    <sheet name="DemoWebshop_ReOrder" sheetId="4" r:id="rId6"/>
+    <sheet name="DemoWebshop_ApplyDiscount" sheetId="7" r:id="rId7"/>
+    <sheet name="OrangeHRM_EditEmployee" sheetId="8" r:id="rId8"/>
+    <sheet name="DemoWebshop_CreateAddress" sheetId="5" r:id="rId9"/>
   </sheets>
   <calcPr calcId="124519"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="103">
   <si>
     <t>S. No</t>
   </si>
@@ -304,13 +305,49 @@
   </si>
   <si>
     <t>23-January-1990</t>
+  </si>
+  <si>
+    <t>TC02_OrangeHRM_EditEmployee</t>
+  </si>
+  <si>
+    <t>OrangeHRM Application Editing Employee</t>
+  </si>
+  <si>
+    <t>S.No</t>
+  </si>
+  <si>
+    <t>Test case name</t>
+  </si>
+  <si>
+    <t>Test case description</t>
+  </si>
+  <si>
+    <t>TC17_DemoWebshop_UpdateShoppingCart</t>
+  </si>
+  <si>
+    <t>Updating shopping cart</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Length in Cm(Jewel)</t>
+  </si>
+  <si>
+    <t>Update Quantity</t>
+  </si>
+  <si>
+    <t>Order Number</t>
+  </si>
+  <si>
+    <t>null</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -361,6 +398,11 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -410,7 +452,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -440,6 +482,9 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -758,8 +803,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -967,6 +1012,182 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="41.85546875" customWidth="1"/>
+    <col min="3" max="3" width="34.28515625" customWidth="1"/>
+    <col min="4" max="4" width="22.5703125" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" customWidth="1"/>
+    <col min="6" max="6" width="23" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>96</v>
+      </c>
+      <c r="C6" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C7" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" t="s">
+        <v>96</v>
+      </c>
+      <c r="C8" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
+        <v>96</v>
+      </c>
+      <c r="C9" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" t="s">
+        <v>96</v>
+      </c>
+      <c r="C10" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" t="s">
+        <v>96</v>
+      </c>
+      <c r="C11" t="s">
+        <v>97</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N11"/>
   <sheetViews>
@@ -1311,7 +1532,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I11"/>
   <sheetViews>
@@ -1415,13 +1636,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1652,7 +1871,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F11"/>
   <sheetViews>
@@ -1883,7 +2102,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K11"/>
   <sheetViews>
@@ -2183,12 +2402,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2247,10 +2466,10 @@
         <v>5</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>37</v>
+        <v>91</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>38</v>
+        <v>92</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>17</v>
@@ -2282,10 +2501,10 @@
         <v>6</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>37</v>
+        <v>91</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>38</v>
+        <v>92</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>17</v>
@@ -2305,10 +2524,10 @@
         <v>7</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>37</v>
+        <v>91</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>38</v>
+        <v>92</v>
       </c>
       <c r="D4" s="10" t="s">
         <v>17</v>
@@ -2328,10 +2547,10 @@
         <v>8</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>37</v>
+        <v>91</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>38</v>
+        <v>92</v>
       </c>
       <c r="D5" s="10" t="s">
         <v>17</v>
@@ -2351,10 +2570,10 @@
         <v>9</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>37</v>
+        <v>91</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>38</v>
+        <v>92</v>
       </c>
       <c r="D6" s="10" t="s">
         <v>17</v>
@@ -2374,10 +2593,10 @@
         <v>10</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>37</v>
+        <v>91</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>38</v>
+        <v>92</v>
       </c>
       <c r="D7" s="10" t="s">
         <v>17</v>
@@ -2397,10 +2616,10 @@
         <v>11</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>37</v>
+        <v>91</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>38</v>
+        <v>92</v>
       </c>
       <c r="D8" s="10" t="s">
         <v>17</v>
@@ -2420,10 +2639,10 @@
         <v>12</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>37</v>
+        <v>91</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>38</v>
+        <v>92</v>
       </c>
       <c r="D9" s="10" t="s">
         <v>17</v>
@@ -2443,10 +2662,10 @@
         <v>13</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>37</v>
+        <v>91</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>38</v>
+        <v>92</v>
       </c>
       <c r="D10" s="10" t="s">
         <v>17</v>
@@ -2466,10 +2685,10 @@
         <v>14</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>37</v>
+        <v>91</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>38</v>
+        <v>92</v>
       </c>
       <c r="D11" s="10" t="s">
         <v>17</v>
@@ -2502,7 +2721,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E1"/>
   <sheetViews>

</xml_diff>

<commit_message>
Excel changes are added in add user testcase
</commit_message>
<xml_diff>
--- a/src/main/resources/AutomationCatalogue_Batch41_TestData.xlsx
+++ b/src/main/resources/AutomationCatalogue_Batch41_TestData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AutomationCatalogue\Projects\TestAutomationCatalogue_Batch41\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AutomationCatalogue\TestAutomationCatalogue_Batch41\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75901A2E-F834-48E0-BC1D-75A4638AA28F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26743185-4F26-41F9-8DB4-DAEEB1914346}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="788" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4360" yWindow="440" windowWidth="14840" windowHeight="9640" tabRatio="788" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OrangeHRM_Login" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="104">
   <si>
     <t>S. No</t>
   </si>
@@ -305,6 +305,45 @@
   </si>
   <si>
     <t>23-January-1990</t>
+  </si>
+  <si>
+    <t>TC03_OrangeHRM_AddUser</t>
+  </si>
+  <si>
+    <t>Orange HRM adding user</t>
+  </si>
+  <si>
+    <t>Admin@124</t>
+  </si>
+  <si>
+    <t>Admin@125</t>
+  </si>
+  <si>
+    <t>Admin@126</t>
+  </si>
+  <si>
+    <t>Admin@127</t>
+  </si>
+  <si>
+    <t>Admin@128</t>
+  </si>
+  <si>
+    <t>Admin@129</t>
+  </si>
+  <si>
+    <t>Admin@130</t>
+  </si>
+  <si>
+    <t>Admin@131</t>
+  </si>
+  <si>
+    <t>Admin@132</t>
+  </si>
+  <si>
+    <t>Charlie Carter</t>
+  </si>
+  <si>
+    <t>CharlieABCDEF</t>
   </si>
 </sst>
 </file>
@@ -760,15 +799,15 @@
       <selection activeCell="Q14" sqref="Q14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="26" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.6328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -785,7 +824,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -802,7 +841,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -819,7 +858,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -836,7 +875,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -853,7 +892,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -870,7 +909,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
@@ -887,7 +926,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
@@ -904,7 +943,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
@@ -921,7 +960,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
@@ -938,7 +977,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
@@ -968,26 +1007,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="30" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="38" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.90625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.453125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.6328125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.90625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1031,7 +1070,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -1072,7 +1111,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -1107,7 +1146,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -1142,7 +1181,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -1174,7 +1213,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -1194,7 +1233,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
@@ -1220,7 +1259,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
@@ -1240,7 +1279,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
@@ -1257,7 +1296,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
@@ -1274,7 +1313,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
@@ -1313,22 +1352,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35" customWidth="1"/>
+    <col min="3" max="3" width="24.7265625" customWidth="1"/>
+    <col min="4" max="4" width="20.7265625" customWidth="1"/>
+    <col min="5" max="5" width="18.54296875" customWidth="1"/>
+    <col min="6" max="6" width="14.90625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.90625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.453125" customWidth="1"/>
+    <col min="9" max="9" width="16.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1357,58 +1397,196 @@
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" t="s">
+        <v>102</v>
+      </c>
+      <c r="G2" t="s">
+        <v>103</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>91</v>
+      </c>
+      <c r="C6" t="s">
+        <v>92</v>
+      </c>
+      <c r="D6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>91</v>
+      </c>
+      <c r="C7" t="s">
+        <v>92</v>
+      </c>
+      <c r="D7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>91</v>
+      </c>
+      <c r="C8" t="s">
+        <v>92</v>
+      </c>
+      <c r="D8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>91</v>
+      </c>
+      <c r="C9" t="s">
+        <v>92</v>
+      </c>
+      <c r="D9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>91</v>
+      </c>
+      <c r="C10" t="s">
+        <v>92</v>
+      </c>
+      <c r="D10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="B11" t="s">
+        <v>91</v>
+      </c>
+      <c r="C11" t="s">
+        <v>92</v>
+      </c>
+      <c r="D11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>101</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{D49D57C7-FC03-4E36-8833-34E76B2D9A99}"/>
+    <hyperlink ref="E3:E11" r:id="rId2" display="Admin@123" xr:uid="{FA95088A-5EAC-46EC-8432-5E533B5B72A7}"/>
+    <hyperlink ref="H2" r:id="rId3" xr:uid="{D138E50B-48D8-4C71-A733-4964EE616AED}"/>
+    <hyperlink ref="I2" r:id="rId4" xr:uid="{9EC16FD4-8165-42E1-BFC4-1CEF48243A31}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1421,17 +1599,17 @@
       <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="41.109375" customWidth="1"/>
+    <col min="2" max="2" width="41.08984375" customWidth="1"/>
     <col min="3" max="3" width="40" customWidth="1"/>
-    <col min="4" max="4" width="24.44140625" customWidth="1"/>
-    <col min="5" max="5" width="19.5546875" customWidth="1"/>
-    <col min="6" max="6" width="22.88671875" customWidth="1"/>
-    <col min="7" max="7" width="20.33203125" customWidth="1"/>
+    <col min="4" max="4" width="24.453125" customWidth="1"/>
+    <col min="5" max="5" width="19.54296875" customWidth="1"/>
+    <col min="6" max="6" width="22.90625" customWidth="1"/>
+    <col min="7" max="7" width="20.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1454,7 +1632,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -1477,7 +1655,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -1494,7 +1672,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -1511,7 +1689,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -1528,7 +1706,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -1545,7 +1723,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
@@ -1562,7 +1740,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
@@ -1579,7 +1757,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
@@ -1596,7 +1774,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
@@ -1613,7 +1791,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
@@ -1658,16 +1836,16 @@
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="28" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="34" customWidth="1"/>
     <col min="4" max="4" width="23" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" customWidth="1"/>
-    <col min="6" max="6" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.36328125" customWidth="1"/>
+    <col min="6" max="6" width="21.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1687,7 +1865,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -1707,7 +1885,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -1724,7 +1902,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -1741,7 +1919,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -1758,7 +1936,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -1775,7 +1953,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
@@ -1792,7 +1970,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
@@ -1809,7 +1987,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
@@ -1826,7 +2004,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
@@ -1843,7 +2021,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
@@ -1889,20 +2067,20 @@
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="6.44140625" customWidth="1"/>
-    <col min="2" max="2" width="34.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="40.109375" customWidth="1"/>
-    <col min="4" max="4" width="22.6640625" customWidth="1"/>
-    <col min="5" max="5" width="12.44140625" customWidth="1"/>
-    <col min="6" max="6" width="21.44140625" customWidth="1"/>
-    <col min="7" max="7" width="21.109375" customWidth="1"/>
-    <col min="8" max="8" width="18.33203125" customWidth="1"/>
-    <col min="9" max="9" width="9.33203125" customWidth="1"/>
+    <col min="1" max="1" width="6.453125" customWidth="1"/>
+    <col min="2" max="2" width="34.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.08984375" customWidth="1"/>
+    <col min="4" max="4" width="22.6328125" customWidth="1"/>
+    <col min="5" max="5" width="12.453125" customWidth="1"/>
+    <col min="6" max="6" width="21.453125" customWidth="1"/>
+    <col min="7" max="7" width="21.08984375" customWidth="1"/>
+    <col min="8" max="8" width="18.36328125" customWidth="1"/>
+    <col min="9" max="9" width="9.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1929,7 +2107,7 @@
       <c r="J1" s="5"/>
       <c r="K1" s="1"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -1954,7 +2132,7 @@
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -1977,7 +2155,7 @@
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -2000,7 +2178,7 @@
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -2023,7 +2201,7 @@
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -2046,7 +2224,7 @@
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
@@ -2069,7 +2247,7 @@
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
@@ -2092,7 +2270,7 @@
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
@@ -2115,7 +2293,7 @@
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
@@ -2138,7 +2316,7 @@
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
@@ -2185,27 +2363,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="8"/>
-    <col min="2" max="2" width="30.88671875" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39.109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.44140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.5546875" style="8" customWidth="1"/>
-    <col min="8" max="8" width="10.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.08984375" style="8"/>
+    <col min="2" max="2" width="30.90625" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.08984375" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.453125" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.6328125" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.08984375" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.54296875" style="8" customWidth="1"/>
+    <col min="8" max="8" width="10.90625" style="8" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17" style="8" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.6640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.6640625" style="8" customWidth="1"/>
-    <col min="12" max="16384" width="9.109375" style="8"/>
+    <col min="10" max="10" width="20.6328125" style="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.6328125" style="8" customWidth="1"/>
+    <col min="12" max="16384" width="9.08984375" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -2240,7 +2418,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="9" t="s">
         <v>5</v>
       </c>
@@ -2275,7 +2453,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
         <v>6</v>
       </c>
@@ -2298,7 +2476,7 @@
       <c r="J3" s="10"/>
       <c r="K3" s="10"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="9" t="s">
         <v>7</v>
       </c>
@@ -2321,7 +2499,7 @@
       <c r="J4" s="10"/>
       <c r="K4" s="10"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="9" t="s">
         <v>8</v>
       </c>
@@ -2344,7 +2522,7 @@
       <c r="J5" s="10"/>
       <c r="K5" s="10"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="9" t="s">
         <v>9</v>
       </c>
@@ -2367,7 +2545,7 @@
       <c r="J6" s="10"/>
       <c r="K6" s="10"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="9" t="s">
         <v>10</v>
       </c>
@@ -2390,7 +2568,7 @@
       <c r="J7" s="10"/>
       <c r="K7" s="10"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="9" t="s">
         <v>11</v>
       </c>
@@ -2413,7 +2591,7 @@
       <c r="J8" s="10"/>
       <c r="K8" s="10"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="9" t="s">
         <v>12</v>
       </c>
@@ -2436,7 +2614,7 @@
       <c r="J9" s="10"/>
       <c r="K9" s="10"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" s="9" t="s">
         <v>13</v>
       </c>
@@ -2459,7 +2637,7 @@
       <c r="J10" s="10"/>
       <c r="K10" s="10"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" s="9" t="s">
         <v>14</v>
       </c>
@@ -2507,15 +2685,15 @@
       <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Excel Utils are added and testcases are adjusted
</commit_message>
<xml_diff>
--- a/src/main/resources/AutomationCatalogue_Batch41_TestData.xlsx
+++ b/src/main/resources/AutomationCatalogue_Batch41_TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AutomationCatalogue\Projects\TestAutomationCatalogue_Batch41\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{339C1403-EB4E-4969-823E-EFDDC38155BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C528329F-3D91-4B45-8906-A045527BA0FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="944" firstSheet="2" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="944" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="10" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1156" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1160" uniqueCount="351">
   <si>
     <t>S. No</t>
   </si>
@@ -1081,6 +1081,12 @@
   </si>
   <si>
     <t>110</t>
+  </si>
+  <si>
+    <t>Anjaneyulu</t>
+  </si>
+  <si>
+    <t>anjanyulu</t>
   </si>
 </sst>
 </file>
@@ -1552,7 +1558,7 @@
   <dimension ref="A1:F122"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K118" sqref="K118"/>
+      <selection activeCell="B76" sqref="B76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3245,7 +3251,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
@@ -3581,7 +3587,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3827,8 +3833,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:O11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L29" sqref="L29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -4228,7 +4234,7 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -4240,6 +4246,7 @@
     <col min="6" max="6" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.77734375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4476,6 +4483,18 @@
         <v>17</v>
       </c>
       <c r="F10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" t="s">
+        <v>349</v>
+      </c>
+      <c r="H10" t="s">
+        <v>350</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J10" s="3" t="s">
         <v>18</v>
       </c>
     </row>
@@ -4508,6 +4527,8 @@
     <hyperlink ref="F3:F11" r:id="rId4" display="Admin@123" xr:uid="{3CAF8F96-E222-4F94-8A70-9C685341A998}"/>
     <hyperlink ref="I5" r:id="rId5" xr:uid="{7EF764BC-844B-47F7-A73F-C9D41C057AD3}"/>
     <hyperlink ref="J5" r:id="rId6" xr:uid="{0611619D-9970-4F64-A28C-D8BAC5BF4492}"/>
+    <hyperlink ref="I10" r:id="rId7" xr:uid="{552B24E7-9F5D-4166-8001-7B76A5A7756F}"/>
+    <hyperlink ref="J10" r:id="rId8" xr:uid="{36C8351A-57C7-498A-9EC5-851023D83150}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4518,7 +4539,7 @@
   <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+      <selection activeCell="G8" sqref="G8:L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="14.4"/>
@@ -4875,7 +4896,7 @@
   <dimension ref="A1:P11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:P2"/>
+      <selection activeCell="G2" sqref="G2:P11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -5173,7 +5194,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="G3" sqref="G3:G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>

</xml_diff>

<commit_message>
completed OrangeHRM goals TC and updated pages
</commit_message>
<xml_diff>
--- a/src/main/resources/AutomationCatalogue_Batch41_TestData.xlsx
+++ b/src/main/resources/AutomationCatalogue_Batch41_TestData.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sarika\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Automation Catalogue\Projects\TestAutomationCatalogue_Batch41\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{525B0CCC-9136-4093-8E47-EA9412C25566}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="706" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10305" tabRatio="706" firstSheet="6" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="OrangeHRM_Login" sheetId="1" r:id="rId1"/>
@@ -22,6 +21,7 @@
     <sheet name="DemoWebshop_ApplyDiscount" sheetId="7" r:id="rId7"/>
     <sheet name="OrangeHRM_EditEmployee" sheetId="8" r:id="rId8"/>
     <sheet name="DemoWebshop_CreateAddress" sheetId="5" r:id="rId9"/>
+    <sheet name="OrangeHRM_Goals" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="124519"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="123">
   <si>
     <t>S. No</t>
   </si>
@@ -350,17 +350,65 @@
     <t>Orange HRM adding user</t>
   </si>
   <si>
-    <t>Charlie Carter</t>
-  </si>
-  <si>
     <t>CharlieABCDEF</t>
+  </si>
+  <si>
+    <t>Charlie Car</t>
+  </si>
+  <si>
+    <t>Employee Name</t>
+  </si>
+  <si>
+    <t>TC20_orangeHRM_Goals</t>
+  </si>
+  <si>
+    <t>Adding and updating the goals</t>
+  </si>
+  <si>
+    <t>Aaliyah Haq</t>
+  </si>
+  <si>
+    <t>First Goal Date</t>
+  </si>
+  <si>
+    <t>Second Goal Date</t>
+  </si>
+  <si>
+    <t>Third Goal Date</t>
+  </si>
+  <si>
+    <t>23-September-2023</t>
+  </si>
+  <si>
+    <t>First Goal Priority</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>Second Goal Priority</t>
+  </si>
+  <si>
+    <t>Third Goal Priority</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>28-January-2024</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>12-March-2024</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -465,7 +513,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -496,6 +544,31 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="7" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -810,22 +883,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView topLeftCell="A11" workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="26" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -842,7 +915,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -859,7 +932,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -876,7 +949,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -893,7 +966,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -910,7 +983,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -927,7 +1000,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
@@ -944,7 +1017,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
@@ -961,7 +1034,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
@@ -978,7 +1051,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
@@ -995,7 +1068,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
@@ -1014,33 +1087,395 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="E3:E11" r:id="rId2" display="Admin@123" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="E2" r:id="rId1"/>
+    <hyperlink ref="E3:E11" r:id="rId2" display="Admin@123"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="32" customWidth="1"/>
+    <col min="3" max="3" width="47.28515625" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" customWidth="1"/>
+    <col min="7" max="7" width="16.140625" customWidth="1"/>
+    <col min="8" max="8" width="20.28515625" customWidth="1"/>
+    <col min="9" max="9" width="19.28515625" customWidth="1"/>
+    <col min="10" max="10" width="16.5703125" customWidth="1"/>
+    <col min="11" max="11" width="16.85546875" customWidth="1"/>
+    <col min="12" max="12" width="15.140625" customWidth="1"/>
+    <col min="13" max="13" width="15" customWidth="1"/>
+    <col min="14" max="14" width="18.5703125" customWidth="1"/>
+    <col min="15" max="15" width="17.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
+    </row>
+    <row r="2" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="G2" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="H2" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="I2" s="19" t="s">
+        <v>119</v>
+      </c>
+      <c r="J2" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="K2" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="L2" s="21" t="s">
+        <v>122</v>
+      </c>
+      <c r="M2" s="22"/>
+      <c r="N2" s="22"/>
+      <c r="O2" s="22"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="22"/>
+      <c r="I3" s="22"/>
+      <c r="J3" s="22"/>
+      <c r="K3" s="22"/>
+      <c r="L3" s="22"/>
+      <c r="M3" s="22"/>
+      <c r="N3" s="22"/>
+      <c r="O3" s="22"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="22"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="22"/>
+      <c r="I4" s="22"/>
+      <c r="J4" s="22"/>
+      <c r="K4" s="22"/>
+      <c r="L4" s="22"/>
+      <c r="M4" s="22"/>
+      <c r="N4" s="22"/>
+      <c r="O4" s="22"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="22"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="22"/>
+      <c r="I5" s="22"/>
+      <c r="J5" s="22"/>
+      <c r="K5" s="22"/>
+      <c r="L5" s="22"/>
+      <c r="M5" s="22"/>
+      <c r="N5" s="22"/>
+      <c r="O5" s="22"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="22"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="22"/>
+      <c r="I6" s="22"/>
+      <c r="J6" s="22"/>
+      <c r="K6" s="22"/>
+      <c r="L6" s="22"/>
+      <c r="M6" s="22"/>
+      <c r="N6" s="22"/>
+      <c r="O6" s="22"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" s="22"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="22"/>
+      <c r="I7" s="22"/>
+      <c r="J7" s="22"/>
+      <c r="K7" s="22"/>
+      <c r="L7" s="22"/>
+      <c r="M7" s="22"/>
+      <c r="N7" s="22"/>
+      <c r="O7" s="22"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="22"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="22"/>
+      <c r="I8" s="22"/>
+      <c r="J8" s="22"/>
+      <c r="K8" s="22"/>
+      <c r="L8" s="22"/>
+      <c r="M8" s="22"/>
+      <c r="N8" s="22"/>
+      <c r="O8" s="22"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="22"/>
+      <c r="J9" s="22"/>
+      <c r="K9" s="22"/>
+      <c r="L9" s="22"/>
+      <c r="M9" s="22"/>
+      <c r="N9" s="22"/>
+      <c r="O9" s="22"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
+      <c r="I10" s="22"/>
+      <c r="J10" s="22"/>
+      <c r="K10" s="22"/>
+      <c r="L10" s="22"/>
+      <c r="M10" s="22"/>
+      <c r="N10" s="22"/>
+      <c r="O10" s="22"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" s="22"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="22"/>
+      <c r="J11" s="22"/>
+      <c r="K11" s="22"/>
+      <c r="L11" s="22"/>
+      <c r="M11" s="22"/>
+      <c r="N11" s="22"/>
+      <c r="O11" s="22"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1"/>
+    <hyperlink ref="E3" r:id="rId2"/>
+    <hyperlink ref="E4:E11" r:id="rId3" display="Admin@123"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="41.81640625" customWidth="1"/>
-    <col min="3" max="3" width="34.26953125" customWidth="1"/>
-    <col min="4" max="4" width="22.54296875" customWidth="1"/>
-    <col min="5" max="5" width="11.26953125" customWidth="1"/>
+    <col min="2" max="2" width="41.85546875" customWidth="1"/>
+    <col min="3" max="3" width="34.28515625" customWidth="1"/>
+    <col min="4" max="4" width="22.5703125" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" customWidth="1"/>
     <col min="6" max="6" width="23" customWidth="1"/>
-    <col min="7" max="7" width="15.7265625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.7265625" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>93</v>
       </c>
@@ -1066,7 +1501,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -1092,7 +1527,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -1103,7 +1538,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -1114,7 +1549,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -1125,7 +1560,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -1136,7 +1571,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
@@ -1147,7 +1582,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
@@ -1158,7 +1593,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
@@ -1169,7 +1604,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
@@ -1180,7 +1615,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
@@ -1198,29 +1633,29 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="30" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="38" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.26953125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.81640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1264,7 +1699,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -1305,7 +1740,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -1340,7 +1775,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -1375,7 +1810,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -1407,7 +1842,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -1427,7 +1862,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
@@ -1453,7 +1888,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
@@ -1473,7 +1908,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
@@ -1490,7 +1925,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
@@ -1507,7 +1942,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
@@ -1527,41 +1962,41 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
-    <hyperlink ref="E3" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
-    <hyperlink ref="E4" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
-    <hyperlink ref="E5" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
-    <hyperlink ref="E6" r:id="rId5" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
-    <hyperlink ref="E7" r:id="rId6" xr:uid="{00000000-0004-0000-0200-000005000000}"/>
-    <hyperlink ref="E8" r:id="rId7" xr:uid="{00000000-0004-0000-0200-000006000000}"/>
-    <hyperlink ref="E9" r:id="rId8" xr:uid="{00000000-0004-0000-0200-000007000000}"/>
-    <hyperlink ref="E10" r:id="rId9" xr:uid="{00000000-0004-0000-0200-000008000000}"/>
-    <hyperlink ref="E11" r:id="rId10" xr:uid="{00000000-0004-0000-0200-000009000000}"/>
+    <hyperlink ref="E2" r:id="rId1"/>
+    <hyperlink ref="E3" r:id="rId2"/>
+    <hyperlink ref="E4" r:id="rId3"/>
+    <hyperlink ref="E5" r:id="rId4"/>
+    <hyperlink ref="E6" r:id="rId5"/>
+    <hyperlink ref="E7" r:id="rId6"/>
+    <hyperlink ref="E8" r:id="rId7"/>
+    <hyperlink ref="E9" r:id="rId8"/>
+    <hyperlink ref="E10" r:id="rId9"/>
+    <hyperlink ref="E11" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.81640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1590,7 +2025,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -1607,11 +2042,11 @@
         <v>18</v>
       </c>
       <c r="F2" t="s">
+        <v>106</v>
+      </c>
+      <c r="G2" t="s">
         <v>105</v>
       </c>
-      <c r="G2" t="s">
-        <v>106</v>
-      </c>
       <c r="H2" s="3" t="s">
         <v>18</v>
       </c>
@@ -1619,7 +2054,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -1636,7 +2071,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -1653,7 +2088,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -1670,7 +2105,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -1687,7 +2122,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
@@ -1704,7 +2139,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
@@ -1721,7 +2156,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
@@ -1738,7 +2173,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
@@ -1755,7 +2190,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
@@ -1775,32 +2210,32 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{A86743D9-EA7F-423D-BAA6-68A740AC3D80}"/>
-    <hyperlink ref="H2" r:id="rId2" xr:uid="{E7CFB2BD-C6BE-44EB-AE4C-FA39C50580F1}"/>
-    <hyperlink ref="I2" r:id="rId3" xr:uid="{717D2B13-45AD-48C1-A07A-146CDADB5D82}"/>
-    <hyperlink ref="E3:E11" r:id="rId4" display="Admin@123" xr:uid="{3CAF8F96-E222-4F94-8A70-9C685341A998}"/>
+    <hyperlink ref="E2" r:id="rId1"/>
+    <hyperlink ref="H2" r:id="rId2"/>
+    <hyperlink ref="I2" r:id="rId3"/>
+    <hyperlink ref="E3:E11" r:id="rId4" display="Admin@123"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="41.1796875" customWidth="1"/>
+    <col min="2" max="2" width="41.140625" customWidth="1"/>
     <col min="3" max="3" width="40" customWidth="1"/>
-    <col min="4" max="4" width="24.453125" customWidth="1"/>
-    <col min="5" max="5" width="19.54296875" customWidth="1"/>
-    <col min="6" max="6" width="22.81640625" customWidth="1"/>
-    <col min="7" max="7" width="20.26953125" customWidth="1"/>
+    <col min="4" max="4" width="24.42578125" customWidth="1"/>
+    <col min="5" max="5" width="19.5703125" customWidth="1"/>
+    <col min="6" max="6" width="22.85546875" customWidth="1"/>
+    <col min="7" max="7" width="20.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1823,7 +2258,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -1846,7 +2281,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -1863,7 +2298,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -1880,7 +2315,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -1897,7 +2332,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -1914,7 +2349,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
@@ -1931,7 +2366,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
@@ -1948,7 +2383,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
@@ -1965,7 +2400,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
@@ -1982,7 +2417,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
@@ -2001,18 +2436,18 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
-    <hyperlink ref="D3:D11" r:id="rId2" display="aarosagarch@gmail.com" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
-    <hyperlink ref="E2" r:id="rId3" xr:uid="{00000000-0004-0000-0400-000002000000}"/>
-    <hyperlink ref="E3" r:id="rId4" xr:uid="{00000000-0004-0000-0400-000003000000}"/>
-    <hyperlink ref="E4" r:id="rId5" xr:uid="{00000000-0004-0000-0400-000004000000}"/>
-    <hyperlink ref="E5" r:id="rId6" xr:uid="{00000000-0004-0000-0400-000005000000}"/>
-    <hyperlink ref="E6" r:id="rId7" xr:uid="{00000000-0004-0000-0400-000006000000}"/>
-    <hyperlink ref="E7" r:id="rId8" xr:uid="{00000000-0004-0000-0400-000007000000}"/>
-    <hyperlink ref="E8" r:id="rId9" xr:uid="{00000000-0004-0000-0400-000008000000}"/>
-    <hyperlink ref="E9" r:id="rId10" xr:uid="{00000000-0004-0000-0400-000009000000}"/>
-    <hyperlink ref="E10" r:id="rId11" xr:uid="{00000000-0004-0000-0400-00000A000000}"/>
-    <hyperlink ref="E11" r:id="rId12" xr:uid="{00000000-0004-0000-0400-00000B000000}"/>
+    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="D3:D11" r:id="rId2" display="aarosagarch@gmail.com"/>
+    <hyperlink ref="E2" r:id="rId3"/>
+    <hyperlink ref="E3" r:id="rId4"/>
+    <hyperlink ref="E4" r:id="rId5"/>
+    <hyperlink ref="E5" r:id="rId6"/>
+    <hyperlink ref="E6" r:id="rId7"/>
+    <hyperlink ref="E7" r:id="rId8"/>
+    <hyperlink ref="E8" r:id="rId9"/>
+    <hyperlink ref="E9" r:id="rId10"/>
+    <hyperlink ref="E10" r:id="rId11"/>
+    <hyperlink ref="E11" r:id="rId12"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId13"/>
@@ -2020,23 +2455,23 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="28" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="34" customWidth="1"/>
     <col min="4" max="4" width="23" customWidth="1"/>
-    <col min="5" max="5" width="11.26953125" customWidth="1"/>
-    <col min="6" max="6" width="21.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" customWidth="1"/>
+    <col min="6" max="6" width="21.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2056,7 +2491,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -2076,7 +2511,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -2093,7 +2528,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -2110,7 +2545,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -2127,7 +2562,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -2144,7 +2579,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
@@ -2161,7 +2596,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
@@ -2178,7 +2613,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
@@ -2195,7 +2630,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
@@ -2212,7 +2647,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
@@ -2232,18 +2667,18 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
-    <hyperlink ref="D3:D11" r:id="rId2" display="aarosagarch@gmail.com" xr:uid="{00000000-0004-0000-0500-000001000000}"/>
-    <hyperlink ref="E2" r:id="rId3" xr:uid="{00000000-0004-0000-0500-000002000000}"/>
-    <hyperlink ref="E3" r:id="rId4" xr:uid="{00000000-0004-0000-0500-000003000000}"/>
-    <hyperlink ref="E4" r:id="rId5" xr:uid="{00000000-0004-0000-0500-000004000000}"/>
-    <hyperlink ref="E5" r:id="rId6" xr:uid="{00000000-0004-0000-0500-000005000000}"/>
-    <hyperlink ref="E6" r:id="rId7" xr:uid="{00000000-0004-0000-0500-000006000000}"/>
-    <hyperlink ref="E7" r:id="rId8" xr:uid="{00000000-0004-0000-0500-000007000000}"/>
-    <hyperlink ref="E8" r:id="rId9" xr:uid="{00000000-0004-0000-0500-000008000000}"/>
-    <hyperlink ref="E9" r:id="rId10" xr:uid="{00000000-0004-0000-0500-000009000000}"/>
-    <hyperlink ref="E10" r:id="rId11" xr:uid="{00000000-0004-0000-0500-00000A000000}"/>
-    <hyperlink ref="E11" r:id="rId12" xr:uid="{00000000-0004-0000-0500-00000B000000}"/>
+    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="D3:D11" r:id="rId2" display="aarosagarch@gmail.com"/>
+    <hyperlink ref="E2" r:id="rId3"/>
+    <hyperlink ref="E3" r:id="rId4"/>
+    <hyperlink ref="E4" r:id="rId5"/>
+    <hyperlink ref="E5" r:id="rId6"/>
+    <hyperlink ref="E6" r:id="rId7"/>
+    <hyperlink ref="E7" r:id="rId8"/>
+    <hyperlink ref="E8" r:id="rId9"/>
+    <hyperlink ref="E9" r:id="rId10"/>
+    <hyperlink ref="E10" r:id="rId11"/>
+    <hyperlink ref="E11" r:id="rId12"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId13"/>
@@ -2251,27 +2686,27 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.453125" customWidth="1"/>
-    <col min="2" max="2" width="34.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="40.1796875" customWidth="1"/>
-    <col min="4" max="4" width="22.7265625" customWidth="1"/>
-    <col min="5" max="5" width="12.453125" customWidth="1"/>
-    <col min="6" max="6" width="21.453125" customWidth="1"/>
-    <col min="7" max="7" width="21.1796875" customWidth="1"/>
-    <col min="8" max="8" width="18.26953125" customWidth="1"/>
-    <col min="9" max="9" width="9.26953125" customWidth="1"/>
+    <col min="1" max="1" width="6.42578125" customWidth="1"/>
+    <col min="2" max="2" width="34.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.140625" customWidth="1"/>
+    <col min="4" max="4" width="22.7109375" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" customWidth="1"/>
+    <col min="6" max="6" width="21.42578125" customWidth="1"/>
+    <col min="7" max="7" width="21.140625" customWidth="1"/>
+    <col min="8" max="8" width="18.28515625" customWidth="1"/>
+    <col min="9" max="9" width="9.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2298,7 +2733,7 @@
       <c r="J1" s="5"/>
       <c r="K1" s="1"/>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -2323,7 +2758,7 @@
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -2346,7 +2781,7 @@
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -2369,7 +2804,7 @@
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -2392,7 +2827,7 @@
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -2415,7 +2850,7 @@
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
@@ -2438,7 +2873,7 @@
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
@@ -2461,7 +2896,7 @@
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
@@ -2484,7 +2919,7 @@
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
@@ -2507,7 +2942,7 @@
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
@@ -2532,18 +2967,18 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
-    <hyperlink ref="D3:D11" r:id="rId2" display="aarosagarch@gmail.com" xr:uid="{00000000-0004-0000-0600-000001000000}"/>
-    <hyperlink ref="E2" r:id="rId3" xr:uid="{00000000-0004-0000-0600-000002000000}"/>
-    <hyperlink ref="E3" r:id="rId4" xr:uid="{00000000-0004-0000-0600-000003000000}"/>
-    <hyperlink ref="E4" r:id="rId5" xr:uid="{00000000-0004-0000-0600-000004000000}"/>
-    <hyperlink ref="E5" r:id="rId6" xr:uid="{00000000-0004-0000-0600-000005000000}"/>
-    <hyperlink ref="E6" r:id="rId7" xr:uid="{00000000-0004-0000-0600-000006000000}"/>
-    <hyperlink ref="E7" r:id="rId8" xr:uid="{00000000-0004-0000-0600-000007000000}"/>
-    <hyperlink ref="E8" r:id="rId9" xr:uid="{00000000-0004-0000-0600-000008000000}"/>
-    <hyperlink ref="E9" r:id="rId10" xr:uid="{00000000-0004-0000-0600-000009000000}"/>
-    <hyperlink ref="E10" r:id="rId11" xr:uid="{00000000-0004-0000-0600-00000A000000}"/>
-    <hyperlink ref="E11" r:id="rId12" xr:uid="{00000000-0004-0000-0600-00000B000000}"/>
+    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="D3:D11" r:id="rId2" display="aarosagarch@gmail.com"/>
+    <hyperlink ref="E2" r:id="rId3"/>
+    <hyperlink ref="E3" r:id="rId4"/>
+    <hyperlink ref="E4" r:id="rId5"/>
+    <hyperlink ref="E5" r:id="rId6"/>
+    <hyperlink ref="E6" r:id="rId7"/>
+    <hyperlink ref="E7" r:id="rId8"/>
+    <hyperlink ref="E8" r:id="rId9"/>
+    <hyperlink ref="E9" r:id="rId10"/>
+    <hyperlink ref="E10" r:id="rId11"/>
+    <hyperlink ref="E11" r:id="rId12"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -2551,30 +2986,30 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E11"/>
+      <selection sqref="A1:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.1796875" style="8"/>
-    <col min="2" max="2" width="30.81640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39.1796875" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.453125" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.7265625" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.1796875" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.54296875" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.81640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="8"/>
+    <col min="2" max="2" width="30.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.85546875" style="8" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17" style="8" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.7265625" style="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.7265625" style="8" customWidth="1"/>
-    <col min="12" max="16384" width="9.1796875" style="8"/>
+    <col min="10" max="10" width="20.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.7109375" style="8" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="29">
+    <row r="1" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -2609,7 +3044,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="29">
+    <row r="2" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>5</v>
       </c>
@@ -2644,7 +3079,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>6</v>
       </c>
@@ -2667,7 +3102,7 @@
       <c r="J3" s="10"/>
       <c r="K3" s="10"/>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>7</v>
       </c>
@@ -2690,7 +3125,7 @@
       <c r="J4" s="10"/>
       <c r="K4" s="10"/>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>8</v>
       </c>
@@ -2713,7 +3148,7 @@
       <c r="J5" s="10"/>
       <c r="K5" s="10"/>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>9</v>
       </c>
@@ -2736,7 +3171,7 @@
       <c r="J6" s="10"/>
       <c r="K6" s="10"/>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>10</v>
       </c>
@@ -2759,7 +3194,7 @@
       <c r="J7" s="10"/>
       <c r="K7" s="10"/>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>11</v>
       </c>
@@ -2782,7 +3217,7 @@
       <c r="J8" s="10"/>
       <c r="K8" s="10"/>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>12</v>
       </c>
@@ -2805,7 +3240,7 @@
       <c r="J9" s="10"/>
       <c r="K9" s="10"/>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>13</v>
       </c>
@@ -2828,7 +3263,7 @@
       <c r="J10" s="10"/>
       <c r="K10" s="10"/>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>14</v>
       </c>
@@ -2853,16 +3288,16 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E11" r:id="rId1" xr:uid="{00000000-0004-0000-0700-000000000000}"/>
-    <hyperlink ref="E10" r:id="rId2" xr:uid="{00000000-0004-0000-0700-000001000000}"/>
-    <hyperlink ref="E9" r:id="rId3" xr:uid="{00000000-0004-0000-0700-000002000000}"/>
-    <hyperlink ref="E8" r:id="rId4" xr:uid="{00000000-0004-0000-0700-000003000000}"/>
-    <hyperlink ref="E7" r:id="rId5" xr:uid="{00000000-0004-0000-0700-000004000000}"/>
-    <hyperlink ref="E6" r:id="rId6" xr:uid="{00000000-0004-0000-0700-000005000000}"/>
-    <hyperlink ref="E5" r:id="rId7" xr:uid="{00000000-0004-0000-0700-000006000000}"/>
-    <hyperlink ref="E4" r:id="rId8" xr:uid="{00000000-0004-0000-0700-000007000000}"/>
-    <hyperlink ref="E3" r:id="rId9" xr:uid="{00000000-0004-0000-0700-000008000000}"/>
-    <hyperlink ref="E2" r:id="rId10" xr:uid="{00000000-0004-0000-0700-000009000000}"/>
+    <hyperlink ref="E11" r:id="rId1"/>
+    <hyperlink ref="E10" r:id="rId2"/>
+    <hyperlink ref="E9" r:id="rId3"/>
+    <hyperlink ref="E8" r:id="rId4"/>
+    <hyperlink ref="E7" r:id="rId5"/>
+    <hyperlink ref="E6" r:id="rId6"/>
+    <hyperlink ref="E5" r:id="rId7"/>
+    <hyperlink ref="E4" r:id="rId8"/>
+    <hyperlink ref="E3" r:id="rId9"/>
+    <hyperlink ref="E2" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId11"/>
@@ -2870,22 +3305,22 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Added changes to my TC03
</commit_message>
<xml_diff>
--- a/src/main/resources/AutomationCatalogue_Batch41_TestData.xlsx
+++ b/src/main/resources/AutomationCatalogue_Batch41_TestData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sarika\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AutomationCatalogue\TestAutomationCatalogue_Batch41\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{525B0CCC-9136-4093-8E47-EA9412C25566}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D080218E-CB4B-4BB7-8C66-62D091F0DDB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="706" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="133">
   <si>
     <t>S. No</t>
   </si>
@@ -350,10 +350,88 @@
     <t>Orange HRM adding user</t>
   </si>
   <si>
-    <t>Charlie Carter</t>
-  </si>
-  <si>
     <t>CharlieABCDEF</t>
+  </si>
+  <si>
+    <t>Sarika_1</t>
+  </si>
+  <si>
+    <t>Sarika_2</t>
+  </si>
+  <si>
+    <t>Sarika_3</t>
+  </si>
+  <si>
+    <t>Sarika_4</t>
+  </si>
+  <si>
+    <t>Sarika_5</t>
+  </si>
+  <si>
+    <t>Sarika_6</t>
+  </si>
+  <si>
+    <t>Sarika_7</t>
+  </si>
+  <si>
+    <t>Sarika_8</t>
+  </si>
+  <si>
+    <t>Sarika_9</t>
+  </si>
+  <si>
+    <t>Charlie_1</t>
+  </si>
+  <si>
+    <t>Charlie_2</t>
+  </si>
+  <si>
+    <t>Charlie_3</t>
+  </si>
+  <si>
+    <t>Charlie_4</t>
+  </si>
+  <si>
+    <t>Charlie_5</t>
+  </si>
+  <si>
+    <t>Charlie_6</t>
+  </si>
+  <si>
+    <t>Charlie_7</t>
+  </si>
+  <si>
+    <t>Charlie_8</t>
+  </si>
+  <si>
+    <t>Charlie_9</t>
+  </si>
+  <si>
+    <t>Admin@124</t>
+  </si>
+  <si>
+    <t>Admin@125</t>
+  </si>
+  <si>
+    <t>Admin@126</t>
+  </si>
+  <si>
+    <t>Admin@127</t>
+  </si>
+  <si>
+    <t>Admin@128</t>
+  </si>
+  <si>
+    <t>Admin@129</t>
+  </si>
+  <si>
+    <t>Admin@130</t>
+  </si>
+  <si>
+    <t>Admin@131</t>
+  </si>
+  <si>
+    <t>Charlie Car</t>
   </si>
 </sst>
 </file>
@@ -557,7 +635,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -609,7 +687,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1547,7 +1625,7 @@
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1558,6 +1636,7 @@
     <col min="5" max="5" width="9.1796875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.81640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18" customWidth="1"/>
     <col min="9" max="9" width="16.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1607,10 +1686,10 @@
         <v>18</v>
       </c>
       <c r="F2" t="s">
+        <v>132</v>
+      </c>
+      <c r="G2" t="s">
         <v>105</v>
-      </c>
-      <c r="G2" t="s">
-        <v>106</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>18</v>
@@ -1635,6 +1714,18 @@
       <c r="E3" s="3" t="s">
         <v>18</v>
       </c>
+      <c r="F3" t="s">
+        <v>106</v>
+      </c>
+      <c r="G3" t="s">
+        <v>115</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="2" t="s">
@@ -1652,6 +1743,18 @@
       <c r="E4" s="3" t="s">
         <v>18</v>
       </c>
+      <c r="F4" t="s">
+        <v>107</v>
+      </c>
+      <c r="G4" t="s">
+        <v>116</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="2" t="s">
@@ -1669,6 +1772,18 @@
       <c r="E5" s="3" t="s">
         <v>18</v>
       </c>
+      <c r="F5" t="s">
+        <v>108</v>
+      </c>
+      <c r="G5" t="s">
+        <v>117</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="2" t="s">
@@ -1686,6 +1801,18 @@
       <c r="E6" s="3" t="s">
         <v>18</v>
       </c>
+      <c r="F6" t="s">
+        <v>109</v>
+      </c>
+      <c r="G6" t="s">
+        <v>118</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="2" t="s">
@@ -1703,6 +1830,18 @@
       <c r="E7" s="3" t="s">
         <v>18</v>
       </c>
+      <c r="F7" t="s">
+        <v>110</v>
+      </c>
+      <c r="G7" t="s">
+        <v>119</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="2" t="s">
@@ -1720,6 +1859,18 @@
       <c r="E8" s="3" t="s">
         <v>18</v>
       </c>
+      <c r="F8" t="s">
+        <v>111</v>
+      </c>
+      <c r="G8" t="s">
+        <v>120</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="2" t="s">
@@ -1737,6 +1888,18 @@
       <c r="E9" s="3" t="s">
         <v>18</v>
       </c>
+      <c r="F9" t="s">
+        <v>112</v>
+      </c>
+      <c r="G9" t="s">
+        <v>121</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="2" t="s">
@@ -1754,6 +1917,18 @@
       <c r="E10" s="3" t="s">
         <v>18</v>
       </c>
+      <c r="F10" t="s">
+        <v>113</v>
+      </c>
+      <c r="G10" t="s">
+        <v>122</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="2" t="s">
@@ -1770,6 +1945,18 @@
       </c>
       <c r="E11" s="3" t="s">
         <v>18</v>
+      </c>
+      <c r="F11" t="s">
+        <v>114</v>
+      </c>
+      <c r="G11" t="s">
+        <v>123</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -1779,6 +1966,10 @@
     <hyperlink ref="H2" r:id="rId2" xr:uid="{E7CFB2BD-C6BE-44EB-AE4C-FA39C50580F1}"/>
     <hyperlink ref="I2" r:id="rId3" xr:uid="{717D2B13-45AD-48C1-A07A-146CDADB5D82}"/>
     <hyperlink ref="E3:E11" r:id="rId4" display="Admin@123" xr:uid="{3CAF8F96-E222-4F94-8A70-9C685341A998}"/>
+    <hyperlink ref="H3" r:id="rId5" xr:uid="{9CAC30B5-85D4-44A0-992D-A92009C6D540}"/>
+    <hyperlink ref="H4:H11" r:id="rId6" display="Admin@123" xr:uid="{7FB30BD1-4F5F-445F-92A7-19BB4217F22B}"/>
+    <hyperlink ref="I3" r:id="rId7" xr:uid="{1C3F3B0D-A906-4FF4-B2EE-05228718BB7C}"/>
+    <hyperlink ref="I4:I11" r:id="rId8" display="Admin@123" xr:uid="{07B1E1BF-9514-48A6-BE4B-D454E5036E67}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Final changes are done in TC03
</commit_message>
<xml_diff>
--- a/src/main/resources/AutomationCatalogue_Batch41_TestData.xlsx
+++ b/src/main/resources/AutomationCatalogue_Batch41_TestData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AutomationCatalogue\Projects\TestAutomationCatalogue_Batch41\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AutomationCatalogue\TestAutomationCatalogue_Batch41\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C528329F-3D91-4B45-8906-A045527BA0FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBEC8E3E-2F44-4AC1-9379-46477E25F28A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="944" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="944" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="10" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1160" uniqueCount="351">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1188" uniqueCount="365">
   <si>
     <t>S. No</t>
   </si>
@@ -1086,7 +1086,49 @@
     <t>Anjaneyulu</t>
   </si>
   <si>
-    <t>anjanyulu</t>
+    <t>RamaKrishna</t>
+  </si>
+  <si>
+    <t>RamaKrishna123</t>
+  </si>
+  <si>
+    <t>Ravali</t>
+  </si>
+  <si>
+    <t>Ravali123</t>
+  </si>
+  <si>
+    <t>Haritha</t>
+  </si>
+  <si>
+    <t>Haritha123</t>
+  </si>
+  <si>
+    <t>Ramya</t>
+  </si>
+  <si>
+    <t>Ramya123</t>
+  </si>
+  <si>
+    <t>Sunitha</t>
+  </si>
+  <si>
+    <t>Sunitha123</t>
+  </si>
+  <si>
+    <t>Sarika</t>
+  </si>
+  <si>
+    <t>Sarika123</t>
+  </si>
+  <si>
+    <t>anjanyulu123</t>
+  </si>
+  <si>
+    <t>Shiva</t>
+  </si>
+  <si>
+    <t>Shiva123</t>
   </si>
 </sst>
 </file>
@@ -1561,13 +1603,13 @@
       <selection activeCell="B76" sqref="B76"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.81640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="39" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="38" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -3255,18 +3297,18 @@
       <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="6.44140625" customWidth="1"/>
-    <col min="2" max="2" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="40.21875" customWidth="1"/>
-    <col min="5" max="5" width="22.77734375" customWidth="1"/>
-    <col min="6" max="6" width="12.44140625" customWidth="1"/>
-    <col min="7" max="7" width="21.44140625" customWidth="1"/>
-    <col min="8" max="8" width="21.21875" customWidth="1"/>
-    <col min="9" max="9" width="18.21875" customWidth="1"/>
-    <col min="10" max="10" width="9.21875" customWidth="1"/>
+    <col min="1" max="1" width="6.453125" customWidth="1"/>
+    <col min="2" max="2" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.1796875" customWidth="1"/>
+    <col min="5" max="5" width="22.81640625" customWidth="1"/>
+    <col min="6" max="6" width="12.453125" customWidth="1"/>
+    <col min="7" max="7" width="21.453125" customWidth="1"/>
+    <col min="8" max="8" width="21.1796875" customWidth="1"/>
+    <col min="9" max="9" width="18.1796875" customWidth="1"/>
+    <col min="10" max="10" width="9.1796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -3590,13 +3632,13 @@
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="2" max="2" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.81640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26" customWidth="1"/>
-    <col min="4" max="4" width="24.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -3833,24 +3875,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:O11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L29" sqref="L29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="2" max="2" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.81640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="38" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.453125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.77734375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.81640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
@@ -4233,21 +4275,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="2" max="2" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.77734375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.77734375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -4333,6 +4375,18 @@
       <c r="F3" s="3" t="s">
         <v>18</v>
       </c>
+      <c r="G3" t="s">
+        <v>350</v>
+      </c>
+      <c r="H3" t="s">
+        <v>351</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="2" t="s">
@@ -4353,6 +4407,18 @@
       <c r="F4" s="3" t="s">
         <v>18</v>
       </c>
+      <c r="G4" t="s">
+        <v>352</v>
+      </c>
+      <c r="H4" t="s">
+        <v>353</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="2" t="s">
@@ -4405,6 +4471,18 @@
       <c r="F6" s="3" t="s">
         <v>18</v>
       </c>
+      <c r="G6" t="s">
+        <v>354</v>
+      </c>
+      <c r="H6" t="s">
+        <v>355</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="2" t="s">
@@ -4425,6 +4503,18 @@
       <c r="F7" s="3" t="s">
         <v>18</v>
       </c>
+      <c r="G7" t="s">
+        <v>356</v>
+      </c>
+      <c r="H7" t="s">
+        <v>357</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="2" t="s">
@@ -4445,6 +4535,18 @@
       <c r="F8" s="3" t="s">
         <v>18</v>
       </c>
+      <c r="G8" t="s">
+        <v>358</v>
+      </c>
+      <c r="H8" t="s">
+        <v>359</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" s="2" t="s">
@@ -4465,6 +4567,18 @@
       <c r="F9" s="3" t="s">
         <v>18</v>
       </c>
+      <c r="G9" t="s">
+        <v>363</v>
+      </c>
+      <c r="H9" t="s">
+        <v>364</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="10" spans="1:10">
       <c r="A10" s="2" t="s">
@@ -4489,7 +4603,7 @@
         <v>349</v>
       </c>
       <c r="H10" t="s">
-        <v>350</v>
+        <v>362</v>
       </c>
       <c r="I10" s="3" t="s">
         <v>18</v>
@@ -4515,6 +4629,18 @@
         <v>17</v>
       </c>
       <c r="F11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G11" t="s">
+        <v>360</v>
+      </c>
+      <c r="H11" t="s">
+        <v>361</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J11" s="3" t="s">
         <v>18</v>
       </c>
     </row>
@@ -4529,6 +4655,20 @@
     <hyperlink ref="J5" r:id="rId6" xr:uid="{0611619D-9970-4F64-A28C-D8BAC5BF4492}"/>
     <hyperlink ref="I10" r:id="rId7" xr:uid="{552B24E7-9F5D-4166-8001-7B76A5A7756F}"/>
     <hyperlink ref="J10" r:id="rId8" xr:uid="{36C8351A-57C7-498A-9EC5-851023D83150}"/>
+    <hyperlink ref="I3" r:id="rId9" xr:uid="{74500D77-3191-4D3A-B38D-9A9B437B1D2C}"/>
+    <hyperlink ref="J3" r:id="rId10" xr:uid="{D80E1DC6-301D-4B36-A23B-F0ED070EA48A}"/>
+    <hyperlink ref="I4" r:id="rId11" xr:uid="{D0FB0770-1811-46F1-9B6D-5D94B2642134}"/>
+    <hyperlink ref="J4" r:id="rId12" xr:uid="{A6B89123-2950-4007-9715-C1145EBE1956}"/>
+    <hyperlink ref="I6" r:id="rId13" xr:uid="{6CBCC207-C3CB-4C41-BEE9-72674CD42365}"/>
+    <hyperlink ref="J6" r:id="rId14" xr:uid="{2F51CA17-67A8-4C0D-9746-0D42AA7A809E}"/>
+    <hyperlink ref="I7" r:id="rId15" xr:uid="{D219FFF8-A3B5-4EC7-9347-0397F0230672}"/>
+    <hyperlink ref="J7" r:id="rId16" xr:uid="{12FA5EE8-4C09-460E-8F38-BA97B5D357F3}"/>
+    <hyperlink ref="I8" r:id="rId17" xr:uid="{5FA32375-585B-400C-9421-75EF8535B8E0}"/>
+    <hyperlink ref="J8" r:id="rId18" xr:uid="{100829E3-DEBC-49C7-8C02-933F9244F088}"/>
+    <hyperlink ref="I9" r:id="rId19" xr:uid="{C5A3A326-62C4-4ECC-A103-2EE061C4FBFC}"/>
+    <hyperlink ref="J9" r:id="rId20" xr:uid="{FA1ACB88-801C-4E23-9860-65C5DA5AD410}"/>
+    <hyperlink ref="I11" r:id="rId21" xr:uid="{D4141781-F0F4-4400-A207-A1C61514AE56}"/>
+    <hyperlink ref="J11" r:id="rId22" xr:uid="{CFFF25C1-32E4-4B1D-9BC9-EA7C19E17A49}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4542,24 +4682,24 @@
       <selection activeCell="G8" sqref="G8:L8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="9.21875" style="8"/>
-    <col min="2" max="2" width="15.88671875" style="8" customWidth="1"/>
-    <col min="3" max="3" width="30.77734375" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="39.21875" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.44140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.77734375" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.21875" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.5546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.77734375" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.1796875" style="8"/>
+    <col min="2" max="2" width="15.90625" style="8" customWidth="1"/>
+    <col min="3" max="3" width="30.81640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.1796875" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.453125" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.81640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.1796875" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.54296875" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.81640625" style="8" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17" style="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.77734375" style="8" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.77734375" style="8" customWidth="1"/>
-    <col min="13" max="16384" width="9.21875" style="8"/>
+    <col min="11" max="11" width="20.81640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.81640625" style="8" customWidth="1"/>
+    <col min="13" max="16384" width="9.1796875" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="28.8">
+    <row r="1" spans="1:12" ht="29">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -4597,7 +4737,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="28.8">
+    <row r="2" spans="1:12" ht="29">
       <c r="A2" s="9" t="s">
         <v>5</v>
       </c>
@@ -4899,16 +5039,16 @@
       <selection activeCell="G2" sqref="G2:P11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="2" max="2" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.90625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.08984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="9.90625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.08984375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16">
@@ -5197,14 +5337,14 @@
       <selection activeCell="G3" sqref="G3:G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="2" max="2" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.81640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="28" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="34" customWidth="1"/>
     <col min="5" max="5" width="23" customWidth="1"/>
-    <col min="6" max="6" width="11.21875" customWidth="1"/>
-    <col min="7" max="7" width="21.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.1796875" customWidth="1"/>
+    <col min="7" max="7" width="21.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -5462,15 +5602,15 @@
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="2" max="2" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="41.21875" customWidth="1"/>
+    <col min="2" max="2" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.1796875" customWidth="1"/>
     <col min="4" max="4" width="40" customWidth="1"/>
-    <col min="5" max="5" width="24.44140625" customWidth="1"/>
-    <col min="6" max="6" width="19.5546875" customWidth="1"/>
-    <col min="7" max="7" width="22.77734375" customWidth="1"/>
-    <col min="8" max="8" width="20.21875" customWidth="1"/>
+    <col min="5" max="5" width="24.453125" customWidth="1"/>
+    <col min="6" max="6" width="19.54296875" customWidth="1"/>
+    <col min="7" max="7" width="22.81640625" customWidth="1"/>
+    <col min="8" max="8" width="20.1796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -5734,16 +5874,16 @@
       <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="2" max="2" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="41.77734375" customWidth="1"/>
-    <col min="4" max="4" width="34.21875" customWidth="1"/>
-    <col min="5" max="5" width="22.5546875" customWidth="1"/>
-    <col min="6" max="6" width="11.21875" customWidth="1"/>
+    <col min="2" max="2" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.81640625" customWidth="1"/>
+    <col min="4" max="4" width="34.1796875" customWidth="1"/>
+    <col min="5" max="5" width="22.54296875" customWidth="1"/>
+    <col min="6" max="6" width="11.1796875" customWidth="1"/>
     <col min="7" max="7" width="23" customWidth="1"/>
-    <col min="8" max="8" width="15.77734375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.77734375" customWidth="1"/>
+    <col min="8" max="8" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">

</xml_diff>

<commit_message>
Done Enhancements in TC04
</commit_message>
<xml_diff>
--- a/src/main/resources/AutomationCatalogue_Batch41_TestData.xlsx
+++ b/src/main/resources/AutomationCatalogue_Batch41_TestData.xlsx
@@ -1,28 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AutomationCatalogue\Projects\TestAutomationCatalogue_Batch41\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Automation Catalogue\Projects\TestAutomationCatalogue_Batch41\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C528329F-3D91-4B45-8906-A045527BA0FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="944" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="944" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="10" r:id="rId1"/>
-    <sheet name="OrangeHRM_Login" sheetId="1" r:id="rId2"/>
-    <sheet name="OrangeHRM_AddEmployee" sheetId="2" r:id="rId3"/>
-    <sheet name="OrangeHRM_AddUser" sheetId="3" r:id="rId4"/>
-    <sheet name="OrangeHRM_EditEmployee" sheetId="8" r:id="rId5"/>
-    <sheet name="DemoWebshop_CreateAddress" sheetId="5" r:id="rId6"/>
-    <sheet name="DemoWebshop_ReOrder" sheetId="4" r:id="rId7"/>
-    <sheet name="DemoWebshop_TotalOrders" sheetId="6" r:id="rId8"/>
-    <sheet name="DemoWebshop_UpdateShoppingCart" sheetId="9" r:id="rId9"/>
-    <sheet name="DemoWebshop_ApplyDiscount" sheetId="7" r:id="rId10"/>
+    <sheet name="OrangeHRM_Goals" sheetId="11" r:id="rId2"/>
+    <sheet name="OrangeHRM_Login" sheetId="1" r:id="rId3"/>
+    <sheet name="OrangeHRM_AddEmployee" sheetId="2" r:id="rId4"/>
+    <sheet name="OrangeHRM_AddUser" sheetId="3" r:id="rId5"/>
+    <sheet name="OrangeHRM_EditEmployee" sheetId="8" r:id="rId6"/>
+    <sheet name="DemoWebshop_CreateAddress" sheetId="5" r:id="rId7"/>
+    <sheet name="DemoWebshop_ReOrder" sheetId="4" r:id="rId8"/>
+    <sheet name="DemoWebshop_TotalOrders" sheetId="6" r:id="rId9"/>
+    <sheet name="DemoWebshop_UpdateShoppingCart" sheetId="9" r:id="rId10"/>
+    <sheet name="DemoWebshop_ApplyDiscount" sheetId="7" r:id="rId11"/>
   </sheets>
   <calcPr calcId="124519"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1160" uniqueCount="351">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1240" uniqueCount="375">
   <si>
     <t>S. No</t>
   </si>
@@ -1087,13 +1087,85 @@
   </si>
   <si>
     <t>anjanyulu</t>
+  </si>
+  <si>
+    <t>TC20_01</t>
+  </si>
+  <si>
+    <t>TC20_02</t>
+  </si>
+  <si>
+    <t>TC20_03</t>
+  </si>
+  <si>
+    <t>TC20_04</t>
+  </si>
+  <si>
+    <t>TC20_05</t>
+  </si>
+  <si>
+    <t>TC20_06</t>
+  </si>
+  <si>
+    <t>TC20_07</t>
+  </si>
+  <si>
+    <t>TC20_08</t>
+  </si>
+  <si>
+    <t>TC20_09</t>
+  </si>
+  <si>
+    <t>TC20_10</t>
+  </si>
+  <si>
+    <t>Employee Name</t>
+  </si>
+  <si>
+    <t>First Goal Priority</t>
+  </si>
+  <si>
+    <t>First Goal Date</t>
+  </si>
+  <si>
+    <t>Second Goal Priority</t>
+  </si>
+  <si>
+    <t>Second Goal Date</t>
+  </si>
+  <si>
+    <t>Third Goal Priority</t>
+  </si>
+  <si>
+    <t>Third Goal Date</t>
+  </si>
+  <si>
+    <t>Aaliyah Haq</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>23-September-2023</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>10-January-2024</t>
+  </si>
+  <si>
+    <t>23-March-2024</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1204,7 +1276,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -1240,6 +1312,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1554,23 +1627,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90270A87-C874-4975-9C16-F9436E7DA963}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F122"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B76" sqref="B76"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="39" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="38" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>89</v>
       </c>
@@ -1590,7 +1663,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>116</v>
       </c>
@@ -1600,7 +1673,7 @@
       <c r="E2" s="14"/>
       <c r="F2" s="14"/>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -1614,7 +1687,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -1628,7 +1701,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -1642,7 +1715,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
@@ -1656,7 +1729,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
@@ -1670,7 +1743,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
@@ -1684,7 +1757,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>11</v>
       </c>
@@ -1698,7 +1771,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>12</v>
       </c>
@@ -1712,7 +1785,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>13</v>
       </c>
@@ -1726,7 +1799,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>14</v>
       </c>
@@ -1740,7 +1813,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
         <v>117</v>
       </c>
@@ -1750,7 +1823,7 @@
       <c r="E13" s="15"/>
       <c r="F13" s="15"/>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>118</v>
       </c>
@@ -1764,7 +1837,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>119</v>
       </c>
@@ -1778,7 +1851,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>120</v>
       </c>
@@ -1792,7 +1865,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>121</v>
       </c>
@@ -1806,7 +1879,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>122</v>
       </c>
@@ -1820,7 +1893,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>123</v>
       </c>
@@ -1834,7 +1907,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>124</v>
       </c>
@@ -1848,7 +1921,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>125</v>
       </c>
@@ -1862,7 +1935,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>126</v>
       </c>
@@ -1876,7 +1949,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>127</v>
       </c>
@@ -1890,7 +1963,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="15" t="s">
         <v>138</v>
       </c>
@@ -1900,7 +1973,7 @@
       <c r="E24" s="15"/>
       <c r="F24" s="15"/>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>139</v>
       </c>
@@ -1914,7 +1987,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>140</v>
       </c>
@@ -1928,7 +2001,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>141</v>
       </c>
@@ -1942,7 +2015,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>142</v>
       </c>
@@ -1956,7 +2029,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>143</v>
       </c>
@@ -1970,7 +2043,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>144</v>
       </c>
@@ -1984,7 +2057,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>145</v>
       </c>
@@ -1998,7 +2071,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>146</v>
       </c>
@@ -2012,7 +2085,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>147</v>
       </c>
@@ -2026,7 +2099,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>148</v>
       </c>
@@ -2040,7 +2113,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="15" t="s">
         <v>159</v>
       </c>
@@ -2050,7 +2123,7 @@
       <c r="E35" s="15"/>
       <c r="F35" s="15"/>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>164</v>
       </c>
@@ -2064,7 +2137,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>165</v>
       </c>
@@ -2078,7 +2151,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>166</v>
       </c>
@@ -2092,7 +2165,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>167</v>
       </c>
@@ -2106,7 +2179,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="40" spans="1:6">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>168</v>
       </c>
@@ -2120,7 +2193,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>169</v>
       </c>
@@ -2134,7 +2207,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>170</v>
       </c>
@@ -2148,7 +2221,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="43" spans="1:6">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>171</v>
       </c>
@@ -2162,7 +2235,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="44" spans="1:6">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>172</v>
       </c>
@@ -2176,7 +2249,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="45" spans="1:6">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>173</v>
       </c>
@@ -2190,7 +2263,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="46" spans="1:6">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="15" t="s">
         <v>185</v>
       </c>
@@ -2200,7 +2273,7 @@
       <c r="E46" s="15"/>
       <c r="F46" s="15"/>
     </row>
-    <row r="47" spans="1:6">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>186</v>
       </c>
@@ -2214,7 +2287,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="48" spans="1:6">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>187</v>
       </c>
@@ -2228,7 +2301,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="49" spans="1:6">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>188</v>
       </c>
@@ -2242,7 +2315,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="50" spans="1:6">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>189</v>
       </c>
@@ -2256,7 +2329,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="51" spans="1:6">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>190</v>
       </c>
@@ -2270,7 +2343,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="52" spans="1:6">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>191</v>
       </c>
@@ -2284,7 +2357,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="53" spans="1:6">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>192</v>
       </c>
@@ -2298,7 +2371,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="54" spans="1:6">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>193</v>
       </c>
@@ -2312,7 +2385,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="55" spans="1:6">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>194</v>
       </c>
@@ -2326,7 +2399,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="56" spans="1:6">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>195</v>
       </c>
@@ -2340,7 +2413,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="57" spans="1:6">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="15" t="s">
         <v>208</v>
       </c>
@@ -2350,7 +2423,7 @@
       <c r="E57" s="15"/>
       <c r="F57" s="15"/>
     </row>
-    <row r="58" spans="1:6">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>209</v>
       </c>
@@ -2364,7 +2437,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="59" spans="1:6">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>210</v>
       </c>
@@ -2378,7 +2451,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="60" spans="1:6">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>211</v>
       </c>
@@ -2392,7 +2465,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="61" spans="1:6">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>212</v>
       </c>
@@ -2406,7 +2479,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="62" spans="1:6">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>213</v>
       </c>
@@ -2420,7 +2493,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="63" spans="1:6">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>214</v>
       </c>
@@ -2434,7 +2507,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="64" spans="1:6">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>215</v>
       </c>
@@ -2448,7 +2521,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="65" spans="1:6">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>216</v>
       </c>
@@ -2462,7 +2535,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="66" spans="1:6">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>217</v>
       </c>
@@ -2476,7 +2549,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="67" spans="1:6">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>218</v>
       </c>
@@ -2490,7 +2563,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="68" spans="1:6">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="15" t="s">
         <v>230</v>
       </c>
@@ -2500,7 +2573,7 @@
       <c r="E68" s="15"/>
       <c r="F68" s="15"/>
     </row>
-    <row r="69" spans="1:6">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>251</v>
       </c>
@@ -2514,7 +2587,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="70" spans="1:6">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>252</v>
       </c>
@@ -2528,7 +2601,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="71" spans="1:6">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>253</v>
       </c>
@@ -2542,7 +2615,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="72" spans="1:6">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>254</v>
       </c>
@@ -2556,7 +2629,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="73" spans="1:6">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>255</v>
       </c>
@@ -2570,7 +2643,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="74" spans="1:6">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>256</v>
       </c>
@@ -2584,7 +2657,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="75" spans="1:6">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>257</v>
       </c>
@@ -2598,7 +2671,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="76" spans="1:6">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>258</v>
       </c>
@@ -2612,7 +2685,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="77" spans="1:6">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>259</v>
       </c>
@@ -2626,7 +2699,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="78" spans="1:6">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>260</v>
       </c>
@@ -2640,7 +2713,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="79" spans="1:6">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="15" t="s">
         <v>262</v>
       </c>
@@ -2650,7 +2723,7 @@
       <c r="E79" s="15"/>
       <c r="F79" s="15"/>
     </row>
-    <row r="80" spans="1:6">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
         <v>263</v>
       </c>
@@ -2664,7 +2737,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="81" spans="1:6">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>264</v>
       </c>
@@ -2678,7 +2751,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="82" spans="1:6">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>265</v>
       </c>
@@ -2692,7 +2765,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="83" spans="1:6">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>266</v>
       </c>
@@ -2706,7 +2779,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="84" spans="1:6">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>267</v>
       </c>
@@ -2720,7 +2793,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="85" spans="1:6">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>268</v>
       </c>
@@ -2734,7 +2807,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="86" spans="1:6">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
         <v>269</v>
       </c>
@@ -2748,7 +2821,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="87" spans="1:6">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>270</v>
       </c>
@@ -2762,7 +2835,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="88" spans="1:6">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
         <v>271</v>
       </c>
@@ -2776,7 +2849,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="89" spans="1:6">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
         <v>272</v>
       </c>
@@ -2790,7 +2863,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="90" spans="1:6">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="15" t="s">
         <v>283</v>
       </c>
@@ -2800,7 +2873,7 @@
       <c r="E90" s="15"/>
       <c r="F90" s="15"/>
     </row>
-    <row r="91" spans="1:6">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
         <v>284</v>
       </c>
@@ -2814,7 +2887,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="92" spans="1:6">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
         <v>285</v>
       </c>
@@ -2828,7 +2901,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="93" spans="1:6">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
         <v>286</v>
       </c>
@@ -2842,7 +2915,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="94" spans="1:6">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
         <v>287</v>
       </c>
@@ -2856,7 +2929,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="95" spans="1:6">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
         <v>288</v>
       </c>
@@ -2870,7 +2943,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="96" spans="1:6">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
         <v>289</v>
       </c>
@@ -2884,7 +2957,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="97" spans="1:6">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
         <v>290</v>
       </c>
@@ -2898,7 +2971,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="98" spans="1:6">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
         <v>291</v>
       </c>
@@ -2912,7 +2985,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="99" spans="1:6">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
         <v>292</v>
       </c>
@@ -2926,7 +2999,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="100" spans="1:6">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
         <v>293</v>
       </c>
@@ -2940,7 +3013,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="101" spans="1:6">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" s="15" t="s">
         <v>316</v>
       </c>
@@ -2950,7 +3023,7 @@
       <c r="E101" s="15"/>
       <c r="F101" s="15"/>
     </row>
-    <row r="102" spans="1:6">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
         <v>317</v>
       </c>
@@ -2964,7 +3037,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="103" spans="1:6">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
         <v>318</v>
       </c>
@@ -2978,7 +3051,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="104" spans="1:6">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
         <v>319</v>
       </c>
@@ -2992,7 +3065,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="105" spans="1:6">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
         <v>320</v>
       </c>
@@ -3006,7 +3079,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="106" spans="1:6">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
         <v>321</v>
       </c>
@@ -3020,7 +3093,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="107" spans="1:6">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
         <v>322</v>
       </c>
@@ -3034,7 +3107,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="108" spans="1:6">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
         <v>323</v>
       </c>
@@ -3048,7 +3121,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="109" spans="1:6">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
         <v>324</v>
       </c>
@@ -3062,7 +3135,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="110" spans="1:6">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
         <v>325</v>
       </c>
@@ -3076,7 +3149,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="111" spans="1:6">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
         <v>326</v>
       </c>
@@ -3090,7 +3163,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="112" spans="1:6">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" s="15" t="s">
         <v>338</v>
       </c>
@@ -3100,7 +3173,7 @@
       <c r="E112" s="15"/>
       <c r="F112" s="15"/>
     </row>
-    <row r="113" spans="1:4">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
         <v>339</v>
       </c>
@@ -3114,7 +3187,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="114" spans="1:4">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
         <v>340</v>
       </c>
@@ -3128,7 +3201,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="115" spans="1:4">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
         <v>341</v>
       </c>
@@ -3142,7 +3215,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="116" spans="1:4">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
         <v>342</v>
       </c>
@@ -3156,7 +3229,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="117" spans="1:4">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
         <v>343</v>
       </c>
@@ -3170,7 +3243,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="118" spans="1:4">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
         <v>344</v>
       </c>
@@ -3184,7 +3257,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="119" spans="1:4">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
         <v>345</v>
       </c>
@@ -3198,7 +3271,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="120" spans="1:4">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
         <v>346</v>
       </c>
@@ -3212,7 +3285,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="121" spans="1:4">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" s="2" t="s">
         <v>347</v>
       </c>
@@ -3226,7 +3299,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="122" spans="1:4">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" s="2" t="s">
         <v>348</v>
       </c>
@@ -3248,28 +3321,293 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.7109375" customWidth="1"/>
+    <col min="4" max="4" width="34.28515625" customWidth="1"/>
+    <col min="5" max="5" width="22.5703125" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" customWidth="1"/>
+    <col min="7" max="7" width="23" customWidth="1"/>
+    <col min="8" max="8" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="C2" t="s">
+        <v>305</v>
+      </c>
+      <c r="D2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="C3" t="s">
+        <v>305</v>
+      </c>
+      <c r="D3" t="s">
+        <v>92</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="C4" t="s">
+        <v>305</v>
+      </c>
+      <c r="D4" t="s">
+        <v>92</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="C5" t="s">
+        <v>305</v>
+      </c>
+      <c r="D5" t="s">
+        <v>92</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="C6" t="s">
+        <v>305</v>
+      </c>
+      <c r="D6" t="s">
+        <v>92</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="C7" t="s">
+        <v>305</v>
+      </c>
+      <c r="D7" t="s">
+        <v>92</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="F7" s="13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="C8" t="s">
+        <v>305</v>
+      </c>
+      <c r="D8" t="s">
+        <v>92</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="C9" t="s">
+        <v>305</v>
+      </c>
+      <c r="D9" t="s">
+        <v>92</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="C10" t="s">
+        <v>305</v>
+      </c>
+      <c r="D10" t="s">
+        <v>92</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="F10" s="13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="C11" t="s">
+        <v>305</v>
+      </c>
+      <c r="D11" t="s">
+        <v>92</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.44140625" customWidth="1"/>
-    <col min="2" max="2" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="40.21875" customWidth="1"/>
-    <col min="5" max="5" width="22.77734375" customWidth="1"/>
-    <col min="6" max="6" width="12.44140625" customWidth="1"/>
-    <col min="7" max="7" width="21.44140625" customWidth="1"/>
-    <col min="8" max="8" width="21.21875" customWidth="1"/>
-    <col min="9" max="9" width="18.21875" customWidth="1"/>
-    <col min="10" max="10" width="9.21875" customWidth="1"/>
+    <col min="1" max="1" width="6.42578125" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.28515625" customWidth="1"/>
+    <col min="5" max="5" width="22.7109375" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" customWidth="1"/>
+    <col min="7" max="7" width="21.42578125" customWidth="1"/>
+    <col min="8" max="8" width="21.28515625" customWidth="1"/>
+    <col min="9" max="9" width="18.28515625" customWidth="1"/>
+    <col min="10" max="10" width="9.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3299,7 +3637,7 @@
       <c r="K1" s="5"/>
       <c r="L1" s="1"/>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -3327,7 +3665,7 @@
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -3353,7 +3691,7 @@
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -3379,7 +3717,7 @@
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -3405,7 +3743,7 @@
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -3431,7 +3769,7 @@
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
@@ -3457,7 +3795,7 @@
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
@@ -3483,7 +3821,7 @@
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
@@ -3509,7 +3847,7 @@
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
@@ -3535,7 +3873,7 @@
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
@@ -3564,18 +3902,18 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
-    <hyperlink ref="E3:E11" r:id="rId2" display="aarosagarch@gmail.com" xr:uid="{00000000-0004-0000-0600-000001000000}"/>
-    <hyperlink ref="F2" r:id="rId3" xr:uid="{00000000-0004-0000-0600-000002000000}"/>
-    <hyperlink ref="F3" r:id="rId4" xr:uid="{00000000-0004-0000-0600-000003000000}"/>
-    <hyperlink ref="F4" r:id="rId5" xr:uid="{00000000-0004-0000-0600-000004000000}"/>
-    <hyperlink ref="F5" r:id="rId6" xr:uid="{00000000-0004-0000-0600-000005000000}"/>
-    <hyperlink ref="F6" r:id="rId7" xr:uid="{00000000-0004-0000-0600-000006000000}"/>
-    <hyperlink ref="F7" r:id="rId8" xr:uid="{00000000-0004-0000-0600-000007000000}"/>
-    <hyperlink ref="F8" r:id="rId9" xr:uid="{00000000-0004-0000-0600-000008000000}"/>
-    <hyperlink ref="F9" r:id="rId10" xr:uid="{00000000-0004-0000-0600-000009000000}"/>
-    <hyperlink ref="F10" r:id="rId11" xr:uid="{00000000-0004-0000-0600-00000A000000}"/>
-    <hyperlink ref="F11" r:id="rId12" xr:uid="{00000000-0004-0000-0600-00000B000000}"/>
+    <hyperlink ref="E2" r:id="rId1"/>
+    <hyperlink ref="E3:E11" r:id="rId2" display="aarosagarch@gmail.com"/>
+    <hyperlink ref="F2" r:id="rId3"/>
+    <hyperlink ref="F3" r:id="rId4"/>
+    <hyperlink ref="F4" r:id="rId5"/>
+    <hyperlink ref="F5" r:id="rId6"/>
+    <hyperlink ref="F6" r:id="rId7"/>
+    <hyperlink ref="F7" r:id="rId8"/>
+    <hyperlink ref="F8" r:id="rId9"/>
+    <hyperlink ref="F9" r:id="rId10"/>
+    <hyperlink ref="F10" r:id="rId11"/>
+    <hyperlink ref="F11" r:id="rId12"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -3583,23 +3921,30 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26" customWidth="1"/>
-    <col min="4" max="4" width="24.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" customWidth="1"/>
+    <col min="3" max="3" width="30.42578125" customWidth="1"/>
+    <col min="4" max="4" width="25.5703125" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" customWidth="1"/>
+    <col min="8" max="8" width="17" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" customWidth="1"/>
+    <col min="10" max="10" width="19.42578125" customWidth="1"/>
+    <col min="11" max="11" width="15.85546875" customWidth="1"/>
+    <col min="12" max="12" width="18" customWidth="1"/>
+    <col min="13" max="13" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3618,13 +3963,34 @@
       <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="G1" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>106</v>
+        <v>351</v>
       </c>
       <c r="C2" t="s">
         <v>15</v>
@@ -3638,13 +4004,34 @@
       <c r="F2" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="G2" t="s">
+        <v>368</v>
+      </c>
+      <c r="H2" t="s">
+        <v>369</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="J2" t="s">
+        <v>371</v>
+      </c>
+      <c r="K2" s="17" t="s">
+        <v>373</v>
+      </c>
+      <c r="L2" t="s">
+        <v>372</v>
+      </c>
+      <c r="M2" s="17" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>107</v>
+        <v>352</v>
       </c>
       <c r="C3" t="s">
         <v>15</v>
@@ -3653,18 +4040,18 @@
         <v>16</v>
       </c>
       <c r="E3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>108</v>
+        <v>353</v>
       </c>
       <c r="C4" t="s">
         <v>15</v>
@@ -3673,18 +4060,18 @@
         <v>16</v>
       </c>
       <c r="E4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>109</v>
+        <v>354</v>
       </c>
       <c r="C5" t="s">
         <v>15</v>
@@ -3693,18 +4080,18 @@
         <v>16</v>
       </c>
       <c r="E5" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>110</v>
+        <v>355</v>
       </c>
       <c r="C6" t="s">
         <v>15</v>
@@ -3713,18 +4100,18 @@
         <v>16</v>
       </c>
       <c r="E6" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>111</v>
+        <v>356</v>
       </c>
       <c r="C7" t="s">
         <v>15</v>
@@ -3733,18 +4120,18 @@
         <v>16</v>
       </c>
       <c r="E7" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>112</v>
+        <v>357</v>
       </c>
       <c r="C8" t="s">
         <v>15</v>
@@ -3753,18 +4140,18 @@
         <v>16</v>
       </c>
       <c r="E8" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>113</v>
+        <v>358</v>
       </c>
       <c r="C9" t="s">
         <v>15</v>
@@ -3773,18 +4160,18 @@
         <v>16</v>
       </c>
       <c r="E9" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>114</v>
+        <v>359</v>
       </c>
       <c r="C10" t="s">
         <v>15</v>
@@ -3793,18 +4180,18 @@
         <v>16</v>
       </c>
       <c r="E10" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>115</v>
+        <v>360</v>
       </c>
       <c r="C11" t="s">
         <v>15</v>
@@ -3813,47 +4200,39 @@
         <v>16</v>
       </c>
       <c r="E11" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>18</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="F3:F11" r:id="rId2" display="Admin@123" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="F2" r:id="rId1"/>
+    <hyperlink ref="F3:F11" r:id="rId2" display="Admin@123"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:O11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L29" sqref="L29"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.77734375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26" customWidth="1"/>
+    <col min="4" max="4" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3872,46 +4251,19 @@
       <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="O1" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>128</v>
+      <c r="B2" t="s">
+        <v>106</v>
       </c>
       <c r="C2" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="D2" t="s">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="E2" t="s">
         <v>17</v>
@@ -3919,293 +4271,182 @@
       <c r="F2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G2" t="s">
-        <v>39</v>
-      </c>
-      <c r="H2" t="s">
-        <v>40</v>
-      </c>
-      <c r="I2" t="s">
-        <v>58</v>
-      </c>
-      <c r="J2" t="s">
-        <v>41</v>
-      </c>
-      <c r="K2" t="s">
-        <v>42</v>
-      </c>
-      <c r="L2" t="s">
-        <v>43</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="N2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>136</v>
+      <c r="B3" t="s">
+        <v>107</v>
       </c>
       <c r="C3" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="D3" t="s">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="E3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I3" t="s">
-        <v>56</v>
-      </c>
-      <c r="J3" t="s">
-        <v>46</v>
-      </c>
-      <c r="K3" t="s">
-        <v>48</v>
-      </c>
-      <c r="L3" t="s">
-        <v>44</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="N3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>129</v>
+      <c r="B4" t="s">
+        <v>108</v>
       </c>
       <c r="C4" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="E4" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I4" t="s">
-        <v>57</v>
-      </c>
-      <c r="J4" t="s">
-        <v>47</v>
-      </c>
-      <c r="K4" t="s">
-        <v>49</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="M4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="N4" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>130</v>
+      <c r="B5" t="s">
+        <v>109</v>
       </c>
       <c r="C5" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="D5" t="s">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="E5" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I5" t="s">
-        <v>59</v>
-      </c>
-      <c r="J5" t="s">
-        <v>41</v>
-      </c>
-      <c r="K5" t="s">
-        <v>48</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="N5" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>131</v>
+      <c r="B6" t="s">
+        <v>110</v>
       </c>
       <c r="C6" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="D6" t="s">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="E6" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G6" t="s">
-        <v>162</v>
-      </c>
-      <c r="H6" t="s">
-        <v>163</v>
-      </c>
-      <c r="I6" t="s">
-        <v>58</v>
-      </c>
-      <c r="J6" t="s">
-        <v>41</v>
-      </c>
-      <c r="K6" t="s">
-        <v>42</v>
-      </c>
-      <c r="L6" t="s">
-        <v>43</v>
-      </c>
-      <c r="M6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="N6" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15">
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>132</v>
+      <c r="B7" t="s">
+        <v>111</v>
       </c>
       <c r="C7" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="D7" t="s">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="E7" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="J7" t="s">
-        <v>46</v>
-      </c>
-      <c r="K7" t="s">
-        <v>42</v>
-      </c>
-      <c r="N7" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15">
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>133</v>
+      <c r="B8" t="s">
+        <v>112</v>
       </c>
       <c r="C8" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="D8" t="s">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="E8" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="N8" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15">
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>134</v>
+      <c r="B9" t="s">
+        <v>113</v>
       </c>
       <c r="C9" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="D9" t="s">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="E9" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>135</v>
+      <c r="B10" t="s">
+        <v>114</v>
       </c>
       <c r="C10" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="D10" t="s">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="E10" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>137</v>
+      <c r="B11" t="s">
+        <v>115</v>
       </c>
       <c r="C11" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="D11" t="s">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="E11" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>18</v>
@@ -4214,43 +4455,435 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
-    <hyperlink ref="F3" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
-    <hyperlink ref="F4" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
-    <hyperlink ref="F5" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
-    <hyperlink ref="F6" r:id="rId5" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
-    <hyperlink ref="F7" r:id="rId6" xr:uid="{00000000-0004-0000-0200-000005000000}"/>
-    <hyperlink ref="F8" r:id="rId7" xr:uid="{00000000-0004-0000-0200-000006000000}"/>
-    <hyperlink ref="F9" r:id="rId8" xr:uid="{00000000-0004-0000-0200-000007000000}"/>
-    <hyperlink ref="F10" r:id="rId9" xr:uid="{00000000-0004-0000-0200-000008000000}"/>
-    <hyperlink ref="F11" r:id="rId10" xr:uid="{00000000-0004-0000-0200-000009000000}"/>
+    <hyperlink ref="F2" r:id="rId1"/>
+    <hyperlink ref="F3:F11" r:id="rId2" display="Admin@123"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L29" sqref="L29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I2" t="s">
+        <v>58</v>
+      </c>
+      <c r="J2" t="s">
+        <v>41</v>
+      </c>
+      <c r="K2" t="s">
+        <v>42</v>
+      </c>
+      <c r="L2" t="s">
+        <v>43</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="N2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="C3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" t="s">
+        <v>56</v>
+      </c>
+      <c r="J3" t="s">
+        <v>46</v>
+      </c>
+      <c r="K3" t="s">
+        <v>48</v>
+      </c>
+      <c r="L3" t="s">
+        <v>44</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="N3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I4" t="s">
+        <v>57</v>
+      </c>
+      <c r="J4" t="s">
+        <v>47</v>
+      </c>
+      <c r="K4" t="s">
+        <v>49</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="N4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I5" t="s">
+        <v>59</v>
+      </c>
+      <c r="J5" t="s">
+        <v>41</v>
+      </c>
+      <c r="K5" t="s">
+        <v>48</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="N5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="C6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" t="s">
+        <v>162</v>
+      </c>
+      <c r="H6" t="s">
+        <v>163</v>
+      </c>
+      <c r="I6" t="s">
+        <v>58</v>
+      </c>
+      <c r="J6" t="s">
+        <v>41</v>
+      </c>
+      <c r="K6" t="s">
+        <v>42</v>
+      </c>
+      <c r="L6" t="s">
+        <v>43</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="N6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J7" t="s">
+        <v>46</v>
+      </c>
+      <c r="K7" t="s">
+        <v>42</v>
+      </c>
+      <c r="N7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="C8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="N8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="C9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="F2" r:id="rId1"/>
+    <hyperlink ref="F3" r:id="rId2"/>
+    <hyperlink ref="F4" r:id="rId3"/>
+    <hyperlink ref="F5" r:id="rId4"/>
+    <hyperlink ref="F6" r:id="rId5"/>
+    <hyperlink ref="F7" r:id="rId6"/>
+    <hyperlink ref="F8" r:id="rId7"/>
+    <hyperlink ref="F9" r:id="rId8"/>
+    <hyperlink ref="F10" r:id="rId9"/>
+    <hyperlink ref="F11" r:id="rId10"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.77734375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.77734375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4282,7 +4915,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -4314,7 +4947,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -4334,7 +4967,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -4354,7 +4987,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -4386,7 +5019,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -4406,7 +5039,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
@@ -4426,7 +5059,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
@@ -4446,7 +5079,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
@@ -4466,7 +5099,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
@@ -4498,7 +5131,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
@@ -4521,45 +5154,45 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{A86743D9-EA7F-423D-BAA6-68A740AC3D80}"/>
-    <hyperlink ref="I2" r:id="rId2" xr:uid="{E7CFB2BD-C6BE-44EB-AE4C-FA39C50580F1}"/>
-    <hyperlink ref="J2" r:id="rId3" xr:uid="{717D2B13-45AD-48C1-A07A-146CDADB5D82}"/>
-    <hyperlink ref="F3:F11" r:id="rId4" display="Admin@123" xr:uid="{3CAF8F96-E222-4F94-8A70-9C685341A998}"/>
-    <hyperlink ref="I5" r:id="rId5" xr:uid="{7EF764BC-844B-47F7-A73F-C9D41C057AD3}"/>
-    <hyperlink ref="J5" r:id="rId6" xr:uid="{0611619D-9970-4F64-A28C-D8BAC5BF4492}"/>
-    <hyperlink ref="I10" r:id="rId7" xr:uid="{552B24E7-9F5D-4166-8001-7B76A5A7756F}"/>
-    <hyperlink ref="J10" r:id="rId8" xr:uid="{36C8351A-57C7-498A-9EC5-851023D83150}"/>
+    <hyperlink ref="F2" r:id="rId1"/>
+    <hyperlink ref="I2" r:id="rId2"/>
+    <hyperlink ref="J2" r:id="rId3"/>
+    <hyperlink ref="F3:F11" r:id="rId4" display="Admin@123"/>
+    <hyperlink ref="I5" r:id="rId5"/>
+    <hyperlink ref="J5" r:id="rId6"/>
+    <hyperlink ref="I10" r:id="rId7"/>
+    <hyperlink ref="J10" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G8" sqref="G8:L8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.21875" style="8"/>
-    <col min="2" max="2" width="15.88671875" style="8" customWidth="1"/>
-    <col min="3" max="3" width="30.77734375" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="39.21875" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.44140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.77734375" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.21875" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.5546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.77734375" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.28515625" style="8"/>
+    <col min="2" max="2" width="15.85546875" style="8" customWidth="1"/>
+    <col min="3" max="3" width="30.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" style="8" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17" style="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.77734375" style="8" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.77734375" style="8" customWidth="1"/>
-    <col min="13" max="16384" width="9.21875" style="8"/>
+    <col min="11" max="11" width="20.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.7109375" style="8" customWidth="1"/>
+    <col min="13" max="16384" width="9.28515625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="28.8">
+    <row r="1" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -4597,7 +5230,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="28.8">
+    <row r="2" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>5</v>
       </c>
@@ -4635,7 +5268,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>6</v>
       </c>
@@ -4661,7 +5294,7 @@
       <c r="K3" s="10"/>
       <c r="L3" s="10"/>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>7</v>
       </c>
@@ -4687,7 +5320,7 @@
       <c r="K4" s="10"/>
       <c r="L4" s="10"/>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>8</v>
       </c>
@@ -4713,7 +5346,7 @@
       <c r="K5" s="10"/>
       <c r="L5" s="10"/>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>9</v>
       </c>
@@ -4739,7 +5372,7 @@
       <c r="K6" s="10"/>
       <c r="L6" s="10"/>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>10</v>
       </c>
@@ -4765,7 +5398,7 @@
       <c r="K7" s="10"/>
       <c r="L7" s="10"/>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>11</v>
       </c>
@@ -4791,7 +5424,7 @@
       <c r="K8" s="10"/>
       <c r="L8" s="10"/>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>12</v>
       </c>
@@ -4817,7 +5450,7 @@
       <c r="K9" s="10"/>
       <c r="L9" s="10"/>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>13</v>
       </c>
@@ -4843,7 +5476,7 @@
       <c r="K10" s="10"/>
       <c r="L10" s="10"/>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>14</v>
       </c>
@@ -4869,49 +5502,49 @@
       <c r="K11" s="10"/>
       <c r="L11" s="10"/>
     </row>
-    <row r="17" spans="7:7">
+    <row r="17" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G17" s="16"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="F11" r:id="rId1" xr:uid="{00000000-0004-0000-0700-000000000000}"/>
-    <hyperlink ref="F10" r:id="rId2" xr:uid="{00000000-0004-0000-0700-000001000000}"/>
-    <hyperlink ref="F9" r:id="rId3" xr:uid="{00000000-0004-0000-0700-000002000000}"/>
-    <hyperlink ref="F8" r:id="rId4" xr:uid="{00000000-0004-0000-0700-000003000000}"/>
-    <hyperlink ref="F7" r:id="rId5" xr:uid="{00000000-0004-0000-0700-000004000000}"/>
-    <hyperlink ref="F6" r:id="rId6" xr:uid="{00000000-0004-0000-0700-000005000000}"/>
-    <hyperlink ref="F5" r:id="rId7" xr:uid="{00000000-0004-0000-0700-000006000000}"/>
-    <hyperlink ref="F4" r:id="rId8" xr:uid="{00000000-0004-0000-0700-000007000000}"/>
-    <hyperlink ref="F3" r:id="rId9" xr:uid="{00000000-0004-0000-0700-000008000000}"/>
-    <hyperlink ref="F2" r:id="rId10" xr:uid="{00000000-0004-0000-0700-000009000000}"/>
+    <hyperlink ref="F11" r:id="rId1"/>
+    <hyperlink ref="F10" r:id="rId2"/>
+    <hyperlink ref="F9" r:id="rId3"/>
+    <hyperlink ref="F8" r:id="rId4"/>
+    <hyperlink ref="F7" r:id="rId5"/>
+    <hyperlink ref="F6" r:id="rId6"/>
+    <hyperlink ref="F5" r:id="rId7"/>
+    <hyperlink ref="F4" r:id="rId8"/>
+    <hyperlink ref="F3" r:id="rId9"/>
+    <hyperlink ref="F2" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId11"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="G2:P11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4961,7 +5594,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -4981,7 +5614,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -5001,7 +5634,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -5021,7 +5654,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -5041,7 +5674,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -5061,7 +5694,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
@@ -5081,7 +5714,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
@@ -5101,7 +5734,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
@@ -5121,7 +5754,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
@@ -5141,7 +5774,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:16">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
@@ -5164,50 +5797,50 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{3FC25540-546C-4207-977C-DC1D6263849C}"/>
-    <hyperlink ref="F2" r:id="rId2" xr:uid="{B11E9984-9A8C-4926-8F34-9841DFCCE15C}"/>
-    <hyperlink ref="E3" r:id="rId3" xr:uid="{7933D716-122A-4B5A-861B-F3FE8C7EA461}"/>
-    <hyperlink ref="E4" r:id="rId4" xr:uid="{3A31F0AE-5B65-4453-8CED-1A89C0738006}"/>
-    <hyperlink ref="E5" r:id="rId5" xr:uid="{80DF605C-575D-4FBA-80E1-9735F9A21964}"/>
-    <hyperlink ref="E6" r:id="rId6" xr:uid="{FBF760A1-06D4-40F1-87EF-C8780018D99F}"/>
-    <hyperlink ref="E7" r:id="rId7" xr:uid="{68C456AD-4CFE-4664-B7ED-3C95ACB453E6}"/>
-    <hyperlink ref="E8" r:id="rId8" xr:uid="{26F76375-2E00-4B03-933C-DA5DD83459AB}"/>
-    <hyperlink ref="E9" r:id="rId9" xr:uid="{496C49AF-735A-48F8-B9E9-C498518B5C74}"/>
-    <hyperlink ref="E10" r:id="rId10" xr:uid="{1E948641-3A9E-4A24-AC96-5C92156AE295}"/>
-    <hyperlink ref="E11" r:id="rId11" xr:uid="{E2918D78-FCDD-48C4-BE45-C22C26315337}"/>
-    <hyperlink ref="F3" r:id="rId12" xr:uid="{9D625209-54EB-4E01-BD02-BF477AEB854A}"/>
-    <hyperlink ref="F4" r:id="rId13" xr:uid="{29FC461B-6E07-4982-9ADA-67D134ACC0BD}"/>
-    <hyperlink ref="F5" r:id="rId14" xr:uid="{4C858938-BDEA-459E-BC03-F648CFF14EAD}"/>
-    <hyperlink ref="F6" r:id="rId15" xr:uid="{5405D72C-30A0-4455-92C1-6513942346A2}"/>
-    <hyperlink ref="F7" r:id="rId16" xr:uid="{04372048-749D-4069-A80B-1E6122BE8D09}"/>
-    <hyperlink ref="F8" r:id="rId17" xr:uid="{110FD36F-6728-43BE-9952-48C4E78C155B}"/>
-    <hyperlink ref="F9" r:id="rId18" xr:uid="{47DAE3DC-D76E-43E8-B6E2-51D8031FA458}"/>
-    <hyperlink ref="F10" r:id="rId19" xr:uid="{4DEFE580-B6D8-4BF7-9740-A553E2FA1EC5}"/>
-    <hyperlink ref="F11" r:id="rId20" xr:uid="{4F6BB619-7603-498D-AD13-E73CF263ADAD}"/>
+    <hyperlink ref="E2" r:id="rId1"/>
+    <hyperlink ref="F2" r:id="rId2"/>
+    <hyperlink ref="E3" r:id="rId3"/>
+    <hyperlink ref="E4" r:id="rId4"/>
+    <hyperlink ref="E5" r:id="rId5"/>
+    <hyperlink ref="E6" r:id="rId6"/>
+    <hyperlink ref="E7" r:id="rId7"/>
+    <hyperlink ref="E8" r:id="rId8"/>
+    <hyperlink ref="E9" r:id="rId9"/>
+    <hyperlink ref="E10" r:id="rId10"/>
+    <hyperlink ref="E11" r:id="rId11"/>
+    <hyperlink ref="F3" r:id="rId12"/>
+    <hyperlink ref="F4" r:id="rId13"/>
+    <hyperlink ref="F5" r:id="rId14"/>
+    <hyperlink ref="F6" r:id="rId15"/>
+    <hyperlink ref="F7" r:id="rId16"/>
+    <hyperlink ref="F8" r:id="rId17"/>
+    <hyperlink ref="F9" r:id="rId18"/>
+    <hyperlink ref="F10" r:id="rId19"/>
+    <hyperlink ref="F11" r:id="rId20"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G3" sqref="G3:G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="28" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="34" customWidth="1"/>
     <col min="5" max="5" width="23" customWidth="1"/>
-    <col min="6" max="6" width="11.21875" customWidth="1"/>
-    <col min="7" max="7" width="21.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" customWidth="1"/>
+    <col min="7" max="7" width="21.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5230,7 +5863,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -5253,7 +5886,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -5273,7 +5906,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -5293,7 +5926,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -5313,7 +5946,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -5333,7 +5966,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
@@ -5353,7 +5986,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
@@ -5373,7 +6006,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
@@ -5393,7 +6026,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
@@ -5413,7 +6046,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
@@ -5436,290 +6069,18 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
-    <hyperlink ref="E3:E11" r:id="rId2" display="aarosagarch@gmail.com" xr:uid="{00000000-0004-0000-0500-000001000000}"/>
-    <hyperlink ref="F2" r:id="rId3" xr:uid="{00000000-0004-0000-0500-000002000000}"/>
-    <hyperlink ref="F3" r:id="rId4" xr:uid="{00000000-0004-0000-0500-000003000000}"/>
-    <hyperlink ref="F4" r:id="rId5" xr:uid="{00000000-0004-0000-0500-000004000000}"/>
-    <hyperlink ref="F5" r:id="rId6" xr:uid="{00000000-0004-0000-0500-000005000000}"/>
-    <hyperlink ref="F6" r:id="rId7" xr:uid="{00000000-0004-0000-0500-000006000000}"/>
-    <hyperlink ref="F7" r:id="rId8" xr:uid="{00000000-0004-0000-0500-000007000000}"/>
-    <hyperlink ref="F8" r:id="rId9" xr:uid="{00000000-0004-0000-0500-000008000000}"/>
-    <hyperlink ref="F9" r:id="rId10" xr:uid="{00000000-0004-0000-0500-000009000000}"/>
-    <hyperlink ref="F10" r:id="rId11" xr:uid="{00000000-0004-0000-0500-00000A000000}"/>
-    <hyperlink ref="F11" r:id="rId12" xr:uid="{00000000-0004-0000-0500-00000B000000}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId13"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:H11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
-  <cols>
-    <col min="2" max="2" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="41.21875" customWidth="1"/>
-    <col min="4" max="4" width="40" customWidth="1"/>
-    <col min="5" max="5" width="24.44140625" customWidth="1"/>
-    <col min="6" max="6" width="19.5546875" customWidth="1"/>
-    <col min="7" max="7" width="22.77734375" customWidth="1"/>
-    <col min="8" max="8" width="20.21875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>295</v>
-      </c>
-      <c r="C2" t="s">
-        <v>294</v>
-      </c>
-      <c r="D2" t="s">
-        <v>66</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2" t="s">
-        <v>69</v>
-      </c>
-      <c r="H2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>303</v>
-      </c>
-      <c r="C3" t="s">
-        <v>294</v>
-      </c>
-      <c r="D3" t="s">
-        <v>66</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>296</v>
-      </c>
-      <c r="C4" t="s">
-        <v>294</v>
-      </c>
-      <c r="D4" t="s">
-        <v>66</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>297</v>
-      </c>
-      <c r="C5" t="s">
-        <v>294</v>
-      </c>
-      <c r="D5" t="s">
-        <v>66</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="C6" t="s">
-        <v>294</v>
-      </c>
-      <c r="D6" t="s">
-        <v>66</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>299</v>
-      </c>
-      <c r="C7" t="s">
-        <v>294</v>
-      </c>
-      <c r="D7" t="s">
-        <v>66</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>300</v>
-      </c>
-      <c r="C8" t="s">
-        <v>294</v>
-      </c>
-      <c r="D8" t="s">
-        <v>66</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>301</v>
-      </c>
-      <c r="C9" t="s">
-        <v>294</v>
-      </c>
-      <c r="D9" t="s">
-        <v>66</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="A10" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>302</v>
-      </c>
-      <c r="C10" t="s">
-        <v>294</v>
-      </c>
-      <c r="D10" t="s">
-        <v>66</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="A11" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>304</v>
-      </c>
-      <c r="C11" t="s">
-        <v>294</v>
-      </c>
-      <c r="D11" t="s">
-        <v>66</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
-    <hyperlink ref="E3:E11" r:id="rId2" display="aarosagarch@gmail.com" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
-    <hyperlink ref="F2" r:id="rId3" xr:uid="{00000000-0004-0000-0400-000002000000}"/>
-    <hyperlink ref="F3" r:id="rId4" xr:uid="{00000000-0004-0000-0400-000003000000}"/>
-    <hyperlink ref="F4" r:id="rId5" xr:uid="{00000000-0004-0000-0400-000004000000}"/>
-    <hyperlink ref="F5" r:id="rId6" xr:uid="{00000000-0004-0000-0400-000005000000}"/>
-    <hyperlink ref="F6" r:id="rId7" xr:uid="{00000000-0004-0000-0400-000006000000}"/>
-    <hyperlink ref="F7" r:id="rId8" xr:uid="{00000000-0004-0000-0400-000007000000}"/>
-    <hyperlink ref="F8" r:id="rId9" xr:uid="{00000000-0004-0000-0400-000008000000}"/>
-    <hyperlink ref="F9" r:id="rId10" xr:uid="{00000000-0004-0000-0400-000009000000}"/>
-    <hyperlink ref="F10" r:id="rId11" xr:uid="{00000000-0004-0000-0400-00000A000000}"/>
-    <hyperlink ref="F11" r:id="rId12" xr:uid="{00000000-0004-0000-0400-00000B000000}"/>
+    <hyperlink ref="E2" r:id="rId1"/>
+    <hyperlink ref="E3:E11" r:id="rId2" display="aarosagarch@gmail.com"/>
+    <hyperlink ref="F2" r:id="rId3"/>
+    <hyperlink ref="F3" r:id="rId4"/>
+    <hyperlink ref="F4" r:id="rId5"/>
+    <hyperlink ref="F5" r:id="rId6"/>
+    <hyperlink ref="F6" r:id="rId7"/>
+    <hyperlink ref="F7" r:id="rId8"/>
+    <hyperlink ref="F8" r:id="rId9"/>
+    <hyperlink ref="F9" r:id="rId10"/>
+    <hyperlink ref="F10" r:id="rId11"/>
+    <hyperlink ref="F11" r:id="rId12"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId13"/>
@@ -5727,266 +6088,273 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="41.77734375" customWidth="1"/>
-    <col min="4" max="4" width="34.21875" customWidth="1"/>
-    <col min="5" max="5" width="22.5546875" customWidth="1"/>
-    <col min="6" max="6" width="11.21875" customWidth="1"/>
-    <col min="7" max="7" width="23" customWidth="1"/>
-    <col min="8" max="8" width="15.77734375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.77734375" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.28515625" customWidth="1"/>
+    <col min="4" max="4" width="40" customWidth="1"/>
+    <col min="5" max="5" width="24.42578125" customWidth="1"/>
+    <col min="6" max="6" width="19.5703125" customWidth="1"/>
+    <col min="7" max="7" width="22.7109375" customWidth="1"/>
+    <col min="8" max="8" width="20.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>89</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>102</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>90</v>
+        <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>91</v>
+        <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>93</v>
+        <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>94</v>
+        <v>67</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>306</v>
+        <v>295</v>
       </c>
       <c r="C2" t="s">
-        <v>305</v>
+        <v>294</v>
       </c>
       <c r="D2" t="s">
-        <v>92</v>
-      </c>
-      <c r="E2" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="F2" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I2" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
+      <c r="F2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" t="s">
+        <v>69</v>
+      </c>
+      <c r="H2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>314</v>
+        <v>303</v>
       </c>
       <c r="C3" t="s">
-        <v>305</v>
+        <v>294</v>
       </c>
       <c r="D3" t="s">
-        <v>92</v>
-      </c>
-      <c r="E3" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="F3" s="13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
+      <c r="F3" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>307</v>
+        <v>296</v>
       </c>
       <c r="C4" t="s">
-        <v>305</v>
+        <v>294</v>
       </c>
       <c r="D4" t="s">
-        <v>92</v>
-      </c>
-      <c r="E4" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="F4" s="13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
+      <c r="F4" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>308</v>
+        <v>297</v>
       </c>
       <c r="C5" t="s">
-        <v>305</v>
+        <v>294</v>
       </c>
       <c r="D5" t="s">
-        <v>92</v>
-      </c>
-      <c r="E5" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="F5" s="13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
+      <c r="F5" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>309</v>
+        <v>298</v>
       </c>
       <c r="C6" t="s">
-        <v>305</v>
+        <v>294</v>
       </c>
       <c r="D6" t="s">
-        <v>92</v>
-      </c>
-      <c r="E6" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="F6" s="13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
+      <c r="F6" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>310</v>
+        <v>299</v>
       </c>
       <c r="C7" t="s">
-        <v>305</v>
+        <v>294</v>
       </c>
       <c r="D7" t="s">
-        <v>92</v>
-      </c>
-      <c r="E7" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="F7" s="13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
+      <c r="F7" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>311</v>
+        <v>300</v>
       </c>
       <c r="C8" t="s">
-        <v>305</v>
+        <v>294</v>
       </c>
       <c r="D8" t="s">
-        <v>92</v>
-      </c>
-      <c r="E8" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="F8" s="13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
+      <c r="F8" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>312</v>
+        <v>301</v>
       </c>
       <c r="C9" t="s">
-        <v>305</v>
+        <v>294</v>
       </c>
       <c r="D9" t="s">
-        <v>92</v>
-      </c>
-      <c r="E9" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="E9" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="F9" s="13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
+      <c r="F9" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>313</v>
+        <v>302</v>
       </c>
       <c r="C10" t="s">
-        <v>305</v>
+        <v>294</v>
       </c>
       <c r="D10" t="s">
-        <v>92</v>
-      </c>
-      <c r="E10" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="E10" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="F10" s="13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
+      <c r="F10" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>315</v>
+        <v>304</v>
       </c>
       <c r="C11" t="s">
-        <v>305</v>
+        <v>294</v>
       </c>
       <c r="D11" t="s">
-        <v>92</v>
-      </c>
-      <c r="E11" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="E11" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="F11" s="13" t="s">
+      <c r="F11" s="3" t="s">
         <v>18</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1"/>
+    <hyperlink ref="E3:E11" r:id="rId2" display="aarosagarch@gmail.com"/>
+    <hyperlink ref="F2" r:id="rId3"/>
+    <hyperlink ref="F3" r:id="rId4"/>
+    <hyperlink ref="F4" r:id="rId5"/>
+    <hyperlink ref="F5" r:id="rId6"/>
+    <hyperlink ref="F6" r:id="rId7"/>
+    <hyperlink ref="F7" r:id="rId8"/>
+    <hyperlink ref="F8" r:id="rId9"/>
+    <hyperlink ref="F9" r:id="rId10"/>
+    <hyperlink ref="F10" r:id="rId11"/>
+    <hyperlink ref="F11" r:id="rId12"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId13"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Excel Utilities are enhanced and ITestResult Listener is added
</commit_message>
<xml_diff>
--- a/src/main/resources/AutomationCatalogue_Batch41_TestData.xlsx
+++ b/src/main/resources/AutomationCatalogue_Batch41_TestData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AutomationCatalogue\TestAutomationCatalogue_Batch41\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AutomationCatalogue\Projects\TestAutomationCatalogue_Batch41\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBEC8E3E-2F44-4AC1-9379-46477E25F28A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C6883C3-486F-4A07-95B8-60CB7AACED24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="944" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="944" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="10" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1188" uniqueCount="365">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1192" uniqueCount="369">
   <si>
     <t>S. No</t>
   </si>
@@ -1129,6 +1129,18 @@
   </si>
   <si>
     <t>Shiva123</t>
+  </si>
+  <si>
+    <t>Order number: 1488790</t>
+  </si>
+  <si>
+    <t>PASSED</t>
+  </si>
+  <si>
+    <t>FAILED</t>
+  </si>
+  <si>
+    <t>Title is not matched</t>
   </si>
 </sst>
 </file>
@@ -1599,17 +1611,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90270A87-C874-4975-9C16-F9436E7DA963}">
   <dimension ref="A1:F122"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B76" sqref="B76"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="39" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="38" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1955,6 +1967,12 @@
       <c r="D25" t="s">
         <v>99</v>
       </c>
+      <c r="E25" t="s">
+        <v>367</v>
+      </c>
+      <c r="F25" t="s">
+        <v>368</v>
+      </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="2" t="s">
@@ -2802,6 +2820,9 @@
       </c>
       <c r="D87" t="s">
         <v>64</v>
+      </c>
+      <c r="E87" t="s">
+        <v>366</v>
       </c>
     </row>
     <row r="88" spans="1:6">
@@ -3297,18 +3318,18 @@
       <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="6.453125" customWidth="1"/>
-    <col min="2" max="2" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="40.1796875" customWidth="1"/>
-    <col min="5" max="5" width="22.81640625" customWidth="1"/>
-    <col min="6" max="6" width="12.453125" customWidth="1"/>
-    <col min="7" max="7" width="21.453125" customWidth="1"/>
-    <col min="8" max="8" width="21.1796875" customWidth="1"/>
-    <col min="9" max="9" width="18.1796875" customWidth="1"/>
-    <col min="10" max="10" width="9.1796875" customWidth="1"/>
+    <col min="1" max="1" width="6.44140625" customWidth="1"/>
+    <col min="2" max="2" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.21875" customWidth="1"/>
+    <col min="5" max="5" width="22.77734375" customWidth="1"/>
+    <col min="6" max="6" width="12.44140625" customWidth="1"/>
+    <col min="7" max="7" width="21.44140625" customWidth="1"/>
+    <col min="8" max="8" width="21.21875" customWidth="1"/>
+    <col min="9" max="9" width="18.21875" customWidth="1"/>
+    <col min="10" max="10" width="9.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -3632,13 +3653,13 @@
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26" customWidth="1"/>
-    <col min="4" max="4" width="24.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -3879,20 +3900,20 @@
       <selection activeCell="L29" sqref="L29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="38" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.44140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.81640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
@@ -4275,21 +4296,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.08984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.36328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.81640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.81640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.36328125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -4682,24 +4703,24 @@
       <selection activeCell="G8" sqref="G8:L8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="9.1796875" style="8"/>
-    <col min="2" max="2" width="15.90625" style="8" customWidth="1"/>
-    <col min="3" max="3" width="30.81640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="39.1796875" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.453125" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.81640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.1796875" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.54296875" style="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.81640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.21875" style="8"/>
+    <col min="2" max="2" width="15.88671875" style="8" customWidth="1"/>
+    <col min="3" max="3" width="30.77734375" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.21875" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.44140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.77734375" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.21875" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.77734375" style="8" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17" style="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.81640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.81640625" style="8" customWidth="1"/>
-    <col min="13" max="16384" width="9.1796875" style="8"/>
+    <col min="11" max="11" width="20.77734375" style="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.77734375" style="8" customWidth="1"/>
+    <col min="13" max="16384" width="9.21875" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="29">
+    <row r="1" spans="1:12" ht="28.8">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -4737,7 +4758,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="29">
+    <row r="2" spans="1:12" ht="28.8">
       <c r="A2" s="9" t="s">
         <v>5</v>
       </c>
@@ -5039,16 +5060,16 @@
       <selection activeCell="G2" sqref="G2:P11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.90625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.08984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.36328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="9.90625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.08984375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16">
@@ -5337,14 +5358,14 @@
       <selection activeCell="G3" sqref="G3:G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="28" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="34" customWidth="1"/>
     <col min="5" max="5" width="23" customWidth="1"/>
-    <col min="6" max="6" width="11.1796875" customWidth="1"/>
-    <col min="7" max="7" width="21.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.21875" customWidth="1"/>
+    <col min="7" max="7" width="21.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -5531,6 +5552,9 @@
       </c>
       <c r="F9" s="3" t="s">
         <v>18</v>
+      </c>
+      <c r="G9" t="s">
+        <v>365</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -5602,15 +5626,15 @@
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="41.1796875" customWidth="1"/>
+    <col min="2" max="2" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.21875" customWidth="1"/>
     <col min="4" max="4" width="40" customWidth="1"/>
-    <col min="5" max="5" width="24.453125" customWidth="1"/>
-    <col min="6" max="6" width="19.54296875" customWidth="1"/>
-    <col min="7" max="7" width="22.81640625" customWidth="1"/>
-    <col min="8" max="8" width="20.1796875" customWidth="1"/>
+    <col min="5" max="5" width="24.44140625" customWidth="1"/>
+    <col min="6" max="6" width="19.5546875" customWidth="1"/>
+    <col min="7" max="7" width="22.77734375" customWidth="1"/>
+    <col min="8" max="8" width="20.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -5874,16 +5898,16 @@
       <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="41.81640625" customWidth="1"/>
-    <col min="4" max="4" width="34.1796875" customWidth="1"/>
-    <col min="5" max="5" width="22.54296875" customWidth="1"/>
-    <col min="6" max="6" width="11.1796875" customWidth="1"/>
+    <col min="2" max="2" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.77734375" customWidth="1"/>
+    <col min="4" max="4" width="34.21875" customWidth="1"/>
+    <col min="5" max="5" width="22.5546875" customWidth="1"/>
+    <col min="6" max="6" width="11.21875" customWidth="1"/>
     <col min="7" max="7" width="23" customWidth="1"/>
-    <col min="8" max="8" width="15.81640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.81640625" customWidth="1"/>
+    <col min="8" max="8" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">

</xml_diff>

<commit_message>
Changes made to the TC05_OrangeHRM_Travel request test case.
</commit_message>
<xml_diff>
--- a/src/main/resources/AutomationCatalogue_Batch41_TestData.xlsx
+++ b/src/main/resources/AutomationCatalogue_Batch41_TestData.xlsx
@@ -5,36 +5,48 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AutomationCatalogue\Projects\TestAutomationCatalogue_Batch41\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Automation Catalogue\TestAutomationCatalogue_Batch41\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{339C1403-EB4E-4969-823E-EFDDC38155BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17661E78-B2A7-4C97-A3B9-F15F5309B848}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="944" firstSheet="2" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-1095" windowWidth="29040" windowHeight="15720" tabRatio="944" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="10" r:id="rId1"/>
     <sheet name="OrangeHRM_Login" sheetId="1" r:id="rId2"/>
     <sheet name="OrangeHRM_AddEmployee" sheetId="2" r:id="rId3"/>
-    <sheet name="OrangeHRM_AddUser" sheetId="3" r:id="rId4"/>
-    <sheet name="OrangeHRM_EditEmployee" sheetId="8" r:id="rId5"/>
-    <sheet name="DemoWebshop_CreateAddress" sheetId="5" r:id="rId6"/>
-    <sheet name="DemoWebshop_ReOrder" sheetId="4" r:id="rId7"/>
-    <sheet name="DemoWebshop_TotalOrders" sheetId="6" r:id="rId8"/>
-    <sheet name="DemoWebshop_UpdateShoppingCart" sheetId="9" r:id="rId9"/>
-    <sheet name="DemoWebshop_ApplyDiscount" sheetId="7" r:id="rId10"/>
+    <sheet name="OrangeHRM_TravelExpense" sheetId="11" r:id="rId4"/>
+    <sheet name="OrangeHRM_AddUser" sheetId="3" r:id="rId5"/>
+    <sheet name="OrangeHRM_EditEmployee" sheetId="8" r:id="rId6"/>
+    <sheet name="DemoWebshop_CreateAddress" sheetId="5" r:id="rId7"/>
+    <sheet name="DemoWebshop_ReOrder" sheetId="4" r:id="rId8"/>
+    <sheet name="DemoWebshop_TotalOrders" sheetId="6" r:id="rId9"/>
+    <sheet name="DemoWebshop_UpdateShoppingCart" sheetId="9" r:id="rId10"/>
+    <sheet name="DemoWebshop_ApplyDiscount" sheetId="7" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1156" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1387" uniqueCount="450">
   <si>
     <t>S. No</t>
   </si>
@@ -522,12 +534,6 @@
     <t>Sagar123</t>
   </si>
   <si>
-    <t>Automation</t>
-  </si>
-  <si>
-    <t>Catalogue</t>
-  </si>
-  <si>
     <t>31</t>
   </si>
   <si>
@@ -1081,6 +1087,315 @@
   </si>
   <si>
     <t>110</t>
+  </si>
+  <si>
+    <t>Christopher</t>
+  </si>
+  <si>
+    <t>Anderson</t>
+  </si>
+  <si>
+    <t>Ronald</t>
+  </si>
+  <si>
+    <t>Clark</t>
+  </si>
+  <si>
+    <t>Mary</t>
+  </si>
+  <si>
+    <t>Wright</t>
+  </si>
+  <si>
+    <t>Lisa</t>
+  </si>
+  <si>
+    <t>Mitchell</t>
+  </si>
+  <si>
+    <t>Jamaica training center</t>
+  </si>
+  <si>
+    <t>Michelle</t>
+  </si>
+  <si>
+    <t>Johnson</t>
+  </si>
+  <si>
+    <t>Kenya Satalite office</t>
+  </si>
+  <si>
+    <t>Thomas</t>
+  </si>
+  <si>
+    <t>Philippine call center</t>
+  </si>
+  <si>
+    <t>Daniel</t>
+  </si>
+  <si>
+    <t>Rodriguez</t>
+  </si>
+  <si>
+    <t>European Office</t>
+  </si>
+  <si>
+    <t>Anthony</t>
+  </si>
+  <si>
+    <t>Lopez</t>
+  </si>
+  <si>
+    <t>Sheffield Office</t>
+  </si>
+  <si>
+    <t>Patricia</t>
+  </si>
+  <si>
+    <t>Perez</t>
+  </si>
+  <si>
+    <t>US Office</t>
+  </si>
+  <si>
+    <t>New Password</t>
+  </si>
+  <si>
+    <t>Currency</t>
+  </si>
+  <si>
+    <t>Destination</t>
+  </si>
+  <si>
+    <t>Travel From</t>
+  </si>
+  <si>
+    <t>Travel To</t>
+  </si>
+  <si>
+    <t>Expense Type</t>
+  </si>
+  <si>
+    <t>Currency Paidin</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>Paid by</t>
+  </si>
+  <si>
+    <t>Employee Name</t>
+  </si>
+  <si>
+    <t>Travel Req Id</t>
+  </si>
+  <si>
+    <t>Request Status</t>
+  </si>
+  <si>
+    <t>Supervisor Username</t>
+  </si>
+  <si>
+    <t>TC05_OrangeHRM_AddEmployee</t>
+  </si>
+  <si>
+    <t>AED - Utd. Arab Emir. Dirham</t>
+  </si>
+  <si>
+    <t>London</t>
+  </si>
+  <si>
+    <t>1-Jan-2022</t>
+  </si>
+  <si>
+    <t>15-Jan-2022</t>
+  </si>
+  <si>
+    <t>Airfare</t>
+  </si>
+  <si>
+    <t>CAD - Canadian Dollar</t>
+  </si>
+  <si>
+    <t>Chicago</t>
+  </si>
+  <si>
+    <t>1-Feb-2022</t>
+  </si>
+  <si>
+    <t>15-Feb-2022</t>
+  </si>
+  <si>
+    <t>Charitable Donations</t>
+  </si>
+  <si>
+    <t>Staff</t>
+  </si>
+  <si>
+    <t>AUD - Australian Dollar</t>
+  </si>
+  <si>
+    <t>Texas</t>
+  </si>
+  <si>
+    <t>1-Mar-2022</t>
+  </si>
+  <si>
+    <t>15-Mar-2022</t>
+  </si>
+  <si>
+    <t>Entertainment</t>
+  </si>
+  <si>
+    <t>EUR - Euro</t>
+  </si>
+  <si>
+    <t>Canada</t>
+  </si>
+  <si>
+    <t>1-Apr-2022</t>
+  </si>
+  <si>
+    <t>15-Apr-2022</t>
+  </si>
+  <si>
+    <t>Food &amp; Beverage</t>
+  </si>
+  <si>
+    <t>JPY - Japanese Yen</t>
+  </si>
+  <si>
+    <t>Germany</t>
+  </si>
+  <si>
+    <t>1-May-2022</t>
+  </si>
+  <si>
+    <t>15-May-2022</t>
+  </si>
+  <si>
+    <t>Fuel</t>
+  </si>
+  <si>
+    <t>LKR - Sri Lanka Rupee</t>
+  </si>
+  <si>
+    <t>Paris</t>
+  </si>
+  <si>
+    <t>1-Jun-2022</t>
+  </si>
+  <si>
+    <t>15-Jun-2022</t>
+  </si>
+  <si>
+    <t>Ground Transportation</t>
+  </si>
+  <si>
+    <t>PHP - Philippine Peso</t>
+  </si>
+  <si>
+    <t>NewYork</t>
+  </si>
+  <si>
+    <t>1-Jul-2022</t>
+  </si>
+  <si>
+    <t>15-Jul-2022</t>
+  </si>
+  <si>
+    <t>Hotel</t>
+  </si>
+  <si>
+    <t>USD - United States Dollar</t>
+  </si>
+  <si>
+    <t>Vegas</t>
+  </si>
+  <si>
+    <t>1-Aug-2022</t>
+  </si>
+  <si>
+    <t>15-Aug-2022</t>
+  </si>
+  <si>
+    <t>Maintenance &amp; Repairs</t>
+  </si>
+  <si>
+    <t>MXN - Mexican New Peso</t>
+  </si>
+  <si>
+    <t>Pittsburgh</t>
+  </si>
+  <si>
+    <t>1-Sep-2022</t>
+  </si>
+  <si>
+    <t>15-Sep-2022</t>
+  </si>
+  <si>
+    <t>ZMK - Zambian Kwacha</t>
+  </si>
+  <si>
+    <t>NewJersy</t>
+  </si>
+  <si>
+    <t>1-OCt-2022</t>
+  </si>
+  <si>
+    <t>15-Oct-2022</t>
+  </si>
+  <si>
+    <t>Office Supplies</t>
+  </si>
+  <si>
+    <t>Brody Naidu</t>
+  </si>
+  <si>
+    <t>2500</t>
+  </si>
+  <si>
+    <t>500</t>
+  </si>
+  <si>
+    <t>200</t>
+  </si>
+  <si>
+    <t>250</t>
+  </si>
+  <si>
+    <t>150</t>
+  </si>
+  <si>
+    <t>1500</t>
+  </si>
+  <si>
+    <t>John Mikel</t>
+  </si>
+  <si>
+    <t>Christopher Anderson</t>
+  </si>
+  <si>
+    <t>Ronald Clark</t>
+  </si>
+  <si>
+    <t>Mary Wright</t>
+  </si>
+  <si>
+    <t>Lisa Mitchell</t>
+  </si>
+  <si>
+    <t>Michelle Johnson</t>
+  </si>
+  <si>
+    <t>John Thomas</t>
+  </si>
+  <si>
+    <t>Daniel Rodriguez</t>
+  </si>
+  <si>
+    <t>Anthony Lopez</t>
   </si>
 </sst>
 </file>
@@ -1552,7 +1867,7 @@
   <dimension ref="A1:F122"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K118" sqref="K118"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2046,13 +2361,13 @@
     </row>
     <row r="36" spans="1:6">
       <c r="A36" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B36" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C36" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>88</v>
@@ -2060,13 +2375,13 @@
     </row>
     <row r="37" spans="1:6">
       <c r="A37" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B37" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C37" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>88</v>
@@ -2074,13 +2389,13 @@
     </row>
     <row r="38" spans="1:6">
       <c r="A38" s="2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B38" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C38" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>88</v>
@@ -2088,13 +2403,13 @@
     </row>
     <row r="39" spans="1:6">
       <c r="A39" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B39" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C39" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>88</v>
@@ -2102,13 +2417,13 @@
     </row>
     <row r="40" spans="1:6">
       <c r="A40" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B40" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C40" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>88</v>
@@ -2116,13 +2431,13 @@
     </row>
     <row r="41" spans="1:6">
       <c r="A41" s="2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B41" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C41" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>88</v>
@@ -2130,13 +2445,13 @@
     </row>
     <row r="42" spans="1:6">
       <c r="A42" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B42" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C42" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>88</v>
@@ -2144,13 +2459,13 @@
     </row>
     <row r="43" spans="1:6">
       <c r="A43" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B43" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C43" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>88</v>
@@ -2158,13 +2473,13 @@
     </row>
     <row r="44" spans="1:6">
       <c r="A44" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="B44" t="s">
+        <v>180</v>
+      </c>
+      <c r="C44" t="s">
         <v>172</v>
-      </c>
-      <c r="B44" t="s">
-        <v>182</v>
-      </c>
-      <c r="C44" t="s">
-        <v>174</v>
       </c>
       <c r="D44" s="2" t="s">
         <v>88</v>
@@ -2172,13 +2487,13 @@
     </row>
     <row r="45" spans="1:6">
       <c r="A45" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B45" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C45" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>88</v>
@@ -2186,7 +2501,7 @@
     </row>
     <row r="46" spans="1:6">
       <c r="A46" s="15" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B46" s="15"/>
       <c r="C46" s="15"/>
@@ -2196,147 +2511,147 @@
     </row>
     <row r="47" spans="1:6">
       <c r="A47" s="2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B47" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C47" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D47" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="48" spans="1:6">
       <c r="A48" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B48" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C48" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D48" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="49" spans="1:6">
       <c r="A49" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B49" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C49" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D49" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="50" spans="1:6">
       <c r="A50" s="2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B50" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C50" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D50" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="51" spans="1:6">
       <c r="A51" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B51" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C51" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D51" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="52" spans="1:6">
       <c r="A52" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B52" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C52" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D52" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="53" spans="1:6">
       <c r="A53" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B53" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C53" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D53" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="54" spans="1:6">
       <c r="A54" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B54" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C54" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D54" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="55" spans="1:6">
       <c r="A55" s="2" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B55" t="s">
+        <v>202</v>
+      </c>
+      <c r="C55" t="s">
         <v>204</v>
       </c>
-      <c r="C55" t="s">
-        <v>206</v>
-      </c>
       <c r="D55" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="56" spans="1:6">
       <c r="A56" s="2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B56" t="s">
+        <v>203</v>
+      </c>
+      <c r="C56" t="s">
+        <v>204</v>
+      </c>
+      <c r="D56" t="s">
         <v>205</v>
-      </c>
-      <c r="C56" t="s">
-        <v>206</v>
-      </c>
-      <c r="D56" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="57" spans="1:6">
       <c r="A57" s="15" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B57" s="15"/>
       <c r="C57" s="15"/>
@@ -2346,147 +2661,147 @@
     </row>
     <row r="58" spans="1:6">
       <c r="A58" s="2" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B58" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C58" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D58" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="59" spans="1:6">
       <c r="A59" s="2" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B59" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C59" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D59" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="60" spans="1:6">
       <c r="A60" s="2" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B60" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C60" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D60" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="61" spans="1:6">
       <c r="A61" s="2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B61" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C61" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D61" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="62" spans="1:6">
       <c r="A62" s="2" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B62" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C62" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D62" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="63" spans="1:6">
       <c r="A63" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B63" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C63" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D63" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="64" spans="1:6">
       <c r="A64" s="2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B64" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C64" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D64" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="65" spans="1:6">
       <c r="A65" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B65" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C65" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D65" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="66" spans="1:6">
       <c r="A66" s="2" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B66" t="s">
+        <v>225</v>
+      </c>
+      <c r="C66" t="s">
         <v>227</v>
       </c>
-      <c r="C66" t="s">
-        <v>229</v>
-      </c>
       <c r="D66" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="67" spans="1:6">
       <c r="A67" s="2" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B67" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C67" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D67" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="68" spans="1:6">
       <c r="A68" s="15" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B68" s="15"/>
       <c r="C68" s="15"/>
@@ -2496,147 +2811,147 @@
     </row>
     <row r="69" spans="1:6">
       <c r="A69" s="2" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C69" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="D69" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="70" spans="1:6">
       <c r="A70" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C70" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="D70" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="71" spans="1:6">
       <c r="A71" s="2" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C71" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="D71" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="72" spans="1:6">
       <c r="A72" s="2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C72" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="D72" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="73" spans="1:6">
       <c r="A73" s="2" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C73" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="D73" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="74" spans="1:6">
       <c r="A74" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C74" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="D74" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="75" spans="1:6">
       <c r="A75" s="2" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C75" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="D75" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="76" spans="1:6">
       <c r="A76" s="2" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C76" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="D76" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="77" spans="1:6">
       <c r="A77" s="2" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B77" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="C77" t="s">
         <v>239</v>
       </c>
-      <c r="C77" t="s">
-        <v>241</v>
-      </c>
       <c r="D77" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="78" spans="1:6">
       <c r="A78" s="2" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B78" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="C78" t="s">
+        <v>239</v>
+      </c>
+      <c r="D78" t="s">
         <v>240</v>
-      </c>
-      <c r="C78" t="s">
-        <v>241</v>
-      </c>
-      <c r="D78" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="79" spans="1:6">
       <c r="A79" s="15" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B79" s="15"/>
       <c r="C79" s="15"/>
@@ -2646,13 +2961,13 @@
     </row>
     <row r="80" spans="1:6">
       <c r="A80" s="2" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B80" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C80" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D80" t="s">
         <v>64</v>
@@ -2660,13 +2975,13 @@
     </row>
     <row r="81" spans="1:6">
       <c r="A81" s="2" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B81" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C81" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D81" t="s">
         <v>64</v>
@@ -2674,13 +2989,13 @@
     </row>
     <row r="82" spans="1:6">
       <c r="A82" s="2" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B82" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C82" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D82" t="s">
         <v>64</v>
@@ -2688,13 +3003,13 @@
     </row>
     <row r="83" spans="1:6">
       <c r="A83" s="2" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B83" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C83" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D83" t="s">
         <v>64</v>
@@ -2702,13 +3017,13 @@
     </row>
     <row r="84" spans="1:6">
       <c r="A84" s="2" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B84" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C84" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D84" t="s">
         <v>64</v>
@@ -2716,13 +3031,13 @@
     </row>
     <row r="85" spans="1:6">
       <c r="A85" s="2" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B85" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C85" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D85" t="s">
         <v>64</v>
@@ -2730,13 +3045,13 @@
     </row>
     <row r="86" spans="1:6">
       <c r="A86" s="2" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B86" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C86" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D86" t="s">
         <v>64</v>
@@ -2744,13 +3059,13 @@
     </row>
     <row r="87" spans="1:6">
       <c r="A87" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B87" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C87" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D87" t="s">
         <v>64</v>
@@ -2758,13 +3073,13 @@
     </row>
     <row r="88" spans="1:6">
       <c r="A88" s="2" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B88" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C88" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D88" t="s">
         <v>64</v>
@@ -2772,13 +3087,13 @@
     </row>
     <row r="89" spans="1:6">
       <c r="A89" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B89" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C89" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D89" t="s">
         <v>64</v>
@@ -2786,7 +3101,7 @@
     </row>
     <row r="90" spans="1:6">
       <c r="A90" s="15" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B90" s="15"/>
       <c r="C90" s="15"/>
@@ -2796,13 +3111,13 @@
     </row>
     <row r="91" spans="1:6">
       <c r="A91" s="2" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C91" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D91" t="s">
         <v>66</v>
@@ -2810,13 +3125,13 @@
     </row>
     <row r="92" spans="1:6">
       <c r="A92" s="2" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C92" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D92" t="s">
         <v>66</v>
@@ -2824,13 +3139,13 @@
     </row>
     <row r="93" spans="1:6">
       <c r="A93" s="2" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C93" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D93" t="s">
         <v>66</v>
@@ -2838,13 +3153,13 @@
     </row>
     <row r="94" spans="1:6">
       <c r="A94" s="2" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="C94" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D94" t="s">
         <v>66</v>
@@ -2852,13 +3167,13 @@
     </row>
     <row r="95" spans="1:6">
       <c r="A95" s="2" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C95" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D95" t="s">
         <v>66</v>
@@ -2866,13 +3181,13 @@
     </row>
     <row r="96" spans="1:6">
       <c r="A96" s="2" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C96" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D96" t="s">
         <v>66</v>
@@ -2880,13 +3195,13 @@
     </row>
     <row r="97" spans="1:6">
       <c r="A97" s="2" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="C97" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D97" t="s">
         <v>66</v>
@@ -2894,13 +3209,13 @@
     </row>
     <row r="98" spans="1:6">
       <c r="A98" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C98" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D98" t="s">
         <v>66</v>
@@ -2908,13 +3223,13 @@
     </row>
     <row r="99" spans="1:6">
       <c r="A99" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="C99" t="s">
         <v>292</v>
-      </c>
-      <c r="B99" s="2" t="s">
-        <v>302</v>
-      </c>
-      <c r="C99" t="s">
-        <v>294</v>
       </c>
       <c r="D99" t="s">
         <v>66</v>
@@ -2922,13 +3237,13 @@
     </row>
     <row r="100" spans="1:6">
       <c r="A100" s="2" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="C100" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D100" t="s">
         <v>66</v>
@@ -2936,7 +3251,7 @@
     </row>
     <row r="101" spans="1:6">
       <c r="A101" s="15" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B101" s="15"/>
       <c r="C101" s="15"/>
@@ -2946,13 +3261,13 @@
     </row>
     <row r="102" spans="1:6">
       <c r="A102" s="2" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="C102" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D102" t="s">
         <v>92</v>
@@ -2960,13 +3275,13 @@
     </row>
     <row r="103" spans="1:6">
       <c r="A103" s="2" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="C103" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D103" t="s">
         <v>92</v>
@@ -2974,13 +3289,13 @@
     </row>
     <row r="104" spans="1:6">
       <c r="A104" s="2" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C104" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D104" t="s">
         <v>92</v>
@@ -2988,13 +3303,13 @@
     </row>
     <row r="105" spans="1:6">
       <c r="A105" s="2" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C105" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D105" t="s">
         <v>92</v>
@@ -3002,13 +3317,13 @@
     </row>
     <row r="106" spans="1:6">
       <c r="A106" s="2" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C106" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D106" t="s">
         <v>92</v>
@@ -3016,13 +3331,13 @@
     </row>
     <row r="107" spans="1:6">
       <c r="A107" s="2" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C107" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D107" t="s">
         <v>92</v>
@@ -3030,13 +3345,13 @@
     </row>
     <row r="108" spans="1:6">
       <c r="A108" s="2" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C108" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D108" t="s">
         <v>92</v>
@@ -3044,13 +3359,13 @@
     </row>
     <row r="109" spans="1:6">
       <c r="A109" s="2" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C109" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D109" t="s">
         <v>92</v>
@@ -3058,13 +3373,13 @@
     </row>
     <row r="110" spans="1:6">
       <c r="A110" s="2" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C110" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D110" t="s">
         <v>92</v>
@@ -3072,13 +3387,13 @@
     </row>
     <row r="111" spans="1:6">
       <c r="A111" s="2" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C111" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D111" t="s">
         <v>92</v>
@@ -3086,7 +3401,7 @@
     </row>
     <row r="112" spans="1:6">
       <c r="A112" s="15" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="B112" s="15"/>
       <c r="C112" s="15"/>
@@ -3096,13 +3411,13 @@
     </row>
     <row r="113" spans="1:4">
       <c r="A113" s="2" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B113" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="C113" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D113" t="s">
         <v>72</v>
@@ -3110,13 +3425,13 @@
     </row>
     <row r="114" spans="1:4">
       <c r="A114" s="2" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="B114" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="C114" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D114" t="s">
         <v>72</v>
@@ -3124,13 +3439,13 @@
     </row>
     <row r="115" spans="1:4">
       <c r="A115" s="2" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B115" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C115" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D115" t="s">
         <v>72</v>
@@ -3138,13 +3453,13 @@
     </row>
     <row r="116" spans="1:4">
       <c r="A116" s="2" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B116" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="C116" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D116" t="s">
         <v>72</v>
@@ -3152,13 +3467,13 @@
     </row>
     <row r="117" spans="1:4">
       <c r="A117" s="2" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B117" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="C117" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D117" t="s">
         <v>72</v>
@@ -3166,13 +3481,13 @@
     </row>
     <row r="118" spans="1:4">
       <c r="A118" s="2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B118" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="C118" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D118" t="s">
         <v>72</v>
@@ -3180,13 +3495,13 @@
     </row>
     <row r="119" spans="1:4">
       <c r="A119" s="2" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="B119" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="C119" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D119" t="s">
         <v>72</v>
@@ -3194,13 +3509,13 @@
     </row>
     <row r="120" spans="1:4">
       <c r="A120" s="2" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B120" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="C120" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D120" t="s">
         <v>72</v>
@@ -3208,13 +3523,13 @@
     </row>
     <row r="121" spans="1:4">
       <c r="A121" s="2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="B121" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C121" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D121" t="s">
         <v>72</v>
@@ -3222,13 +3537,13 @@
     </row>
     <row r="122" spans="1:4">
       <c r="A122" s="2" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="B122" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C122" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D122" t="s">
         <v>72</v>
@@ -3242,10 +3557,275 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:I11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="2" max="2" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.77734375" customWidth="1"/>
+    <col min="4" max="4" width="34.21875" customWidth="1"/>
+    <col min="5" max="5" width="22.5546875" customWidth="1"/>
+    <col min="6" max="6" width="11.21875" customWidth="1"/>
+    <col min="7" max="7" width="23" customWidth="1"/>
+    <col min="8" max="8" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="C2" t="s">
+        <v>303</v>
+      </c>
+      <c r="D2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="C3" t="s">
+        <v>303</v>
+      </c>
+      <c r="D3" t="s">
+        <v>92</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="C4" t="s">
+        <v>303</v>
+      </c>
+      <c r="D4" t="s">
+        <v>92</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="C5" t="s">
+        <v>303</v>
+      </c>
+      <c r="D5" t="s">
+        <v>92</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="C6" t="s">
+        <v>303</v>
+      </c>
+      <c r="D6" t="s">
+        <v>92</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="C7" t="s">
+        <v>303</v>
+      </c>
+      <c r="D7" t="s">
+        <v>92</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="F7" s="13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="C8" t="s">
+        <v>303</v>
+      </c>
+      <c r="D8" t="s">
+        <v>92</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="C9" t="s">
+        <v>303</v>
+      </c>
+      <c r="D9" t="s">
+        <v>92</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="C10" t="s">
+        <v>303</v>
+      </c>
+      <c r="D10" t="s">
+        <v>92</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="F10" s="13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="C11" t="s">
+        <v>303</v>
+      </c>
+      <c r="D11" t="s">
+        <v>92</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
@@ -3298,10 +3878,10 @@
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="C2" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D2" t="s">
         <v>72</v>
@@ -3326,10 +3906,10 @@
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="C3" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D3" t="s">
         <v>72</v>
@@ -3352,10 +3932,10 @@
         <v>7</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C4" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D4" t="s">
         <v>72</v>
@@ -3378,10 +3958,10 @@
         <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="C5" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D5" t="s">
         <v>72</v>
@@ -3404,10 +3984,10 @@
         <v>9</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="C6" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D6" t="s">
         <v>72</v>
@@ -3430,10 +4010,10 @@
         <v>10</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="C7" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D7" t="s">
         <v>72</v>
@@ -3456,10 +4036,10 @@
         <v>11</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="C8" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D8" t="s">
         <v>72</v>
@@ -3482,10 +4062,10 @@
         <v>12</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="C9" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D9" t="s">
         <v>72</v>
@@ -3508,10 +4088,10 @@
         <v>13</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C10" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D10" t="s">
         <v>72</v>
@@ -3534,10 +4114,10 @@
         <v>14</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C11" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D11" t="s">
         <v>72</v>
@@ -3825,10 +4405,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:O11"/>
+  <dimension ref="A1:O25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="H16" sqref="H16:H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3957,6 +4537,12 @@
       <c r="F3" s="3" t="s">
         <v>18</v>
       </c>
+      <c r="G3" t="s">
+        <v>347</v>
+      </c>
+      <c r="H3" t="s">
+        <v>348</v>
+      </c>
       <c r="I3" t="s">
         <v>56</v>
       </c>
@@ -3973,7 +4559,7 @@
         <v>51</v>
       </c>
       <c r="N3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:15">
@@ -3995,6 +4581,12 @@
       <c r="F4" s="3" t="s">
         <v>18</v>
       </c>
+      <c r="G4" t="s">
+        <v>349</v>
+      </c>
+      <c r="H4" t="s">
+        <v>350</v>
+      </c>
       <c r="I4" t="s">
         <v>57</v>
       </c>
@@ -4033,6 +4625,12 @@
       <c r="F5" s="3" t="s">
         <v>18</v>
       </c>
+      <c r="G5" t="s">
+        <v>351</v>
+      </c>
+      <c r="H5" t="s">
+        <v>352</v>
+      </c>
       <c r="I5" t="s">
         <v>59</v>
       </c>
@@ -4044,6 +4642,9 @@
       </c>
       <c r="L5" s="2" t="s">
         <v>45</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>50</v>
       </c>
       <c r="N5" t="s">
         <v>55</v>
@@ -4069,22 +4670,22 @@
         <v>18</v>
       </c>
       <c r="G6" t="s">
-        <v>162</v>
+        <v>353</v>
       </c>
       <c r="H6" t="s">
-        <v>163</v>
+        <v>354</v>
       </c>
       <c r="I6" t="s">
-        <v>58</v>
+        <v>355</v>
       </c>
       <c r="J6" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="K6" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="L6" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="M6" s="2" t="s">
         <v>5</v>
@@ -4112,11 +4713,26 @@
       <c r="F7" s="3" t="s">
         <v>18</v>
       </c>
+      <c r="G7" t="s">
+        <v>356</v>
+      </c>
+      <c r="H7" t="s">
+        <v>357</v>
+      </c>
+      <c r="I7" t="s">
+        <v>358</v>
+      </c>
       <c r="J7" t="s">
         <v>46</v>
       </c>
       <c r="K7" t="s">
         <v>42</v>
+      </c>
+      <c r="L7" t="s">
+        <v>44</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="N7" t="s">
         <v>52</v>
@@ -4141,6 +4757,27 @@
       <c r="F8" s="3" t="s">
         <v>18</v>
       </c>
+      <c r="G8" t="s">
+        <v>39</v>
+      </c>
+      <c r="H8" t="s">
+        <v>359</v>
+      </c>
+      <c r="I8" t="s">
+        <v>360</v>
+      </c>
+      <c r="J8" t="s">
+        <v>41</v>
+      </c>
+      <c r="K8" t="s">
+        <v>48</v>
+      </c>
+      <c r="L8" t="s">
+        <v>43</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>51</v>
+      </c>
       <c r="N8" t="s">
         <v>54</v>
       </c>
@@ -4164,6 +4801,30 @@
       <c r="F9" s="3" t="s">
         <v>18</v>
       </c>
+      <c r="G9" t="s">
+        <v>361</v>
+      </c>
+      <c r="H9" t="s">
+        <v>362</v>
+      </c>
+      <c r="I9" t="s">
+        <v>363</v>
+      </c>
+      <c r="J9" t="s">
+        <v>46</v>
+      </c>
+      <c r="K9" t="s">
+        <v>48</v>
+      </c>
+      <c r="L9" t="s">
+        <v>45</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="N9" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="10" spans="1:15">
       <c r="A10" s="2" t="s">
@@ -4184,6 +4845,30 @@
       <c r="F10" s="3" t="s">
         <v>18</v>
       </c>
+      <c r="G10" t="s">
+        <v>364</v>
+      </c>
+      <c r="H10" t="s">
+        <v>365</v>
+      </c>
+      <c r="I10" t="s">
+        <v>366</v>
+      </c>
+      <c r="J10" t="s">
+        <v>46</v>
+      </c>
+      <c r="K10" t="s">
+        <v>42</v>
+      </c>
+      <c r="L10" t="s">
+        <v>43</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="N10" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="11" spans="1:15">
       <c r="A11" s="2" t="s">
@@ -4203,6 +4888,110 @@
       </c>
       <c r="F11" s="3" t="s">
         <v>18</v>
+      </c>
+      <c r="G11" t="s">
+        <v>367</v>
+      </c>
+      <c r="H11" t="s">
+        <v>368</v>
+      </c>
+      <c r="I11" t="s">
+        <v>369</v>
+      </c>
+      <c r="J11" t="s">
+        <v>47</v>
+      </c>
+      <c r="K11" t="s">
+        <v>42</v>
+      </c>
+      <c r="L11" t="s">
+        <v>43</v>
+      </c>
+      <c r="M11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="N11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15">
+      <c r="F16" t="s">
+        <v>39</v>
+      </c>
+      <c r="G16" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="6:7">
+      <c r="F17" t="s">
+        <v>347</v>
+      </c>
+      <c r="G17" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="18" spans="6:7">
+      <c r="F18" t="s">
+        <v>349</v>
+      </c>
+      <c r="G18" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="19" spans="6:7">
+      <c r="F19" t="s">
+        <v>351</v>
+      </c>
+      <c r="G19" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="20" spans="6:7">
+      <c r="F20" t="s">
+        <v>353</v>
+      </c>
+      <c r="G20" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="21" spans="6:7">
+      <c r="F21" t="s">
+        <v>356</v>
+      </c>
+      <c r="G21" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="22" spans="6:7">
+      <c r="F22" t="s">
+        <v>39</v>
+      </c>
+      <c r="G22" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="23" spans="6:7">
+      <c r="F23" t="s">
+        <v>361</v>
+      </c>
+      <c r="G23" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="24" spans="6:7">
+      <c r="F24" t="s">
+        <v>364</v>
+      </c>
+      <c r="G24" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="25" spans="6:7">
+      <c r="F25" t="s">
+        <v>367</v>
+      </c>
+      <c r="G25" t="s">
+        <v>368</v>
       </c>
     </row>
   </sheetData>
@@ -4224,6 +5013,591 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B26C6E52-E5E5-4D9E-897F-B24CFADC5889}">
+  <dimension ref="A1:R11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="O20" sqref="O20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="5.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.21875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="26.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18">
+      <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>383</v>
+      </c>
+      <c r="C2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" t="s">
+        <v>384</v>
+      </c>
+      <c r="H2" t="s">
+        <v>385</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="K2" t="s">
+        <v>388</v>
+      </c>
+      <c r="L2" t="s">
+        <v>384</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>435</v>
+      </c>
+      <c r="N2" t="s">
+        <v>242</v>
+      </c>
+      <c r="O2" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>383</v>
+      </c>
+      <c r="C3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" t="s">
+        <v>389</v>
+      </c>
+      <c r="H3" t="s">
+        <v>390</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>392</v>
+      </c>
+      <c r="K3" t="s">
+        <v>393</v>
+      </c>
+      <c r="L3" t="s">
+        <v>384</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>436</v>
+      </c>
+      <c r="N3" t="s">
+        <v>394</v>
+      </c>
+      <c r="O3" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18">
+      <c r="A4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>383</v>
+      </c>
+      <c r="C4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" t="s">
+        <v>395</v>
+      </c>
+      <c r="H4" t="s">
+        <v>396</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="K4" t="s">
+        <v>399</v>
+      </c>
+      <c r="L4" t="s">
+        <v>384</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>437</v>
+      </c>
+      <c r="N4" t="s">
+        <v>394</v>
+      </c>
+      <c r="O4" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18">
+      <c r="A5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>383</v>
+      </c>
+      <c r="C5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" t="s">
+        <v>400</v>
+      </c>
+      <c r="H5" t="s">
+        <v>401</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>402</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="K5" t="s">
+        <v>404</v>
+      </c>
+      <c r="L5" t="s">
+        <v>384</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>436</v>
+      </c>
+      <c r="N5" t="s">
+        <v>394</v>
+      </c>
+      <c r="O5" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18">
+      <c r="A6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>383</v>
+      </c>
+      <c r="C6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" t="s">
+        <v>405</v>
+      </c>
+      <c r="H6" t="s">
+        <v>406</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="K6" t="s">
+        <v>409</v>
+      </c>
+      <c r="L6" t="s">
+        <v>384</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>438</v>
+      </c>
+      <c r="N6" t="s">
+        <v>394</v>
+      </c>
+      <c r="O6" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18">
+      <c r="A7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>383</v>
+      </c>
+      <c r="C7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" t="s">
+        <v>410</v>
+      </c>
+      <c r="H7" t="s">
+        <v>411</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>413</v>
+      </c>
+      <c r="K7" t="s">
+        <v>414</v>
+      </c>
+      <c r="L7" t="s">
+        <v>384</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="N7" t="s">
+        <v>394</v>
+      </c>
+      <c r="O7" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18">
+      <c r="A8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" t="s">
+        <v>383</v>
+      </c>
+      <c r="C8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" t="s">
+        <v>415</v>
+      </c>
+      <c r="H8" t="s">
+        <v>416</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="K8" t="s">
+        <v>419</v>
+      </c>
+      <c r="L8" t="s">
+        <v>384</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>438</v>
+      </c>
+      <c r="N8" t="s">
+        <v>242</v>
+      </c>
+      <c r="O8" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18">
+      <c r="A9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
+        <v>383</v>
+      </c>
+      <c r="C9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" t="s">
+        <v>420</v>
+      </c>
+      <c r="H9" t="s">
+        <v>421</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>422</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>423</v>
+      </c>
+      <c r="K9" t="s">
+        <v>424</v>
+      </c>
+      <c r="L9" t="s">
+        <v>384</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>436</v>
+      </c>
+      <c r="N9" t="s">
+        <v>394</v>
+      </c>
+      <c r="O9" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18">
+      <c r="A10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" t="s">
+        <v>383</v>
+      </c>
+      <c r="C10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" t="s">
+        <v>425</v>
+      </c>
+      <c r="H10" t="s">
+        <v>426</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>427</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="K10" t="s">
+        <v>388</v>
+      </c>
+      <c r="L10" t="s">
+        <v>384</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>440</v>
+      </c>
+      <c r="N10" t="s">
+        <v>242</v>
+      </c>
+      <c r="O10" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18">
+      <c r="A11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" t="s">
+        <v>383</v>
+      </c>
+      <c r="C11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G11" t="s">
+        <v>429</v>
+      </c>
+      <c r="H11" t="s">
+        <v>430</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>431</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>432</v>
+      </c>
+      <c r="K11" t="s">
+        <v>433</v>
+      </c>
+      <c r="L11" t="s">
+        <v>384</v>
+      </c>
+      <c r="M11" s="2" t="s">
+        <v>436</v>
+      </c>
+      <c r="N11" t="s">
+        <v>394</v>
+      </c>
+      <c r="O11" t="s">
+        <v>449</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{8C11662A-BCAC-45AA-8736-25E364CF41AF}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{D7BCD4AF-B7E3-4884-9BE6-AF2407193468}"/>
+    <hyperlink ref="E4" r:id="rId3" xr:uid="{E96CBB08-7725-4EC4-8B97-4381B62A20AC}"/>
+    <hyperlink ref="E5" r:id="rId4" xr:uid="{3C222BD2-F739-4534-9DE6-60B8489DFEA6}"/>
+    <hyperlink ref="E6" r:id="rId5" xr:uid="{D0F42A5C-9B12-451F-BF7F-A05B601FCE1D}"/>
+    <hyperlink ref="E7" r:id="rId6" xr:uid="{BB67F6A5-24A1-45FD-BC5A-2F42E027FC30}"/>
+    <hyperlink ref="E8" r:id="rId7" xr:uid="{C5608EAE-2CE3-49B9-B528-6671D8ADF2C0}"/>
+    <hyperlink ref="E9" r:id="rId8" xr:uid="{AA5D4E6F-E01B-411F-9811-8938FC530979}"/>
+    <hyperlink ref="E10" r:id="rId9" xr:uid="{F56E5482-98B3-41B5-9B8C-199812EC3EBC}"/>
+    <hyperlink ref="E11" r:id="rId10" xr:uid="{52BE2A0A-8174-46F7-A506-1DA84FCDED7F}"/>
+    <hyperlink ref="F2" r:id="rId11" xr:uid="{AD6AAC71-2E98-4420-A716-60E66A3E2464}"/>
+    <hyperlink ref="F3" r:id="rId12" xr:uid="{EB9EDB1A-7760-4FDA-83B6-81CA08496AAF}"/>
+    <hyperlink ref="F4" r:id="rId13" xr:uid="{C4091AFA-6247-408D-B67E-FC7B9FF24FFC}"/>
+    <hyperlink ref="F5" r:id="rId14" xr:uid="{F0D72094-CB20-4A88-BD6E-763773B520EE}"/>
+    <hyperlink ref="F6" r:id="rId15" xr:uid="{708CDE5D-0E4C-4F69-92B6-9156EF596F8D}"/>
+    <hyperlink ref="F7" r:id="rId16" xr:uid="{770D6A80-5F8F-4383-AD2E-12629E1F70E5}"/>
+    <hyperlink ref="F8" r:id="rId17" xr:uid="{33B40313-CF60-45E1-B044-B89F8FC075E7}"/>
+    <hyperlink ref="F9" r:id="rId18" xr:uid="{13CB37C1-C34F-4489-B35C-6BF4FFC2DD0D}"/>
+    <hyperlink ref="F10" r:id="rId19" xr:uid="{3102A8D1-CA80-4DB4-A4BC-97C976B6B2D2}"/>
+    <hyperlink ref="F11" r:id="rId20" xr:uid="{78781037-EF74-469B-AF17-58A15339BF9E}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId21"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:J11"/>
   <sheetViews>
@@ -4513,12 +5887,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="14.4"/>
@@ -4581,10 +5955,10 @@
         <v>5</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>88</v>
@@ -4619,10 +5993,10 @@
         <v>6</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>88</v>
@@ -4645,10 +6019,10 @@
         <v>7</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D4" s="10" t="s">
         <v>88</v>
@@ -4671,10 +6045,10 @@
         <v>8</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D5" s="10" t="s">
         <v>88</v>
@@ -4697,10 +6071,10 @@
         <v>9</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D6" s="10" t="s">
         <v>88</v>
@@ -4723,10 +6097,10 @@
         <v>10</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D7" s="10" t="s">
         <v>88</v>
@@ -4749,10 +6123,10 @@
         <v>11</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D8" s="10" t="s">
         <v>88</v>
@@ -4775,10 +6149,10 @@
         <v>12</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D9" s="10" t="s">
         <v>88</v>
@@ -4801,10 +6175,10 @@
         <v>13</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D10" s="10" t="s">
         <v>88</v>
@@ -4827,10 +6201,10 @@
         <v>14</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D11" s="10" t="s">
         <v>88</v>
@@ -4870,7 +6244,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:P11"/>
   <sheetViews>
@@ -4916,28 +6290,28 @@
         <v>76</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>248</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="2" spans="1:16">
@@ -4945,13 +6319,13 @@
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C2" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="D2" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>65</v>
@@ -4965,13 +6339,13 @@
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C3" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="D3" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>65</v>
@@ -4985,13 +6359,13 @@
         <v>7</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C4" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="D4" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>65</v>
@@ -5005,13 +6379,13 @@
         <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C5" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="D5" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>65</v>
@@ -5025,13 +6399,13 @@
         <v>9</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C6" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="D6" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>65</v>
@@ -5045,13 +6419,13 @@
         <v>10</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C7" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="D7" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>65</v>
@@ -5065,13 +6439,13 @@
         <v>11</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C8" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="D8" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>65</v>
@@ -5085,13 +6459,13 @@
         <v>12</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C9" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="D9" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>65</v>
@@ -5105,13 +6479,13 @@
         <v>13</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="C10" t="s">
         <v>239</v>
       </c>
-      <c r="C10" t="s">
-        <v>241</v>
-      </c>
       <c r="D10" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>65</v>
@@ -5125,13 +6499,13 @@
         <v>14</v>
       </c>
       <c r="B11" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="C11" t="s">
+        <v>239</v>
+      </c>
+      <c r="D11" t="s">
         <v>240</v>
-      </c>
-      <c r="C11" t="s">
-        <v>241</v>
-      </c>
-      <c r="D11" t="s">
-        <v>242</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>65</v>
@@ -5168,7 +6542,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:G11"/>
   <sheetViews>
@@ -5214,10 +6588,10 @@
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C2" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D2" t="s">
         <v>64</v>
@@ -5237,10 +6611,10 @@
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C3" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D3" t="s">
         <v>64</v>
@@ -5257,10 +6631,10 @@
         <v>7</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C4" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D4" t="s">
         <v>64</v>
@@ -5277,10 +6651,10 @@
         <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C5" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D5" t="s">
         <v>64</v>
@@ -5297,10 +6671,10 @@
         <v>9</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C6" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D6" t="s">
         <v>64</v>
@@ -5317,10 +6691,10 @@
         <v>10</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C7" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D7" t="s">
         <v>64</v>
@@ -5337,10 +6711,10 @@
         <v>11</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C8" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D8" t="s">
         <v>64</v>
@@ -5357,10 +6731,10 @@
         <v>12</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C9" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D9" t="s">
         <v>64</v>
@@ -5377,10 +6751,10 @@
         <v>13</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C10" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D10" t="s">
         <v>64</v>
@@ -5397,10 +6771,10 @@
         <v>14</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C11" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D11" t="s">
         <v>64</v>
@@ -5433,7 +6807,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:H11"/>
   <sheetViews>
@@ -5483,10 +6857,10 @@
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C2" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D2" t="s">
         <v>66</v>
@@ -5509,10 +6883,10 @@
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C3" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D3" t="s">
         <v>66</v>
@@ -5529,10 +6903,10 @@
         <v>7</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C4" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D4" t="s">
         <v>66</v>
@@ -5549,10 +6923,10 @@
         <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="C5" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D5" t="s">
         <v>66</v>
@@ -5569,10 +6943,10 @@
         <v>9</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C6" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D6" t="s">
         <v>66</v>
@@ -5589,10 +6963,10 @@
         <v>10</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C7" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D7" t="s">
         <v>66</v>
@@ -5609,10 +6983,10 @@
         <v>11</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="C8" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D8" t="s">
         <v>66</v>
@@ -5629,10 +7003,10 @@
         <v>12</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C9" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D9" t="s">
         <v>66</v>
@@ -5649,10 +7023,10 @@
         <v>13</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C10" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D10" t="s">
         <v>66</v>
@@ -5669,10 +7043,10 @@
         <v>14</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="C11" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D11" t="s">
         <v>66</v>
@@ -5703,269 +7077,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId13"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
-  <cols>
-    <col min="2" max="2" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="41.77734375" customWidth="1"/>
-    <col min="4" max="4" width="34.21875" customWidth="1"/>
-    <col min="5" max="5" width="22.5546875" customWidth="1"/>
-    <col min="6" max="6" width="11.21875" customWidth="1"/>
-    <col min="7" max="7" width="23" customWidth="1"/>
-    <col min="8" max="8" width="15.77734375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.77734375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9">
-      <c r="A1" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
-      <c r="A2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>306</v>
-      </c>
-      <c r="C2" t="s">
-        <v>305</v>
-      </c>
-      <c r="D2" t="s">
-        <v>92</v>
-      </c>
-      <c r="E2" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="F2" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I2" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>314</v>
-      </c>
-      <c r="C3" t="s">
-        <v>305</v>
-      </c>
-      <c r="D3" t="s">
-        <v>92</v>
-      </c>
-      <c r="E3" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="F3" s="13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>307</v>
-      </c>
-      <c r="C4" t="s">
-        <v>305</v>
-      </c>
-      <c r="D4" t="s">
-        <v>92</v>
-      </c>
-      <c r="E4" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="F4" s="13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>308</v>
-      </c>
-      <c r="C5" t="s">
-        <v>305</v>
-      </c>
-      <c r="D5" t="s">
-        <v>92</v>
-      </c>
-      <c r="E5" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="F5" s="13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="A6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>309</v>
-      </c>
-      <c r="C6" t="s">
-        <v>305</v>
-      </c>
-      <c r="D6" t="s">
-        <v>92</v>
-      </c>
-      <c r="E6" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="F6" s="13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>310</v>
-      </c>
-      <c r="C7" t="s">
-        <v>305</v>
-      </c>
-      <c r="D7" t="s">
-        <v>92</v>
-      </c>
-      <c r="E7" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="F7" s="13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="A8" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>311</v>
-      </c>
-      <c r="C8" t="s">
-        <v>305</v>
-      </c>
-      <c r="D8" t="s">
-        <v>92</v>
-      </c>
-      <c r="E8" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="F8" s="13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="A9" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>312</v>
-      </c>
-      <c r="C9" t="s">
-        <v>305</v>
-      </c>
-      <c r="D9" t="s">
-        <v>92</v>
-      </c>
-      <c r="E9" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="F9" s="13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="A10" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>313</v>
-      </c>
-      <c r="C10" t="s">
-        <v>305</v>
-      </c>
-      <c r="D10" t="s">
-        <v>92</v>
-      </c>
-      <c r="E10" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="F10" s="13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="A11" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>315</v>
-      </c>
-      <c r="C11" t="s">
-        <v>305</v>
-      </c>
-      <c r="D11" t="s">
-        <v>92</v>
-      </c>
-      <c r="E11" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="F11" s="13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Changes made to the TestData.xlsx
</commit_message>
<xml_diff>
--- a/src/main/resources/AutomationCatalogue_Batch41_TestData.xlsx
+++ b/src/main/resources/AutomationCatalogue_Batch41_TestData.xlsx
@@ -5,36 +5,48 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AutomationCatalogue\Projects\TestAutomationCatalogue_Batch41\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Automation Catalogue\TestAutomationCatalogue_Batch41\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{339C1403-EB4E-4969-823E-EFDDC38155BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17661E78-B2A7-4C97-A3B9-F15F5309B848}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="944" firstSheet="2" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-1095" windowWidth="29040" windowHeight="15720" tabRatio="944" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="10" r:id="rId1"/>
     <sheet name="OrangeHRM_Login" sheetId="1" r:id="rId2"/>
     <sheet name="OrangeHRM_AddEmployee" sheetId="2" r:id="rId3"/>
-    <sheet name="OrangeHRM_AddUser" sheetId="3" r:id="rId4"/>
-    <sheet name="OrangeHRM_EditEmployee" sheetId="8" r:id="rId5"/>
-    <sheet name="DemoWebshop_CreateAddress" sheetId="5" r:id="rId6"/>
-    <sheet name="DemoWebshop_ReOrder" sheetId="4" r:id="rId7"/>
-    <sheet name="DemoWebshop_TotalOrders" sheetId="6" r:id="rId8"/>
-    <sheet name="DemoWebshop_UpdateShoppingCart" sheetId="9" r:id="rId9"/>
-    <sheet name="DemoWebshop_ApplyDiscount" sheetId="7" r:id="rId10"/>
+    <sheet name="OrangeHRM_TravelExpense" sheetId="11" r:id="rId4"/>
+    <sheet name="OrangeHRM_AddUser" sheetId="3" r:id="rId5"/>
+    <sheet name="OrangeHRM_EditEmployee" sheetId="8" r:id="rId6"/>
+    <sheet name="DemoWebshop_CreateAddress" sheetId="5" r:id="rId7"/>
+    <sheet name="DemoWebshop_ReOrder" sheetId="4" r:id="rId8"/>
+    <sheet name="DemoWebshop_TotalOrders" sheetId="6" r:id="rId9"/>
+    <sheet name="DemoWebshop_UpdateShoppingCart" sheetId="9" r:id="rId10"/>
+    <sheet name="DemoWebshop_ApplyDiscount" sheetId="7" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1156" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1387" uniqueCount="450">
   <si>
     <t>S. No</t>
   </si>
@@ -522,12 +534,6 @@
     <t>Sagar123</t>
   </si>
   <si>
-    <t>Automation</t>
-  </si>
-  <si>
-    <t>Catalogue</t>
-  </si>
-  <si>
     <t>31</t>
   </si>
   <si>
@@ -1081,6 +1087,315 @@
   </si>
   <si>
     <t>110</t>
+  </si>
+  <si>
+    <t>Christopher</t>
+  </si>
+  <si>
+    <t>Anderson</t>
+  </si>
+  <si>
+    <t>Ronald</t>
+  </si>
+  <si>
+    <t>Clark</t>
+  </si>
+  <si>
+    <t>Mary</t>
+  </si>
+  <si>
+    <t>Wright</t>
+  </si>
+  <si>
+    <t>Lisa</t>
+  </si>
+  <si>
+    <t>Mitchell</t>
+  </si>
+  <si>
+    <t>Jamaica training center</t>
+  </si>
+  <si>
+    <t>Michelle</t>
+  </si>
+  <si>
+    <t>Johnson</t>
+  </si>
+  <si>
+    <t>Kenya Satalite office</t>
+  </si>
+  <si>
+    <t>Thomas</t>
+  </si>
+  <si>
+    <t>Philippine call center</t>
+  </si>
+  <si>
+    <t>Daniel</t>
+  </si>
+  <si>
+    <t>Rodriguez</t>
+  </si>
+  <si>
+    <t>European Office</t>
+  </si>
+  <si>
+    <t>Anthony</t>
+  </si>
+  <si>
+    <t>Lopez</t>
+  </si>
+  <si>
+    <t>Sheffield Office</t>
+  </si>
+  <si>
+    <t>Patricia</t>
+  </si>
+  <si>
+    <t>Perez</t>
+  </si>
+  <si>
+    <t>US Office</t>
+  </si>
+  <si>
+    <t>New Password</t>
+  </si>
+  <si>
+    <t>Currency</t>
+  </si>
+  <si>
+    <t>Destination</t>
+  </si>
+  <si>
+    <t>Travel From</t>
+  </si>
+  <si>
+    <t>Travel To</t>
+  </si>
+  <si>
+    <t>Expense Type</t>
+  </si>
+  <si>
+    <t>Currency Paidin</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>Paid by</t>
+  </si>
+  <si>
+    <t>Employee Name</t>
+  </si>
+  <si>
+    <t>Travel Req Id</t>
+  </si>
+  <si>
+    <t>Request Status</t>
+  </si>
+  <si>
+    <t>Supervisor Username</t>
+  </si>
+  <si>
+    <t>TC05_OrangeHRM_AddEmployee</t>
+  </si>
+  <si>
+    <t>AED - Utd. Arab Emir. Dirham</t>
+  </si>
+  <si>
+    <t>London</t>
+  </si>
+  <si>
+    <t>1-Jan-2022</t>
+  </si>
+  <si>
+    <t>15-Jan-2022</t>
+  </si>
+  <si>
+    <t>Airfare</t>
+  </si>
+  <si>
+    <t>CAD - Canadian Dollar</t>
+  </si>
+  <si>
+    <t>Chicago</t>
+  </si>
+  <si>
+    <t>1-Feb-2022</t>
+  </si>
+  <si>
+    <t>15-Feb-2022</t>
+  </si>
+  <si>
+    <t>Charitable Donations</t>
+  </si>
+  <si>
+    <t>Staff</t>
+  </si>
+  <si>
+    <t>AUD - Australian Dollar</t>
+  </si>
+  <si>
+    <t>Texas</t>
+  </si>
+  <si>
+    <t>1-Mar-2022</t>
+  </si>
+  <si>
+    <t>15-Mar-2022</t>
+  </si>
+  <si>
+    <t>Entertainment</t>
+  </si>
+  <si>
+    <t>EUR - Euro</t>
+  </si>
+  <si>
+    <t>Canada</t>
+  </si>
+  <si>
+    <t>1-Apr-2022</t>
+  </si>
+  <si>
+    <t>15-Apr-2022</t>
+  </si>
+  <si>
+    <t>Food &amp; Beverage</t>
+  </si>
+  <si>
+    <t>JPY - Japanese Yen</t>
+  </si>
+  <si>
+    <t>Germany</t>
+  </si>
+  <si>
+    <t>1-May-2022</t>
+  </si>
+  <si>
+    <t>15-May-2022</t>
+  </si>
+  <si>
+    <t>Fuel</t>
+  </si>
+  <si>
+    <t>LKR - Sri Lanka Rupee</t>
+  </si>
+  <si>
+    <t>Paris</t>
+  </si>
+  <si>
+    <t>1-Jun-2022</t>
+  </si>
+  <si>
+    <t>15-Jun-2022</t>
+  </si>
+  <si>
+    <t>Ground Transportation</t>
+  </si>
+  <si>
+    <t>PHP - Philippine Peso</t>
+  </si>
+  <si>
+    <t>NewYork</t>
+  </si>
+  <si>
+    <t>1-Jul-2022</t>
+  </si>
+  <si>
+    <t>15-Jul-2022</t>
+  </si>
+  <si>
+    <t>Hotel</t>
+  </si>
+  <si>
+    <t>USD - United States Dollar</t>
+  </si>
+  <si>
+    <t>Vegas</t>
+  </si>
+  <si>
+    <t>1-Aug-2022</t>
+  </si>
+  <si>
+    <t>15-Aug-2022</t>
+  </si>
+  <si>
+    <t>Maintenance &amp; Repairs</t>
+  </si>
+  <si>
+    <t>MXN - Mexican New Peso</t>
+  </si>
+  <si>
+    <t>Pittsburgh</t>
+  </si>
+  <si>
+    <t>1-Sep-2022</t>
+  </si>
+  <si>
+    <t>15-Sep-2022</t>
+  </si>
+  <si>
+    <t>ZMK - Zambian Kwacha</t>
+  </si>
+  <si>
+    <t>NewJersy</t>
+  </si>
+  <si>
+    <t>1-OCt-2022</t>
+  </si>
+  <si>
+    <t>15-Oct-2022</t>
+  </si>
+  <si>
+    <t>Office Supplies</t>
+  </si>
+  <si>
+    <t>Brody Naidu</t>
+  </si>
+  <si>
+    <t>2500</t>
+  </si>
+  <si>
+    <t>500</t>
+  </si>
+  <si>
+    <t>200</t>
+  </si>
+  <si>
+    <t>250</t>
+  </si>
+  <si>
+    <t>150</t>
+  </si>
+  <si>
+    <t>1500</t>
+  </si>
+  <si>
+    <t>John Mikel</t>
+  </si>
+  <si>
+    <t>Christopher Anderson</t>
+  </si>
+  <si>
+    <t>Ronald Clark</t>
+  </si>
+  <si>
+    <t>Mary Wright</t>
+  </si>
+  <si>
+    <t>Lisa Mitchell</t>
+  </si>
+  <si>
+    <t>Michelle Johnson</t>
+  </si>
+  <si>
+    <t>John Thomas</t>
+  </si>
+  <si>
+    <t>Daniel Rodriguez</t>
+  </si>
+  <si>
+    <t>Anthony Lopez</t>
   </si>
 </sst>
 </file>
@@ -1552,7 +1867,7 @@
   <dimension ref="A1:F122"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K118" sqref="K118"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2046,13 +2361,13 @@
     </row>
     <row r="36" spans="1:6">
       <c r="A36" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B36" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C36" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>88</v>
@@ -2060,13 +2375,13 @@
     </row>
     <row r="37" spans="1:6">
       <c r="A37" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B37" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C37" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>88</v>
@@ -2074,13 +2389,13 @@
     </row>
     <row r="38" spans="1:6">
       <c r="A38" s="2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B38" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C38" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>88</v>
@@ -2088,13 +2403,13 @@
     </row>
     <row r="39" spans="1:6">
       <c r="A39" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B39" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C39" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>88</v>
@@ -2102,13 +2417,13 @@
     </row>
     <row r="40" spans="1:6">
       <c r="A40" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B40" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C40" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>88</v>
@@ -2116,13 +2431,13 @@
     </row>
     <row r="41" spans="1:6">
       <c r="A41" s="2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B41" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C41" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>88</v>
@@ -2130,13 +2445,13 @@
     </row>
     <row r="42" spans="1:6">
       <c r="A42" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B42" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C42" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>88</v>
@@ -2144,13 +2459,13 @@
     </row>
     <row r="43" spans="1:6">
       <c r="A43" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B43" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C43" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>88</v>
@@ -2158,13 +2473,13 @@
     </row>
     <row r="44" spans="1:6">
       <c r="A44" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="B44" t="s">
+        <v>180</v>
+      </c>
+      <c r="C44" t="s">
         <v>172</v>
-      </c>
-      <c r="B44" t="s">
-        <v>182</v>
-      </c>
-      <c r="C44" t="s">
-        <v>174</v>
       </c>
       <c r="D44" s="2" t="s">
         <v>88</v>
@@ -2172,13 +2487,13 @@
     </row>
     <row r="45" spans="1:6">
       <c r="A45" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B45" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C45" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>88</v>
@@ -2186,7 +2501,7 @@
     </row>
     <row r="46" spans="1:6">
       <c r="A46" s="15" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B46" s="15"/>
       <c r="C46" s="15"/>
@@ -2196,147 +2511,147 @@
     </row>
     <row r="47" spans="1:6">
       <c r="A47" s="2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B47" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C47" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D47" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="48" spans="1:6">
       <c r="A48" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B48" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C48" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D48" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="49" spans="1:6">
       <c r="A49" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B49" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C49" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D49" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="50" spans="1:6">
       <c r="A50" s="2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B50" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C50" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D50" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="51" spans="1:6">
       <c r="A51" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B51" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C51" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D51" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="52" spans="1:6">
       <c r="A52" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B52" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C52" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D52" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="53" spans="1:6">
       <c r="A53" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B53" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C53" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D53" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="54" spans="1:6">
       <c r="A54" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B54" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C54" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D54" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="55" spans="1:6">
       <c r="A55" s="2" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B55" t="s">
+        <v>202</v>
+      </c>
+      <c r="C55" t="s">
         <v>204</v>
       </c>
-      <c r="C55" t="s">
-        <v>206</v>
-      </c>
       <c r="D55" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="56" spans="1:6">
       <c r="A56" s="2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B56" t="s">
+        <v>203</v>
+      </c>
+      <c r="C56" t="s">
+        <v>204</v>
+      </c>
+      <c r="D56" t="s">
         <v>205</v>
-      </c>
-      <c r="C56" t="s">
-        <v>206</v>
-      </c>
-      <c r="D56" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="57" spans="1:6">
       <c r="A57" s="15" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B57" s="15"/>
       <c r="C57" s="15"/>
@@ -2346,147 +2661,147 @@
     </row>
     <row r="58" spans="1:6">
       <c r="A58" s="2" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B58" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C58" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D58" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="59" spans="1:6">
       <c r="A59" s="2" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B59" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C59" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D59" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="60" spans="1:6">
       <c r="A60" s="2" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B60" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C60" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D60" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="61" spans="1:6">
       <c r="A61" s="2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B61" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C61" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D61" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="62" spans="1:6">
       <c r="A62" s="2" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B62" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C62" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D62" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="63" spans="1:6">
       <c r="A63" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B63" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C63" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D63" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="64" spans="1:6">
       <c r="A64" s="2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B64" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C64" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D64" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="65" spans="1:6">
       <c r="A65" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B65" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C65" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D65" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="66" spans="1:6">
       <c r="A66" s="2" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B66" t="s">
+        <v>225</v>
+      </c>
+      <c r="C66" t="s">
         <v>227</v>
       </c>
-      <c r="C66" t="s">
-        <v>229</v>
-      </c>
       <c r="D66" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="67" spans="1:6">
       <c r="A67" s="2" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B67" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C67" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D67" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="68" spans="1:6">
       <c r="A68" s="15" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B68" s="15"/>
       <c r="C68" s="15"/>
@@ -2496,147 +2811,147 @@
     </row>
     <row r="69" spans="1:6">
       <c r="A69" s="2" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C69" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="D69" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="70" spans="1:6">
       <c r="A70" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C70" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="D70" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="71" spans="1:6">
       <c r="A71" s="2" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C71" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="D71" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="72" spans="1:6">
       <c r="A72" s="2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C72" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="D72" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="73" spans="1:6">
       <c r="A73" s="2" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C73" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="D73" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="74" spans="1:6">
       <c r="A74" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C74" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="D74" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="75" spans="1:6">
       <c r="A75" s="2" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C75" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="D75" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="76" spans="1:6">
       <c r="A76" s="2" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C76" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="D76" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="77" spans="1:6">
       <c r="A77" s="2" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B77" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="C77" t="s">
         <v>239</v>
       </c>
-      <c r="C77" t="s">
-        <v>241</v>
-      </c>
       <c r="D77" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="78" spans="1:6">
       <c r="A78" s="2" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B78" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="C78" t="s">
+        <v>239</v>
+      </c>
+      <c r="D78" t="s">
         <v>240</v>
-      </c>
-      <c r="C78" t="s">
-        <v>241</v>
-      </c>
-      <c r="D78" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="79" spans="1:6">
       <c r="A79" s="15" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B79" s="15"/>
       <c r="C79" s="15"/>
@@ -2646,13 +2961,13 @@
     </row>
     <row r="80" spans="1:6">
       <c r="A80" s="2" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B80" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C80" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D80" t="s">
         <v>64</v>
@@ -2660,13 +2975,13 @@
     </row>
     <row r="81" spans="1:6">
       <c r="A81" s="2" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B81" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C81" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D81" t="s">
         <v>64</v>
@@ -2674,13 +2989,13 @@
     </row>
     <row r="82" spans="1:6">
       <c r="A82" s="2" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B82" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C82" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D82" t="s">
         <v>64</v>
@@ -2688,13 +3003,13 @@
     </row>
     <row r="83" spans="1:6">
       <c r="A83" s="2" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B83" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C83" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D83" t="s">
         <v>64</v>
@@ -2702,13 +3017,13 @@
     </row>
     <row r="84" spans="1:6">
       <c r="A84" s="2" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B84" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C84" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D84" t="s">
         <v>64</v>
@@ -2716,13 +3031,13 @@
     </row>
     <row r="85" spans="1:6">
       <c r="A85" s="2" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B85" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C85" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D85" t="s">
         <v>64</v>
@@ -2730,13 +3045,13 @@
     </row>
     <row r="86" spans="1:6">
       <c r="A86" s="2" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B86" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C86" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D86" t="s">
         <v>64</v>
@@ -2744,13 +3059,13 @@
     </row>
     <row r="87" spans="1:6">
       <c r="A87" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B87" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C87" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D87" t="s">
         <v>64</v>
@@ -2758,13 +3073,13 @@
     </row>
     <row r="88" spans="1:6">
       <c r="A88" s="2" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B88" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C88" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D88" t="s">
         <v>64</v>
@@ -2772,13 +3087,13 @@
     </row>
     <row r="89" spans="1:6">
       <c r="A89" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B89" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C89" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D89" t="s">
         <v>64</v>
@@ -2786,7 +3101,7 @@
     </row>
     <row r="90" spans="1:6">
       <c r="A90" s="15" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B90" s="15"/>
       <c r="C90" s="15"/>
@@ -2796,13 +3111,13 @@
     </row>
     <row r="91" spans="1:6">
       <c r="A91" s="2" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C91" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D91" t="s">
         <v>66</v>
@@ -2810,13 +3125,13 @@
     </row>
     <row r="92" spans="1:6">
       <c r="A92" s="2" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C92" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D92" t="s">
         <v>66</v>
@@ -2824,13 +3139,13 @@
     </row>
     <row r="93" spans="1:6">
       <c r="A93" s="2" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C93" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D93" t="s">
         <v>66</v>
@@ -2838,13 +3153,13 @@
     </row>
     <row r="94" spans="1:6">
       <c r="A94" s="2" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="C94" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D94" t="s">
         <v>66</v>
@@ -2852,13 +3167,13 @@
     </row>
     <row r="95" spans="1:6">
       <c r="A95" s="2" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C95" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D95" t="s">
         <v>66</v>
@@ -2866,13 +3181,13 @@
     </row>
     <row r="96" spans="1:6">
       <c r="A96" s="2" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C96" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D96" t="s">
         <v>66</v>
@@ -2880,13 +3195,13 @@
     </row>
     <row r="97" spans="1:6">
       <c r="A97" s="2" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="C97" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D97" t="s">
         <v>66</v>
@@ -2894,13 +3209,13 @@
     </row>
     <row r="98" spans="1:6">
       <c r="A98" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C98" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D98" t="s">
         <v>66</v>
@@ -2908,13 +3223,13 @@
     </row>
     <row r="99" spans="1:6">
       <c r="A99" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="C99" t="s">
         <v>292</v>
-      </c>
-      <c r="B99" s="2" t="s">
-        <v>302</v>
-      </c>
-      <c r="C99" t="s">
-        <v>294</v>
       </c>
       <c r="D99" t="s">
         <v>66</v>
@@ -2922,13 +3237,13 @@
     </row>
     <row r="100" spans="1:6">
       <c r="A100" s="2" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="C100" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D100" t="s">
         <v>66</v>
@@ -2936,7 +3251,7 @@
     </row>
     <row r="101" spans="1:6">
       <c r="A101" s="15" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B101" s="15"/>
       <c r="C101" s="15"/>
@@ -2946,13 +3261,13 @@
     </row>
     <row r="102" spans="1:6">
       <c r="A102" s="2" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="C102" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D102" t="s">
         <v>92</v>
@@ -2960,13 +3275,13 @@
     </row>
     <row r="103" spans="1:6">
       <c r="A103" s="2" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="C103" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D103" t="s">
         <v>92</v>
@@ -2974,13 +3289,13 @@
     </row>
     <row r="104" spans="1:6">
       <c r="A104" s="2" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C104" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D104" t="s">
         <v>92</v>
@@ -2988,13 +3303,13 @@
     </row>
     <row r="105" spans="1:6">
       <c r="A105" s="2" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C105" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D105" t="s">
         <v>92</v>
@@ -3002,13 +3317,13 @@
     </row>
     <row r="106" spans="1:6">
       <c r="A106" s="2" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C106" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D106" t="s">
         <v>92</v>
@@ -3016,13 +3331,13 @@
     </row>
     <row r="107" spans="1:6">
       <c r="A107" s="2" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C107" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D107" t="s">
         <v>92</v>
@@ -3030,13 +3345,13 @@
     </row>
     <row r="108" spans="1:6">
       <c r="A108" s="2" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C108" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D108" t="s">
         <v>92</v>
@@ -3044,13 +3359,13 @@
     </row>
     <row r="109" spans="1:6">
       <c r="A109" s="2" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C109" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D109" t="s">
         <v>92</v>
@@ -3058,13 +3373,13 @@
     </row>
     <row r="110" spans="1:6">
       <c r="A110" s="2" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C110" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D110" t="s">
         <v>92</v>
@@ -3072,13 +3387,13 @@
     </row>
     <row r="111" spans="1:6">
       <c r="A111" s="2" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C111" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D111" t="s">
         <v>92</v>
@@ -3086,7 +3401,7 @@
     </row>
     <row r="112" spans="1:6">
       <c r="A112" s="15" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="B112" s="15"/>
       <c r="C112" s="15"/>
@@ -3096,13 +3411,13 @@
     </row>
     <row r="113" spans="1:4">
       <c r="A113" s="2" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B113" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="C113" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D113" t="s">
         <v>72</v>
@@ -3110,13 +3425,13 @@
     </row>
     <row r="114" spans="1:4">
       <c r="A114" s="2" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="B114" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="C114" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D114" t="s">
         <v>72</v>
@@ -3124,13 +3439,13 @@
     </row>
     <row r="115" spans="1:4">
       <c r="A115" s="2" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B115" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C115" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D115" t="s">
         <v>72</v>
@@ -3138,13 +3453,13 @@
     </row>
     <row r="116" spans="1:4">
       <c r="A116" s="2" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B116" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="C116" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D116" t="s">
         <v>72</v>
@@ -3152,13 +3467,13 @@
     </row>
     <row r="117" spans="1:4">
       <c r="A117" s="2" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B117" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="C117" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D117" t="s">
         <v>72</v>
@@ -3166,13 +3481,13 @@
     </row>
     <row r="118" spans="1:4">
       <c r="A118" s="2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B118" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="C118" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D118" t="s">
         <v>72</v>
@@ -3180,13 +3495,13 @@
     </row>
     <row r="119" spans="1:4">
       <c r="A119" s="2" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="B119" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="C119" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D119" t="s">
         <v>72</v>
@@ -3194,13 +3509,13 @@
     </row>
     <row r="120" spans="1:4">
       <c r="A120" s="2" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B120" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="C120" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D120" t="s">
         <v>72</v>
@@ -3208,13 +3523,13 @@
     </row>
     <row r="121" spans="1:4">
       <c r="A121" s="2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="B121" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C121" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D121" t="s">
         <v>72</v>
@@ -3222,13 +3537,13 @@
     </row>
     <row r="122" spans="1:4">
       <c r="A122" s="2" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="B122" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C122" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D122" t="s">
         <v>72</v>
@@ -3242,10 +3557,275 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:I11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="2" max="2" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.77734375" customWidth="1"/>
+    <col min="4" max="4" width="34.21875" customWidth="1"/>
+    <col min="5" max="5" width="22.5546875" customWidth="1"/>
+    <col min="6" max="6" width="11.21875" customWidth="1"/>
+    <col min="7" max="7" width="23" customWidth="1"/>
+    <col min="8" max="8" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="C2" t="s">
+        <v>303</v>
+      </c>
+      <c r="D2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="C3" t="s">
+        <v>303</v>
+      </c>
+      <c r="D3" t="s">
+        <v>92</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="C4" t="s">
+        <v>303</v>
+      </c>
+      <c r="D4" t="s">
+        <v>92</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="C5" t="s">
+        <v>303</v>
+      </c>
+      <c r="D5" t="s">
+        <v>92</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="C6" t="s">
+        <v>303</v>
+      </c>
+      <c r="D6" t="s">
+        <v>92</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="C7" t="s">
+        <v>303</v>
+      </c>
+      <c r="D7" t="s">
+        <v>92</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="F7" s="13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="C8" t="s">
+        <v>303</v>
+      </c>
+      <c r="D8" t="s">
+        <v>92</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="C9" t="s">
+        <v>303</v>
+      </c>
+      <c r="D9" t="s">
+        <v>92</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="C10" t="s">
+        <v>303</v>
+      </c>
+      <c r="D10" t="s">
+        <v>92</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="F10" s="13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="C11" t="s">
+        <v>303</v>
+      </c>
+      <c r="D11" t="s">
+        <v>92</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
@@ -3298,10 +3878,10 @@
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="C2" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D2" t="s">
         <v>72</v>
@@ -3326,10 +3906,10 @@
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="C3" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D3" t="s">
         <v>72</v>
@@ -3352,10 +3932,10 @@
         <v>7</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C4" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D4" t="s">
         <v>72</v>
@@ -3378,10 +3958,10 @@
         <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="C5" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D5" t="s">
         <v>72</v>
@@ -3404,10 +3984,10 @@
         <v>9</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="C6" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D6" t="s">
         <v>72</v>
@@ -3430,10 +4010,10 @@
         <v>10</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="C7" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D7" t="s">
         <v>72</v>
@@ -3456,10 +4036,10 @@
         <v>11</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="C8" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D8" t="s">
         <v>72</v>
@@ -3482,10 +4062,10 @@
         <v>12</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="C9" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D9" t="s">
         <v>72</v>
@@ -3508,10 +4088,10 @@
         <v>13</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C10" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D10" t="s">
         <v>72</v>
@@ -3534,10 +4114,10 @@
         <v>14</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C11" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D11" t="s">
         <v>72</v>
@@ -3825,10 +4405,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:O11"/>
+  <dimension ref="A1:O25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="H16" sqref="H16:H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3957,6 +4537,12 @@
       <c r="F3" s="3" t="s">
         <v>18</v>
       </c>
+      <c r="G3" t="s">
+        <v>347</v>
+      </c>
+      <c r="H3" t="s">
+        <v>348</v>
+      </c>
       <c r="I3" t="s">
         <v>56</v>
       </c>
@@ -3973,7 +4559,7 @@
         <v>51</v>
       </c>
       <c r="N3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:15">
@@ -3995,6 +4581,12 @@
       <c r="F4" s="3" t="s">
         <v>18</v>
       </c>
+      <c r="G4" t="s">
+        <v>349</v>
+      </c>
+      <c r="H4" t="s">
+        <v>350</v>
+      </c>
       <c r="I4" t="s">
         <v>57</v>
       </c>
@@ -4033,6 +4625,12 @@
       <c r="F5" s="3" t="s">
         <v>18</v>
       </c>
+      <c r="G5" t="s">
+        <v>351</v>
+      </c>
+      <c r="H5" t="s">
+        <v>352</v>
+      </c>
       <c r="I5" t="s">
         <v>59</v>
       </c>
@@ -4044,6 +4642,9 @@
       </c>
       <c r="L5" s="2" t="s">
         <v>45</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>50</v>
       </c>
       <c r="N5" t="s">
         <v>55</v>
@@ -4069,22 +4670,22 @@
         <v>18</v>
       </c>
       <c r="G6" t="s">
-        <v>162</v>
+        <v>353</v>
       </c>
       <c r="H6" t="s">
-        <v>163</v>
+        <v>354</v>
       </c>
       <c r="I6" t="s">
-        <v>58</v>
+        <v>355</v>
       </c>
       <c r="J6" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="K6" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="L6" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="M6" s="2" t="s">
         <v>5</v>
@@ -4112,11 +4713,26 @@
       <c r="F7" s="3" t="s">
         <v>18</v>
       </c>
+      <c r="G7" t="s">
+        <v>356</v>
+      </c>
+      <c r="H7" t="s">
+        <v>357</v>
+      </c>
+      <c r="I7" t="s">
+        <v>358</v>
+      </c>
       <c r="J7" t="s">
         <v>46</v>
       </c>
       <c r="K7" t="s">
         <v>42</v>
+      </c>
+      <c r="L7" t="s">
+        <v>44</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="N7" t="s">
         <v>52</v>
@@ -4141,6 +4757,27 @@
       <c r="F8" s="3" t="s">
         <v>18</v>
       </c>
+      <c r="G8" t="s">
+        <v>39</v>
+      </c>
+      <c r="H8" t="s">
+        <v>359</v>
+      </c>
+      <c r="I8" t="s">
+        <v>360</v>
+      </c>
+      <c r="J8" t="s">
+        <v>41</v>
+      </c>
+      <c r="K8" t="s">
+        <v>48</v>
+      </c>
+      <c r="L8" t="s">
+        <v>43</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>51</v>
+      </c>
       <c r="N8" t="s">
         <v>54</v>
       </c>
@@ -4164,6 +4801,30 @@
       <c r="F9" s="3" t="s">
         <v>18</v>
       </c>
+      <c r="G9" t="s">
+        <v>361</v>
+      </c>
+      <c r="H9" t="s">
+        <v>362</v>
+      </c>
+      <c r="I9" t="s">
+        <v>363</v>
+      </c>
+      <c r="J9" t="s">
+        <v>46</v>
+      </c>
+      <c r="K9" t="s">
+        <v>48</v>
+      </c>
+      <c r="L9" t="s">
+        <v>45</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="N9" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="10" spans="1:15">
       <c r="A10" s="2" t="s">
@@ -4184,6 +4845,30 @@
       <c r="F10" s="3" t="s">
         <v>18</v>
       </c>
+      <c r="G10" t="s">
+        <v>364</v>
+      </c>
+      <c r="H10" t="s">
+        <v>365</v>
+      </c>
+      <c r="I10" t="s">
+        <v>366</v>
+      </c>
+      <c r="J10" t="s">
+        <v>46</v>
+      </c>
+      <c r="K10" t="s">
+        <v>42</v>
+      </c>
+      <c r="L10" t="s">
+        <v>43</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="N10" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="11" spans="1:15">
       <c r="A11" s="2" t="s">
@@ -4203,6 +4888,110 @@
       </c>
       <c r="F11" s="3" t="s">
         <v>18</v>
+      </c>
+      <c r="G11" t="s">
+        <v>367</v>
+      </c>
+      <c r="H11" t="s">
+        <v>368</v>
+      </c>
+      <c r="I11" t="s">
+        <v>369</v>
+      </c>
+      <c r="J11" t="s">
+        <v>47</v>
+      </c>
+      <c r="K11" t="s">
+        <v>42</v>
+      </c>
+      <c r="L11" t="s">
+        <v>43</v>
+      </c>
+      <c r="M11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="N11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15">
+      <c r="F16" t="s">
+        <v>39</v>
+      </c>
+      <c r="G16" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="6:7">
+      <c r="F17" t="s">
+        <v>347</v>
+      </c>
+      <c r="G17" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="18" spans="6:7">
+      <c r="F18" t="s">
+        <v>349</v>
+      </c>
+      <c r="G18" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="19" spans="6:7">
+      <c r="F19" t="s">
+        <v>351</v>
+      </c>
+      <c r="G19" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="20" spans="6:7">
+      <c r="F20" t="s">
+        <v>353</v>
+      </c>
+      <c r="G20" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="21" spans="6:7">
+      <c r="F21" t="s">
+        <v>356</v>
+      </c>
+      <c r="G21" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="22" spans="6:7">
+      <c r="F22" t="s">
+        <v>39</v>
+      </c>
+      <c r="G22" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="23" spans="6:7">
+      <c r="F23" t="s">
+        <v>361</v>
+      </c>
+      <c r="G23" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="24" spans="6:7">
+      <c r="F24" t="s">
+        <v>364</v>
+      </c>
+      <c r="G24" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="25" spans="6:7">
+      <c r="F25" t="s">
+        <v>367</v>
+      </c>
+      <c r="G25" t="s">
+        <v>368</v>
       </c>
     </row>
   </sheetData>
@@ -4224,6 +5013,591 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B26C6E52-E5E5-4D9E-897F-B24CFADC5889}">
+  <dimension ref="A1:R11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="O20" sqref="O20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="5.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.21875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="26.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18">
+      <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>383</v>
+      </c>
+      <c r="C2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" t="s">
+        <v>384</v>
+      </c>
+      <c r="H2" t="s">
+        <v>385</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="K2" t="s">
+        <v>388</v>
+      </c>
+      <c r="L2" t="s">
+        <v>384</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>435</v>
+      </c>
+      <c r="N2" t="s">
+        <v>242</v>
+      </c>
+      <c r="O2" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>383</v>
+      </c>
+      <c r="C3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" t="s">
+        <v>389</v>
+      </c>
+      <c r="H3" t="s">
+        <v>390</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>392</v>
+      </c>
+      <c r="K3" t="s">
+        <v>393</v>
+      </c>
+      <c r="L3" t="s">
+        <v>384</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>436</v>
+      </c>
+      <c r="N3" t="s">
+        <v>394</v>
+      </c>
+      <c r="O3" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18">
+      <c r="A4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>383</v>
+      </c>
+      <c r="C4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" t="s">
+        <v>395</v>
+      </c>
+      <c r="H4" t="s">
+        <v>396</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="K4" t="s">
+        <v>399</v>
+      </c>
+      <c r="L4" t="s">
+        <v>384</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>437</v>
+      </c>
+      <c r="N4" t="s">
+        <v>394</v>
+      </c>
+      <c r="O4" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18">
+      <c r="A5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>383</v>
+      </c>
+      <c r="C5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" t="s">
+        <v>400</v>
+      </c>
+      <c r="H5" t="s">
+        <v>401</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>402</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="K5" t="s">
+        <v>404</v>
+      </c>
+      <c r="L5" t="s">
+        <v>384</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>436</v>
+      </c>
+      <c r="N5" t="s">
+        <v>394</v>
+      </c>
+      <c r="O5" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18">
+      <c r="A6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>383</v>
+      </c>
+      <c r="C6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" t="s">
+        <v>405</v>
+      </c>
+      <c r="H6" t="s">
+        <v>406</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="K6" t="s">
+        <v>409</v>
+      </c>
+      <c r="L6" t="s">
+        <v>384</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>438</v>
+      </c>
+      <c r="N6" t="s">
+        <v>394</v>
+      </c>
+      <c r="O6" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18">
+      <c r="A7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>383</v>
+      </c>
+      <c r="C7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" t="s">
+        <v>410</v>
+      </c>
+      <c r="H7" t="s">
+        <v>411</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>413</v>
+      </c>
+      <c r="K7" t="s">
+        <v>414</v>
+      </c>
+      <c r="L7" t="s">
+        <v>384</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="N7" t="s">
+        <v>394</v>
+      </c>
+      <c r="O7" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18">
+      <c r="A8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" t="s">
+        <v>383</v>
+      </c>
+      <c r="C8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" t="s">
+        <v>415</v>
+      </c>
+      <c r="H8" t="s">
+        <v>416</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="K8" t="s">
+        <v>419</v>
+      </c>
+      <c r="L8" t="s">
+        <v>384</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>438</v>
+      </c>
+      <c r="N8" t="s">
+        <v>242</v>
+      </c>
+      <c r="O8" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18">
+      <c r="A9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
+        <v>383</v>
+      </c>
+      <c r="C9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" t="s">
+        <v>420</v>
+      </c>
+      <c r="H9" t="s">
+        <v>421</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>422</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>423</v>
+      </c>
+      <c r="K9" t="s">
+        <v>424</v>
+      </c>
+      <c r="L9" t="s">
+        <v>384</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>436</v>
+      </c>
+      <c r="N9" t="s">
+        <v>394</v>
+      </c>
+      <c r="O9" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18">
+      <c r="A10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" t="s">
+        <v>383</v>
+      </c>
+      <c r="C10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" t="s">
+        <v>425</v>
+      </c>
+      <c r="H10" t="s">
+        <v>426</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>427</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="K10" t="s">
+        <v>388</v>
+      </c>
+      <c r="L10" t="s">
+        <v>384</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>440</v>
+      </c>
+      <c r="N10" t="s">
+        <v>242</v>
+      </c>
+      <c r="O10" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18">
+      <c r="A11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" t="s">
+        <v>383</v>
+      </c>
+      <c r="C11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G11" t="s">
+        <v>429</v>
+      </c>
+      <c r="H11" t="s">
+        <v>430</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>431</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>432</v>
+      </c>
+      <c r="K11" t="s">
+        <v>433</v>
+      </c>
+      <c r="L11" t="s">
+        <v>384</v>
+      </c>
+      <c r="M11" s="2" t="s">
+        <v>436</v>
+      </c>
+      <c r="N11" t="s">
+        <v>394</v>
+      </c>
+      <c r="O11" t="s">
+        <v>449</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{8C11662A-BCAC-45AA-8736-25E364CF41AF}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{D7BCD4AF-B7E3-4884-9BE6-AF2407193468}"/>
+    <hyperlink ref="E4" r:id="rId3" xr:uid="{E96CBB08-7725-4EC4-8B97-4381B62A20AC}"/>
+    <hyperlink ref="E5" r:id="rId4" xr:uid="{3C222BD2-F739-4534-9DE6-60B8489DFEA6}"/>
+    <hyperlink ref="E6" r:id="rId5" xr:uid="{D0F42A5C-9B12-451F-BF7F-A05B601FCE1D}"/>
+    <hyperlink ref="E7" r:id="rId6" xr:uid="{BB67F6A5-24A1-45FD-BC5A-2F42E027FC30}"/>
+    <hyperlink ref="E8" r:id="rId7" xr:uid="{C5608EAE-2CE3-49B9-B528-6671D8ADF2C0}"/>
+    <hyperlink ref="E9" r:id="rId8" xr:uid="{AA5D4E6F-E01B-411F-9811-8938FC530979}"/>
+    <hyperlink ref="E10" r:id="rId9" xr:uid="{F56E5482-98B3-41B5-9B8C-199812EC3EBC}"/>
+    <hyperlink ref="E11" r:id="rId10" xr:uid="{52BE2A0A-8174-46F7-A506-1DA84FCDED7F}"/>
+    <hyperlink ref="F2" r:id="rId11" xr:uid="{AD6AAC71-2E98-4420-A716-60E66A3E2464}"/>
+    <hyperlink ref="F3" r:id="rId12" xr:uid="{EB9EDB1A-7760-4FDA-83B6-81CA08496AAF}"/>
+    <hyperlink ref="F4" r:id="rId13" xr:uid="{C4091AFA-6247-408D-B67E-FC7B9FF24FFC}"/>
+    <hyperlink ref="F5" r:id="rId14" xr:uid="{F0D72094-CB20-4A88-BD6E-763773B520EE}"/>
+    <hyperlink ref="F6" r:id="rId15" xr:uid="{708CDE5D-0E4C-4F69-92B6-9156EF596F8D}"/>
+    <hyperlink ref="F7" r:id="rId16" xr:uid="{770D6A80-5F8F-4383-AD2E-12629E1F70E5}"/>
+    <hyperlink ref="F8" r:id="rId17" xr:uid="{33B40313-CF60-45E1-B044-B89F8FC075E7}"/>
+    <hyperlink ref="F9" r:id="rId18" xr:uid="{13CB37C1-C34F-4489-B35C-6BF4FFC2DD0D}"/>
+    <hyperlink ref="F10" r:id="rId19" xr:uid="{3102A8D1-CA80-4DB4-A4BC-97C976B6B2D2}"/>
+    <hyperlink ref="F11" r:id="rId20" xr:uid="{78781037-EF74-469B-AF17-58A15339BF9E}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId21"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:J11"/>
   <sheetViews>
@@ -4513,12 +5887,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="14.4"/>
@@ -4581,10 +5955,10 @@
         <v>5</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>88</v>
@@ -4619,10 +5993,10 @@
         <v>6</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>88</v>
@@ -4645,10 +6019,10 @@
         <v>7</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D4" s="10" t="s">
         <v>88</v>
@@ -4671,10 +6045,10 @@
         <v>8</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D5" s="10" t="s">
         <v>88</v>
@@ -4697,10 +6071,10 @@
         <v>9</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D6" s="10" t="s">
         <v>88</v>
@@ -4723,10 +6097,10 @@
         <v>10</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D7" s="10" t="s">
         <v>88</v>
@@ -4749,10 +6123,10 @@
         <v>11</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D8" s="10" t="s">
         <v>88</v>
@@ -4775,10 +6149,10 @@
         <v>12</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D9" s="10" t="s">
         <v>88</v>
@@ -4801,10 +6175,10 @@
         <v>13</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D10" s="10" t="s">
         <v>88</v>
@@ -4827,10 +6201,10 @@
         <v>14</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D11" s="10" t="s">
         <v>88</v>
@@ -4870,7 +6244,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:P11"/>
   <sheetViews>
@@ -4916,28 +6290,28 @@
         <v>76</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>248</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="2" spans="1:16">
@@ -4945,13 +6319,13 @@
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C2" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="D2" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>65</v>
@@ -4965,13 +6339,13 @@
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C3" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="D3" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>65</v>
@@ -4985,13 +6359,13 @@
         <v>7</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C4" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="D4" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>65</v>
@@ -5005,13 +6379,13 @@
         <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C5" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="D5" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>65</v>
@@ -5025,13 +6399,13 @@
         <v>9</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C6" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="D6" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>65</v>
@@ -5045,13 +6419,13 @@
         <v>10</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C7" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="D7" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>65</v>
@@ -5065,13 +6439,13 @@
         <v>11</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C8" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="D8" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>65</v>
@@ -5085,13 +6459,13 @@
         <v>12</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C9" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="D9" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>65</v>
@@ -5105,13 +6479,13 @@
         <v>13</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="C10" t="s">
         <v>239</v>
       </c>
-      <c r="C10" t="s">
-        <v>241</v>
-      </c>
       <c r="D10" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>65</v>
@@ -5125,13 +6499,13 @@
         <v>14</v>
       </c>
       <c r="B11" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="C11" t="s">
+        <v>239</v>
+      </c>
+      <c r="D11" t="s">
         <v>240</v>
-      </c>
-      <c r="C11" t="s">
-        <v>241</v>
-      </c>
-      <c r="D11" t="s">
-        <v>242</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>65</v>
@@ -5168,7 +6542,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:G11"/>
   <sheetViews>
@@ -5214,10 +6588,10 @@
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C2" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D2" t="s">
         <v>64</v>
@@ -5237,10 +6611,10 @@
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C3" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D3" t="s">
         <v>64</v>
@@ -5257,10 +6631,10 @@
         <v>7</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C4" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D4" t="s">
         <v>64</v>
@@ -5277,10 +6651,10 @@
         <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C5" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D5" t="s">
         <v>64</v>
@@ -5297,10 +6671,10 @@
         <v>9</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C6" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D6" t="s">
         <v>64</v>
@@ -5317,10 +6691,10 @@
         <v>10</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C7" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D7" t="s">
         <v>64</v>
@@ -5337,10 +6711,10 @@
         <v>11</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C8" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D8" t="s">
         <v>64</v>
@@ -5357,10 +6731,10 @@
         <v>12</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C9" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D9" t="s">
         <v>64</v>
@@ -5377,10 +6751,10 @@
         <v>13</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C10" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D10" t="s">
         <v>64</v>
@@ -5397,10 +6771,10 @@
         <v>14</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C11" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D11" t="s">
         <v>64</v>
@@ -5433,7 +6807,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:H11"/>
   <sheetViews>
@@ -5483,10 +6857,10 @@
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C2" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D2" t="s">
         <v>66</v>
@@ -5509,10 +6883,10 @@
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C3" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D3" t="s">
         <v>66</v>
@@ -5529,10 +6903,10 @@
         <v>7</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C4" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D4" t="s">
         <v>66</v>
@@ -5549,10 +6923,10 @@
         <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="C5" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D5" t="s">
         <v>66</v>
@@ -5569,10 +6943,10 @@
         <v>9</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C6" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D6" t="s">
         <v>66</v>
@@ -5589,10 +6963,10 @@
         <v>10</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C7" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D7" t="s">
         <v>66</v>
@@ -5609,10 +6983,10 @@
         <v>11</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="C8" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D8" t="s">
         <v>66</v>
@@ -5629,10 +7003,10 @@
         <v>12</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C9" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D9" t="s">
         <v>66</v>
@@ -5649,10 +7023,10 @@
         <v>13</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C10" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D10" t="s">
         <v>66</v>
@@ -5669,10 +7043,10 @@
         <v>14</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="C11" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D11" t="s">
         <v>66</v>
@@ -5703,269 +7077,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId13"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
-  <cols>
-    <col min="2" max="2" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="41.77734375" customWidth="1"/>
-    <col min="4" max="4" width="34.21875" customWidth="1"/>
-    <col min="5" max="5" width="22.5546875" customWidth="1"/>
-    <col min="6" max="6" width="11.21875" customWidth="1"/>
-    <col min="7" max="7" width="23" customWidth="1"/>
-    <col min="8" max="8" width="15.77734375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.77734375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9">
-      <c r="A1" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
-      <c r="A2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>306</v>
-      </c>
-      <c r="C2" t="s">
-        <v>305</v>
-      </c>
-      <c r="D2" t="s">
-        <v>92</v>
-      </c>
-      <c r="E2" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="F2" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I2" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>314</v>
-      </c>
-      <c r="C3" t="s">
-        <v>305</v>
-      </c>
-      <c r="D3" t="s">
-        <v>92</v>
-      </c>
-      <c r="E3" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="F3" s="13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>307</v>
-      </c>
-      <c r="C4" t="s">
-        <v>305</v>
-      </c>
-      <c r="D4" t="s">
-        <v>92</v>
-      </c>
-      <c r="E4" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="F4" s="13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>308</v>
-      </c>
-      <c r="C5" t="s">
-        <v>305</v>
-      </c>
-      <c r="D5" t="s">
-        <v>92</v>
-      </c>
-      <c r="E5" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="F5" s="13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="A6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>309</v>
-      </c>
-      <c r="C6" t="s">
-        <v>305</v>
-      </c>
-      <c r="D6" t="s">
-        <v>92</v>
-      </c>
-      <c r="E6" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="F6" s="13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>310</v>
-      </c>
-      <c r="C7" t="s">
-        <v>305</v>
-      </c>
-      <c r="D7" t="s">
-        <v>92</v>
-      </c>
-      <c r="E7" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="F7" s="13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="A8" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>311</v>
-      </c>
-      <c r="C8" t="s">
-        <v>305</v>
-      </c>
-      <c r="D8" t="s">
-        <v>92</v>
-      </c>
-      <c r="E8" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="F8" s="13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="A9" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>312</v>
-      </c>
-      <c r="C9" t="s">
-        <v>305</v>
-      </c>
-      <c r="D9" t="s">
-        <v>92</v>
-      </c>
-      <c r="E9" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="F9" s="13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="A10" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>313</v>
-      </c>
-      <c r="C10" t="s">
-        <v>305</v>
-      </c>
-      <c r="D10" t="s">
-        <v>92</v>
-      </c>
-      <c r="E10" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="F10" s="13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="A11" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>315</v>
-      </c>
-      <c r="C11" t="s">
-        <v>305</v>
-      </c>
-      <c r="D11" t="s">
-        <v>92</v>
-      </c>
-      <c r="E11" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="F11" s="13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
partial changes done to Travel expense Test case.
</commit_message>
<xml_diff>
--- a/src/main/resources/AutomationCatalogue_Batch41_TestData.xlsx
+++ b/src/main/resources/AutomationCatalogue_Batch41_TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Automation Catalogue\TestAutomationCatalogue_Batch41\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55A76453-BA0E-4FF5-8AA8-EF8757939A81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B77F0DB-24BC-4FD2-B1E5-F27FAE088218}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="944" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1387" uniqueCount="450">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1370" uniqueCount="442">
   <si>
     <t>S. No</t>
   </si>
@@ -1185,217 +1185,193 @@
     <t>Paid by</t>
   </si>
   <si>
+    <t>Request Status</t>
+  </si>
+  <si>
+    <t>TC05_OrangeHRM_AddEmployee</t>
+  </si>
+  <si>
+    <t>AED - Utd. Arab Emir. Dirham</t>
+  </si>
+  <si>
+    <t>London</t>
+  </si>
+  <si>
+    <t>1-Jan-2022</t>
+  </si>
+  <si>
+    <t>15-Jan-2022</t>
+  </si>
+  <si>
+    <t>Airfare</t>
+  </si>
+  <si>
+    <t>CAD - Canadian Dollar</t>
+  </si>
+  <si>
+    <t>Chicago</t>
+  </si>
+  <si>
+    <t>1-Feb-2022</t>
+  </si>
+  <si>
+    <t>15-Feb-2022</t>
+  </si>
+  <si>
+    <t>Charitable Donations</t>
+  </si>
+  <si>
+    <t>Staff</t>
+  </si>
+  <si>
+    <t>AUD - Australian Dollar</t>
+  </si>
+  <si>
+    <t>Texas</t>
+  </si>
+  <si>
+    <t>1-Mar-2022</t>
+  </si>
+  <si>
+    <t>15-Mar-2022</t>
+  </si>
+  <si>
+    <t>Entertainment</t>
+  </si>
+  <si>
+    <t>EUR - Euro</t>
+  </si>
+  <si>
+    <t>Canada</t>
+  </si>
+  <si>
+    <t>1-Apr-2022</t>
+  </si>
+  <si>
+    <t>15-Apr-2022</t>
+  </si>
+  <si>
+    <t>Food &amp; Beverage</t>
+  </si>
+  <si>
+    <t>JPY - Japanese Yen</t>
+  </si>
+  <si>
+    <t>Germany</t>
+  </si>
+  <si>
+    <t>1-May-2022</t>
+  </si>
+  <si>
+    <t>15-May-2022</t>
+  </si>
+  <si>
+    <t>Fuel</t>
+  </si>
+  <si>
+    <t>LKR - Sri Lanka Rupee</t>
+  </si>
+  <si>
+    <t>Paris</t>
+  </si>
+  <si>
+    <t>1-Jun-2022</t>
+  </si>
+  <si>
+    <t>15-Jun-2022</t>
+  </si>
+  <si>
+    <t>Ground Transportation</t>
+  </si>
+  <si>
+    <t>PHP - Philippine Peso</t>
+  </si>
+  <si>
+    <t>NewYork</t>
+  </si>
+  <si>
+    <t>1-Jul-2022</t>
+  </si>
+  <si>
+    <t>15-Jul-2022</t>
+  </si>
+  <si>
+    <t>Hotel</t>
+  </si>
+  <si>
+    <t>USD - United States Dollar</t>
+  </si>
+  <si>
+    <t>Vegas</t>
+  </si>
+  <si>
+    <t>1-Aug-2022</t>
+  </si>
+  <si>
+    <t>15-Aug-2022</t>
+  </si>
+  <si>
+    <t>Maintenance &amp; Repairs</t>
+  </si>
+  <si>
+    <t>MXN - Mexican New Peso</t>
+  </si>
+  <si>
+    <t>Pittsburgh</t>
+  </si>
+  <si>
+    <t>1-Sep-2022</t>
+  </si>
+  <si>
+    <t>15-Sep-2022</t>
+  </si>
+  <si>
+    <t>ZMK - Zambian Kwacha</t>
+  </si>
+  <si>
+    <t>NewJersy</t>
+  </si>
+  <si>
+    <t>1-OCt-2022</t>
+  </si>
+  <si>
+    <t>15-Oct-2022</t>
+  </si>
+  <si>
+    <t>Office Supplies</t>
+  </si>
+  <si>
+    <t>2500</t>
+  </si>
+  <si>
+    <t>500</t>
+  </si>
+  <si>
+    <t>200</t>
+  </si>
+  <si>
+    <t>250</t>
+  </si>
+  <si>
+    <t>150</t>
+  </si>
+  <si>
+    <t>1500</t>
+  </si>
+  <si>
+    <t>Req Id</t>
+  </si>
+  <si>
+    <t>0164</t>
+  </si>
+  <si>
+    <t>PASSED</t>
+  </si>
+  <si>
     <t>Employee Name</t>
   </si>
   <si>
-    <t>Request Status</t>
-  </si>
-  <si>
-    <t>Supervisor Username</t>
-  </si>
-  <si>
-    <t>TC05_OrangeHRM_AddEmployee</t>
-  </si>
-  <si>
-    <t>AED - Utd. Arab Emir. Dirham</t>
-  </si>
-  <si>
-    <t>London</t>
-  </si>
-  <si>
-    <t>1-Jan-2022</t>
-  </si>
-  <si>
-    <t>15-Jan-2022</t>
-  </si>
-  <si>
-    <t>Airfare</t>
-  </si>
-  <si>
-    <t>CAD - Canadian Dollar</t>
-  </si>
-  <si>
-    <t>Chicago</t>
-  </si>
-  <si>
-    <t>1-Feb-2022</t>
-  </si>
-  <si>
-    <t>15-Feb-2022</t>
-  </si>
-  <si>
-    <t>Charitable Donations</t>
-  </si>
-  <si>
-    <t>Staff</t>
-  </si>
-  <si>
-    <t>AUD - Australian Dollar</t>
-  </si>
-  <si>
-    <t>Texas</t>
-  </si>
-  <si>
-    <t>1-Mar-2022</t>
-  </si>
-  <si>
-    <t>15-Mar-2022</t>
-  </si>
-  <si>
-    <t>Entertainment</t>
-  </si>
-  <si>
-    <t>EUR - Euro</t>
-  </si>
-  <si>
-    <t>Canada</t>
-  </si>
-  <si>
-    <t>1-Apr-2022</t>
-  </si>
-  <si>
-    <t>15-Apr-2022</t>
-  </si>
-  <si>
-    <t>Food &amp; Beverage</t>
-  </si>
-  <si>
-    <t>JPY - Japanese Yen</t>
-  </si>
-  <si>
-    <t>Germany</t>
-  </si>
-  <si>
-    <t>1-May-2022</t>
-  </si>
-  <si>
-    <t>15-May-2022</t>
-  </si>
-  <si>
-    <t>Fuel</t>
-  </si>
-  <si>
-    <t>LKR - Sri Lanka Rupee</t>
-  </si>
-  <si>
-    <t>Paris</t>
-  </si>
-  <si>
-    <t>1-Jun-2022</t>
-  </si>
-  <si>
-    <t>15-Jun-2022</t>
-  </si>
-  <si>
-    <t>Ground Transportation</t>
-  </si>
-  <si>
-    <t>PHP - Philippine Peso</t>
-  </si>
-  <si>
-    <t>NewYork</t>
-  </si>
-  <si>
-    <t>1-Jul-2022</t>
-  </si>
-  <si>
-    <t>15-Jul-2022</t>
-  </si>
-  <si>
-    <t>Hotel</t>
-  </si>
-  <si>
-    <t>USD - United States Dollar</t>
-  </si>
-  <si>
-    <t>Vegas</t>
-  </si>
-  <si>
-    <t>1-Aug-2022</t>
-  </si>
-  <si>
-    <t>15-Aug-2022</t>
-  </si>
-  <si>
-    <t>Maintenance &amp; Repairs</t>
-  </si>
-  <si>
-    <t>MXN - Mexican New Peso</t>
-  </si>
-  <si>
-    <t>Pittsburgh</t>
-  </si>
-  <si>
-    <t>1-Sep-2022</t>
-  </si>
-  <si>
-    <t>15-Sep-2022</t>
-  </si>
-  <si>
-    <t>ZMK - Zambian Kwacha</t>
-  </si>
-  <si>
-    <t>NewJersy</t>
-  </si>
-  <si>
-    <t>1-OCt-2022</t>
-  </si>
-  <si>
-    <t>15-Oct-2022</t>
-  </si>
-  <si>
-    <t>Office Supplies</t>
-  </si>
-  <si>
-    <t>Brody Naidu</t>
-  </si>
-  <si>
-    <t>2500</t>
-  </si>
-  <si>
-    <t>500</t>
-  </si>
-  <si>
-    <t>200</t>
-  </si>
-  <si>
-    <t>250</t>
-  </si>
-  <si>
-    <t>150</t>
-  </si>
-  <si>
-    <t>1500</t>
-  </si>
-  <si>
-    <t>John Mikel</t>
-  </si>
-  <si>
-    <t>Christopher Anderson</t>
-  </si>
-  <si>
-    <t>Ronald Clark</t>
-  </si>
-  <si>
-    <t>Mary Wright</t>
-  </si>
-  <si>
-    <t>Lisa Mitchell</t>
-  </si>
-  <si>
-    <t>Michelle Johnson</t>
-  </si>
-  <si>
-    <t>John Thomas</t>
-  </si>
-  <si>
-    <t>Daniel Rodriguez</t>
-  </si>
-  <si>
-    <t>Anthony Lopez</t>
-  </si>
-  <si>
-    <t>Req Id</t>
+    <t>Aaliyah Haq</t>
   </si>
 </sst>
 </file>
@@ -1867,7 +1843,7 @@
   <dimension ref="A1:F122"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2071,6 +2047,9 @@
       </c>
       <c r="D14" t="s">
         <v>38</v>
+      </c>
+      <c r="E14" t="s">
+        <v>439</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -4405,10 +4384,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:O25"/>
+  <dimension ref="A1:O11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H16" sqref="H16:H25"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -4517,6 +4496,9 @@
       <c r="N2" t="s">
         <v>52</v>
       </c>
+      <c r="O2" t="s">
+        <v>438</v>
+      </c>
     </row>
     <row r="3" spans="1:15">
       <c r="A3" s="2" t="s">
@@ -4912,86 +4894,6 @@
       </c>
       <c r="N11" t="s">
         <v>55</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15">
-      <c r="F16" t="s">
-        <v>39</v>
-      </c>
-      <c r="G16" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="17" spans="6:7">
-      <c r="F17" t="s">
-        <v>347</v>
-      </c>
-      <c r="G17" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="18" spans="6:7">
-      <c r="F18" t="s">
-        <v>349</v>
-      </c>
-      <c r="G18" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="19" spans="6:7">
-      <c r="F19" t="s">
-        <v>351</v>
-      </c>
-      <c r="G19" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="20" spans="6:7">
-      <c r="F20" t="s">
-        <v>353</v>
-      </c>
-      <c r="G20" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="21" spans="6:7">
-      <c r="F21" t="s">
-        <v>356</v>
-      </c>
-      <c r="G21" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="22" spans="6:7">
-      <c r="F22" t="s">
-        <v>39</v>
-      </c>
-      <c r="G22" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="23" spans="6:7">
-      <c r="F23" t="s">
-        <v>361</v>
-      </c>
-      <c r="G23" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="24" spans="6:7">
-      <c r="F24" t="s">
-        <v>364</v>
-      </c>
-      <c r="G24" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="25" spans="6:7">
-      <c r="F25" t="s">
-        <v>367</v>
-      </c>
-      <c r="G25" t="s">
-        <v>368</v>
       </c>
     </row>
   </sheetData>
@@ -5016,30 +4918,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B26C6E52-E5E5-4D9E-897F-B24CFADC5889}">
   <dimension ref="A1:R11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="P13" sqref="P13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="5.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.21875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="26.109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.88671875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.21875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="26.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9" customWidth="1"/>
+    <col min="17" max="17" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.5546875" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="10.5546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5048,549 +4950,553 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>370</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>371</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>372</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>373</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>376</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>377</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>378</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="R1" s="1" t="s">
         <v>379</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>449</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>380</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>381</v>
       </c>
     </row>
     <row r="2" spans="1:18">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="C2" t="s">
+        <v>380</v>
+      </c>
+      <c r="D2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" t="s">
+        <v>381</v>
+      </c>
+      <c r="I2" t="s">
         <v>382</v>
       </c>
-      <c r="C2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="J2" s="2" t="s">
         <v>383</v>
       </c>
-      <c r="H2" t="s">
+      <c r="K2" s="2" t="s">
         <v>384</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="L2" t="s">
         <v>385</v>
       </c>
-      <c r="J2" s="2" t="s">
-        <v>386</v>
-      </c>
-      <c r="K2" t="s">
-        <v>387</v>
-      </c>
-      <c r="L2" t="s">
-        <v>383</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>434</v>
-      </c>
-      <c r="N2" t="s">
+      <c r="M2" t="s">
+        <v>381</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>431</v>
+      </c>
+      <c r="O2" t="s">
         <v>242</v>
       </c>
-      <c r="O2" t="s">
-        <v>433</v>
+      <c r="P2" t="s">
+        <v>441</v>
       </c>
     </row>
     <row r="3" spans="1:18">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
-        <v>382</v>
+      <c r="B3" s="2" t="s">
+        <v>195</v>
       </c>
       <c r="C3" t="s">
+        <v>380</v>
+      </c>
+      <c r="D3" t="s">
         <v>38</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>18</v>
-      </c>
       <c r="F3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" t="s">
+        <v>386</v>
+      </c>
+      <c r="I3" t="s">
+        <v>387</v>
+      </c>
+      <c r="J3" s="2" t="s">
         <v>388</v>
       </c>
-      <c r="H3" t="s">
+      <c r="K3" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="L3" t="s">
         <v>390</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="M3" t="s">
+        <v>381</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>432</v>
+      </c>
+      <c r="O3" t="s">
         <v>391</v>
-      </c>
-      <c r="K3" t="s">
-        <v>392</v>
-      </c>
-      <c r="L3" t="s">
-        <v>383</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>435</v>
-      </c>
-      <c r="N3" t="s">
-        <v>393</v>
-      </c>
-      <c r="O3" t="s">
-        <v>440</v>
       </c>
     </row>
     <row r="4" spans="1:18">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B4" t="s">
-        <v>382</v>
+      <c r="B4" s="2" t="s">
+        <v>196</v>
       </c>
       <c r="C4" t="s">
+        <v>380</v>
+      </c>
+      <c r="D4" t="s">
         <v>38</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>18</v>
-      </c>
       <c r="F4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" t="s">
+        <v>392</v>
+      </c>
+      <c r="I4" t="s">
+        <v>393</v>
+      </c>
+      <c r="J4" s="2" t="s">
         <v>394</v>
       </c>
-      <c r="H4" t="s">
+      <c r="K4" s="2" t="s">
         <v>395</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="L4" t="s">
         <v>396</v>
       </c>
-      <c r="J4" s="2" t="s">
-        <v>397</v>
-      </c>
-      <c r="K4" t="s">
-        <v>398</v>
-      </c>
-      <c r="L4" t="s">
-        <v>383</v>
-      </c>
-      <c r="M4" s="2" t="s">
-        <v>436</v>
-      </c>
-      <c r="N4" t="s">
-        <v>393</v>
+      <c r="M4" t="s">
+        <v>381</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>433</v>
       </c>
       <c r="O4" t="s">
-        <v>441</v>
+        <v>391</v>
       </c>
     </row>
     <row r="5" spans="1:18">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B5" t="s">
-        <v>382</v>
+      <c r="B5" s="2" t="s">
+        <v>197</v>
       </c>
       <c r="C5" t="s">
+        <v>380</v>
+      </c>
+      <c r="D5" t="s">
         <v>38</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="3" t="s">
-        <v>18</v>
-      </c>
       <c r="F5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" t="s">
+        <v>397</v>
+      </c>
+      <c r="I5" t="s">
+        <v>398</v>
+      </c>
+      <c r="J5" s="2" t="s">
         <v>399</v>
       </c>
-      <c r="H5" t="s">
+      <c r="K5" s="2" t="s">
         <v>400</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="L5" t="s">
         <v>401</v>
       </c>
-      <c r="J5" s="2" t="s">
-        <v>402</v>
-      </c>
-      <c r="K5" t="s">
-        <v>403</v>
-      </c>
-      <c r="L5" t="s">
-        <v>383</v>
-      </c>
-      <c r="M5" s="2" t="s">
-        <v>435</v>
-      </c>
-      <c r="N5" t="s">
-        <v>393</v>
+      <c r="M5" t="s">
+        <v>381</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>432</v>
       </c>
       <c r="O5" t="s">
-        <v>442</v>
+        <v>391</v>
       </c>
     </row>
     <row r="6" spans="1:18">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B6" t="s">
-        <v>382</v>
+      <c r="B6" s="2" t="s">
+        <v>198</v>
       </c>
       <c r="C6" t="s">
+        <v>380</v>
+      </c>
+      <c r="D6" t="s">
         <v>38</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>18</v>
-      </c>
       <c r="F6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" t="s">
+        <v>402</v>
+      </c>
+      <c r="I6" t="s">
+        <v>403</v>
+      </c>
+      <c r="J6" s="2" t="s">
         <v>404</v>
       </c>
-      <c r="H6" t="s">
+      <c r="K6" s="2" t="s">
         <v>405</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="L6" t="s">
         <v>406</v>
       </c>
-      <c r="J6" s="2" t="s">
-        <v>407</v>
-      </c>
-      <c r="K6" t="s">
-        <v>408</v>
-      </c>
-      <c r="L6" t="s">
-        <v>383</v>
-      </c>
-      <c r="M6" s="2" t="s">
-        <v>437</v>
-      </c>
-      <c r="N6" t="s">
-        <v>393</v>
+      <c r="M6" t="s">
+        <v>381</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>434</v>
       </c>
       <c r="O6" t="s">
-        <v>443</v>
+        <v>391</v>
       </c>
     </row>
     <row r="7" spans="1:18">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B7" t="s">
-        <v>382</v>
+      <c r="B7" s="2" t="s">
+        <v>199</v>
       </c>
       <c r="C7" t="s">
+        <v>380</v>
+      </c>
+      <c r="D7" t="s">
         <v>38</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="3" t="s">
-        <v>18</v>
-      </c>
       <c r="F7" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H7" t="s">
+        <v>407</v>
+      </c>
+      <c r="I7" t="s">
+        <v>408</v>
+      </c>
+      <c r="J7" s="2" t="s">
         <v>409</v>
       </c>
-      <c r="H7" t="s">
+      <c r="K7" s="2" t="s">
         <v>410</v>
       </c>
-      <c r="I7" s="2" t="s">
+      <c r="L7" t="s">
         <v>411</v>
       </c>
-      <c r="J7" s="2" t="s">
-        <v>412</v>
-      </c>
-      <c r="K7" t="s">
-        <v>413</v>
-      </c>
-      <c r="L7" t="s">
-        <v>383</v>
-      </c>
-      <c r="M7" s="2" t="s">
-        <v>438</v>
-      </c>
-      <c r="N7" t="s">
-        <v>393</v>
+      <c r="M7" t="s">
+        <v>381</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>435</v>
       </c>
       <c r="O7" t="s">
-        <v>444</v>
+        <v>391</v>
       </c>
     </row>
     <row r="8" spans="1:18">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B8" t="s">
-        <v>382</v>
+      <c r="B8" s="2" t="s">
+        <v>200</v>
       </c>
       <c r="C8" t="s">
+        <v>380</v>
+      </c>
+      <c r="D8" t="s">
         <v>38</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="3" t="s">
-        <v>18</v>
-      </c>
       <c r="F8" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H8" t="s">
+        <v>412</v>
+      </c>
+      <c r="I8" t="s">
+        <v>413</v>
+      </c>
+      <c r="J8" s="2" t="s">
         <v>414</v>
       </c>
-      <c r="H8" t="s">
+      <c r="K8" s="2" t="s">
         <v>415</v>
       </c>
-      <c r="I8" s="2" t="s">
+      <c r="L8" t="s">
         <v>416</v>
       </c>
-      <c r="J8" s="2" t="s">
-        <v>417</v>
-      </c>
-      <c r="K8" t="s">
-        <v>418</v>
-      </c>
-      <c r="L8" t="s">
-        <v>383</v>
-      </c>
-      <c r="M8" s="2" t="s">
-        <v>437</v>
-      </c>
-      <c r="N8" t="s">
+      <c r="M8" t="s">
+        <v>381</v>
+      </c>
+      <c r="N8" s="2" t="s">
+        <v>434</v>
+      </c>
+      <c r="O8" t="s">
         <v>242</v>
-      </c>
-      <c r="O8" t="s">
-        <v>445</v>
       </c>
     </row>
     <row r="9" spans="1:18">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B9" t="s">
-        <v>382</v>
+      <c r="B9" s="2" t="s">
+        <v>201</v>
       </c>
       <c r="C9" t="s">
+        <v>380</v>
+      </c>
+      <c r="D9" t="s">
         <v>38</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="3" t="s">
-        <v>18</v>
-      </c>
       <c r="F9" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H9" t="s">
+        <v>417</v>
+      </c>
+      <c r="I9" t="s">
+        <v>418</v>
+      </c>
+      <c r="J9" s="2" t="s">
         <v>419</v>
       </c>
-      <c r="H9" t="s">
+      <c r="K9" s="2" t="s">
         <v>420</v>
       </c>
-      <c r="I9" s="2" t="s">
+      <c r="L9" t="s">
         <v>421</v>
       </c>
-      <c r="J9" s="2" t="s">
-        <v>422</v>
-      </c>
-      <c r="K9" t="s">
-        <v>423</v>
-      </c>
-      <c r="L9" t="s">
-        <v>383</v>
-      </c>
-      <c r="M9" s="2" t="s">
-        <v>435</v>
-      </c>
-      <c r="N9" t="s">
-        <v>393</v>
+      <c r="M9" t="s">
+        <v>381</v>
+      </c>
+      <c r="N9" s="2" t="s">
+        <v>432</v>
       </c>
       <c r="O9" t="s">
-        <v>446</v>
+        <v>391</v>
       </c>
     </row>
     <row r="10" spans="1:18">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B10" t="s">
-        <v>382</v>
+      <c r="B10" s="2" t="s">
+        <v>202</v>
       </c>
       <c r="C10" t="s">
+        <v>380</v>
+      </c>
+      <c r="D10" t="s">
         <v>38</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>17</v>
       </c>
-      <c r="E10" s="3" t="s">
-        <v>18</v>
-      </c>
       <c r="F10" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H10" t="s">
+        <v>422</v>
+      </c>
+      <c r="I10" t="s">
+        <v>423</v>
+      </c>
+      <c r="J10" s="2" t="s">
         <v>424</v>
       </c>
-      <c r="H10" t="s">
+      <c r="K10" s="2" t="s">
         <v>425</v>
       </c>
-      <c r="I10" s="2" t="s">
-        <v>426</v>
-      </c>
-      <c r="J10" s="2" t="s">
-        <v>427</v>
-      </c>
-      <c r="K10" t="s">
-        <v>387</v>
-      </c>
       <c r="L10" t="s">
-        <v>383</v>
-      </c>
-      <c r="M10" s="2" t="s">
-        <v>439</v>
-      </c>
-      <c r="N10" t="s">
+        <v>385</v>
+      </c>
+      <c r="M10" t="s">
+        <v>381</v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>436</v>
+      </c>
+      <c r="O10" t="s">
         <v>242</v>
-      </c>
-      <c r="O10" t="s">
-        <v>447</v>
       </c>
     </row>
     <row r="11" spans="1:18">
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B11" t="s">
-        <v>382</v>
+      <c r="B11" s="2" t="s">
+        <v>203</v>
       </c>
       <c r="C11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D11" t="s">
         <v>38</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>17</v>
       </c>
-      <c r="E11" s="3" t="s">
-        <v>18</v>
-      </c>
       <c r="F11" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H11" t="s">
+        <v>426</v>
+      </c>
+      <c r="I11" t="s">
+        <v>427</v>
+      </c>
+      <c r="J11" s="2" t="s">
         <v>428</v>
       </c>
-      <c r="H11" t="s">
+      <c r="K11" s="2" t="s">
         <v>429</v>
       </c>
-      <c r="I11" s="2" t="s">
+      <c r="L11" t="s">
         <v>430</v>
       </c>
-      <c r="J11" s="2" t="s">
-        <v>431</v>
-      </c>
-      <c r="K11" t="s">
+      <c r="M11" t="s">
+        <v>381</v>
+      </c>
+      <c r="N11" s="2" t="s">
         <v>432</v>
       </c>
-      <c r="L11" t="s">
-        <v>383</v>
-      </c>
-      <c r="M11" s="2" t="s">
-        <v>435</v>
-      </c>
-      <c r="N11" t="s">
-        <v>393</v>
-      </c>
       <c r="O11" t="s">
-        <v>448</v>
+        <v>391</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{8C11662A-BCAC-45AA-8736-25E364CF41AF}"/>
-    <hyperlink ref="E3" r:id="rId2" xr:uid="{D7BCD4AF-B7E3-4884-9BE6-AF2407193468}"/>
-    <hyperlink ref="E4" r:id="rId3" xr:uid="{E96CBB08-7725-4EC4-8B97-4381B62A20AC}"/>
-    <hyperlink ref="E5" r:id="rId4" xr:uid="{3C222BD2-F739-4534-9DE6-60B8489DFEA6}"/>
-    <hyperlink ref="E6" r:id="rId5" xr:uid="{D0F42A5C-9B12-451F-BF7F-A05B601FCE1D}"/>
-    <hyperlink ref="E7" r:id="rId6" xr:uid="{BB67F6A5-24A1-45FD-BC5A-2F42E027FC30}"/>
-    <hyperlink ref="E8" r:id="rId7" xr:uid="{C5608EAE-2CE3-49B9-B528-6671D8ADF2C0}"/>
-    <hyperlink ref="E9" r:id="rId8" xr:uid="{AA5D4E6F-E01B-411F-9811-8938FC530979}"/>
-    <hyperlink ref="E10" r:id="rId9" xr:uid="{F56E5482-98B3-41B5-9B8C-199812EC3EBC}"/>
-    <hyperlink ref="E11" r:id="rId10" xr:uid="{52BE2A0A-8174-46F7-A506-1DA84FCDED7F}"/>
-    <hyperlink ref="F2" r:id="rId11" xr:uid="{AD6AAC71-2E98-4420-A716-60E66A3E2464}"/>
-    <hyperlink ref="F3" r:id="rId12" xr:uid="{EB9EDB1A-7760-4FDA-83B6-81CA08496AAF}"/>
-    <hyperlink ref="F4" r:id="rId13" xr:uid="{C4091AFA-6247-408D-B67E-FC7B9FF24FFC}"/>
-    <hyperlink ref="F5" r:id="rId14" xr:uid="{F0D72094-CB20-4A88-BD6E-763773B520EE}"/>
-    <hyperlink ref="F6" r:id="rId15" xr:uid="{708CDE5D-0E4C-4F69-92B6-9156EF596F8D}"/>
-    <hyperlink ref="F7" r:id="rId16" xr:uid="{770D6A80-5F8F-4383-AD2E-12629E1F70E5}"/>
-    <hyperlink ref="F8" r:id="rId17" xr:uid="{33B40313-CF60-45E1-B044-B89F8FC075E7}"/>
-    <hyperlink ref="F9" r:id="rId18" xr:uid="{13CB37C1-C34F-4489-B35C-6BF4FFC2DD0D}"/>
-    <hyperlink ref="F10" r:id="rId19" xr:uid="{3102A8D1-CA80-4DB4-A4BC-97C976B6B2D2}"/>
-    <hyperlink ref="F11" r:id="rId20" xr:uid="{78781037-EF74-469B-AF17-58A15339BF9E}"/>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{8C11662A-BCAC-45AA-8736-25E364CF41AF}"/>
+    <hyperlink ref="F3" r:id="rId2" xr:uid="{D7BCD4AF-B7E3-4884-9BE6-AF2407193468}"/>
+    <hyperlink ref="F4" r:id="rId3" xr:uid="{E96CBB08-7725-4EC4-8B97-4381B62A20AC}"/>
+    <hyperlink ref="F5" r:id="rId4" xr:uid="{3C222BD2-F739-4534-9DE6-60B8489DFEA6}"/>
+    <hyperlink ref="F6" r:id="rId5" xr:uid="{D0F42A5C-9B12-451F-BF7F-A05B601FCE1D}"/>
+    <hyperlink ref="F7" r:id="rId6" xr:uid="{BB67F6A5-24A1-45FD-BC5A-2F42E027FC30}"/>
+    <hyperlink ref="F8" r:id="rId7" xr:uid="{C5608EAE-2CE3-49B9-B528-6671D8ADF2C0}"/>
+    <hyperlink ref="F9" r:id="rId8" xr:uid="{AA5D4E6F-E01B-411F-9811-8938FC530979}"/>
+    <hyperlink ref="F10" r:id="rId9" xr:uid="{F56E5482-98B3-41B5-9B8C-199812EC3EBC}"/>
+    <hyperlink ref="F11" r:id="rId10" xr:uid="{52BE2A0A-8174-46F7-A506-1DA84FCDED7F}"/>
+    <hyperlink ref="G2" r:id="rId11" xr:uid="{AD6AAC71-2E98-4420-A716-60E66A3E2464}"/>
+    <hyperlink ref="G3" r:id="rId12" xr:uid="{EB9EDB1A-7760-4FDA-83B6-81CA08496AAF}"/>
+    <hyperlink ref="G4" r:id="rId13" xr:uid="{C4091AFA-6247-408D-B67E-FC7B9FF24FFC}"/>
+    <hyperlink ref="G5" r:id="rId14" xr:uid="{F0D72094-CB20-4A88-BD6E-763773B520EE}"/>
+    <hyperlink ref="G6" r:id="rId15" xr:uid="{708CDE5D-0E4C-4F69-92B6-9156EF596F8D}"/>
+    <hyperlink ref="G7" r:id="rId16" xr:uid="{770D6A80-5F8F-4383-AD2E-12629E1F70E5}"/>
+    <hyperlink ref="G8" r:id="rId17" xr:uid="{33B40313-CF60-45E1-B044-B89F8FC075E7}"/>
+    <hyperlink ref="G9" r:id="rId18" xr:uid="{13CB37C1-C34F-4489-B35C-6BF4FFC2DD0D}"/>
+    <hyperlink ref="G10" r:id="rId19" xr:uid="{3102A8D1-CA80-4DB4-A4BC-97C976B6B2D2}"/>
+    <hyperlink ref="G11" r:id="rId20" xr:uid="{78781037-EF74-469B-AF17-58A15339BF9E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId21"/>

</xml_diff>

<commit_message>
applied log 4j code changes to Addemployee test case and edit employee test case.
</commit_message>
<xml_diff>
--- a/src/main/resources/AutomationCatalogue_Batch41_TestData.xlsx
+++ b/src/main/resources/AutomationCatalogue_Batch41_TestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Automation Catalogue\TestAutomationCatalogue_Batch41\src\main\resources\"/>
     </mc:Choice>
@@ -27,7 +27,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1370" uniqueCount="442">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1372" uniqueCount="443">
   <si>
     <t>S. No</t>
   </si>
@@ -1372,12 +1372,16 @@
   </si>
   <si>
     <t>Aaliyah Haq</t>
+  </si>
+  <si>
+    <t>0167</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="8">
     <font>
       <sz val="11"/>
@@ -1848,11 +1852,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="5.0"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.77734375"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="39.0"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="38.0"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="9.44140625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1889,13 +1893,13 @@
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>106</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>15</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" t="s" s="0">
         <v>16</v>
       </c>
     </row>
@@ -1903,13 +1907,13 @@
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>107</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" t="s" s="0">
         <v>15</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" t="s" s="0">
         <v>16</v>
       </c>
     </row>
@@ -1917,13 +1921,13 @@
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" t="s" s="0">
         <v>108</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" t="s" s="0">
         <v>15</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" t="s" s="0">
         <v>16</v>
       </c>
     </row>
@@ -1931,13 +1935,13 @@
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" t="s" s="0">
         <v>109</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" t="s" s="0">
         <v>15</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" t="s" s="0">
         <v>16</v>
       </c>
     </row>
@@ -1945,13 +1949,13 @@
       <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" t="s" s="0">
         <v>110</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" t="s" s="0">
         <v>15</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" t="s" s="0">
         <v>16</v>
       </c>
     </row>
@@ -1959,13 +1963,13 @@
       <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" t="s" s="0">
         <v>111</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" t="s" s="0">
         <v>15</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" t="s" s="0">
         <v>16</v>
       </c>
     </row>
@@ -1973,13 +1977,13 @@
       <c r="A9" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" t="s" s="0">
         <v>112</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" t="s" s="0">
         <v>15</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" t="s" s="0">
         <v>16</v>
       </c>
     </row>
@@ -1987,13 +1991,13 @@
       <c r="A10" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" t="s" s="0">
         <v>113</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" t="s" s="0">
         <v>15</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" t="s" s="0">
         <v>16</v>
       </c>
     </row>
@@ -2001,13 +2005,13 @@
       <c r="A11" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" t="s" s="0">
         <v>114</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" t="s" s="0">
         <v>15</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" t="s" s="0">
         <v>16</v>
       </c>
     </row>
@@ -2015,13 +2019,13 @@
       <c r="A12" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" t="s" s="0">
         <v>115</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" t="s" s="0">
         <v>15</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" t="s" s="0">
         <v>16</v>
       </c>
     </row>
@@ -2042,13 +2046,13 @@
       <c r="B14" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" t="s" s="0">
         <v>38</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" t="s" s="0">
         <v>439</v>
       </c>
     </row>
@@ -2059,10 +2063,10 @@
       <c r="B15" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" t="s" s="0">
         <v>38</v>
       </c>
     </row>
@@ -2073,10 +2077,10 @@
       <c r="B16" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" t="s" s="0">
         <v>38</v>
       </c>
     </row>
@@ -2087,10 +2091,10 @@
       <c r="B17" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" t="s" s="0">
         <v>38</v>
       </c>
     </row>
@@ -2101,10 +2105,10 @@
       <c r="B18" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" t="s" s="0">
         <v>38</v>
       </c>
     </row>
@@ -2115,10 +2119,10 @@
       <c r="B19" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" t="s" s="0">
         <v>38</v>
       </c>
     </row>
@@ -2129,10 +2133,10 @@
       <c r="B20" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" t="s" s="0">
         <v>38</v>
       </c>
     </row>
@@ -2143,10 +2147,10 @@
       <c r="B21" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" t="s" s="0">
         <v>38</v>
       </c>
     </row>
@@ -2157,10 +2161,10 @@
       <c r="B22" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" t="s" s="0">
         <v>38</v>
       </c>
     </row>
@@ -2171,10 +2175,10 @@
       <c r="B23" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" t="s" s="0">
         <v>38</v>
       </c>
     </row>
@@ -2195,10 +2199,10 @@
       <c r="B25" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" t="s" s="0">
         <v>98</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" t="s" s="0">
         <v>99</v>
       </c>
     </row>
@@ -2209,10 +2213,10 @@
       <c r="B26" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" t="s" s="0">
         <v>98</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26" t="s" s="0">
         <v>99</v>
       </c>
     </row>
@@ -2223,10 +2227,10 @@
       <c r="B27" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" t="s" s="0">
         <v>98</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D27" t="s" s="0">
         <v>99</v>
       </c>
     </row>
@@ -2237,10 +2241,10 @@
       <c r="B28" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" t="s" s="0">
         <v>98</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D28" t="s" s="0">
         <v>99</v>
       </c>
     </row>
@@ -2251,10 +2255,10 @@
       <c r="B29" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" t="s" s="0">
         <v>98</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D29" t="s" s="0">
         <v>99</v>
       </c>
     </row>
@@ -2265,10 +2269,10 @@
       <c r="B30" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" t="s" s="0">
         <v>98</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D30" t="s" s="0">
         <v>99</v>
       </c>
     </row>
@@ -2279,10 +2283,10 @@
       <c r="B31" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" t="s" s="0">
         <v>98</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D31" t="s" s="0">
         <v>99</v>
       </c>
     </row>
@@ -2293,10 +2297,10 @@
       <c r="B32" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" t="s" s="0">
         <v>98</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D32" t="s" s="0">
         <v>99</v>
       </c>
     </row>
@@ -2307,10 +2311,10 @@
       <c r="B33" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33" t="s" s="0">
         <v>98</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D33" t="s" s="0">
         <v>99</v>
       </c>
     </row>
@@ -2321,10 +2325,10 @@
       <c r="B34" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" t="s" s="0">
         <v>98</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D34" t="s" s="0">
         <v>99</v>
       </c>
     </row>
@@ -2342,10 +2346,10 @@
       <c r="A36" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" t="s" s="0">
         <v>173</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C36" t="s" s="0">
         <v>172</v>
       </c>
       <c r="D36" s="2" t="s">
@@ -2356,10 +2360,10 @@
       <c r="A37" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" t="s" s="0">
         <v>181</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C37" t="s" s="0">
         <v>172</v>
       </c>
       <c r="D37" s="2" t="s">
@@ -2370,10 +2374,10 @@
       <c r="A38" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" t="s" s="0">
         <v>174</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C38" t="s" s="0">
         <v>172</v>
       </c>
       <c r="D38" s="2" t="s">
@@ -2384,10 +2388,10 @@
       <c r="A39" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39" t="s" s="0">
         <v>175</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C39" t="s" s="0">
         <v>172</v>
       </c>
       <c r="D39" s="2" t="s">
@@ -2398,10 +2402,10 @@
       <c r="A40" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" t="s" s="0">
         <v>176</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C40" t="s" s="0">
         <v>172</v>
       </c>
       <c r="D40" s="2" t="s">
@@ -2412,10 +2416,10 @@
       <c r="A41" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" t="s" s="0">
         <v>177</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C41" t="s" s="0">
         <v>172</v>
       </c>
       <c r="D41" s="2" t="s">
@@ -2426,10 +2430,10 @@
       <c r="A42" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42" t="s" s="0">
         <v>178</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C42" t="s" s="0">
         <v>172</v>
       </c>
       <c r="D42" s="2" t="s">
@@ -2440,10 +2444,10 @@
       <c r="A43" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" t="s" s="0">
         <v>179</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C43" t="s" s="0">
         <v>172</v>
       </c>
       <c r="D43" s="2" t="s">
@@ -2454,10 +2458,10 @@
       <c r="A44" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B44" t="s" s="0">
         <v>180</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C44" t="s" s="0">
         <v>172</v>
       </c>
       <c r="D44" s="2" t="s">
@@ -2468,10 +2472,10 @@
       <c r="A45" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B45" t="s" s="0">
         <v>182</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C45" t="s" s="0">
         <v>172</v>
       </c>
       <c r="D45" s="2" t="s">
@@ -2492,13 +2496,13 @@
       <c r="A47" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B47" t="s" s="0">
         <v>194</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C47" t="s" s="0">
         <v>204</v>
       </c>
-      <c r="D47" t="s">
+      <c r="D47" t="s" s="0">
         <v>205</v>
       </c>
     </row>
@@ -2506,13 +2510,13 @@
       <c r="A48" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B48" t="s" s="0">
         <v>195</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C48" t="s" s="0">
         <v>204</v>
       </c>
-      <c r="D48" t="s">
+      <c r="D48" t="s" s="0">
         <v>205</v>
       </c>
     </row>
@@ -2520,13 +2524,13 @@
       <c r="A49" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B49" t="s" s="0">
         <v>196</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C49" t="s" s="0">
         <v>204</v>
       </c>
-      <c r="D49" t="s">
+      <c r="D49" t="s" s="0">
         <v>205</v>
       </c>
     </row>
@@ -2534,13 +2538,13 @@
       <c r="A50" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B50" t="s" s="0">
         <v>197</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C50" t="s" s="0">
         <v>204</v>
       </c>
-      <c r="D50" t="s">
+      <c r="D50" t="s" s="0">
         <v>205</v>
       </c>
     </row>
@@ -2548,13 +2552,13 @@
       <c r="A51" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B51" t="s" s="0">
         <v>198</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C51" t="s" s="0">
         <v>204</v>
       </c>
-      <c r="D51" t="s">
+      <c r="D51" t="s" s="0">
         <v>205</v>
       </c>
     </row>
@@ -2562,13 +2566,13 @@
       <c r="A52" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B52" t="s" s="0">
         <v>199</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C52" t="s" s="0">
         <v>204</v>
       </c>
-      <c r="D52" t="s">
+      <c r="D52" t="s" s="0">
         <v>205</v>
       </c>
     </row>
@@ -2576,13 +2580,13 @@
       <c r="A53" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B53" t="s" s="0">
         <v>200</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C53" t="s" s="0">
         <v>204</v>
       </c>
-      <c r="D53" t="s">
+      <c r="D53" t="s" s="0">
         <v>205</v>
       </c>
     </row>
@@ -2590,13 +2594,13 @@
       <c r="A54" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B54" t="s" s="0">
         <v>201</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C54" t="s" s="0">
         <v>204</v>
       </c>
-      <c r="D54" t="s">
+      <c r="D54" t="s" s="0">
         <v>205</v>
       </c>
     </row>
@@ -2604,13 +2608,13 @@
       <c r="A55" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B55" t="s" s="0">
         <v>202</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C55" t="s" s="0">
         <v>204</v>
       </c>
-      <c r="D55" t="s">
+      <c r="D55" t="s" s="0">
         <v>205</v>
       </c>
     </row>
@@ -2618,13 +2622,13 @@
       <c r="A56" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B56" t="s" s="0">
         <v>203</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C56" t="s" s="0">
         <v>204</v>
       </c>
-      <c r="D56" t="s">
+      <c r="D56" t="s" s="0">
         <v>205</v>
       </c>
     </row>
@@ -2642,13 +2646,13 @@
       <c r="A58" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B58" t="s" s="0">
         <v>217</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C58" t="s" s="0">
         <v>227</v>
       </c>
-      <c r="D58" t="s">
+      <c r="D58" t="s" s="0">
         <v>206</v>
       </c>
     </row>
@@ -2656,13 +2660,13 @@
       <c r="A59" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B59" t="s" s="0">
         <v>218</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C59" t="s" s="0">
         <v>227</v>
       </c>
-      <c r="D59" t="s">
+      <c r="D59" t="s" s="0">
         <v>206</v>
       </c>
     </row>
@@ -2670,13 +2674,13 @@
       <c r="A60" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B60" t="s" s="0">
         <v>219</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C60" t="s" s="0">
         <v>227</v>
       </c>
-      <c r="D60" t="s">
+      <c r="D60" t="s" s="0">
         <v>206</v>
       </c>
     </row>
@@ -2684,13 +2688,13 @@
       <c r="A61" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B61" t="s" s="0">
         <v>220</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C61" t="s" s="0">
         <v>227</v>
       </c>
-      <c r="D61" t="s">
+      <c r="D61" t="s" s="0">
         <v>206</v>
       </c>
     </row>
@@ -2698,13 +2702,13 @@
       <c r="A62" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B62" t="s" s="0">
         <v>221</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C62" t="s" s="0">
         <v>227</v>
       </c>
-      <c r="D62" t="s">
+      <c r="D62" t="s" s="0">
         <v>206</v>
       </c>
     </row>
@@ -2712,13 +2716,13 @@
       <c r="A63" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B63" t="s" s="0">
         <v>222</v>
       </c>
-      <c r="C63" t="s">
+      <c r="C63" t="s" s="0">
         <v>227</v>
       </c>
-      <c r="D63" t="s">
+      <c r="D63" t="s" s="0">
         <v>206</v>
       </c>
     </row>
@@ -2726,13 +2730,13 @@
       <c r="A64" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B64" t="s" s="0">
         <v>223</v>
       </c>
-      <c r="C64" t="s">
+      <c r="C64" t="s" s="0">
         <v>227</v>
       </c>
-      <c r="D64" t="s">
+      <c r="D64" t="s" s="0">
         <v>206</v>
       </c>
     </row>
@@ -2740,13 +2744,13 @@
       <c r="A65" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B65" t="s" s="0">
         <v>224</v>
       </c>
-      <c r="C65" t="s">
+      <c r="C65" t="s" s="0">
         <v>227</v>
       </c>
-      <c r="D65" t="s">
+      <c r="D65" t="s" s="0">
         <v>206</v>
       </c>
     </row>
@@ -2754,13 +2758,13 @@
       <c r="A66" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B66" t="s" s="0">
         <v>225</v>
       </c>
-      <c r="C66" t="s">
+      <c r="C66" t="s" s="0">
         <v>227</v>
       </c>
-      <c r="D66" t="s">
+      <c r="D66" t="s" s="0">
         <v>206</v>
       </c>
     </row>
@@ -2768,13 +2772,13 @@
       <c r="A67" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B67" t="s" s="0">
         <v>226</v>
       </c>
-      <c r="C67" t="s">
+      <c r="C67" t="s" s="0">
         <v>227</v>
       </c>
-      <c r="D67" t="s">
+      <c r="D67" t="s" s="0">
         <v>206</v>
       </c>
     </row>
@@ -2795,10 +2799,10 @@
       <c r="B69" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="C69" t="s">
+      <c r="C69" t="s" s="0">
         <v>239</v>
       </c>
-      <c r="D69" t="s">
+      <c r="D69" t="s" s="0">
         <v>240</v>
       </c>
     </row>
@@ -2809,10 +2813,10 @@
       <c r="B70" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="C70" t="s">
+      <c r="C70" t="s" s="0">
         <v>239</v>
       </c>
-      <c r="D70" t="s">
+      <c r="D70" t="s" s="0">
         <v>240</v>
       </c>
     </row>
@@ -2823,10 +2827,10 @@
       <c r="B71" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="C71" t="s">
+      <c r="C71" t="s" s="0">
         <v>239</v>
       </c>
-      <c r="D71" t="s">
+      <c r="D71" t="s" s="0">
         <v>240</v>
       </c>
     </row>
@@ -2837,10 +2841,10 @@
       <c r="B72" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="C72" t="s">
+      <c r="C72" t="s" s="0">
         <v>239</v>
       </c>
-      <c r="D72" t="s">
+      <c r="D72" t="s" s="0">
         <v>240</v>
       </c>
     </row>
@@ -2851,10 +2855,10 @@
       <c r="B73" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="C73" t="s">
+      <c r="C73" t="s" s="0">
         <v>239</v>
       </c>
-      <c r="D73" t="s">
+      <c r="D73" t="s" s="0">
         <v>240</v>
       </c>
     </row>
@@ -2865,10 +2869,10 @@
       <c r="B74" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="C74" t="s">
+      <c r="C74" t="s" s="0">
         <v>239</v>
       </c>
-      <c r="D74" t="s">
+      <c r="D74" t="s" s="0">
         <v>240</v>
       </c>
     </row>
@@ -2879,10 +2883,10 @@
       <c r="B75" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="C75" t="s">
+      <c r="C75" t="s" s="0">
         <v>239</v>
       </c>
-      <c r="D75" t="s">
+      <c r="D75" t="s" s="0">
         <v>240</v>
       </c>
     </row>
@@ -2893,10 +2897,10 @@
       <c r="B76" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="C76" t="s">
+      <c r="C76" t="s" s="0">
         <v>239</v>
       </c>
-      <c r="D76" t="s">
+      <c r="D76" t="s" s="0">
         <v>240</v>
       </c>
     </row>
@@ -2907,10 +2911,10 @@
       <c r="B77" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="C77" t="s">
+      <c r="C77" t="s" s="0">
         <v>239</v>
       </c>
-      <c r="D77" t="s">
+      <c r="D77" t="s" s="0">
         <v>240</v>
       </c>
     </row>
@@ -2921,10 +2925,10 @@
       <c r="B78" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="C78" t="s">
+      <c r="C78" t="s" s="0">
         <v>239</v>
       </c>
-      <c r="D78" t="s">
+      <c r="D78" t="s" s="0">
         <v>240</v>
       </c>
     </row>
@@ -2942,13 +2946,13 @@
       <c r="A80" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="B80" t="s">
+      <c r="B80" t="s" s="0">
         <v>271</v>
       </c>
-      <c r="C80" t="s">
+      <c r="C80" t="s" s="0">
         <v>259</v>
       </c>
-      <c r="D80" t="s">
+      <c r="D80" t="s" s="0">
         <v>64</v>
       </c>
     </row>
@@ -2956,13 +2960,13 @@
       <c r="A81" s="2" t="s">
         <v>262</v>
       </c>
-      <c r="B81" t="s">
+      <c r="B81" t="s" s="0">
         <v>272</v>
       </c>
-      <c r="C81" t="s">
+      <c r="C81" t="s" s="0">
         <v>259</v>
       </c>
-      <c r="D81" t="s">
+      <c r="D81" t="s" s="0">
         <v>64</v>
       </c>
     </row>
@@ -2970,13 +2974,13 @@
       <c r="A82" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="B82" t="s">
+      <c r="B82" t="s" s="0">
         <v>273</v>
       </c>
-      <c r="C82" t="s">
+      <c r="C82" t="s" s="0">
         <v>259</v>
       </c>
-      <c r="D82" t="s">
+      <c r="D82" t="s" s="0">
         <v>64</v>
       </c>
     </row>
@@ -2984,13 +2988,13 @@
       <c r="A83" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="B83" t="s">
+      <c r="B83" t="s" s="0">
         <v>274</v>
       </c>
-      <c r="C83" t="s">
+      <c r="C83" t="s" s="0">
         <v>259</v>
       </c>
-      <c r="D83" t="s">
+      <c r="D83" t="s" s="0">
         <v>64</v>
       </c>
     </row>
@@ -2998,13 +3002,13 @@
       <c r="A84" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="B84" t="s">
+      <c r="B84" t="s" s="0">
         <v>275</v>
       </c>
-      <c r="C84" t="s">
+      <c r="C84" t="s" s="0">
         <v>259</v>
       </c>
-      <c r="D84" t="s">
+      <c r="D84" t="s" s="0">
         <v>64</v>
       </c>
     </row>
@@ -3012,13 +3016,13 @@
       <c r="A85" s="2" t="s">
         <v>266</v>
       </c>
-      <c r="B85" t="s">
+      <c r="B85" t="s" s="0">
         <v>276</v>
       </c>
-      <c r="C85" t="s">
+      <c r="C85" t="s" s="0">
         <v>259</v>
       </c>
-      <c r="D85" t="s">
+      <c r="D85" t="s" s="0">
         <v>64</v>
       </c>
     </row>
@@ -3026,13 +3030,13 @@
       <c r="A86" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="B86" t="s">
+      <c r="B86" t="s" s="0">
         <v>277</v>
       </c>
-      <c r="C86" t="s">
+      <c r="C86" t="s" s="0">
         <v>259</v>
       </c>
-      <c r="D86" t="s">
+      <c r="D86" t="s" s="0">
         <v>64</v>
       </c>
     </row>
@@ -3040,13 +3044,13 @@
       <c r="A87" s="2" t="s">
         <v>268</v>
       </c>
-      <c r="B87" t="s">
+      <c r="B87" t="s" s="0">
         <v>278</v>
       </c>
-      <c r="C87" t="s">
+      <c r="C87" t="s" s="0">
         <v>259</v>
       </c>
-      <c r="D87" t="s">
+      <c r="D87" t="s" s="0">
         <v>64</v>
       </c>
     </row>
@@ -3054,13 +3058,13 @@
       <c r="A88" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="B88" t="s">
+      <c r="B88" t="s" s="0">
         <v>279</v>
       </c>
-      <c r="C88" t="s">
+      <c r="C88" t="s" s="0">
         <v>259</v>
       </c>
-      <c r="D88" t="s">
+      <c r="D88" t="s" s="0">
         <v>64</v>
       </c>
     </row>
@@ -3068,13 +3072,13 @@
       <c r="A89" s="2" t="s">
         <v>270</v>
       </c>
-      <c r="B89" t="s">
+      <c r="B89" t="s" s="0">
         <v>280</v>
       </c>
-      <c r="C89" t="s">
+      <c r="C89" t="s" s="0">
         <v>259</v>
       </c>
-      <c r="D89" t="s">
+      <c r="D89" t="s" s="0">
         <v>64</v>
       </c>
     </row>
@@ -3095,10 +3099,10 @@
       <c r="B91" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="C91" t="s">
+      <c r="C91" t="s" s="0">
         <v>292</v>
       </c>
-      <c r="D91" t="s">
+      <c r="D91" t="s" s="0">
         <v>66</v>
       </c>
     </row>
@@ -3109,10 +3113,10 @@
       <c r="B92" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="C92" t="s">
+      <c r="C92" t="s" s="0">
         <v>292</v>
       </c>
-      <c r="D92" t="s">
+      <c r="D92" t="s" s="0">
         <v>66</v>
       </c>
     </row>
@@ -3123,10 +3127,10 @@
       <c r="B93" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="C93" t="s">
+      <c r="C93" t="s" s="0">
         <v>292</v>
       </c>
-      <c r="D93" t="s">
+      <c r="D93" t="s" s="0">
         <v>66</v>
       </c>
     </row>
@@ -3137,10 +3141,10 @@
       <c r="B94" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="C94" t="s">
+      <c r="C94" t="s" s="0">
         <v>292</v>
       </c>
-      <c r="D94" t="s">
+      <c r="D94" t="s" s="0">
         <v>66</v>
       </c>
     </row>
@@ -3151,10 +3155,10 @@
       <c r="B95" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="C95" t="s">
+      <c r="C95" t="s" s="0">
         <v>292</v>
       </c>
-      <c r="D95" t="s">
+      <c r="D95" t="s" s="0">
         <v>66</v>
       </c>
     </row>
@@ -3165,10 +3169,10 @@
       <c r="B96" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="C96" t="s">
+      <c r="C96" t="s" s="0">
         <v>292</v>
       </c>
-      <c r="D96" t="s">
+      <c r="D96" t="s" s="0">
         <v>66</v>
       </c>
     </row>
@@ -3179,10 +3183,10 @@
       <c r="B97" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="C97" t="s">
+      <c r="C97" t="s" s="0">
         <v>292</v>
       </c>
-      <c r="D97" t="s">
+      <c r="D97" t="s" s="0">
         <v>66</v>
       </c>
     </row>
@@ -3193,10 +3197,10 @@
       <c r="B98" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="C98" t="s">
+      <c r="C98" t="s" s="0">
         <v>292</v>
       </c>
-      <c r="D98" t="s">
+      <c r="D98" t="s" s="0">
         <v>66</v>
       </c>
     </row>
@@ -3207,10 +3211,10 @@
       <c r="B99" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="C99" t="s">
+      <c r="C99" t="s" s="0">
         <v>292</v>
       </c>
-      <c r="D99" t="s">
+      <c r="D99" t="s" s="0">
         <v>66</v>
       </c>
     </row>
@@ -3221,10 +3225,10 @@
       <c r="B100" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="C100" t="s">
+      <c r="C100" t="s" s="0">
         <v>292</v>
       </c>
-      <c r="D100" t="s">
+      <c r="D100" t="s" s="0">
         <v>66</v>
       </c>
     </row>
@@ -3245,10 +3249,10 @@
       <c r="B102" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="C102" t="s">
+      <c r="C102" t="s" s="0">
         <v>303</v>
       </c>
-      <c r="D102" t="s">
+      <c r="D102" t="s" s="0">
         <v>92</v>
       </c>
     </row>
@@ -3259,10 +3263,10 @@
       <c r="B103" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="C103" t="s">
+      <c r="C103" t="s" s="0">
         <v>303</v>
       </c>
-      <c r="D103" t="s">
+      <c r="D103" t="s" s="0">
         <v>92</v>
       </c>
     </row>
@@ -3273,10 +3277,10 @@
       <c r="B104" s="2" t="s">
         <v>305</v>
       </c>
-      <c r="C104" t="s">
+      <c r="C104" t="s" s="0">
         <v>303</v>
       </c>
-      <c r="D104" t="s">
+      <c r="D104" t="s" s="0">
         <v>92</v>
       </c>
     </row>
@@ -3287,10 +3291,10 @@
       <c r="B105" s="2" t="s">
         <v>306</v>
       </c>
-      <c r="C105" t="s">
+      <c r="C105" t="s" s="0">
         <v>303</v>
       </c>
-      <c r="D105" t="s">
+      <c r="D105" t="s" s="0">
         <v>92</v>
       </c>
     </row>
@@ -3301,10 +3305,10 @@
       <c r="B106" s="2" t="s">
         <v>307</v>
       </c>
-      <c r="C106" t="s">
+      <c r="C106" t="s" s="0">
         <v>303</v>
       </c>
-      <c r="D106" t="s">
+      <c r="D106" t="s" s="0">
         <v>92</v>
       </c>
     </row>
@@ -3315,10 +3319,10 @@
       <c r="B107" s="2" t="s">
         <v>308</v>
       </c>
-      <c r="C107" t="s">
+      <c r="C107" t="s" s="0">
         <v>303</v>
       </c>
-      <c r="D107" t="s">
+      <c r="D107" t="s" s="0">
         <v>92</v>
       </c>
     </row>
@@ -3329,10 +3333,10 @@
       <c r="B108" s="2" t="s">
         <v>309</v>
       </c>
-      <c r="C108" t="s">
+      <c r="C108" t="s" s="0">
         <v>303</v>
       </c>
-      <c r="D108" t="s">
+      <c r="D108" t="s" s="0">
         <v>92</v>
       </c>
     </row>
@@ -3343,10 +3347,10 @@
       <c r="B109" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="C109" t="s">
+      <c r="C109" t="s" s="0">
         <v>303</v>
       </c>
-      <c r="D109" t="s">
+      <c r="D109" t="s" s="0">
         <v>92</v>
       </c>
     </row>
@@ -3357,10 +3361,10 @@
       <c r="B110" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="C110" t="s">
+      <c r="C110" t="s" s="0">
         <v>303</v>
       </c>
-      <c r="D110" t="s">
+      <c r="D110" t="s" s="0">
         <v>92</v>
       </c>
     </row>
@@ -3371,10 +3375,10 @@
       <c r="B111" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="C111" t="s">
+      <c r="C111" t="s" s="0">
         <v>303</v>
       </c>
-      <c r="D111" t="s">
+      <c r="D111" t="s" s="0">
         <v>92</v>
       </c>
     </row>
@@ -3392,13 +3396,13 @@
       <c r="A113" s="2" t="s">
         <v>337</v>
       </c>
-      <c r="B113" t="s">
+      <c r="B113" t="s" s="0">
         <v>326</v>
       </c>
-      <c r="C113" t="s">
+      <c r="C113" t="s" s="0">
         <v>325</v>
       </c>
-      <c r="D113" t="s">
+      <c r="D113" t="s" s="0">
         <v>72</v>
       </c>
     </row>
@@ -3406,13 +3410,13 @@
       <c r="A114" s="2" t="s">
         <v>338</v>
       </c>
-      <c r="B114" t="s">
+      <c r="B114" t="s" s="0">
         <v>334</v>
       </c>
-      <c r="C114" t="s">
+      <c r="C114" t="s" s="0">
         <v>325</v>
       </c>
-      <c r="D114" t="s">
+      <c r="D114" t="s" s="0">
         <v>72</v>
       </c>
     </row>
@@ -3420,13 +3424,13 @@
       <c r="A115" s="2" t="s">
         <v>339</v>
       </c>
-      <c r="B115" t="s">
+      <c r="B115" t="s" s="0">
         <v>327</v>
       </c>
-      <c r="C115" t="s">
+      <c r="C115" t="s" s="0">
         <v>325</v>
       </c>
-      <c r="D115" t="s">
+      <c r="D115" t="s" s="0">
         <v>72</v>
       </c>
     </row>
@@ -3434,13 +3438,13 @@
       <c r="A116" s="2" t="s">
         <v>340</v>
       </c>
-      <c r="B116" t="s">
+      <c r="B116" t="s" s="0">
         <v>328</v>
       </c>
-      <c r="C116" t="s">
+      <c r="C116" t="s" s="0">
         <v>325</v>
       </c>
-      <c r="D116" t="s">
+      <c r="D116" t="s" s="0">
         <v>72</v>
       </c>
     </row>
@@ -3448,13 +3452,13 @@
       <c r="A117" s="2" t="s">
         <v>341</v>
       </c>
-      <c r="B117" t="s">
+      <c r="B117" t="s" s="0">
         <v>329</v>
       </c>
-      <c r="C117" t="s">
+      <c r="C117" t="s" s="0">
         <v>325</v>
       </c>
-      <c r="D117" t="s">
+      <c r="D117" t="s" s="0">
         <v>72</v>
       </c>
     </row>
@@ -3462,13 +3466,13 @@
       <c r="A118" s="2" t="s">
         <v>342</v>
       </c>
-      <c r="B118" t="s">
+      <c r="B118" t="s" s="0">
         <v>330</v>
       </c>
-      <c r="C118" t="s">
+      <c r="C118" t="s" s="0">
         <v>325</v>
       </c>
-      <c r="D118" t="s">
+      <c r="D118" t="s" s="0">
         <v>72</v>
       </c>
     </row>
@@ -3476,13 +3480,13 @@
       <c r="A119" s="2" t="s">
         <v>343</v>
       </c>
-      <c r="B119" t="s">
+      <c r="B119" t="s" s="0">
         <v>331</v>
       </c>
-      <c r="C119" t="s">
+      <c r="C119" t="s" s="0">
         <v>325</v>
       </c>
-      <c r="D119" t="s">
+      <c r="D119" t="s" s="0">
         <v>72</v>
       </c>
     </row>
@@ -3490,13 +3494,13 @@
       <c r="A120" s="2" t="s">
         <v>344</v>
       </c>
-      <c r="B120" t="s">
+      <c r="B120" t="s" s="0">
         <v>332</v>
       </c>
-      <c r="C120" t="s">
+      <c r="C120" t="s" s="0">
         <v>325</v>
       </c>
-      <c r="D120" t="s">
+      <c r="D120" t="s" s="0">
         <v>72</v>
       </c>
     </row>
@@ -3504,13 +3508,13 @@
       <c r="A121" s="2" t="s">
         <v>345</v>
       </c>
-      <c r="B121" t="s">
+      <c r="B121" t="s" s="0">
         <v>333</v>
       </c>
-      <c r="C121" t="s">
+      <c r="C121" t="s" s="0">
         <v>325</v>
       </c>
-      <c r="D121" t="s">
+      <c r="D121" t="s" s="0">
         <v>72</v>
       </c>
     </row>
@@ -3518,13 +3522,13 @@
       <c r="A122" s="2" t="s">
         <v>346</v>
       </c>
-      <c r="B122" t="s">
+      <c r="B122" t="s" s="0">
         <v>335</v>
       </c>
-      <c r="C122" t="s">
+      <c r="C122" t="s" s="0">
         <v>325</v>
       </c>
-      <c r="D122" t="s">
+      <c r="D122" t="s" s="0">
         <v>72</v>
       </c>
     </row>
@@ -3545,14 +3549,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="41.77734375" customWidth="1"/>
-    <col min="4" max="4" width="34.21875" customWidth="1"/>
-    <col min="5" max="5" width="22.5546875" customWidth="1"/>
-    <col min="6" max="6" width="11.21875" customWidth="1"/>
-    <col min="7" max="7" width="23" customWidth="1"/>
-    <col min="8" max="8" width="15.77734375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.77734375" customWidth="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.77734375"/>
+    <col min="3" max="3" customWidth="true" width="41.77734375"/>
+    <col min="4" max="4" customWidth="true" width="34.21875"/>
+    <col min="5" max="5" customWidth="true" width="22.5546875"/>
+    <col min="6" max="6" customWidth="true" width="11.21875"/>
+    <col min="7" max="7" customWidth="true" width="23.0"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="15.77734375"/>
+    <col min="9" max="9" customWidth="true" width="14.77734375"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -3591,10 +3595,10 @@
       <c r="B2" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>303</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="0">
         <v>92</v>
       </c>
       <c r="E2" s="13" t="s">
@@ -3609,7 +3613,7 @@
       <c r="H2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" t="s" s="0">
         <v>97</v>
       </c>
     </row>
@@ -3620,10 +3624,10 @@
       <c r="B3" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>303</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" t="s" s="0">
         <v>92</v>
       </c>
       <c r="E3" s="13" t="s">
@@ -3640,10 +3644,10 @@
       <c r="B4" s="2" t="s">
         <v>305</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" t="s" s="0">
         <v>303</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" t="s" s="0">
         <v>92</v>
       </c>
       <c r="E4" s="13" t="s">
@@ -3660,10 +3664,10 @@
       <c r="B5" s="2" t="s">
         <v>306</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" t="s" s="0">
         <v>303</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" t="s" s="0">
         <v>92</v>
       </c>
       <c r="E5" s="13" t="s">
@@ -3680,10 +3684,10 @@
       <c r="B6" s="2" t="s">
         <v>307</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" t="s" s="0">
         <v>303</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" t="s" s="0">
         <v>92</v>
       </c>
       <c r="E6" s="13" t="s">
@@ -3700,10 +3704,10 @@
       <c r="B7" s="2" t="s">
         <v>308</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" t="s" s="0">
         <v>303</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" t="s" s="0">
         <v>92</v>
       </c>
       <c r="E7" s="13" t="s">
@@ -3720,10 +3724,10 @@
       <c r="B8" s="2" t="s">
         <v>309</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" t="s" s="0">
         <v>303</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" t="s" s="0">
         <v>92</v>
       </c>
       <c r="E8" s="13" t="s">
@@ -3740,10 +3744,10 @@
       <c r="B9" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" t="s" s="0">
         <v>303</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" t="s" s="0">
         <v>92</v>
       </c>
       <c r="E9" s="13" t="s">
@@ -3760,10 +3764,10 @@
       <c r="B10" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" t="s" s="0">
         <v>303</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" t="s" s="0">
         <v>92</v>
       </c>
       <c r="E10" s="13" t="s">
@@ -3780,10 +3784,10 @@
       <c r="B11" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" t="s" s="0">
         <v>303</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" t="s" s="0">
         <v>92</v>
       </c>
       <c r="E11" s="13" t="s">
@@ -3810,16 +3814,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="6.44140625" customWidth="1"/>
-    <col min="2" max="2" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="40.21875" customWidth="1"/>
-    <col min="5" max="5" width="22.77734375" customWidth="1"/>
-    <col min="6" max="6" width="12.44140625" customWidth="1"/>
-    <col min="7" max="7" width="21.44140625" customWidth="1"/>
-    <col min="8" max="8" width="21.21875" customWidth="1"/>
-    <col min="9" max="9" width="18.21875" customWidth="1"/>
-    <col min="10" max="10" width="9.21875" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="6.44140625"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.77734375"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="34.5546875"/>
+    <col min="4" max="4" customWidth="true" width="40.21875"/>
+    <col min="5" max="5" customWidth="true" width="22.77734375"/>
+    <col min="6" max="6" customWidth="true" width="12.44140625"/>
+    <col min="7" max="7" customWidth="true" width="21.44140625"/>
+    <col min="8" max="8" customWidth="true" width="21.21875"/>
+    <col min="9" max="9" customWidth="true" width="18.21875"/>
+    <col min="10" max="10" customWidth="true" width="9.21875"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -3859,10 +3863,10 @@
       <c r="B2" s="2" t="s">
         <v>326</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>325</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="0">
         <v>72</v>
       </c>
       <c r="E2" s="3" t="s">
@@ -3871,7 +3875,7 @@
       <c r="F2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" t="s" s="0">
         <v>74</v>
       </c>
       <c r="H2" s="2" t="s">
@@ -3887,10 +3891,10 @@
       <c r="B3" s="2" t="s">
         <v>334</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>325</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" t="s" s="0">
         <v>72</v>
       </c>
       <c r="E3" s="3" t="s">
@@ -3899,7 +3903,7 @@
       <c r="F3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" t="s" s="0">
         <v>74</v>
       </c>
       <c r="H3" s="2"/>
@@ -3913,10 +3917,10 @@
       <c r="B4" s="2" t="s">
         <v>327</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" t="s" s="0">
         <v>325</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" t="s" s="0">
         <v>72</v>
       </c>
       <c r="E4" s="3" t="s">
@@ -3925,7 +3929,7 @@
       <c r="F4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" t="s" s="0">
         <v>74</v>
       </c>
       <c r="H4" s="2"/>
@@ -3939,10 +3943,10 @@
       <c r="B5" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" t="s" s="0">
         <v>325</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" t="s" s="0">
         <v>72</v>
       </c>
       <c r="E5" s="3" t="s">
@@ -3951,7 +3955,7 @@
       <c r="F5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" t="s" s="0">
         <v>74</v>
       </c>
       <c r="H5" s="2"/>
@@ -3965,10 +3969,10 @@
       <c r="B6" s="2" t="s">
         <v>329</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" t="s" s="0">
         <v>325</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" t="s" s="0">
         <v>72</v>
       </c>
       <c r="E6" s="3" t="s">
@@ -3977,7 +3981,7 @@
       <c r="F6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" t="s" s="0">
         <v>74</v>
       </c>
       <c r="H6" s="2"/>
@@ -3991,10 +3995,10 @@
       <c r="B7" s="2" t="s">
         <v>330</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" t="s" s="0">
         <v>325</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" t="s" s="0">
         <v>72</v>
       </c>
       <c r="E7" s="3" t="s">
@@ -4003,7 +4007,7 @@
       <c r="F7" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" t="s" s="0">
         <v>74</v>
       </c>
       <c r="H7" s="2"/>
@@ -4017,10 +4021,10 @@
       <c r="B8" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" t="s" s="0">
         <v>325</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" t="s" s="0">
         <v>72</v>
       </c>
       <c r="E8" s="3" t="s">
@@ -4029,7 +4033,7 @@
       <c r="F8" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8" t="s" s="0">
         <v>74</v>
       </c>
       <c r="H8" s="2"/>
@@ -4043,10 +4047,10 @@
       <c r="B9" s="2" t="s">
         <v>332</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" t="s" s="0">
         <v>325</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" t="s" s="0">
         <v>72</v>
       </c>
       <c r="E9" s="3" t="s">
@@ -4055,7 +4059,7 @@
       <c r="F9" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G9" t="s" s="0">
         <v>74</v>
       </c>
       <c r="H9" s="2"/>
@@ -4069,10 +4073,10 @@
       <c r="B10" s="2" t="s">
         <v>333</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" t="s" s="0">
         <v>325</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" t="s" s="0">
         <v>72</v>
       </c>
       <c r="E10" s="3" t="s">
@@ -4081,7 +4085,7 @@
       <c r="F10" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G10" t="s" s="0">
         <v>74</v>
       </c>
       <c r="H10" s="2"/>
@@ -4095,10 +4099,10 @@
       <c r="B11" s="2" t="s">
         <v>335</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" t="s" s="0">
         <v>325</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" t="s" s="0">
         <v>72</v>
       </c>
       <c r="E11" s="3" t="s">
@@ -4107,7 +4111,7 @@
       <c r="F11" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G11" t="s" s="0">
         <v>74</v>
       </c>
       <c r="H11" s="2"/>
@@ -4145,11 +4149,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26" customWidth="1"/>
-    <col min="4" max="4" width="24.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.77734375"/>
+    <col min="3" max="3" customWidth="true" width="26.0"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="24.44140625"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="10.77734375"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="11.21875"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -4176,16 +4180,16 @@
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>106</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>15</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="0">
         <v>16</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" t="s" s="0">
         <v>17</v>
       </c>
       <c r="F2" s="3" t="s">
@@ -4196,16 +4200,16 @@
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>107</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>15</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" t="s" s="0">
         <v>16</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" t="s" s="0">
         <v>19</v>
       </c>
       <c r="F3" s="3" t="s">
@@ -4216,16 +4220,16 @@
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>108</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" t="s" s="0">
         <v>15</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" t="s" s="0">
         <v>16</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" t="s" s="0">
         <v>20</v>
       </c>
       <c r="F4" s="3" t="s">
@@ -4236,16 +4240,16 @@
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" t="s" s="0">
         <v>109</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" t="s" s="0">
         <v>15</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" t="s" s="0">
         <v>16</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" t="s" s="0">
         <v>21</v>
       </c>
       <c r="F5" s="3" t="s">
@@ -4256,16 +4260,16 @@
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" t="s" s="0">
         <v>110</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" t="s" s="0">
         <v>15</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" t="s" s="0">
         <v>16</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" t="s" s="0">
         <v>22</v>
       </c>
       <c r="F6" s="3" t="s">
@@ -4276,16 +4280,16 @@
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" t="s" s="0">
         <v>111</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" t="s" s="0">
         <v>15</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" t="s" s="0">
         <v>16</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" t="s" s="0">
         <v>23</v>
       </c>
       <c r="F7" s="3" t="s">
@@ -4296,16 +4300,16 @@
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" t="s" s="0">
         <v>112</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" t="s" s="0">
         <v>15</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" t="s" s="0">
         <v>16</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" t="s" s="0">
         <v>24</v>
       </c>
       <c r="F8" s="3" t="s">
@@ -4316,16 +4320,16 @@
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" t="s" s="0">
         <v>113</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" t="s" s="0">
         <v>15</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" t="s" s="0">
         <v>16</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" t="s" s="0">
         <v>25</v>
       </c>
       <c r="F9" s="3" t="s">
@@ -4336,16 +4340,16 @@
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" t="s" s="0">
         <v>114</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" t="s" s="0">
         <v>15</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" t="s" s="0">
         <v>16</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" t="s" s="0">
         <v>26</v>
       </c>
       <c r="F10" s="3" t="s">
@@ -4356,16 +4360,16 @@
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" t="s" s="0">
         <v>115</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" t="s" s="0">
         <v>15</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" t="s" s="0">
         <v>16</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" t="s" s="0">
         <v>27</v>
       </c>
       <c r="F11" s="3" t="s">
@@ -4392,18 +4396,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.77734375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.77734375"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="30.0"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="38.0"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="10.21875"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="11.21875"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="9.77734375"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="9.44140625"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="25.44140625"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="13.0"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="10.77734375"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="16.77734375"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="11.21875"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
@@ -4460,44 +4464,44 @@
       <c r="B2" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="0">
         <v>38</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" t="s" s="0">
         <v>17</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" t="s" s="0">
         <v>39</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" t="s" s="0">
         <v>40</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" t="s" s="0">
         <v>58</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" t="s" s="0">
         <v>41</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" t="s" s="0">
         <v>42</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L2" t="s" s="0">
         <v>43</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="N2" t="s">
+      <c r="N2" t="s" s="0">
         <v>52</v>
       </c>
-      <c r="O2" t="s">
-        <v>438</v>
+      <c r="O2" t="s" s="0">
+        <v>442</v>
       </c>
     </row>
     <row r="3" spans="1:15">
@@ -4507,40 +4511,40 @@
       <c r="B3" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" t="s" s="0">
         <v>38</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" t="s" s="0">
         <v>17</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" t="s" s="0">
         <v>347</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" t="s" s="0">
         <v>348</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" t="s" s="0">
         <v>56</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" t="s" s="0">
         <v>46</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K3" t="s" s="0">
         <v>48</v>
       </c>
-      <c r="L3" t="s">
+      <c r="L3" t="s" s="0">
         <v>44</v>
       </c>
       <c r="M3" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="N3" t="s">
+      <c r="N3" t="s" s="0">
         <v>55</v>
       </c>
     </row>
@@ -4551,31 +4555,31 @@
       <c r="B4" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" t="s" s="0">
         <v>38</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" t="s" s="0">
         <v>17</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" t="s" s="0">
         <v>349</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" t="s" s="0">
         <v>350</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" t="s" s="0">
         <v>57</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" t="s" s="0">
         <v>47</v>
       </c>
-      <c r="K4" t="s">
+      <c r="K4" t="s" s="0">
         <v>49</v>
       </c>
       <c r="L4" s="2" t="s">
@@ -4584,7 +4588,7 @@
       <c r="M4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="N4" t="s">
+      <c r="N4" t="s" s="0">
         <v>54</v>
       </c>
     </row>
@@ -4595,31 +4599,31 @@
       <c r="B5" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" t="s" s="0">
         <v>38</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" t="s" s="0">
         <v>17</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" t="s" s="0">
         <v>351</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" t="s" s="0">
         <v>352</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I5" t="s" s="0">
         <v>59</v>
       </c>
-      <c r="J5" t="s">
+      <c r="J5" t="s" s="0">
         <v>41</v>
       </c>
-      <c r="K5" t="s">
+      <c r="K5" t="s" s="0">
         <v>48</v>
       </c>
       <c r="L5" s="2" t="s">
@@ -4628,7 +4632,7 @@
       <c r="M5" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="N5" t="s">
+      <c r="N5" t="s" s="0">
         <v>55</v>
       </c>
     </row>
@@ -4639,40 +4643,40 @@
       <c r="B6" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" t="s" s="0">
         <v>38</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" t="s" s="0">
         <v>17</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" t="s" s="0">
         <v>353</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" t="s" s="0">
         <v>354</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I6" t="s" s="0">
         <v>355</v>
       </c>
-      <c r="J6" t="s">
+      <c r="J6" t="s" s="0">
         <v>47</v>
       </c>
-      <c r="K6" t="s">
+      <c r="K6" t="s" s="0">
         <v>49</v>
       </c>
-      <c r="L6" t="s">
+      <c r="L6" t="s" s="0">
         <v>44</v>
       </c>
       <c r="M6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="N6" t="s">
+      <c r="N6" t="s" s="0">
         <v>53</v>
       </c>
     </row>
@@ -4683,40 +4687,40 @@
       <c r="B7" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" t="s" s="0">
         <v>38</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" t="s" s="0">
         <v>17</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" t="s" s="0">
         <v>356</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H7" t="s" s="0">
         <v>357</v>
       </c>
-      <c r="I7" t="s">
+      <c r="I7" t="s" s="0">
         <v>358</v>
       </c>
-      <c r="J7" t="s">
+      <c r="J7" t="s" s="0">
         <v>46</v>
       </c>
-      <c r="K7" t="s">
+      <c r="K7" t="s" s="0">
         <v>42</v>
       </c>
-      <c r="L7" t="s">
+      <c r="L7" t="s" s="0">
         <v>44</v>
       </c>
       <c r="M7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="N7" t="s">
+      <c r="N7" t="s" s="0">
         <v>52</v>
       </c>
     </row>
@@ -4727,40 +4731,40 @@
       <c r="B8" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" t="s" s="0">
         <v>38</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" t="s" s="0">
         <v>17</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8" t="s" s="0">
         <v>39</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H8" t="s" s="0">
         <v>359</v>
       </c>
-      <c r="I8" t="s">
+      <c r="I8" t="s" s="0">
         <v>360</v>
       </c>
-      <c r="J8" t="s">
+      <c r="J8" t="s" s="0">
         <v>41</v>
       </c>
-      <c r="K8" t="s">
+      <c r="K8" t="s" s="0">
         <v>48</v>
       </c>
-      <c r="L8" t="s">
+      <c r="L8" t="s" s="0">
         <v>43</v>
       </c>
       <c r="M8" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="N8" t="s">
+      <c r="N8" t="s" s="0">
         <v>54</v>
       </c>
     </row>
@@ -4771,40 +4775,40 @@
       <c r="B9" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" t="s" s="0">
         <v>38</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" t="s" s="0">
         <v>17</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G9" t="s" s="0">
         <v>361</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H9" t="s" s="0">
         <v>362</v>
       </c>
-      <c r="I9" t="s">
+      <c r="I9" t="s" s="0">
         <v>363</v>
       </c>
-      <c r="J9" t="s">
+      <c r="J9" t="s" s="0">
         <v>46</v>
       </c>
-      <c r="K9" t="s">
+      <c r="K9" t="s" s="0">
         <v>48</v>
       </c>
-      <c r="L9" t="s">
+      <c r="L9" t="s" s="0">
         <v>45</v>
       </c>
       <c r="M9" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="N9" t="s">
+      <c r="N9" t="s" s="0">
         <v>53</v>
       </c>
     </row>
@@ -4815,40 +4819,40 @@
       <c r="B10" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" t="s" s="0">
         <v>38</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" t="s" s="0">
         <v>17</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G10" t="s" s="0">
         <v>364</v>
       </c>
-      <c r="H10" t="s">
+      <c r="H10" t="s" s="0">
         <v>365</v>
       </c>
-      <c r="I10" t="s">
+      <c r="I10" t="s" s="0">
         <v>366</v>
       </c>
-      <c r="J10" t="s">
+      <c r="J10" t="s" s="0">
         <v>46</v>
       </c>
-      <c r="K10" t="s">
+      <c r="K10" t="s" s="0">
         <v>42</v>
       </c>
-      <c r="L10" t="s">
+      <c r="L10" t="s" s="0">
         <v>43</v>
       </c>
       <c r="M10" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="N10" t="s">
+      <c r="N10" t="s" s="0">
         <v>53</v>
       </c>
     </row>
@@ -4859,40 +4863,40 @@
       <c r="B11" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" t="s" s="0">
         <v>38</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" t="s" s="0">
         <v>17</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G11" t="s" s="0">
         <v>367</v>
       </c>
-      <c r="H11" t="s">
+      <c r="H11" t="s" s="0">
         <v>368</v>
       </c>
-      <c r="I11" t="s">
+      <c r="I11" t="s" s="0">
         <v>369</v>
       </c>
-      <c r="J11" t="s">
+      <c r="J11" t="s" s="0">
         <v>47</v>
       </c>
-      <c r="K11" t="s">
+      <c r="K11" t="s" s="0">
         <v>42</v>
       </c>
-      <c r="L11" t="s">
+      <c r="L11" t="s" s="0">
         <v>43</v>
       </c>
       <c r="M11" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="N11" t="s">
+      <c r="N11" t="s" s="0">
         <v>55</v>
       </c>
     </row>
@@ -4924,25 +4928,25 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="5.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21.21875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="26.109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7.88671875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9" customWidth="1"/>
-    <col min="17" max="17" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.5546875" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="5.44140625"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.77734375"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="28.5546875"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="35.44140625"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="9.77734375"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="10.88671875"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="13.33203125"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="25.0"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="10.5546875"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="10.88671875"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="11.88671875"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="21.21875"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="26.109375"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="7.88671875"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="9.0"/>
+    <col min="16" max="16" customWidth="true" width="9.0"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="11.88671875"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="13.5546875"/>
+    <col min="19" max="19" customWidth="true" width="10.5546875"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18">
@@ -5008,13 +5012,13 @@
       <c r="B2" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>380</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="0">
         <v>38</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" t="s" s="0">
         <v>17</v>
       </c>
       <c r="F2" s="3" t="s">
@@ -5023,10 +5027,10 @@
       <c r="G2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" t="s" s="0">
         <v>381</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" t="s" s="0">
         <v>382</v>
       </c>
       <c r="J2" s="2" t="s">
@@ -5035,19 +5039,19 @@
       <c r="K2" s="2" t="s">
         <v>384</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L2" t="s" s="0">
         <v>385</v>
       </c>
-      <c r="M2" t="s">
+      <c r="M2" t="s" s="0">
         <v>381</v>
       </c>
       <c r="N2" s="2" t="s">
         <v>431</v>
       </c>
-      <c r="O2" t="s">
+      <c r="O2" t="s" s="0">
         <v>242</v>
       </c>
-      <c r="P2" t="s">
+      <c r="P2" t="s" s="0">
         <v>441</v>
       </c>
     </row>
@@ -5058,13 +5062,13 @@
       <c r="B3" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>380</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" t="s" s="0">
         <v>38</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" t="s" s="0">
         <v>17</v>
       </c>
       <c r="F3" s="3" t="s">
@@ -5073,10 +5077,10 @@
       <c r="G3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" t="s" s="0">
         <v>386</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" t="s" s="0">
         <v>387</v>
       </c>
       <c r="J3" s="2" t="s">
@@ -5085,16 +5089,16 @@
       <c r="K3" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="L3" t="s">
+      <c r="L3" t="s" s="0">
         <v>390</v>
       </c>
-      <c r="M3" t="s">
+      <c r="M3" t="s" s="0">
         <v>381</v>
       </c>
       <c r="N3" s="2" t="s">
         <v>432</v>
       </c>
-      <c r="O3" t="s">
+      <c r="O3" t="s" s="0">
         <v>391</v>
       </c>
     </row>
@@ -5105,13 +5109,13 @@
       <c r="B4" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" t="s" s="0">
         <v>380</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" t="s" s="0">
         <v>38</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" t="s" s="0">
         <v>17</v>
       </c>
       <c r="F4" s="3" t="s">
@@ -5120,10 +5124,10 @@
       <c r="G4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" t="s" s="0">
         <v>392</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" t="s" s="0">
         <v>393</v>
       </c>
       <c r="J4" s="2" t="s">
@@ -5132,16 +5136,16 @@
       <c r="K4" s="2" t="s">
         <v>395</v>
       </c>
-      <c r="L4" t="s">
+      <c r="L4" t="s" s="0">
         <v>396</v>
       </c>
-      <c r="M4" t="s">
+      <c r="M4" t="s" s="0">
         <v>381</v>
       </c>
       <c r="N4" s="2" t="s">
         <v>433</v>
       </c>
-      <c r="O4" t="s">
+      <c r="O4" t="s" s="0">
         <v>391</v>
       </c>
     </row>
@@ -5152,13 +5156,13 @@
       <c r="B5" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" t="s" s="0">
         <v>380</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" t="s" s="0">
         <v>38</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" t="s" s="0">
         <v>17</v>
       </c>
       <c r="F5" s="3" t="s">
@@ -5167,10 +5171,10 @@
       <c r="G5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" t="s" s="0">
         <v>397</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I5" t="s" s="0">
         <v>398</v>
       </c>
       <c r="J5" s="2" t="s">
@@ -5179,16 +5183,16 @@
       <c r="K5" s="2" t="s">
         <v>400</v>
       </c>
-      <c r="L5" t="s">
+      <c r="L5" t="s" s="0">
         <v>401</v>
       </c>
-      <c r="M5" t="s">
+      <c r="M5" t="s" s="0">
         <v>381</v>
       </c>
       <c r="N5" s="2" t="s">
         <v>432</v>
       </c>
-      <c r="O5" t="s">
+      <c r="O5" t="s" s="0">
         <v>391</v>
       </c>
     </row>
@@ -5199,13 +5203,13 @@
       <c r="B6" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" t="s" s="0">
         <v>380</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" t="s" s="0">
         <v>38</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" t="s" s="0">
         <v>17</v>
       </c>
       <c r="F6" s="3" t="s">
@@ -5214,10 +5218,10 @@
       <c r="G6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" t="s" s="0">
         <v>402</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I6" t="s" s="0">
         <v>403</v>
       </c>
       <c r="J6" s="2" t="s">
@@ -5226,16 +5230,16 @@
       <c r="K6" s="2" t="s">
         <v>405</v>
       </c>
-      <c r="L6" t="s">
+      <c r="L6" t="s" s="0">
         <v>406</v>
       </c>
-      <c r="M6" t="s">
+      <c r="M6" t="s" s="0">
         <v>381</v>
       </c>
       <c r="N6" s="2" t="s">
         <v>434</v>
       </c>
-      <c r="O6" t="s">
+      <c r="O6" t="s" s="0">
         <v>391</v>
       </c>
     </row>
@@ -5246,13 +5250,13 @@
       <c r="B7" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" t="s" s="0">
         <v>380</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" t="s" s="0">
         <v>38</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" t="s" s="0">
         <v>17</v>
       </c>
       <c r="F7" s="3" t="s">
@@ -5261,10 +5265,10 @@
       <c r="G7" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H7" t="s" s="0">
         <v>407</v>
       </c>
-      <c r="I7" t="s">
+      <c r="I7" t="s" s="0">
         <v>408</v>
       </c>
       <c r="J7" s="2" t="s">
@@ -5273,16 +5277,16 @@
       <c r="K7" s="2" t="s">
         <v>410</v>
       </c>
-      <c r="L7" t="s">
+      <c r="L7" t="s" s="0">
         <v>411</v>
       </c>
-      <c r="M7" t="s">
+      <c r="M7" t="s" s="0">
         <v>381</v>
       </c>
       <c r="N7" s="2" t="s">
         <v>435</v>
       </c>
-      <c r="O7" t="s">
+      <c r="O7" t="s" s="0">
         <v>391</v>
       </c>
     </row>
@@ -5293,13 +5297,13 @@
       <c r="B8" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" t="s" s="0">
         <v>380</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" t="s" s="0">
         <v>38</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" t="s" s="0">
         <v>17</v>
       </c>
       <c r="F8" s="3" t="s">
@@ -5308,10 +5312,10 @@
       <c r="G8" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H8" t="s" s="0">
         <v>412</v>
       </c>
-      <c r="I8" t="s">
+      <c r="I8" t="s" s="0">
         <v>413</v>
       </c>
       <c r="J8" s="2" t="s">
@@ -5320,16 +5324,16 @@
       <c r="K8" s="2" t="s">
         <v>415</v>
       </c>
-      <c r="L8" t="s">
+      <c r="L8" t="s" s="0">
         <v>416</v>
       </c>
-      <c r="M8" t="s">
+      <c r="M8" t="s" s="0">
         <v>381</v>
       </c>
       <c r="N8" s="2" t="s">
         <v>434</v>
       </c>
-      <c r="O8" t="s">
+      <c r="O8" t="s" s="0">
         <v>242</v>
       </c>
     </row>
@@ -5340,13 +5344,13 @@
       <c r="B9" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" t="s" s="0">
         <v>380</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" t="s" s="0">
         <v>38</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" t="s" s="0">
         <v>17</v>
       </c>
       <c r="F9" s="3" t="s">
@@ -5355,10 +5359,10 @@
       <c r="G9" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H9" t="s" s="0">
         <v>417</v>
       </c>
-      <c r="I9" t="s">
+      <c r="I9" t="s" s="0">
         <v>418</v>
       </c>
       <c r="J9" s="2" t="s">
@@ -5367,16 +5371,16 @@
       <c r="K9" s="2" t="s">
         <v>420</v>
       </c>
-      <c r="L9" t="s">
+      <c r="L9" t="s" s="0">
         <v>421</v>
       </c>
-      <c r="M9" t="s">
+      <c r="M9" t="s" s="0">
         <v>381</v>
       </c>
       <c r="N9" s="2" t="s">
         <v>432</v>
       </c>
-      <c r="O9" t="s">
+      <c r="O9" t="s" s="0">
         <v>391</v>
       </c>
     </row>
@@ -5387,13 +5391,13 @@
       <c r="B10" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" t="s" s="0">
         <v>380</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" t="s" s="0">
         <v>38</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" t="s" s="0">
         <v>17</v>
       </c>
       <c r="F10" s="3" t="s">
@@ -5402,10 +5406,10 @@
       <c r="G10" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="H10" t="s">
+      <c r="H10" t="s" s="0">
         <v>422</v>
       </c>
-      <c r="I10" t="s">
+      <c r="I10" t="s" s="0">
         <v>423</v>
       </c>
       <c r="J10" s="2" t="s">
@@ -5414,16 +5418,16 @@
       <c r="K10" s="2" t="s">
         <v>425</v>
       </c>
-      <c r="L10" t="s">
+      <c r="L10" t="s" s="0">
         <v>385</v>
       </c>
-      <c r="M10" t="s">
+      <c r="M10" t="s" s="0">
         <v>381</v>
       </c>
       <c r="N10" s="2" t="s">
         <v>436</v>
       </c>
-      <c r="O10" t="s">
+      <c r="O10" t="s" s="0">
         <v>242</v>
       </c>
     </row>
@@ -5434,13 +5438,13 @@
       <c r="B11" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" t="s" s="0">
         <v>380</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" t="s" s="0">
         <v>38</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" t="s" s="0">
         <v>17</v>
       </c>
       <c r="F11" s="3" t="s">
@@ -5449,10 +5453,10 @@
       <c r="G11" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="H11" t="s">
+      <c r="H11" t="s" s="0">
         <v>426</v>
       </c>
-      <c r="I11" t="s">
+      <c r="I11" t="s" s="0">
         <v>427</v>
       </c>
       <c r="J11" s="2" t="s">
@@ -5461,16 +5465,16 @@
       <c r="K11" s="2" t="s">
         <v>429</v>
       </c>
-      <c r="L11" t="s">
+      <c r="L11" t="s" s="0">
         <v>430</v>
       </c>
-      <c r="M11" t="s">
+      <c r="M11" t="s" s="0">
         <v>381</v>
       </c>
       <c r="N11" s="2" t="s">
         <v>432</v>
       </c>
-      <c r="O11" t="s">
+      <c r="O11" t="s" s="0">
         <v>391</v>
       </c>
     </row>
@@ -5513,14 +5517,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.77734375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.77734375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.77734375"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="25.109375"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="22.44140625"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="10.21875"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="11.33203125"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="14.77734375"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="18.77734375"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="16.21875"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -5562,22 +5566,22 @@
       <c r="B2" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>98</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="0">
         <v>99</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" t="s" s="0">
         <v>17</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" t="s" s="0">
         <v>100</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" t="s" s="0">
         <v>101</v>
       </c>
       <c r="I2" s="3" t="s">
@@ -5594,13 +5598,13 @@
       <c r="B3" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>98</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" t="s" s="0">
         <v>99</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" t="s" s="0">
         <v>17</v>
       </c>
       <c r="F3" s="3" t="s">
@@ -5614,13 +5618,13 @@
       <c r="B4" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" t="s" s="0">
         <v>98</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" t="s" s="0">
         <v>99</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" t="s" s="0">
         <v>17</v>
       </c>
       <c r="F4" s="3" t="s">
@@ -5634,22 +5638,22 @@
       <c r="B5" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" t="s" s="0">
         <v>98</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" t="s" s="0">
         <v>99</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" t="s" s="0">
         <v>17</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" t="s" s="0">
         <v>160</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" t="s" s="0">
         <v>161</v>
       </c>
       <c r="I5" s="3" t="s">
@@ -5666,13 +5670,13 @@
       <c r="B6" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" t="s" s="0">
         <v>98</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" t="s" s="0">
         <v>99</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" t="s" s="0">
         <v>17</v>
       </c>
       <c r="F6" s="3" t="s">
@@ -5686,13 +5690,13 @@
       <c r="B7" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" t="s" s="0">
         <v>98</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" t="s" s="0">
         <v>99</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" t="s" s="0">
         <v>17</v>
       </c>
       <c r="F7" s="3" t="s">
@@ -5706,13 +5710,13 @@
       <c r="B8" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" t="s" s="0">
         <v>98</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" t="s" s="0">
         <v>99</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" t="s" s="0">
         <v>17</v>
       </c>
       <c r="F8" s="3" t="s">
@@ -5726,13 +5730,13 @@
       <c r="B9" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" t="s" s="0">
         <v>98</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" t="s" s="0">
         <v>99</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" t="s" s="0">
         <v>17</v>
       </c>
       <c r="F9" s="3" t="s">
@@ -5746,13 +5750,13 @@
       <c r="B10" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" t="s" s="0">
         <v>98</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" t="s" s="0">
         <v>99</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" t="s" s="0">
         <v>17</v>
       </c>
       <c r="F10" s="3" t="s">
@@ -5766,13 +5770,13 @@
       <c r="B11" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" t="s" s="0">
         <v>98</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" t="s" s="0">
         <v>99</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" t="s" s="0">
         <v>17</v>
       </c>
       <c r="F11" s="3" t="s">
@@ -5803,19 +5807,19 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="9.21875" style="8"/>
-    <col min="2" max="2" width="15.88671875" style="8" customWidth="1"/>
-    <col min="3" max="3" width="30.77734375" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="39.21875" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.44140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.77734375" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.21875" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.5546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.77734375" style="8" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17" style="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.77734375" style="8" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.77734375" style="8" customWidth="1"/>
-    <col min="13" max="16384" width="9.21875" style="8"/>
+    <col min="1" max="1" style="8" width="9.21875"/>
+    <col min="2" max="2" customWidth="true" style="8" width="15.88671875"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="8" width="30.77734375"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="8" width="39.21875"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="8" width="10.44140625"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="8" width="11.77734375"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="8" width="10.21875"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="8" width="12.5546875"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="8" width="10.77734375"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" style="8" width="17.0"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="8" width="20.77734375"/>
+    <col min="12" max="12" customWidth="true" style="8" width="15.77734375"/>
+    <col min="13" max="16384" style="8" width="9.21875"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="28.8">
@@ -6160,14 +6164,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.77734375"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="33.88671875"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="30.109375"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="22.21875"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="11.33203125"/>
+    <col min="7" max="8" bestFit="true" customWidth="true" width="9.88671875"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="14.109375"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="11.33203125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16">
@@ -6227,10 +6231,10 @@
       <c r="B2" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>239</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="0">
         <v>240</v>
       </c>
       <c r="E2" s="3" t="s">
@@ -6247,10 +6251,10 @@
       <c r="B3" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>239</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" t="s" s="0">
         <v>240</v>
       </c>
       <c r="E3" s="3" t="s">
@@ -6267,10 +6271,10 @@
       <c r="B4" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" t="s" s="0">
         <v>239</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" t="s" s="0">
         <v>240</v>
       </c>
       <c r="E4" s="3" t="s">
@@ -6287,10 +6291,10 @@
       <c r="B5" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" t="s" s="0">
         <v>239</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" t="s" s="0">
         <v>240</v>
       </c>
       <c r="E5" s="3" t="s">
@@ -6307,10 +6311,10 @@
       <c r="B6" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" t="s" s="0">
         <v>239</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" t="s" s="0">
         <v>240</v>
       </c>
       <c r="E6" s="3" t="s">
@@ -6327,10 +6331,10 @@
       <c r="B7" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" t="s" s="0">
         <v>239</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" t="s" s="0">
         <v>240</v>
       </c>
       <c r="E7" s="3" t="s">
@@ -6347,10 +6351,10 @@
       <c r="B8" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" t="s" s="0">
         <v>239</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" t="s" s="0">
         <v>240</v>
       </c>
       <c r="E8" s="3" t="s">
@@ -6367,10 +6371,10 @@
       <c r="B9" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" t="s" s="0">
         <v>239</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" t="s" s="0">
         <v>240</v>
       </c>
       <c r="E9" s="3" t="s">
@@ -6387,10 +6391,10 @@
       <c r="B10" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" t="s" s="0">
         <v>239</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" t="s" s="0">
         <v>240</v>
       </c>
       <c r="E10" s="3" t="s">
@@ -6407,10 +6411,10 @@
       <c r="B11" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" t="s" s="0">
         <v>239</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" t="s" s="0">
         <v>240</v>
       </c>
       <c r="E11" s="3" t="s">
@@ -6458,12 +6462,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34" customWidth="1"/>
-    <col min="5" max="5" width="23" customWidth="1"/>
-    <col min="6" max="6" width="11.21875" customWidth="1"/>
-    <col min="7" max="7" width="21.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.77734375"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="28.0"/>
+    <col min="4" max="4" customWidth="true" width="34.0"/>
+    <col min="5" max="5" customWidth="true" width="23.0"/>
+    <col min="6" max="6" customWidth="true" width="11.21875"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="21.21875"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -6496,10 +6500,10 @@
       <c r="B2" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>259</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="0">
         <v>64</v>
       </c>
       <c r="E2" s="3" t="s">
@@ -6508,7 +6512,7 @@
       <c r="F2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" t="s" s="0">
         <v>68</v>
       </c>
     </row>
@@ -6519,10 +6523,10 @@
       <c r="B3" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>259</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" t="s" s="0">
         <v>64</v>
       </c>
       <c r="E3" s="3" t="s">
@@ -6539,10 +6543,10 @@
       <c r="B4" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" t="s" s="0">
         <v>259</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" t="s" s="0">
         <v>64</v>
       </c>
       <c r="E4" s="3" t="s">
@@ -6559,10 +6563,10 @@
       <c r="B5" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" t="s" s="0">
         <v>259</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" t="s" s="0">
         <v>64</v>
       </c>
       <c r="E5" s="3" t="s">
@@ -6579,10 +6583,10 @@
       <c r="B6" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" t="s" s="0">
         <v>259</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" t="s" s="0">
         <v>64</v>
       </c>
       <c r="E6" s="3" t="s">
@@ -6599,10 +6603,10 @@
       <c r="B7" s="2" t="s">
         <v>276</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" t="s" s="0">
         <v>259</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" t="s" s="0">
         <v>64</v>
       </c>
       <c r="E7" s="3" t="s">
@@ -6619,10 +6623,10 @@
       <c r="B8" s="2" t="s">
         <v>277</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" t="s" s="0">
         <v>259</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" t="s" s="0">
         <v>64</v>
       </c>
       <c r="E8" s="3" t="s">
@@ -6639,10 +6643,10 @@
       <c r="B9" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" t="s" s="0">
         <v>259</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" t="s" s="0">
         <v>64</v>
       </c>
       <c r="E9" s="3" t="s">
@@ -6659,10 +6663,10 @@
       <c r="B10" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" t="s" s="0">
         <v>259</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" t="s" s="0">
         <v>64</v>
       </c>
       <c r="E10" s="3" t="s">
@@ -6679,10 +6683,10 @@
       <c r="B11" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" t="s" s="0">
         <v>259</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" t="s" s="0">
         <v>64</v>
       </c>
       <c r="E11" s="3" t="s">
@@ -6723,13 +6727,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="41.21875" customWidth="1"/>
-    <col min="4" max="4" width="40" customWidth="1"/>
-    <col min="5" max="5" width="24.44140625" customWidth="1"/>
-    <col min="6" max="6" width="19.5546875" customWidth="1"/>
-    <col min="7" max="7" width="22.77734375" customWidth="1"/>
-    <col min="8" max="8" width="20.21875" customWidth="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.77734375"/>
+    <col min="3" max="3" customWidth="true" width="41.21875"/>
+    <col min="4" max="4" customWidth="true" width="40.0"/>
+    <col min="5" max="5" customWidth="true" width="24.44140625"/>
+    <col min="6" max="6" customWidth="true" width="19.5546875"/>
+    <col min="7" max="7" customWidth="true" width="22.77734375"/>
+    <col min="8" max="8" customWidth="true" width="20.21875"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -6765,10 +6769,10 @@
       <c r="B2" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>292</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="0">
         <v>66</v>
       </c>
       <c r="E2" s="3" t="s">
@@ -6777,10 +6781,10 @@
       <c r="F2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" t="s" s="0">
         <v>69</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" t="s" s="0">
         <v>71</v>
       </c>
     </row>
@@ -6791,10 +6795,10 @@
       <c r="B3" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>292</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" t="s" s="0">
         <v>66</v>
       </c>
       <c r="E3" s="3" t="s">
@@ -6811,10 +6815,10 @@
       <c r="B4" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" t="s" s="0">
         <v>292</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" t="s" s="0">
         <v>66</v>
       </c>
       <c r="E4" s="3" t="s">
@@ -6831,10 +6835,10 @@
       <c r="B5" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" t="s" s="0">
         <v>292</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" t="s" s="0">
         <v>66</v>
       </c>
       <c r="E5" s="3" t="s">
@@ -6851,10 +6855,10 @@
       <c r="B6" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" t="s" s="0">
         <v>292</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" t="s" s="0">
         <v>66</v>
       </c>
       <c r="E6" s="3" t="s">
@@ -6871,10 +6875,10 @@
       <c r="B7" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" t="s" s="0">
         <v>292</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" t="s" s="0">
         <v>66</v>
       </c>
       <c r="E7" s="3" t="s">
@@ -6891,10 +6895,10 @@
       <c r="B8" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" t="s" s="0">
         <v>292</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" t="s" s="0">
         <v>66</v>
       </c>
       <c r="E8" s="3" t="s">
@@ -6911,10 +6915,10 @@
       <c r="B9" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" t="s" s="0">
         <v>292</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" t="s" s="0">
         <v>66</v>
       </c>
       <c r="E9" s="3" t="s">
@@ -6931,10 +6935,10 @@
       <c r="B10" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" t="s" s="0">
         <v>292</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" t="s" s="0">
         <v>66</v>
       </c>
       <c r="E10" s="3" t="s">
@@ -6951,10 +6955,10 @@
       <c r="B11" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" t="s" s="0">
         <v>292</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" t="s" s="0">
         <v>66</v>
       </c>
       <c r="E11" s="3" t="s">

</xml_diff>

<commit_message>
added projectpath to DemoWebshop_CreateAddress
</commit_message>
<xml_diff>
--- a/src/main/resources/AutomationCatalogue_Batch41_TestData.xlsx
+++ b/src/main/resources/AutomationCatalogue_Batch41_TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AutomationCatalogue\Projects\TestAutomationCatalogue_Batch41\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\INSPIRON\IdeaProjects\TestAutomationCatalogue_Batch41\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75901A2E-F834-48E0-BC1D-75A4638AA28F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FECACCF-4334-4515-9264-0A5DB7F789AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="788" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="788" firstSheet="5" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OrangeHRM_Login" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="201">
   <si>
     <t>S. No</t>
   </si>
@@ -305,6 +305,336 @@
   </si>
   <si>
     <t>23-January-1990</t>
+  </si>
+  <si>
+    <t>TC12_DemoWebShop_CreateAddress</t>
+  </si>
+  <si>
+    <t>DemoWebShop Application CreateAddress</t>
+  </si>
+  <si>
+    <t>Admin@124</t>
+  </si>
+  <si>
+    <t>Admin@125</t>
+  </si>
+  <si>
+    <t>Admin@126</t>
+  </si>
+  <si>
+    <t>Admin@127</t>
+  </si>
+  <si>
+    <t>Admin@128</t>
+  </si>
+  <si>
+    <t>Admin@129</t>
+  </si>
+  <si>
+    <t>Admin@130</t>
+  </si>
+  <si>
+    <t>Admin@131</t>
+  </si>
+  <si>
+    <t>Admin@132</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Company</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>Address1</t>
+  </si>
+  <si>
+    <t>Address2</t>
+  </si>
+  <si>
+    <t>ZipPostalCode</t>
+  </si>
+  <si>
+    <t>PhoneNumber</t>
+  </si>
+  <si>
+    <t>FaxNumber</t>
+  </si>
+  <si>
+    <t>Rama</t>
+  </si>
+  <si>
+    <t>Krishna</t>
+  </si>
+  <si>
+    <t>Amazon</t>
+  </si>
+  <si>
+    <t>Hyderabad</t>
+  </si>
+  <si>
+    <t>101</t>
+  </si>
+  <si>
+    <t>102</t>
+  </si>
+  <si>
+    <t>103</t>
+  </si>
+  <si>
+    <t>104</t>
+  </si>
+  <si>
+    <t>105</t>
+  </si>
+  <si>
+    <t>106</t>
+  </si>
+  <si>
+    <t>107</t>
+  </si>
+  <si>
+    <t>108</t>
+  </si>
+  <si>
+    <t>109</t>
+  </si>
+  <si>
+    <t>110</t>
+  </si>
+  <si>
+    <t>220</t>
+  </si>
+  <si>
+    <t>221</t>
+  </si>
+  <si>
+    <t>222</t>
+  </si>
+  <si>
+    <t>223</t>
+  </si>
+  <si>
+    <t>224</t>
+  </si>
+  <si>
+    <t>225</t>
+  </si>
+  <si>
+    <t>226</t>
+  </si>
+  <si>
+    <t>227</t>
+  </si>
+  <si>
+    <t>228</t>
+  </si>
+  <si>
+    <t>229</t>
+  </si>
+  <si>
+    <t>500023</t>
+  </si>
+  <si>
+    <t>500024</t>
+  </si>
+  <si>
+    <t>500025</t>
+  </si>
+  <si>
+    <t>500026</t>
+  </si>
+  <si>
+    <t>500027</t>
+  </si>
+  <si>
+    <t>500028</t>
+  </si>
+  <si>
+    <t>500029</t>
+  </si>
+  <si>
+    <t>500030</t>
+  </si>
+  <si>
+    <t>500031</t>
+  </si>
+  <si>
+    <t>500032</t>
+  </si>
+  <si>
+    <t>809546781</t>
+  </si>
+  <si>
+    <t>809546783</t>
+  </si>
+  <si>
+    <t>809546784</t>
+  </si>
+  <si>
+    <t>809546785</t>
+  </si>
+  <si>
+    <t>809546786</t>
+  </si>
+  <si>
+    <t>809546787</t>
+  </si>
+  <si>
+    <t>809546788</t>
+  </si>
+  <si>
+    <t>809546789</t>
+  </si>
+  <si>
+    <t>809546782</t>
+  </si>
+  <si>
+    <t>809546790</t>
+  </si>
+  <si>
+    <t>22341</t>
+  </si>
+  <si>
+    <t>22342</t>
+  </si>
+  <si>
+    <t>22343</t>
+  </si>
+  <si>
+    <t>22344</t>
+  </si>
+  <si>
+    <t>22345</t>
+  </si>
+  <si>
+    <t>22346</t>
+  </si>
+  <si>
+    <t>22347</t>
+  </si>
+  <si>
+    <t>22348</t>
+  </si>
+  <si>
+    <t>22349</t>
+  </si>
+  <si>
+    <t>22350</t>
+  </si>
+  <si>
+    <t>Bengaluru</t>
+  </si>
+  <si>
+    <t>Chennai</t>
+  </si>
+  <si>
+    <t>Madras</t>
+  </si>
+  <si>
+    <t>Mumbai</t>
+  </si>
+  <si>
+    <t>Goa</t>
+  </si>
+  <si>
+    <t>Manipur</t>
+  </si>
+  <si>
+    <t>Tamilnadu</t>
+  </si>
+  <si>
+    <t>Kerala</t>
+  </si>
+  <si>
+    <t>Karnataka</t>
+  </si>
+  <si>
+    <t>Wipro</t>
+  </si>
+  <si>
+    <t>Zamzam</t>
+  </si>
+  <si>
+    <t>Joli</t>
+  </si>
+  <si>
+    <t>Zenus</t>
+  </si>
+  <si>
+    <t>Xrey</t>
+  </si>
+  <si>
+    <t>Y axis</t>
+  </si>
+  <si>
+    <t>Q connect</t>
+  </si>
+  <si>
+    <t>Appy</t>
+  </si>
+  <si>
+    <t>Berry</t>
+  </si>
+  <si>
+    <t>ram1@gmail.com</t>
+  </si>
+  <si>
+    <t>Ryas</t>
+  </si>
+  <si>
+    <t>Kery</t>
+  </si>
+  <si>
+    <t>blan</t>
+  </si>
+  <si>
+    <t>Zam</t>
+  </si>
+  <si>
+    <t>Kobra</t>
+  </si>
+  <si>
+    <t>Jerry</t>
+  </si>
+  <si>
+    <t>Roan</t>
+  </si>
+  <si>
+    <t>Tommy</t>
+  </si>
+  <si>
+    <t>Blessy</t>
+  </si>
+  <si>
+    <t>Blue</t>
+  </si>
+  <si>
+    <t>Kate</t>
+  </si>
+  <si>
+    <t>Braxy</t>
+  </si>
+  <si>
+    <t>Cody</t>
+  </si>
+  <si>
+    <t>Kin</t>
+  </si>
+  <si>
+    <t>Joe</t>
+  </si>
+  <si>
+    <t>Ret</t>
+  </si>
+  <si>
+    <t>Tin</t>
+  </si>
+  <si>
+    <t>Bru</t>
   </si>
 </sst>
 </file>
@@ -411,7 +741,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -439,6 +769,10 @@
     <xf numFmtId="15" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -760,15 +1094,15 @@
       <selection activeCell="Q14" sqref="Q14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="26" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -785,7 +1119,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -802,7 +1136,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -819,7 +1153,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -836,7 +1170,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -853,7 +1187,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -870,7 +1204,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
@@ -887,7 +1221,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
@@ -904,7 +1238,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
@@ -921,7 +1255,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
@@ -938,7 +1272,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
@@ -972,22 +1306,22 @@
       <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="30" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="38" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1031,7 +1365,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -1072,7 +1406,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -1107,7 +1441,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -1142,7 +1476,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -1174,7 +1508,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -1194,7 +1528,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
@@ -1220,7 +1554,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
@@ -1240,7 +1574,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
@@ -1257,7 +1591,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
@@ -1274,7 +1608,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
@@ -1317,18 +1651,18 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1357,52 +1691,52 @@
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
@@ -1418,20 +1752,20 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="41.109375" customWidth="1"/>
+    <col min="2" max="2" width="41.140625" customWidth="1"/>
     <col min="3" max="3" width="40" customWidth="1"/>
-    <col min="4" max="4" width="24.44140625" customWidth="1"/>
-    <col min="5" max="5" width="19.5546875" customWidth="1"/>
-    <col min="6" max="6" width="22.88671875" customWidth="1"/>
-    <col min="7" max="7" width="20.33203125" customWidth="1"/>
+    <col min="4" max="4" width="24.42578125" customWidth="1"/>
+    <col min="5" max="5" width="19.5703125" customWidth="1"/>
+    <col min="6" max="6" width="22.85546875" customWidth="1"/>
+    <col min="7" max="7" width="20.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1454,7 +1788,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -1477,7 +1811,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -1494,7 +1828,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -1511,7 +1845,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -1528,7 +1862,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -1545,7 +1879,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
@@ -1562,7 +1896,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
@@ -1579,7 +1913,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
@@ -1596,7 +1930,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
@@ -1613,7 +1947,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
@@ -1658,16 +1992,16 @@
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="28" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="34" customWidth="1"/>
     <col min="4" max="4" width="23" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" customWidth="1"/>
-    <col min="6" max="6" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" customWidth="1"/>
+    <col min="6" max="6" width="21.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1687,7 +2021,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -1707,7 +2041,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -1724,7 +2058,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -1741,7 +2075,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -1758,7 +2092,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -1775,7 +2109,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
@@ -1792,7 +2126,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
@@ -1809,7 +2143,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
@@ -1826,7 +2160,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
@@ -1843,7 +2177,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
@@ -1889,20 +2223,20 @@
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.44140625" customWidth="1"/>
-    <col min="2" max="2" width="34.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="40.109375" customWidth="1"/>
-    <col min="4" max="4" width="22.6640625" customWidth="1"/>
-    <col min="5" max="5" width="12.44140625" customWidth="1"/>
-    <col min="6" max="6" width="21.44140625" customWidth="1"/>
-    <col min="7" max="7" width="21.109375" customWidth="1"/>
-    <col min="8" max="8" width="18.33203125" customWidth="1"/>
-    <col min="9" max="9" width="9.33203125" customWidth="1"/>
+    <col min="1" max="1" width="6.42578125" customWidth="1"/>
+    <col min="2" max="2" width="34.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.140625" customWidth="1"/>
+    <col min="4" max="4" width="22.7109375" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" customWidth="1"/>
+    <col min="6" max="6" width="21.42578125" customWidth="1"/>
+    <col min="7" max="7" width="21.140625" customWidth="1"/>
+    <col min="8" max="8" width="18.28515625" customWidth="1"/>
+    <col min="9" max="9" width="9.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1929,7 +2263,7 @@
       <c r="J1" s="5"/>
       <c r="K1" s="1"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -1954,7 +2288,7 @@
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -1977,7 +2311,7 @@
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -2000,7 +2334,7 @@
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -2023,7 +2357,7 @@
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -2046,7 +2380,7 @@
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
@@ -2069,7 +2403,7 @@
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
@@ -2092,7 +2426,7 @@
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
@@ -2115,7 +2449,7 @@
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
@@ -2138,7 +2472,7 @@
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
@@ -2185,27 +2519,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="8"/>
-    <col min="2" max="2" width="30.88671875" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39.109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.44140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.5546875" style="8" customWidth="1"/>
-    <col min="8" max="8" width="10.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="8"/>
+    <col min="2" max="2" width="30.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.5703125" style="8" customWidth="1"/>
+    <col min="8" max="8" width="10.85546875" style="8" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17" style="8" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.6640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.6640625" style="8" customWidth="1"/>
-    <col min="12" max="16384" width="9.109375" style="8"/>
+    <col min="10" max="10" width="20.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.7109375" style="8" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -2240,7 +2574,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>5</v>
       </c>
@@ -2253,7 +2587,7 @@
       <c r="D2" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="13" t="s">
         <v>18</v>
       </c>
       <c r="F2" s="10" t="s">
@@ -2275,7 +2609,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>6</v>
       </c>
@@ -2298,7 +2632,7 @@
       <c r="J3" s="10"/>
       <c r="K3" s="10"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>7</v>
       </c>
@@ -2321,7 +2655,7 @@
       <c r="J4" s="10"/>
       <c r="K4" s="10"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>8</v>
       </c>
@@ -2344,7 +2678,7 @@
       <c r="J5" s="10"/>
       <c r="K5" s="10"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>9</v>
       </c>
@@ -2367,7 +2701,7 @@
       <c r="J6" s="10"/>
       <c r="K6" s="10"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>10</v>
       </c>
@@ -2390,7 +2724,7 @@
       <c r="J7" s="10"/>
       <c r="K7" s="10"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>11</v>
       </c>
@@ -2413,7 +2747,7 @@
       <c r="J8" s="10"/>
       <c r="K8" s="10"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>12</v>
       </c>
@@ -2436,7 +2770,7 @@
       <c r="J9" s="10"/>
       <c r="K9" s="10"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>13</v>
       </c>
@@ -2459,7 +2793,7 @@
       <c r="J10" s="10"/>
       <c r="K10" s="10"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>14</v>
       </c>
@@ -2501,21 +2835,31 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:O11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.42578125" customWidth="1"/>
+    <col min="3" max="3" width="38.5703125" customWidth="1"/>
+    <col min="4" max="4" width="22.28515625" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" customWidth="1"/>
+    <col min="7" max="7" width="9.85546875" customWidth="1"/>
+    <col min="8" max="8" width="19.28515625" customWidth="1"/>
+    <col min="9" max="9" width="12" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" customWidth="1"/>
+    <col min="11" max="11" width="14.140625" customWidth="1"/>
+    <col min="12" max="12" width="13.28515625" customWidth="1"/>
+    <col min="13" max="13" width="13.85546875" customWidth="1"/>
+    <col min="14" max="14" width="15.7109375" customWidth="1"/>
+    <col min="15" max="15" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2531,8 +2875,517 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" t="s">
+        <v>110</v>
+      </c>
+      <c r="G2" t="s">
+        <v>111</v>
+      </c>
+      <c r="H2" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="I2" t="s">
+        <v>112</v>
+      </c>
+      <c r="J2" t="s">
+        <v>113</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="F3" t="s">
+        <v>192</v>
+      </c>
+      <c r="G3" t="s">
+        <v>183</v>
+      </c>
+      <c r="H3" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="I3" t="s">
+        <v>173</v>
+      </c>
+      <c r="J3" t="s">
+        <v>164</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="F4" t="s">
+        <v>193</v>
+      </c>
+      <c r="G4" t="s">
+        <v>184</v>
+      </c>
+      <c r="H4" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="I4" t="s">
+        <v>174</v>
+      </c>
+      <c r="J4" t="s">
+        <v>165</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="F5" t="s">
+        <v>194</v>
+      </c>
+      <c r="G5" t="s">
+        <v>185</v>
+      </c>
+      <c r="H5" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="I5" t="s">
+        <v>175</v>
+      </c>
+      <c r="J5" t="s">
+        <v>166</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>91</v>
+      </c>
+      <c r="C6" t="s">
+        <v>92</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="F6" t="s">
+        <v>195</v>
+      </c>
+      <c r="G6" t="s">
+        <v>186</v>
+      </c>
+      <c r="H6" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="I6" t="s">
+        <v>176</v>
+      </c>
+      <c r="J6" t="s">
+        <v>167</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="O6" s="2" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>91</v>
+      </c>
+      <c r="C7" t="s">
+        <v>92</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="F7" t="s">
+        <v>196</v>
+      </c>
+      <c r="G7" t="s">
+        <v>187</v>
+      </c>
+      <c r="H7" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="I7" t="s">
+        <v>177</v>
+      </c>
+      <c r="J7" t="s">
+        <v>168</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="O7" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" t="s">
+        <v>91</v>
+      </c>
+      <c r="C8" t="s">
+        <v>92</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="F8" t="s">
+        <v>197</v>
+      </c>
+      <c r="G8" t="s">
+        <v>188</v>
+      </c>
+      <c r="H8" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="I8" t="s">
+        <v>178</v>
+      </c>
+      <c r="J8" t="s">
+        <v>169</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="N8" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="O8" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
+        <v>91</v>
+      </c>
+      <c r="C9" t="s">
+        <v>92</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F9" t="s">
+        <v>198</v>
+      </c>
+      <c r="G9" t="s">
+        <v>189</v>
+      </c>
+      <c r="H9" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="I9" t="s">
+        <v>179</v>
+      </c>
+      <c r="J9" t="s">
+        <v>170</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="N9" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="O9" s="2" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" t="s">
+        <v>91</v>
+      </c>
+      <c r="C10" t="s">
+        <v>92</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="F10" t="s">
+        <v>199</v>
+      </c>
+      <c r="G10" t="s">
+        <v>190</v>
+      </c>
+      <c r="H10" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="I10" t="s">
+        <v>180</v>
+      </c>
+      <c r="J10" t="s">
+        <v>171</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="O10" s="2" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" t="s">
+        <v>91</v>
+      </c>
+      <c r="C11" t="s">
+        <v>92</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="F11" t="s">
+        <v>200</v>
+      </c>
+      <c r="G11" t="s">
+        <v>191</v>
+      </c>
+      <c r="H11" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="I11" t="s">
+        <v>181</v>
+      </c>
+      <c r="J11" t="s">
+        <v>172</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="M11" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="N11" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="O11" s="2" t="s">
+        <v>163</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{206FD441-86C1-4524-B3E6-7880821583B1}"/>
+    <hyperlink ref="D3:D11" r:id="rId2" display="aarosagarch@gmail.com" xr:uid="{ED84493B-3D11-4DEB-B1DC-5F1201089DCE}"/>
+    <hyperlink ref="E2" r:id="rId3" xr:uid="{2E524FD9-2DA6-40F2-8531-B69F1118AFF7}"/>
+    <hyperlink ref="E3:E11" r:id="rId4" display="Admin@123" xr:uid="{FC233FAB-13DA-4A4A-93B7-BD860EA79EFF}"/>
+    <hyperlink ref="H2" r:id="rId5" display="ram@gmail.com" xr:uid="{1A4A161D-BFC0-4F4F-B779-7581010A2050}"/>
+    <hyperlink ref="H3:H11" r:id="rId6" display="ram@gmail.com" xr:uid="{6FC41756-B974-4C88-9980-FE44CAF5F426}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
TestNG XML changes implemented
</commit_message>
<xml_diff>
--- a/src/main/resources/AutomationCatalogue_Batch41_TestData.xlsx
+++ b/src/main/resources/AutomationCatalogue_Batch41_TestData.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Automation Catalogue\Projects\TestAutomationCatalogue_Batch41\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AutomationCatalogue\Projects\TestAutomationCatalogue_Batch41\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68887C4F-1860-4271-A739-70455A684833}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="944" firstSheet="5" activeTab="9"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="944" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="10" r:id="rId1"/>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1277" uniqueCount="386">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1292" uniqueCount="388">
   <si>
     <t>S. No</t>
   </si>
@@ -1192,13 +1193,19 @@
   </si>
   <si>
     <t>Third Goal Status</t>
+  </si>
+  <si>
+    <t>RunMode</t>
+  </si>
+  <si>
+    <t>Yes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1661,23 +1668,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F122"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G122"/>
   <sheetViews>
-    <sheetView topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="E59" sqref="E59"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="39" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="38" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>89</v>
       </c>
@@ -1691,13 +1699,16 @@
         <v>102</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="14" t="s">
         <v>115</v>
       </c>
@@ -1706,8 +1717,9 @@
       <c r="D2" s="14"/>
       <c r="E2" s="14"/>
       <c r="F2" s="14"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" s="14"/>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -1721,7 +1733,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -1735,7 +1747,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -1748,8 +1760,11 @@
       <c r="D5" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
@@ -1763,7 +1778,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
@@ -1777,7 +1792,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
@@ -1791,7 +1806,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9" s="2" t="s">
         <v>11</v>
       </c>
@@ -1805,7 +1820,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="A10" s="2" t="s">
         <v>12</v>
       </c>
@@ -1819,7 +1834,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11" s="2" t="s">
         <v>13</v>
       </c>
@@ -1833,7 +1848,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7">
       <c r="A12" s="2" t="s">
         <v>14</v>
       </c>
@@ -1847,7 +1862,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7">
       <c r="A13" s="15" t="s">
         <v>116</v>
       </c>
@@ -1856,8 +1871,9 @@
       <c r="D13" s="15"/>
       <c r="E13" s="15"/>
       <c r="F13" s="15"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G13" s="15"/>
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14" s="2" t="s">
         <v>117</v>
       </c>
@@ -1871,7 +1887,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7">
       <c r="A15" s="2" t="s">
         <v>118</v>
       </c>
@@ -1885,7 +1901,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7">
       <c r="A16" s="2" t="s">
         <v>119</v>
       </c>
@@ -1899,7 +1915,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7">
       <c r="A17" s="2" t="s">
         <v>120</v>
       </c>
@@ -1913,7 +1929,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7">
       <c r="A18" s="2" t="s">
         <v>121</v>
       </c>
@@ -1927,7 +1943,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7">
       <c r="A19" s="2" t="s">
         <v>122</v>
       </c>
@@ -1941,7 +1957,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7">
       <c r="A20" s="2" t="s">
         <v>123</v>
       </c>
@@ -1954,8 +1970,11 @@
       <c r="D20" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E20" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
       <c r="A21" s="2" t="s">
         <v>124</v>
       </c>
@@ -1969,7 +1988,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7">
       <c r="A22" s="2" t="s">
         <v>125</v>
       </c>
@@ -1983,7 +2002,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7">
       <c r="A23" s="2" t="s">
         <v>126</v>
       </c>
@@ -1997,7 +2016,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7">
       <c r="A24" s="15" t="s">
         <v>137</v>
       </c>
@@ -2006,8 +2025,9 @@
       <c r="D24" s="15"/>
       <c r="E24" s="15"/>
       <c r="F24" s="15"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G24" s="15"/>
+    </row>
+    <row r="25" spans="1:7">
       <c r="A25" s="2" t="s">
         <v>138</v>
       </c>
@@ -2020,14 +2040,14 @@
       <c r="D25" t="s">
         <v>98</v>
       </c>
-      <c r="E25" t="s">
+      <c r="F25" t="s">
         <v>366</v>
       </c>
-      <c r="F25" t="s">
+      <c r="G25" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7">
       <c r="A26" s="2" t="s">
         <v>139</v>
       </c>
@@ -2041,7 +2061,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7">
       <c r="A27" s="2" t="s">
         <v>140</v>
       </c>
@@ -2055,7 +2075,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7">
       <c r="A28" s="2" t="s">
         <v>141</v>
       </c>
@@ -2068,8 +2088,11 @@
       <c r="D28" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E28" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
       <c r="A29" s="2" t="s">
         <v>142</v>
       </c>
@@ -2082,8 +2105,11 @@
       <c r="D29" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E29" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
       <c r="A30" s="2" t="s">
         <v>143</v>
       </c>
@@ -2096,8 +2122,11 @@
       <c r="D30" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E30" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
       <c r="A31" s="2" t="s">
         <v>144</v>
       </c>
@@ -2111,7 +2140,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7">
       <c r="A32" s="2" t="s">
         <v>145</v>
       </c>
@@ -2125,7 +2154,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7">
       <c r="A33" s="2" t="s">
         <v>146</v>
       </c>
@@ -2139,7 +2168,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7">
       <c r="A34" s="2" t="s">
         <v>147</v>
       </c>
@@ -2153,7 +2182,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7">
       <c r="A35" s="15" t="s">
         <v>158</v>
       </c>
@@ -2162,8 +2191,9 @@
       <c r="D35" s="15"/>
       <c r="E35" s="15"/>
       <c r="F35" s="15"/>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G35" s="15"/>
+    </row>
+    <row r="36" spans="1:7">
       <c r="A36" s="2" t="s">
         <v>163</v>
       </c>
@@ -2176,8 +2206,9 @@
       <c r="D36" s="2" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E36" s="2"/>
+    </row>
+    <row r="37" spans="1:7">
       <c r="A37" s="2" t="s">
         <v>164</v>
       </c>
@@ -2190,8 +2221,9 @@
       <c r="D37" s="2" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E37" s="2"/>
+    </row>
+    <row r="38" spans="1:7">
       <c r="A38" s="2" t="s">
         <v>165</v>
       </c>
@@ -2204,8 +2236,9 @@
       <c r="D38" s="2" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E38" s="2"/>
+    </row>
+    <row r="39" spans="1:7">
       <c r="A39" s="2" t="s">
         <v>166</v>
       </c>
@@ -2218,8 +2251,9 @@
       <c r="D39" s="2" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E39" s="2"/>
+    </row>
+    <row r="40" spans="1:7">
       <c r="A40" s="2" t="s">
         <v>167</v>
       </c>
@@ -2232,8 +2266,11 @@
       <c r="D40" s="2" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E40" s="2" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
       <c r="A41" s="2" t="s">
         <v>168</v>
       </c>
@@ -2246,8 +2283,9 @@
       <c r="D41" s="2" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E41" s="2"/>
+    </row>
+    <row r="42" spans="1:7">
       <c r="A42" s="2" t="s">
         <v>169</v>
       </c>
@@ -2260,8 +2298,9 @@
       <c r="D42" s="2" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E42" s="2"/>
+    </row>
+    <row r="43" spans="1:7">
       <c r="A43" s="2" t="s">
         <v>170</v>
       </c>
@@ -2274,8 +2313,11 @@
       <c r="D43" s="2" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E43" s="2" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
       <c r="A44" s="2" t="s">
         <v>171</v>
       </c>
@@ -2288,8 +2330,9 @@
       <c r="D44" s="2" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E44" s="2"/>
+    </row>
+    <row r="45" spans="1:7">
       <c r="A45" s="2" t="s">
         <v>172</v>
       </c>
@@ -2302,8 +2345,9 @@
       <c r="D45" s="2" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E45" s="2"/>
+    </row>
+    <row r="46" spans="1:7">
       <c r="A46" s="15" t="s">
         <v>184</v>
       </c>
@@ -2312,8 +2356,9 @@
       <c r="D46" s="15"/>
       <c r="E46" s="15"/>
       <c r="F46" s="15"/>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G46" s="15"/>
+    </row>
+    <row r="47" spans="1:7">
       <c r="A47" s="2" t="s">
         <v>185</v>
       </c>
@@ -2327,7 +2372,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7">
       <c r="A48" s="2" t="s">
         <v>186</v>
       </c>
@@ -2341,7 +2386,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7">
       <c r="A49" s="2" t="s">
         <v>187</v>
       </c>
@@ -2355,7 +2400,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7">
       <c r="A50" s="2" t="s">
         <v>188</v>
       </c>
@@ -2369,7 +2414,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7">
       <c r="A51" s="2" t="s">
         <v>189</v>
       </c>
@@ -2383,7 +2428,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7">
       <c r="A52" s="2" t="s">
         <v>190</v>
       </c>
@@ -2397,7 +2442,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7">
       <c r="A53" s="2" t="s">
         <v>191</v>
       </c>
@@ -2410,8 +2455,11 @@
       <c r="D53" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E53" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7">
       <c r="A54" s="2" t="s">
         <v>192</v>
       </c>
@@ -2425,7 +2473,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7">
       <c r="A55" s="2" t="s">
         <v>193</v>
       </c>
@@ -2439,7 +2487,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7">
       <c r="A56" s="2" t="s">
         <v>194</v>
       </c>
@@ -2453,7 +2501,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7">
       <c r="A57" s="15" t="s">
         <v>207</v>
       </c>
@@ -2462,8 +2510,9 @@
       <c r="D57" s="15"/>
       <c r="E57" s="15"/>
       <c r="F57" s="15"/>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G57" s="15"/>
+    </row>
+    <row r="58" spans="1:7">
       <c r="A58" s="2" t="s">
         <v>208</v>
       </c>
@@ -2476,11 +2525,11 @@
       <c r="D58" t="s">
         <v>207</v>
       </c>
-      <c r="E58" t="s">
+      <c r="F58" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7">
       <c r="A59" s="2" t="s">
         <v>209</v>
       </c>
@@ -2494,7 +2543,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7">
       <c r="A60" s="2" t="s">
         <v>210</v>
       </c>
@@ -2508,7 +2557,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7">
       <c r="A61" s="2" t="s">
         <v>211</v>
       </c>
@@ -2522,7 +2571,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7">
       <c r="A62" s="2" t="s">
         <v>212</v>
       </c>
@@ -2536,7 +2585,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7">
       <c r="A63" s="2" t="s">
         <v>213</v>
       </c>
@@ -2549,8 +2598,11 @@
       <c r="D63" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E63" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7">
       <c r="A64" s="2" t="s">
         <v>214</v>
       </c>
@@ -2564,7 +2616,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7">
       <c r="A65" s="2" t="s">
         <v>215</v>
       </c>
@@ -2578,7 +2630,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7">
       <c r="A66" s="2" t="s">
         <v>216</v>
       </c>
@@ -2592,7 +2644,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7">
       <c r="A67" s="2" t="s">
         <v>217</v>
       </c>
@@ -2606,7 +2658,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7">
       <c r="A68" s="15" t="s">
         <v>229</v>
       </c>
@@ -2615,8 +2667,9 @@
       <c r="D68" s="15"/>
       <c r="E68" s="15"/>
       <c r="F68" s="15"/>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G68" s="15"/>
+    </row>
+    <row r="69" spans="1:7">
       <c r="A69" s="2" t="s">
         <v>250</v>
       </c>
@@ -2630,7 +2683,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7">
       <c r="A70" s="2" t="s">
         <v>251</v>
       </c>
@@ -2644,7 +2697,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7">
       <c r="A71" s="2" t="s">
         <v>252</v>
       </c>
@@ -2658,7 +2711,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7">
       <c r="A72" s="2" t="s">
         <v>253</v>
       </c>
@@ -2671,8 +2724,11 @@
       <c r="D72" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E72" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7">
       <c r="A73" s="2" t="s">
         <v>254</v>
       </c>
@@ -2686,7 +2742,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7">
       <c r="A74" s="2" t="s">
         <v>255</v>
       </c>
@@ -2700,7 +2756,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7">
       <c r="A75" s="2" t="s">
         <v>256</v>
       </c>
@@ -2714,7 +2770,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7">
       <c r="A76" s="2" t="s">
         <v>257</v>
       </c>
@@ -2728,7 +2784,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7">
       <c r="A77" s="2" t="s">
         <v>258</v>
       </c>
@@ -2742,7 +2798,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7">
       <c r="A78" s="2" t="s">
         <v>259</v>
       </c>
@@ -2756,7 +2812,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7">
       <c r="A79" s="15" t="s">
         <v>261</v>
       </c>
@@ -2765,8 +2821,9 @@
       <c r="D79" s="15"/>
       <c r="E79" s="15"/>
       <c r="F79" s="15"/>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G79" s="15"/>
+    </row>
+    <row r="80" spans="1:7">
       <c r="A80" s="2" t="s">
         <v>262</v>
       </c>
@@ -2780,7 +2837,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7">
       <c r="A81" s="2" t="s">
         <v>263</v>
       </c>
@@ -2794,7 +2851,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7">
       <c r="A82" s="2" t="s">
         <v>264</v>
       </c>
@@ -2807,8 +2864,11 @@
       <c r="D82" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E82" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7">
       <c r="A83" s="2" t="s">
         <v>265</v>
       </c>
@@ -2822,7 +2882,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7">
       <c r="A84" s="2" t="s">
         <v>266</v>
       </c>
@@ -2836,7 +2896,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7">
       <c r="A85" s="2" t="s">
         <v>267</v>
       </c>
@@ -2850,7 +2910,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7">
       <c r="A86" s="2" t="s">
         <v>268</v>
       </c>
@@ -2864,7 +2924,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7">
       <c r="A87" s="2" t="s">
         <v>269</v>
       </c>
@@ -2877,11 +2937,11 @@
       <c r="D87" t="s">
         <v>64</v>
       </c>
-      <c r="E87" t="s">
+      <c r="F87" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7">
       <c r="A88" s="2" t="s">
         <v>270</v>
       </c>
@@ -2895,7 +2955,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7">
       <c r="A89" s="2" t="s">
         <v>271</v>
       </c>
@@ -2909,7 +2969,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7">
       <c r="A90" s="15" t="s">
         <v>282</v>
       </c>
@@ -2918,8 +2978,9 @@
       <c r="D90" s="15"/>
       <c r="E90" s="15"/>
       <c r="F90" s="15"/>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G90" s="15"/>
+    </row>
+    <row r="91" spans="1:7">
       <c r="A91" s="2" t="s">
         <v>283</v>
       </c>
@@ -2933,7 +2994,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:7">
       <c r="A92" s="2" t="s">
         <v>284</v>
       </c>
@@ -2947,7 +3008,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:7">
       <c r="A93" s="2" t="s">
         <v>285</v>
       </c>
@@ -2961,7 +3022,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:7">
       <c r="A94" s="2" t="s">
         <v>286</v>
       </c>
@@ -2975,7 +3036,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:7">
       <c r="A95" s="2" t="s">
         <v>287</v>
       </c>
@@ -2989,7 +3050,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:7">
       <c r="A96" s="2" t="s">
         <v>288</v>
       </c>
@@ -3002,8 +3063,11 @@
       <c r="D96" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E96" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7">
       <c r="A97" s="2" t="s">
         <v>289</v>
       </c>
@@ -3017,7 +3081,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:7">
       <c r="A98" s="2" t="s">
         <v>290</v>
       </c>
@@ -3031,7 +3095,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:7">
       <c r="A99" s="2" t="s">
         <v>291</v>
       </c>
@@ -3045,7 +3109,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:7">
       <c r="A100" s="2" t="s">
         <v>292</v>
       </c>
@@ -3059,7 +3123,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:7">
       <c r="A101" s="15" t="s">
         <v>315</v>
       </c>
@@ -3068,8 +3132,9 @@
       <c r="D101" s="15"/>
       <c r="E101" s="15"/>
       <c r="F101" s="15"/>
-    </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G101" s="15"/>
+    </row>
+    <row r="102" spans="1:7">
       <c r="A102" s="2" t="s">
         <v>316</v>
       </c>
@@ -3082,11 +3147,11 @@
       <c r="D102" t="s">
         <v>92</v>
       </c>
-      <c r="E102" t="s">
+      <c r="F102" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:7">
       <c r="A103" s="2" t="s">
         <v>317</v>
       </c>
@@ -3100,7 +3165,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:7">
       <c r="A104" s="2" t="s">
         <v>318</v>
       </c>
@@ -3114,7 +3179,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:7">
       <c r="A105" s="2" t="s">
         <v>319</v>
       </c>
@@ -3128,7 +3193,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:7">
       <c r="A106" s="2" t="s">
         <v>320</v>
       </c>
@@ -3142,7 +3207,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:7">
       <c r="A107" s="2" t="s">
         <v>321</v>
       </c>
@@ -3156,7 +3221,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:7">
       <c r="A108" s="2" t="s">
         <v>322</v>
       </c>
@@ -3169,8 +3234,11 @@
       <c r="D108" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E108" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7">
       <c r="A109" s="2" t="s">
         <v>323</v>
       </c>
@@ -3184,7 +3252,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:7">
       <c r="A110" s="2" t="s">
         <v>324</v>
       </c>
@@ -3198,7 +3266,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:7">
       <c r="A111" s="2" t="s">
         <v>325</v>
       </c>
@@ -3212,7 +3280,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:7">
       <c r="A112" s="15" t="s">
         <v>337</v>
       </c>
@@ -3221,8 +3289,9 @@
       <c r="D112" s="15"/>
       <c r="E112" s="15"/>
       <c r="F112" s="15"/>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G112" s="15"/>
+    </row>
+    <row r="113" spans="1:5">
       <c r="A113" s="2" t="s">
         <v>338</v>
       </c>
@@ -3236,7 +3305,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5">
       <c r="A114" s="2" t="s">
         <v>339</v>
       </c>
@@ -3250,7 +3319,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5">
       <c r="A115" s="2" t="s">
         <v>340</v>
       </c>
@@ -3264,7 +3333,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5">
       <c r="A116" s="2" t="s">
         <v>341</v>
       </c>
@@ -3277,8 +3346,11 @@
       <c r="D116" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E116" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5">
       <c r="A117" s="2" t="s">
         <v>342</v>
       </c>
@@ -3292,7 +3364,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5">
       <c r="A118" s="2" t="s">
         <v>343</v>
       </c>
@@ -3306,7 +3378,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5">
       <c r="A119" s="2" t="s">
         <v>344</v>
       </c>
@@ -3320,7 +3392,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5">
       <c r="A120" s="2" t="s">
         <v>345</v>
       </c>
@@ -3334,7 +3406,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5">
       <c r="A121" s="2" t="s">
         <v>346</v>
       </c>
@@ -3348,7 +3420,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5">
       <c r="A122" s="2" t="s">
         <v>347</v>
       </c>
@@ -3370,33 +3442,33 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:P11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+    <sheetView topLeftCell="G1" workbookViewId="0">
       <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="12.28515625" customWidth="1"/>
-    <col min="3" max="3" width="27.42578125" customWidth="1"/>
-    <col min="4" max="4" width="25.85546875" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" customWidth="1"/>
+    <col min="3" max="3" width="27.44140625" customWidth="1"/>
+    <col min="4" max="4" width="25.88671875" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" customWidth="1"/>
+    <col min="6" max="6" width="11.88671875" customWidth="1"/>
     <col min="7" max="7" width="15" customWidth="1"/>
-    <col min="8" max="8" width="16.5703125" customWidth="1"/>
-    <col min="9" max="9" width="17.85546875" customWidth="1"/>
-    <col min="10" max="10" width="19.28515625" customWidth="1"/>
-    <col min="11" max="11" width="17.85546875" customWidth="1"/>
-    <col min="12" max="12" width="16.85546875" customWidth="1"/>
+    <col min="8" max="8" width="16.5546875" customWidth="1"/>
+    <col min="9" max="9" width="17.88671875" customWidth="1"/>
+    <col min="10" max="10" width="19.33203125" customWidth="1"/>
+    <col min="11" max="11" width="17.88671875" customWidth="1"/>
+    <col min="12" max="12" width="16.88671875" customWidth="1"/>
     <col min="13" max="13" width="17" customWidth="1"/>
-    <col min="14" max="14" width="15.140625" customWidth="1"/>
-    <col min="15" max="15" width="17.7109375" customWidth="1"/>
-    <col min="16" max="16" width="15.5703125" customWidth="1"/>
+    <col min="14" max="14" width="15.109375" customWidth="1"/>
+    <col min="15" max="15" width="17.6640625" customWidth="1"/>
+    <col min="16" max="16" width="15.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" s="17" customFormat="1">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
@@ -3446,7 +3518,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -3487,7 +3559,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -3507,7 +3579,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -3527,7 +3599,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -3547,7 +3619,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -3567,7 +3639,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
@@ -3587,7 +3659,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
@@ -3607,7 +3679,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
@@ -3627,7 +3699,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
@@ -3647,7 +3719,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16">
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
@@ -3673,28 +3745,28 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="6.42578125" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="40.28515625" customWidth="1"/>
-    <col min="5" max="5" width="22.7109375" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" customWidth="1"/>
-    <col min="7" max="7" width="21.42578125" customWidth="1"/>
-    <col min="8" max="8" width="21.28515625" customWidth="1"/>
-    <col min="9" max="9" width="18.28515625" customWidth="1"/>
-    <col min="10" max="10" width="9.28515625" customWidth="1"/>
+    <col min="1" max="1" width="6.44140625" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.33203125" customWidth="1"/>
+    <col min="5" max="5" width="22.6640625" customWidth="1"/>
+    <col min="6" max="6" width="12.44140625" customWidth="1"/>
+    <col min="7" max="7" width="21.44140625" customWidth="1"/>
+    <col min="8" max="8" width="21.33203125" customWidth="1"/>
+    <col min="9" max="9" width="18.33203125" customWidth="1"/>
+    <col min="10" max="10" width="9.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3724,7 +3796,7 @@
       <c r="K1" s="5"/>
       <c r="L1" s="1"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -3752,7 +3824,7 @@
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -3778,7 +3850,7 @@
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -3804,7 +3876,7 @@
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -3830,7 +3902,7 @@
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -3856,7 +3928,7 @@
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
@@ -3882,7 +3954,7 @@
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
@@ -3908,7 +3980,7 @@
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
@@ -3934,7 +4006,7 @@
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
@@ -3960,7 +4032,7 @@
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12">
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
@@ -3989,18 +4061,18 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1"/>
-    <hyperlink ref="E3:E11" r:id="rId2" display="aarosagarch@gmail.com"/>
-    <hyperlink ref="F2" r:id="rId3"/>
-    <hyperlink ref="F3" r:id="rId4"/>
-    <hyperlink ref="F4" r:id="rId5"/>
-    <hyperlink ref="F5" r:id="rId6"/>
-    <hyperlink ref="F6" r:id="rId7"/>
-    <hyperlink ref="F7" r:id="rId8"/>
-    <hyperlink ref="F8" r:id="rId9"/>
-    <hyperlink ref="F9" r:id="rId10"/>
-    <hyperlink ref="F10" r:id="rId11"/>
-    <hyperlink ref="F11" r:id="rId12"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0A00-000000000000}"/>
+    <hyperlink ref="E3:E11" r:id="rId2" display="aarosagarch@gmail.com" xr:uid="{00000000-0004-0000-0A00-000001000000}"/>
+    <hyperlink ref="F2" r:id="rId3" xr:uid="{00000000-0004-0000-0A00-000002000000}"/>
+    <hyperlink ref="F3" r:id="rId4" xr:uid="{00000000-0004-0000-0A00-000003000000}"/>
+    <hyperlink ref="F4" r:id="rId5" xr:uid="{00000000-0004-0000-0A00-000004000000}"/>
+    <hyperlink ref="F5" r:id="rId6" xr:uid="{00000000-0004-0000-0A00-000005000000}"/>
+    <hyperlink ref="F6" r:id="rId7" xr:uid="{00000000-0004-0000-0A00-000006000000}"/>
+    <hyperlink ref="F7" r:id="rId8" xr:uid="{00000000-0004-0000-0A00-000007000000}"/>
+    <hyperlink ref="F8" r:id="rId9" xr:uid="{00000000-0004-0000-0A00-000008000000}"/>
+    <hyperlink ref="F9" r:id="rId10" xr:uid="{00000000-0004-0000-0A00-000009000000}"/>
+    <hyperlink ref="F10" r:id="rId11" xr:uid="{00000000-0004-0000-0A00-00000A000000}"/>
+    <hyperlink ref="F11" r:id="rId12" xr:uid="{00000000-0004-0000-0A00-00000B000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -4008,23 +4080,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26" customWidth="1"/>
-    <col min="4" max="4" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4044,7 +4116,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -4064,7 +4136,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -4084,7 +4156,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -4104,7 +4176,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -4124,7 +4196,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -4144,7 +4216,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
@@ -4164,7 +4236,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
@@ -4184,7 +4256,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
@@ -4204,7 +4276,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
@@ -4224,7 +4296,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6">
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
@@ -4247,38 +4319,38 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1"/>
-    <hyperlink ref="F3:F11" r:id="rId2" display="Admin@123"/>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="F3:F11" r:id="rId2" display="Admin@123" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:O11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="L29" sqref="L29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="38" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.44140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4325,7 +4397,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -4369,7 +4441,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -4407,7 +4479,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -4445,7 +4517,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -4480,7 +4552,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -4524,7 +4596,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
@@ -4553,7 +4625,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
@@ -4576,7 +4648,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
@@ -4596,7 +4668,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
@@ -4616,7 +4688,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15">
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
@@ -4639,43 +4711,43 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1"/>
-    <hyperlink ref="F3" r:id="rId2"/>
-    <hyperlink ref="F4" r:id="rId3"/>
-    <hyperlink ref="F5" r:id="rId4"/>
-    <hyperlink ref="F6" r:id="rId5"/>
-    <hyperlink ref="F7" r:id="rId6"/>
-    <hyperlink ref="F8" r:id="rId7"/>
-    <hyperlink ref="F9" r:id="rId8"/>
-    <hyperlink ref="F10" r:id="rId9"/>
-    <hyperlink ref="F11" r:id="rId10"/>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="F3" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="F4" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+    <hyperlink ref="F5" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
+    <hyperlink ref="F6" r:id="rId5" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
+    <hyperlink ref="F7" r:id="rId6" xr:uid="{00000000-0004-0000-0200-000005000000}"/>
+    <hyperlink ref="F8" r:id="rId7" xr:uid="{00000000-0004-0000-0200-000006000000}"/>
+    <hyperlink ref="F9" r:id="rId8" xr:uid="{00000000-0004-0000-0200-000007000000}"/>
+    <hyperlink ref="F10" r:id="rId9" xr:uid="{00000000-0004-0000-0200-000008000000}"/>
+    <hyperlink ref="F11" r:id="rId10" xr:uid="{00000000-0004-0000-0200-000009000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4707,7 +4779,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -4739,7 +4811,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -4771,7 +4843,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -4803,7 +4875,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -4835,7 +4907,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -4867,7 +4939,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
@@ -4899,7 +4971,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
@@ -4931,7 +5003,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
@@ -4963,7 +5035,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
@@ -4995,7 +5067,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10">
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
@@ -5030,59 +5102,59 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1"/>
-    <hyperlink ref="I2" r:id="rId2"/>
-    <hyperlink ref="J2" r:id="rId3"/>
-    <hyperlink ref="F3:F11" r:id="rId4" display="Admin@123"/>
-    <hyperlink ref="I5" r:id="rId5"/>
-    <hyperlink ref="J5" r:id="rId6"/>
-    <hyperlink ref="I10" r:id="rId7"/>
-    <hyperlink ref="J10" r:id="rId8"/>
-    <hyperlink ref="I3" r:id="rId9"/>
-    <hyperlink ref="J3" r:id="rId10"/>
-    <hyperlink ref="I4" r:id="rId11"/>
-    <hyperlink ref="J4" r:id="rId12"/>
-    <hyperlink ref="I6" r:id="rId13"/>
-    <hyperlink ref="J6" r:id="rId14"/>
-    <hyperlink ref="I7" r:id="rId15"/>
-    <hyperlink ref="J7" r:id="rId16"/>
-    <hyperlink ref="I8" r:id="rId17"/>
-    <hyperlink ref="J8" r:id="rId18"/>
-    <hyperlink ref="I9" r:id="rId19"/>
-    <hyperlink ref="J9" r:id="rId20"/>
-    <hyperlink ref="I11" r:id="rId21"/>
-    <hyperlink ref="J11" r:id="rId22"/>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="I2" r:id="rId2" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
+    <hyperlink ref="J2" r:id="rId3" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
+    <hyperlink ref="F3:F11" r:id="rId4" display="Admin@123" xr:uid="{00000000-0004-0000-0300-000003000000}"/>
+    <hyperlink ref="I5" r:id="rId5" xr:uid="{00000000-0004-0000-0300-000004000000}"/>
+    <hyperlink ref="J5" r:id="rId6" xr:uid="{00000000-0004-0000-0300-000005000000}"/>
+    <hyperlink ref="I10" r:id="rId7" xr:uid="{00000000-0004-0000-0300-000006000000}"/>
+    <hyperlink ref="J10" r:id="rId8" xr:uid="{00000000-0004-0000-0300-000007000000}"/>
+    <hyperlink ref="I3" r:id="rId9" xr:uid="{00000000-0004-0000-0300-000008000000}"/>
+    <hyperlink ref="J3" r:id="rId10" xr:uid="{00000000-0004-0000-0300-000009000000}"/>
+    <hyperlink ref="I4" r:id="rId11" xr:uid="{00000000-0004-0000-0300-00000A000000}"/>
+    <hyperlink ref="J4" r:id="rId12" xr:uid="{00000000-0004-0000-0300-00000B000000}"/>
+    <hyperlink ref="I6" r:id="rId13" xr:uid="{00000000-0004-0000-0300-00000C000000}"/>
+    <hyperlink ref="J6" r:id="rId14" xr:uid="{00000000-0004-0000-0300-00000D000000}"/>
+    <hyperlink ref="I7" r:id="rId15" xr:uid="{00000000-0004-0000-0300-00000E000000}"/>
+    <hyperlink ref="J7" r:id="rId16" xr:uid="{00000000-0004-0000-0300-00000F000000}"/>
+    <hyperlink ref="I8" r:id="rId17" xr:uid="{00000000-0004-0000-0300-000010000000}"/>
+    <hyperlink ref="J8" r:id="rId18" xr:uid="{00000000-0004-0000-0300-000011000000}"/>
+    <hyperlink ref="I9" r:id="rId19" xr:uid="{00000000-0004-0000-0300-000012000000}"/>
+    <hyperlink ref="J9" r:id="rId20" xr:uid="{00000000-0004-0000-0300-000013000000}"/>
+    <hyperlink ref="I11" r:id="rId21" xr:uid="{00000000-0004-0000-0300-000014000000}"/>
+    <hyperlink ref="J11" r:id="rId22" xr:uid="{00000000-0004-0000-0300-000015000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G8" sqref="G8:L8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" style="8"/>
-    <col min="2" max="2" width="15.85546875" style="8" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="39.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.33203125" style="8"/>
+    <col min="2" max="2" width="15.88671875" style="8" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.44140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.6640625" style="8" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17" style="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.7109375" style="8" customWidth="1"/>
-    <col min="13" max="16384" width="9.28515625" style="8"/>
+    <col min="11" max="11" width="20.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.6640625" style="8" customWidth="1"/>
+    <col min="13" max="16384" width="9.33203125" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="28.8">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -5120,7 +5192,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="28.8">
       <c r="A2" s="9" t="s">
         <v>5</v>
       </c>
@@ -5158,7 +5230,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12">
       <c r="A3" s="9" t="s">
         <v>6</v>
       </c>
@@ -5184,7 +5256,7 @@
       <c r="K3" s="10"/>
       <c r="L3" s="10"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12">
       <c r="A4" s="9" t="s">
         <v>7</v>
       </c>
@@ -5210,7 +5282,7 @@
       <c r="K4" s="10"/>
       <c r="L4" s="10"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12">
       <c r="A5" s="9" t="s">
         <v>8</v>
       </c>
@@ -5236,7 +5308,7 @@
       <c r="K5" s="10"/>
       <c r="L5" s="10"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12">
       <c r="A6" s="9" t="s">
         <v>9</v>
       </c>
@@ -5262,7 +5334,7 @@
       <c r="K6" s="10"/>
       <c r="L6" s="10"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12">
       <c r="A7" s="9" t="s">
         <v>10</v>
       </c>
@@ -5288,7 +5360,7 @@
       <c r="K7" s="10"/>
       <c r="L7" s="10"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12">
       <c r="A8" s="9" t="s">
         <v>11</v>
       </c>
@@ -5314,7 +5386,7 @@
       <c r="K8" s="10"/>
       <c r="L8" s="10"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12">
       <c r="A9" s="9" t="s">
         <v>12</v>
       </c>
@@ -5340,7 +5412,7 @@
       <c r="K9" s="10"/>
       <c r="L9" s="10"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12">
       <c r="A10" s="9" t="s">
         <v>13</v>
       </c>
@@ -5366,7 +5438,7 @@
       <c r="K10" s="10"/>
       <c r="L10" s="10"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12">
       <c r="A11" s="9" t="s">
         <v>14</v>
       </c>
@@ -5392,22 +5464,22 @@
       <c r="K11" s="10"/>
       <c r="L11" s="10"/>
     </row>
-    <row r="17" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="7:7">
       <c r="G17" s="16"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="F11" r:id="rId1"/>
-    <hyperlink ref="F10" r:id="rId2"/>
-    <hyperlink ref="F9" r:id="rId3"/>
-    <hyperlink ref="F8" r:id="rId4"/>
-    <hyperlink ref="F7" r:id="rId5"/>
-    <hyperlink ref="F6" r:id="rId6"/>
-    <hyperlink ref="F5" r:id="rId7"/>
-    <hyperlink ref="F4" r:id="rId8"/>
-    <hyperlink ref="F3" r:id="rId9"/>
-    <hyperlink ref="F2" r:id="rId10"/>
+    <hyperlink ref="F11" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
+    <hyperlink ref="F10" r:id="rId2" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
+    <hyperlink ref="F9" r:id="rId3" xr:uid="{00000000-0004-0000-0400-000002000000}"/>
+    <hyperlink ref="F8" r:id="rId4" xr:uid="{00000000-0004-0000-0400-000003000000}"/>
+    <hyperlink ref="F7" r:id="rId5" xr:uid="{00000000-0004-0000-0400-000004000000}"/>
+    <hyperlink ref="F6" r:id="rId6" xr:uid="{00000000-0004-0000-0400-000005000000}"/>
+    <hyperlink ref="F5" r:id="rId7" xr:uid="{00000000-0004-0000-0400-000006000000}"/>
+    <hyperlink ref="F4" r:id="rId8" xr:uid="{00000000-0004-0000-0400-000007000000}"/>
+    <hyperlink ref="F3" r:id="rId9" xr:uid="{00000000-0004-0000-0400-000008000000}"/>
+    <hyperlink ref="F2" r:id="rId10" xr:uid="{00000000-0004-0000-0400-000009000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId11"/>
@@ -5415,26 +5487,26 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:P11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:P11"/>
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5484,7 +5556,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -5504,7 +5576,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -5524,7 +5596,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -5544,7 +5616,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -5564,7 +5636,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -5584,7 +5656,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
@@ -5604,7 +5676,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
@@ -5624,7 +5696,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
@@ -5644,7 +5716,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
@@ -5664,7 +5736,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16">
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
@@ -5687,50 +5759,50 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1"/>
-    <hyperlink ref="F2" r:id="rId2"/>
-    <hyperlink ref="E3" r:id="rId3"/>
-    <hyperlink ref="E4" r:id="rId4"/>
-    <hyperlink ref="E5" r:id="rId5"/>
-    <hyperlink ref="E6" r:id="rId6"/>
-    <hyperlink ref="E7" r:id="rId7"/>
-    <hyperlink ref="E8" r:id="rId8"/>
-    <hyperlink ref="E9" r:id="rId9"/>
-    <hyperlink ref="E10" r:id="rId10"/>
-    <hyperlink ref="E11" r:id="rId11"/>
-    <hyperlink ref="F3" r:id="rId12"/>
-    <hyperlink ref="F4" r:id="rId13"/>
-    <hyperlink ref="F5" r:id="rId14"/>
-    <hyperlink ref="F6" r:id="rId15"/>
-    <hyperlink ref="F7" r:id="rId16"/>
-    <hyperlink ref="F8" r:id="rId17"/>
-    <hyperlink ref="F9" r:id="rId18"/>
-    <hyperlink ref="F10" r:id="rId19"/>
-    <hyperlink ref="F11" r:id="rId20"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
+    <hyperlink ref="F2" r:id="rId2" xr:uid="{00000000-0004-0000-0500-000001000000}"/>
+    <hyperlink ref="E3" r:id="rId3" xr:uid="{00000000-0004-0000-0500-000002000000}"/>
+    <hyperlink ref="E4" r:id="rId4" xr:uid="{00000000-0004-0000-0500-000003000000}"/>
+    <hyperlink ref="E5" r:id="rId5" xr:uid="{00000000-0004-0000-0500-000004000000}"/>
+    <hyperlink ref="E6" r:id="rId6" xr:uid="{00000000-0004-0000-0500-000005000000}"/>
+    <hyperlink ref="E7" r:id="rId7" xr:uid="{00000000-0004-0000-0500-000006000000}"/>
+    <hyperlink ref="E8" r:id="rId8" xr:uid="{00000000-0004-0000-0500-000007000000}"/>
+    <hyperlink ref="E9" r:id="rId9" xr:uid="{00000000-0004-0000-0500-000008000000}"/>
+    <hyperlink ref="E10" r:id="rId10" xr:uid="{00000000-0004-0000-0500-000009000000}"/>
+    <hyperlink ref="E11" r:id="rId11" xr:uid="{00000000-0004-0000-0500-00000A000000}"/>
+    <hyperlink ref="F3" r:id="rId12" xr:uid="{00000000-0004-0000-0500-00000B000000}"/>
+    <hyperlink ref="F4" r:id="rId13" xr:uid="{00000000-0004-0000-0500-00000C000000}"/>
+    <hyperlink ref="F5" r:id="rId14" xr:uid="{00000000-0004-0000-0500-00000D000000}"/>
+    <hyperlink ref="F6" r:id="rId15" xr:uid="{00000000-0004-0000-0500-00000E000000}"/>
+    <hyperlink ref="F7" r:id="rId16" xr:uid="{00000000-0004-0000-0500-00000F000000}"/>
+    <hyperlink ref="F8" r:id="rId17" xr:uid="{00000000-0004-0000-0500-000010000000}"/>
+    <hyperlink ref="F9" r:id="rId18" xr:uid="{00000000-0004-0000-0500-000011000000}"/>
+    <hyperlink ref="F10" r:id="rId19" xr:uid="{00000000-0004-0000-0500-000012000000}"/>
+    <hyperlink ref="F11" r:id="rId20" xr:uid="{00000000-0004-0000-0500-000013000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3:G11"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="28" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="34" customWidth="1"/>
     <col min="5" max="5" width="23" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" customWidth="1"/>
-    <col min="7" max="7" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.33203125" customWidth="1"/>
+    <col min="7" max="7" width="21.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5753,7 +5825,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -5776,7 +5848,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -5796,7 +5868,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -5816,7 +5888,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -5836,7 +5908,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -5856,7 +5928,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
@@ -5876,7 +5948,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
@@ -5896,7 +5968,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
@@ -5919,7 +5991,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
@@ -5939,7 +6011,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
@@ -5962,18 +6034,18 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1"/>
-    <hyperlink ref="E3:E11" r:id="rId2" display="aarosagarch@gmail.com"/>
-    <hyperlink ref="F2" r:id="rId3"/>
-    <hyperlink ref="F3" r:id="rId4"/>
-    <hyperlink ref="F4" r:id="rId5"/>
-    <hyperlink ref="F5" r:id="rId6"/>
-    <hyperlink ref="F6" r:id="rId7"/>
-    <hyperlink ref="F7" r:id="rId8"/>
-    <hyperlink ref="F8" r:id="rId9"/>
-    <hyperlink ref="F9" r:id="rId10"/>
-    <hyperlink ref="F10" r:id="rId11"/>
-    <hyperlink ref="F11" r:id="rId12"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
+    <hyperlink ref="E3:E11" r:id="rId2" display="aarosagarch@gmail.com" xr:uid="{00000000-0004-0000-0600-000001000000}"/>
+    <hyperlink ref="F2" r:id="rId3" xr:uid="{00000000-0004-0000-0600-000002000000}"/>
+    <hyperlink ref="F3" r:id="rId4" xr:uid="{00000000-0004-0000-0600-000003000000}"/>
+    <hyperlink ref="F4" r:id="rId5" xr:uid="{00000000-0004-0000-0600-000004000000}"/>
+    <hyperlink ref="F5" r:id="rId6" xr:uid="{00000000-0004-0000-0600-000005000000}"/>
+    <hyperlink ref="F6" r:id="rId7" xr:uid="{00000000-0004-0000-0600-000006000000}"/>
+    <hyperlink ref="F7" r:id="rId8" xr:uid="{00000000-0004-0000-0600-000007000000}"/>
+    <hyperlink ref="F8" r:id="rId9" xr:uid="{00000000-0004-0000-0600-000008000000}"/>
+    <hyperlink ref="F9" r:id="rId10" xr:uid="{00000000-0004-0000-0600-000009000000}"/>
+    <hyperlink ref="F10" r:id="rId11" xr:uid="{00000000-0004-0000-0600-00000A000000}"/>
+    <hyperlink ref="F11" r:id="rId12" xr:uid="{00000000-0004-0000-0600-00000B000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId13"/>
@@ -5981,25 +6053,25 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="41.28515625" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.33203125" customWidth="1"/>
     <col min="4" max="4" width="40" customWidth="1"/>
-    <col min="5" max="5" width="24.42578125" customWidth="1"/>
-    <col min="6" max="6" width="19.5703125" customWidth="1"/>
-    <col min="7" max="7" width="22.7109375" customWidth="1"/>
-    <col min="8" max="8" width="20.28515625" customWidth="1"/>
+    <col min="5" max="5" width="24.44140625" customWidth="1"/>
+    <col min="6" max="6" width="19.5546875" customWidth="1"/>
+    <col min="7" max="7" width="22.6640625" customWidth="1"/>
+    <col min="8" max="8" width="20.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6025,7 +6097,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -6051,7 +6123,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -6071,7 +6143,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -6091,7 +6163,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -6111,7 +6183,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -6131,7 +6203,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
@@ -6151,7 +6223,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
@@ -6171,7 +6243,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
@@ -6191,7 +6263,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
@@ -6211,7 +6283,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8">
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
@@ -6234,18 +6306,18 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1"/>
-    <hyperlink ref="E3:E11" r:id="rId2" display="aarosagarch@gmail.com"/>
-    <hyperlink ref="F2" r:id="rId3"/>
-    <hyperlink ref="F3" r:id="rId4"/>
-    <hyperlink ref="F4" r:id="rId5"/>
-    <hyperlink ref="F5" r:id="rId6"/>
-    <hyperlink ref="F6" r:id="rId7"/>
-    <hyperlink ref="F7" r:id="rId8"/>
-    <hyperlink ref="F8" r:id="rId9"/>
-    <hyperlink ref="F9" r:id="rId10"/>
-    <hyperlink ref="F10" r:id="rId11"/>
-    <hyperlink ref="F11" r:id="rId12"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0700-000000000000}"/>
+    <hyperlink ref="E3:E11" r:id="rId2" display="aarosagarch@gmail.com" xr:uid="{00000000-0004-0000-0700-000001000000}"/>
+    <hyperlink ref="F2" r:id="rId3" xr:uid="{00000000-0004-0000-0700-000002000000}"/>
+    <hyperlink ref="F3" r:id="rId4" xr:uid="{00000000-0004-0000-0700-000003000000}"/>
+    <hyperlink ref="F4" r:id="rId5" xr:uid="{00000000-0004-0000-0700-000004000000}"/>
+    <hyperlink ref="F5" r:id="rId6" xr:uid="{00000000-0004-0000-0700-000005000000}"/>
+    <hyperlink ref="F6" r:id="rId7" xr:uid="{00000000-0004-0000-0700-000006000000}"/>
+    <hyperlink ref="F7" r:id="rId8" xr:uid="{00000000-0004-0000-0700-000007000000}"/>
+    <hyperlink ref="F8" r:id="rId9" xr:uid="{00000000-0004-0000-0700-000008000000}"/>
+    <hyperlink ref="F9" r:id="rId10" xr:uid="{00000000-0004-0000-0700-000009000000}"/>
+    <hyperlink ref="F10" r:id="rId11" xr:uid="{00000000-0004-0000-0700-00000A000000}"/>
+    <hyperlink ref="F11" r:id="rId12" xr:uid="{00000000-0004-0000-0700-00000B000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId13"/>
@@ -6253,26 +6325,26 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="41.7109375" customWidth="1"/>
-    <col min="4" max="4" width="34.28515625" customWidth="1"/>
-    <col min="5" max="5" width="22.5703125" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.6640625" customWidth="1"/>
+    <col min="4" max="4" width="34.33203125" customWidth="1"/>
+    <col min="5" max="5" width="22.5546875" customWidth="1"/>
+    <col min="6" max="6" width="11.33203125" customWidth="1"/>
     <col min="7" max="7" width="23" customWidth="1"/>
-    <col min="8" max="8" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.7109375" customWidth="1"/>
+    <col min="8" max="8" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>89</v>
       </c>
@@ -6301,7 +6373,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -6330,7 +6402,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -6350,7 +6422,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -6370,7 +6442,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -6390,7 +6462,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -6410,7 +6482,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
@@ -6430,7 +6502,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
@@ -6450,7 +6522,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
@@ -6470,7 +6542,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
@@ -6490,7 +6562,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9">
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>

</xml_diff>

<commit_message>
Stabilization of automation Scripts
</commit_message>
<xml_diff>
--- a/src/main/resources/AutomationCatalogue_Batch41_TestData.xlsx
+++ b/src/main/resources/AutomationCatalogue_Batch41_TestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Automation Catalogue\Projects\TestAutomationCatalogue_Batch41\src\main\resources\"/>
     </mc:Choice>
@@ -26,7 +26,7 @@
   </sheets>
   <calcPr calcId="124519"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1427" uniqueCount="447">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1439" uniqueCount="449">
   <si>
     <t>S. No</t>
   </si>
@@ -1375,12 +1375,19 @@
   </si>
   <si>
     <t>7-November-2024</t>
+  </si>
+  <si>
+    <t>0141</t>
+  </si>
+  <si>
+    <t>addUser</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1856,12 +1863,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="5.0"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.7109375"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="39.0"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="38.0"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="9.42578125"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="18.28515625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -1902,27 +1909,30 @@
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>104</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>15</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" t="s" s="0">
         <v>16</v>
+      </c>
+      <c r="F3" t="s" s="0">
+        <v>364</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>105</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" t="s" s="0">
         <v>15</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" t="s" s="0">
         <v>16</v>
       </c>
     </row>
@@ -1930,16 +1940,16 @@
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" t="s" s="0">
         <v>106</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" t="s" s="0">
         <v>15</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" t="s" s="0">
         <v>16</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" t="s" s="0">
         <v>386</v>
       </c>
     </row>
@@ -1947,13 +1957,13 @@
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" t="s" s="0">
         <v>107</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" t="s" s="0">
         <v>15</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" t="s" s="0">
         <v>16</v>
       </c>
     </row>
@@ -1961,13 +1971,13 @@
       <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" t="s" s="0">
         <v>108</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" t="s" s="0">
         <v>15</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" t="s" s="0">
         <v>16</v>
       </c>
     </row>
@@ -1975,13 +1985,13 @@
       <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" t="s" s="0">
         <v>109</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" t="s" s="0">
         <v>15</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" t="s" s="0">
         <v>16</v>
       </c>
     </row>
@@ -1989,13 +1999,13 @@
       <c r="A9" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" t="s" s="0">
         <v>110</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" t="s" s="0">
         <v>15</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" t="s" s="0">
         <v>16</v>
       </c>
     </row>
@@ -2003,13 +2013,13 @@
       <c r="A10" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" t="s" s="0">
         <v>111</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" t="s" s="0">
         <v>15</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" t="s" s="0">
         <v>16</v>
       </c>
     </row>
@@ -2017,13 +2027,13 @@
       <c r="A11" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" t="s" s="0">
         <v>112</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" t="s" s="0">
         <v>15</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" t="s" s="0">
         <v>16</v>
       </c>
     </row>
@@ -2031,13 +2041,13 @@
       <c r="A12" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" t="s" s="0">
         <v>113</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" t="s" s="0">
         <v>15</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" t="s" s="0">
         <v>16</v>
       </c>
     </row>
@@ -2059,11 +2069,14 @@
       <c r="B14" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" t="s" s="0">
         <v>38</v>
+      </c>
+      <c r="F14" t="s" s="0">
+        <v>364</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -2073,10 +2086,10 @@
       <c r="B15" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" t="s" s="0">
         <v>38</v>
       </c>
     </row>
@@ -2087,10 +2100,10 @@
       <c r="B16" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" t="s" s="0">
         <v>38</v>
       </c>
     </row>
@@ -2101,10 +2114,10 @@
       <c r="B17" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" t="s" s="0">
         <v>38</v>
       </c>
     </row>
@@ -2115,10 +2128,10 @@
       <c r="B18" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" t="s" s="0">
         <v>38</v>
       </c>
     </row>
@@ -2129,10 +2142,10 @@
       <c r="B19" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" t="s" s="0">
         <v>38</v>
       </c>
     </row>
@@ -2143,13 +2156,13 @@
       <c r="B20" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" t="s" s="0">
         <v>38</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" t="s" s="0">
         <v>386</v>
       </c>
     </row>
@@ -2160,10 +2173,10 @@
       <c r="B21" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" t="s" s="0">
         <v>38</v>
       </c>
     </row>
@@ -2174,10 +2187,10 @@
       <c r="B22" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" t="s" s="0">
         <v>38</v>
       </c>
     </row>
@@ -2188,10 +2201,10 @@
       <c r="B23" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" t="s" s="0">
         <v>38</v>
       </c>
     </row>
@@ -2213,16 +2226,16 @@
       <c r="B25" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" t="s" s="0">
         <v>96</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" t="s" s="0">
         <v>97</v>
       </c>
-      <c r="F25" t="s">
-        <v>365</v>
-      </c>
-      <c r="G25" t="s">
+      <c r="F25" t="s" s="0">
+        <v>364</v>
+      </c>
+      <c r="G25" t="s" s="0">
         <v>366</v>
       </c>
     </row>
@@ -2233,10 +2246,10 @@
       <c r="B26" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" t="s" s="0">
         <v>96</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26" t="s" s="0">
         <v>97</v>
       </c>
     </row>
@@ -2247,10 +2260,10 @@
       <c r="B27" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" t="s" s="0">
         <v>96</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D27" t="s" s="0">
         <v>97</v>
       </c>
     </row>
@@ -2261,13 +2274,13 @@
       <c r="B28" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" t="s" s="0">
         <v>96</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D28" t="s" s="0">
         <v>97</v>
       </c>
-      <c r="E28" t="s">
+      <c r="E28" t="s" s="0">
         <v>386</v>
       </c>
     </row>
@@ -2278,13 +2291,13 @@
       <c r="B29" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" t="s" s="0">
         <v>96</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D29" t="s" s="0">
         <v>97</v>
       </c>
-      <c r="E29" t="s">
+      <c r="E29" t="s" s="0">
         <v>386</v>
       </c>
     </row>
@@ -2295,13 +2308,13 @@
       <c r="B30" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" t="s" s="0">
         <v>96</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D30" t="s" s="0">
         <v>97</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E30" t="s" s="0">
         <v>386</v>
       </c>
     </row>
@@ -2312,10 +2325,10 @@
       <c r="B31" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" t="s" s="0">
         <v>96</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D31" t="s" s="0">
         <v>97</v>
       </c>
     </row>
@@ -2326,10 +2339,10 @@
       <c r="B32" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" t="s" s="0">
         <v>96</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D32" t="s" s="0">
         <v>97</v>
       </c>
     </row>
@@ -2340,10 +2353,10 @@
       <c r="B33" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33" t="s" s="0">
         <v>96</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D33" t="s" s="0">
         <v>97</v>
       </c>
     </row>
@@ -2354,10 +2367,10 @@
       <c r="B34" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" t="s" s="0">
         <v>96</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D34" t="s" s="0">
         <v>97</v>
       </c>
     </row>
@@ -2376,25 +2389,28 @@
       <c r="A36" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" t="s" s="0">
         <v>173</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C36" t="s" s="0">
         <v>172</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>87</v>
       </c>
       <c r="E36" s="2"/>
+      <c r="F36" t="s" s="0">
+        <v>364</v>
+      </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" t="s" s="0">
         <v>181</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C37" t="s" s="0">
         <v>172</v>
       </c>
       <c r="D37" s="2" t="s">
@@ -2406,10 +2422,10 @@
       <c r="A38" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" t="s" s="0">
         <v>174</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C38" t="s" s="0">
         <v>172</v>
       </c>
       <c r="D38" s="2" t="s">
@@ -2421,10 +2437,10 @@
       <c r="A39" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39" t="s" s="0">
         <v>175</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C39" t="s" s="0">
         <v>172</v>
       </c>
       <c r="D39" s="2" t="s">
@@ -2436,10 +2452,10 @@
       <c r="A40" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" t="s" s="0">
         <v>176</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C40" t="s" s="0">
         <v>172</v>
       </c>
       <c r="D40" s="2" t="s">
@@ -2453,10 +2469,10 @@
       <c r="A41" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" t="s" s="0">
         <v>177</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C41" t="s" s="0">
         <v>172</v>
       </c>
       <c r="D41" s="2" t="s">
@@ -2468,10 +2484,10 @@
       <c r="A42" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42" t="s" s="0">
         <v>178</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C42" t="s" s="0">
         <v>172</v>
       </c>
       <c r="D42" s="2" t="s">
@@ -2483,10 +2499,10 @@
       <c r="A43" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" t="s" s="0">
         <v>179</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C43" t="s" s="0">
         <v>172</v>
       </c>
       <c r="D43" s="2" t="s">
@@ -2500,10 +2516,10 @@
       <c r="A44" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B44" t="s" s="0">
         <v>180</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C44" t="s" s="0">
         <v>172</v>
       </c>
       <c r="D44" s="2" t="s">
@@ -2515,10 +2531,10 @@
       <c r="A45" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B45" t="s" s="0">
         <v>182</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C45" t="s" s="0">
         <v>172</v>
       </c>
       <c r="D45" s="2" t="s">
@@ -2541,13 +2557,13 @@
       <c r="A47" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B47" t="s" s="0">
         <v>194</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C47" t="s" s="0">
         <v>204</v>
       </c>
-      <c r="D47" t="s">
+      <c r="D47" t="s" s="0">
         <v>205</v>
       </c>
     </row>
@@ -2555,13 +2571,13 @@
       <c r="A48" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B48" t="s" s="0">
         <v>195</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C48" t="s" s="0">
         <v>204</v>
       </c>
-      <c r="D48" t="s">
+      <c r="D48" t="s" s="0">
         <v>205</v>
       </c>
     </row>
@@ -2569,13 +2585,13 @@
       <c r="A49" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B49" t="s" s="0">
         <v>196</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C49" t="s" s="0">
         <v>204</v>
       </c>
-      <c r="D49" t="s">
+      <c r="D49" t="s" s="0">
         <v>205</v>
       </c>
     </row>
@@ -2583,13 +2599,13 @@
       <c r="A50" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B50" t="s" s="0">
         <v>197</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C50" t="s" s="0">
         <v>204</v>
       </c>
-      <c r="D50" t="s">
+      <c r="D50" t="s" s="0">
         <v>205</v>
       </c>
     </row>
@@ -2597,13 +2613,13 @@
       <c r="A51" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B51" t="s" s="0">
         <v>198</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C51" t="s" s="0">
         <v>204</v>
       </c>
-      <c r="D51" t="s">
+      <c r="D51" t="s" s="0">
         <v>205</v>
       </c>
     </row>
@@ -2611,13 +2627,13 @@
       <c r="A52" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B52" t="s" s="0">
         <v>199</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C52" t="s" s="0">
         <v>204</v>
       </c>
-      <c r="D52" t="s">
+      <c r="D52" t="s" s="0">
         <v>205</v>
       </c>
     </row>
@@ -2625,16 +2641,16 @@
       <c r="A53" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B53" t="s" s="0">
         <v>200</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C53" t="s" s="0">
         <v>204</v>
       </c>
-      <c r="D53" t="s">
+      <c r="D53" t="s" s="0">
         <v>205</v>
       </c>
-      <c r="E53" t="s">
+      <c r="E53" t="s" s="0">
         <v>386</v>
       </c>
     </row>
@@ -2642,13 +2658,13 @@
       <c r="A54" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B54" t="s" s="0">
         <v>201</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C54" t="s" s="0">
         <v>204</v>
       </c>
-      <c r="D54" t="s">
+      <c r="D54" t="s" s="0">
         <v>205</v>
       </c>
     </row>
@@ -2656,13 +2672,13 @@
       <c r="A55" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B55" t="s" s="0">
         <v>202</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C55" t="s" s="0">
         <v>204</v>
       </c>
-      <c r="D55" t="s">
+      <c r="D55" t="s" s="0">
         <v>205</v>
       </c>
     </row>
@@ -2670,13 +2686,13 @@
       <c r="A56" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B56" t="s" s="0">
         <v>203</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C56" t="s" s="0">
         <v>204</v>
       </c>
-      <c r="D56" t="s">
+      <c r="D56" t="s" s="0">
         <v>205</v>
       </c>
     </row>
@@ -2695,16 +2711,16 @@
       <c r="A58" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B58" t="s" s="0">
         <v>217</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C58" t="s" s="0">
         <v>227</v>
       </c>
-      <c r="D58" t="s">
+      <c r="D58" t="s" s="0">
         <v>206</v>
       </c>
-      <c r="F58" t="s">
+      <c r="F58" t="s" s="0">
         <v>364</v>
       </c>
     </row>
@@ -2712,13 +2728,13 @@
       <c r="A59" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B59" t="s" s="0">
         <v>218</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C59" t="s" s="0">
         <v>227</v>
       </c>
-      <c r="D59" t="s">
+      <c r="D59" t="s" s="0">
         <v>206</v>
       </c>
     </row>
@@ -2726,13 +2742,13 @@
       <c r="A60" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B60" t="s" s="0">
         <v>219</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C60" t="s" s="0">
         <v>227</v>
       </c>
-      <c r="D60" t="s">
+      <c r="D60" t="s" s="0">
         <v>206</v>
       </c>
     </row>
@@ -2740,13 +2756,13 @@
       <c r="A61" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B61" t="s" s="0">
         <v>220</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C61" t="s" s="0">
         <v>227</v>
       </c>
-      <c r="D61" t="s">
+      <c r="D61" t="s" s="0">
         <v>206</v>
       </c>
     </row>
@@ -2754,13 +2770,13 @@
       <c r="A62" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B62" t="s" s="0">
         <v>221</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C62" t="s" s="0">
         <v>227</v>
       </c>
-      <c r="D62" t="s">
+      <c r="D62" t="s" s="0">
         <v>206</v>
       </c>
     </row>
@@ -2768,16 +2784,16 @@
       <c r="A63" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B63" t="s" s="0">
         <v>222</v>
       </c>
-      <c r="C63" t="s">
+      <c r="C63" t="s" s="0">
         <v>227</v>
       </c>
-      <c r="D63" t="s">
+      <c r="D63" t="s" s="0">
         <v>206</v>
       </c>
-      <c r="E63" t="s">
+      <c r="E63" t="s" s="0">
         <v>386</v>
       </c>
     </row>
@@ -2785,13 +2801,13 @@
       <c r="A64" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B64" t="s" s="0">
         <v>223</v>
       </c>
-      <c r="C64" t="s">
+      <c r="C64" t="s" s="0">
         <v>227</v>
       </c>
-      <c r="D64" t="s">
+      <c r="D64" t="s" s="0">
         <v>206</v>
       </c>
     </row>
@@ -2799,13 +2815,13 @@
       <c r="A65" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B65" t="s" s="0">
         <v>224</v>
       </c>
-      <c r="C65" t="s">
+      <c r="C65" t="s" s="0">
         <v>227</v>
       </c>
-      <c r="D65" t="s">
+      <c r="D65" t="s" s="0">
         <v>206</v>
       </c>
     </row>
@@ -2813,13 +2829,13 @@
       <c r="A66" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B66" t="s" s="0">
         <v>225</v>
       </c>
-      <c r="C66" t="s">
+      <c r="C66" t="s" s="0">
         <v>227</v>
       </c>
-      <c r="D66" t="s">
+      <c r="D66" t="s" s="0">
         <v>206</v>
       </c>
     </row>
@@ -2827,13 +2843,13 @@
       <c r="A67" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B67" t="s" s="0">
         <v>226</v>
       </c>
-      <c r="C67" t="s">
+      <c r="C67" t="s" s="0">
         <v>227</v>
       </c>
-      <c r="D67" t="s">
+      <c r="D67" t="s" s="0">
         <v>206</v>
       </c>
     </row>
@@ -2855,10 +2871,10 @@
       <c r="B69" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="C69" t="s">
+      <c r="C69" t="s" s="0">
         <v>239</v>
       </c>
-      <c r="D69" t="s">
+      <c r="D69" t="s" s="0">
         <v>240</v>
       </c>
     </row>
@@ -2869,10 +2885,10 @@
       <c r="B70" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="C70" t="s">
+      <c r="C70" t="s" s="0">
         <v>239</v>
       </c>
-      <c r="D70" t="s">
+      <c r="D70" t="s" s="0">
         <v>240</v>
       </c>
     </row>
@@ -2883,10 +2899,10 @@
       <c r="B71" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="C71" t="s">
+      <c r="C71" t="s" s="0">
         <v>239</v>
       </c>
-      <c r="D71" t="s">
+      <c r="D71" t="s" s="0">
         <v>240</v>
       </c>
     </row>
@@ -2897,13 +2913,13 @@
       <c r="B72" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="C72" t="s">
+      <c r="C72" t="s" s="0">
         <v>239</v>
       </c>
-      <c r="D72" t="s">
+      <c r="D72" t="s" s="0">
         <v>240</v>
       </c>
-      <c r="E72" t="s">
+      <c r="E72" t="s" s="0">
         <v>386</v>
       </c>
     </row>
@@ -2914,10 +2930,10 @@
       <c r="B73" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="C73" t="s">
+      <c r="C73" t="s" s="0">
         <v>239</v>
       </c>
-      <c r="D73" t="s">
+      <c r="D73" t="s" s="0">
         <v>240</v>
       </c>
     </row>
@@ -2928,10 +2944,10 @@
       <c r="B74" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="C74" t="s">
+      <c r="C74" t="s" s="0">
         <v>239</v>
       </c>
-      <c r="D74" t="s">
+      <c r="D74" t="s" s="0">
         <v>240</v>
       </c>
     </row>
@@ -2942,10 +2958,10 @@
       <c r="B75" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="C75" t="s">
+      <c r="C75" t="s" s="0">
         <v>239</v>
       </c>
-      <c r="D75" t="s">
+      <c r="D75" t="s" s="0">
         <v>240</v>
       </c>
     </row>
@@ -2956,10 +2972,10 @@
       <c r="B76" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="C76" t="s">
+      <c r="C76" t="s" s="0">
         <v>239</v>
       </c>
-      <c r="D76" t="s">
+      <c r="D76" t="s" s="0">
         <v>240</v>
       </c>
     </row>
@@ -2970,10 +2986,10 @@
       <c r="B77" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="C77" t="s">
+      <c r="C77" t="s" s="0">
         <v>239</v>
       </c>
-      <c r="D77" t="s">
+      <c r="D77" t="s" s="0">
         <v>240</v>
       </c>
     </row>
@@ -2984,10 +3000,10 @@
       <c r="B78" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="C78" t="s">
+      <c r="C78" t="s" s="0">
         <v>239</v>
       </c>
-      <c r="D78" t="s">
+      <c r="D78" t="s" s="0">
         <v>240</v>
       </c>
     </row>
@@ -3006,13 +3022,13 @@
       <c r="A80" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="B80" t="s">
+      <c r="B80" t="s" s="0">
         <v>271</v>
       </c>
-      <c r="C80" t="s">
+      <c r="C80" t="s" s="0">
         <v>259</v>
       </c>
-      <c r="D80" t="s">
+      <c r="D80" t="s" s="0">
         <v>64</v>
       </c>
     </row>
@@ -3020,13 +3036,13 @@
       <c r="A81" s="2" t="s">
         <v>262</v>
       </c>
-      <c r="B81" t="s">
+      <c r="B81" t="s" s="0">
         <v>272</v>
       </c>
-      <c r="C81" t="s">
+      <c r="C81" t="s" s="0">
         <v>259</v>
       </c>
-      <c r="D81" t="s">
+      <c r="D81" t="s" s="0">
         <v>64</v>
       </c>
     </row>
@@ -3034,16 +3050,16 @@
       <c r="A82" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="B82" t="s">
+      <c r="B82" t="s" s="0">
         <v>273</v>
       </c>
-      <c r="C82" t="s">
+      <c r="C82" t="s" s="0">
         <v>259</v>
       </c>
-      <c r="D82" t="s">
+      <c r="D82" t="s" s="0">
         <v>64</v>
       </c>
-      <c r="E82" t="s">
+      <c r="E82" t="s" s="0">
         <v>386</v>
       </c>
     </row>
@@ -3051,13 +3067,13 @@
       <c r="A83" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="B83" t="s">
+      <c r="B83" t="s" s="0">
         <v>274</v>
       </c>
-      <c r="C83" t="s">
+      <c r="C83" t="s" s="0">
         <v>259</v>
       </c>
-      <c r="D83" t="s">
+      <c r="D83" t="s" s="0">
         <v>64</v>
       </c>
     </row>
@@ -3065,13 +3081,13 @@
       <c r="A84" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="B84" t="s">
+      <c r="B84" t="s" s="0">
         <v>275</v>
       </c>
-      <c r="C84" t="s">
+      <c r="C84" t="s" s="0">
         <v>259</v>
       </c>
-      <c r="D84" t="s">
+      <c r="D84" t="s" s="0">
         <v>64</v>
       </c>
     </row>
@@ -3079,13 +3095,13 @@
       <c r="A85" s="2" t="s">
         <v>266</v>
       </c>
-      <c r="B85" t="s">
+      <c r="B85" t="s" s="0">
         <v>276</v>
       </c>
-      <c r="C85" t="s">
+      <c r="C85" t="s" s="0">
         <v>259</v>
       </c>
-      <c r="D85" t="s">
+      <c r="D85" t="s" s="0">
         <v>64</v>
       </c>
     </row>
@@ -3093,13 +3109,13 @@
       <c r="A86" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="B86" t="s">
+      <c r="B86" t="s" s="0">
         <v>277</v>
       </c>
-      <c r="C86" t="s">
+      <c r="C86" t="s" s="0">
         <v>259</v>
       </c>
-      <c r="D86" t="s">
+      <c r="D86" t="s" s="0">
         <v>64</v>
       </c>
     </row>
@@ -3107,16 +3123,16 @@
       <c r="A87" s="2" t="s">
         <v>268</v>
       </c>
-      <c r="B87" t="s">
+      <c r="B87" t="s" s="0">
         <v>278</v>
       </c>
-      <c r="C87" t="s">
+      <c r="C87" t="s" s="0">
         <v>259</v>
       </c>
-      <c r="D87" t="s">
+      <c r="D87" t="s" s="0">
         <v>64</v>
       </c>
-      <c r="F87" t="s">
+      <c r="F87" t="s" s="0">
         <v>364</v>
       </c>
     </row>
@@ -3124,13 +3140,13 @@
       <c r="A88" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="B88" t="s">
+      <c r="B88" t="s" s="0">
         <v>279</v>
       </c>
-      <c r="C88" t="s">
+      <c r="C88" t="s" s="0">
         <v>259</v>
       </c>
-      <c r="D88" t="s">
+      <c r="D88" t="s" s="0">
         <v>64</v>
       </c>
     </row>
@@ -3138,13 +3154,13 @@
       <c r="A89" s="2" t="s">
         <v>270</v>
       </c>
-      <c r="B89" t="s">
+      <c r="B89" t="s" s="0">
         <v>280</v>
       </c>
-      <c r="C89" t="s">
+      <c r="C89" t="s" s="0">
         <v>259</v>
       </c>
-      <c r="D89" t="s">
+      <c r="D89" t="s" s="0">
         <v>64</v>
       </c>
     </row>
@@ -3166,10 +3182,10 @@
       <c r="B91" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="C91" t="s">
+      <c r="C91" t="s" s="0">
         <v>292</v>
       </c>
-      <c r="D91" t="s">
+      <c r="D91" t="s" s="0">
         <v>66</v>
       </c>
     </row>
@@ -3180,10 +3196,10 @@
       <c r="B92" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="C92" t="s">
+      <c r="C92" t="s" s="0">
         <v>292</v>
       </c>
-      <c r="D92" t="s">
+      <c r="D92" t="s" s="0">
         <v>66</v>
       </c>
     </row>
@@ -3194,10 +3210,10 @@
       <c r="B93" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="C93" t="s">
+      <c r="C93" t="s" s="0">
         <v>292</v>
       </c>
-      <c r="D93" t="s">
+      <c r="D93" t="s" s="0">
         <v>66</v>
       </c>
     </row>
@@ -3208,10 +3224,10 @@
       <c r="B94" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="C94" t="s">
+      <c r="C94" t="s" s="0">
         <v>292</v>
       </c>
-      <c r="D94" t="s">
+      <c r="D94" t="s" s="0">
         <v>66</v>
       </c>
     </row>
@@ -3222,10 +3238,10 @@
       <c r="B95" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="C95" t="s">
+      <c r="C95" t="s" s="0">
         <v>292</v>
       </c>
-      <c r="D95" t="s">
+      <c r="D95" t="s" s="0">
         <v>66</v>
       </c>
     </row>
@@ -3236,13 +3252,13 @@
       <c r="B96" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="C96" t="s">
+      <c r="C96" t="s" s="0">
         <v>292</v>
       </c>
-      <c r="D96" t="s">
+      <c r="D96" t="s" s="0">
         <v>66</v>
       </c>
-      <c r="E96" t="s">
+      <c r="E96" t="s" s="0">
         <v>386</v>
       </c>
     </row>
@@ -3253,10 +3269,10 @@
       <c r="B97" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="C97" t="s">
+      <c r="C97" t="s" s="0">
         <v>292</v>
       </c>
-      <c r="D97" t="s">
+      <c r="D97" t="s" s="0">
         <v>66</v>
       </c>
     </row>
@@ -3267,10 +3283,10 @@
       <c r="B98" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="C98" t="s">
+      <c r="C98" t="s" s="0">
         <v>292</v>
       </c>
-      <c r="D98" t="s">
+      <c r="D98" t="s" s="0">
         <v>66</v>
       </c>
     </row>
@@ -3281,10 +3297,10 @@
       <c r="B99" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="C99" t="s">
+      <c r="C99" t="s" s="0">
         <v>292</v>
       </c>
-      <c r="D99" t="s">
+      <c r="D99" t="s" s="0">
         <v>66</v>
       </c>
     </row>
@@ -3295,10 +3311,10 @@
       <c r="B100" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="C100" t="s">
+      <c r="C100" t="s" s="0">
         <v>292</v>
       </c>
-      <c r="D100" t="s">
+      <c r="D100" t="s" s="0">
         <v>66</v>
       </c>
     </row>
@@ -3320,13 +3336,13 @@
       <c r="B102" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="C102" t="s">
+      <c r="C102" t="s" s="0">
         <v>303</v>
       </c>
-      <c r="D102" t="s">
+      <c r="D102" t="s" s="0">
         <v>91</v>
       </c>
-      <c r="F102" t="s">
+      <c r="F102" t="s" s="0">
         <v>364</v>
       </c>
     </row>
@@ -3337,10 +3353,10 @@
       <c r="B103" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="C103" t="s">
+      <c r="C103" t="s" s="0">
         <v>303</v>
       </c>
-      <c r="D103" t="s">
+      <c r="D103" t="s" s="0">
         <v>91</v>
       </c>
     </row>
@@ -3351,10 +3367,10 @@
       <c r="B104" s="2" t="s">
         <v>305</v>
       </c>
-      <c r="C104" t="s">
+      <c r="C104" t="s" s="0">
         <v>303</v>
       </c>
-      <c r="D104" t="s">
+      <c r="D104" t="s" s="0">
         <v>91</v>
       </c>
     </row>
@@ -3365,10 +3381,10 @@
       <c r="B105" s="2" t="s">
         <v>306</v>
       </c>
-      <c r="C105" t="s">
+      <c r="C105" t="s" s="0">
         <v>303</v>
       </c>
-      <c r="D105" t="s">
+      <c r="D105" t="s" s="0">
         <v>91</v>
       </c>
     </row>
@@ -3379,10 +3395,10 @@
       <c r="B106" s="2" t="s">
         <v>307</v>
       </c>
-      <c r="C106" t="s">
+      <c r="C106" t="s" s="0">
         <v>303</v>
       </c>
-      <c r="D106" t="s">
+      <c r="D106" t="s" s="0">
         <v>91</v>
       </c>
     </row>
@@ -3393,10 +3409,10 @@
       <c r="B107" s="2" t="s">
         <v>308</v>
       </c>
-      <c r="C107" t="s">
+      <c r="C107" t="s" s="0">
         <v>303</v>
       </c>
-      <c r="D107" t="s">
+      <c r="D107" t="s" s="0">
         <v>91</v>
       </c>
     </row>
@@ -3407,13 +3423,13 @@
       <c r="B108" s="2" t="s">
         <v>309</v>
       </c>
-      <c r="C108" t="s">
+      <c r="C108" t="s" s="0">
         <v>303</v>
       </c>
-      <c r="D108" t="s">
+      <c r="D108" t="s" s="0">
         <v>91</v>
       </c>
-      <c r="E108" t="s">
+      <c r="E108" t="s" s="0">
         <v>386</v>
       </c>
     </row>
@@ -3424,10 +3440,10 @@
       <c r="B109" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="C109" t="s">
+      <c r="C109" t="s" s="0">
         <v>303</v>
       </c>
-      <c r="D109" t="s">
+      <c r="D109" t="s" s="0">
         <v>91</v>
       </c>
     </row>
@@ -3438,10 +3454,10 @@
       <c r="B110" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="C110" t="s">
+      <c r="C110" t="s" s="0">
         <v>303</v>
       </c>
-      <c r="D110" t="s">
+      <c r="D110" t="s" s="0">
         <v>91</v>
       </c>
     </row>
@@ -3452,10 +3468,10 @@
       <c r="B111" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="C111" t="s">
+      <c r="C111" t="s" s="0">
         <v>303</v>
       </c>
-      <c r="D111" t="s">
+      <c r="D111" t="s" s="0">
         <v>91</v>
       </c>
     </row>
@@ -3474,13 +3490,13 @@
       <c r="A113" s="2" t="s">
         <v>337</v>
       </c>
-      <c r="B113" t="s">
+      <c r="B113" t="s" s="0">
         <v>326</v>
       </c>
-      <c r="C113" t="s">
+      <c r="C113" t="s" s="0">
         <v>325</v>
       </c>
-      <c r="D113" t="s">
+      <c r="D113" t="s" s="0">
         <v>72</v>
       </c>
     </row>
@@ -3488,13 +3504,13 @@
       <c r="A114" s="2" t="s">
         <v>338</v>
       </c>
-      <c r="B114" t="s">
+      <c r="B114" t="s" s="0">
         <v>334</v>
       </c>
-      <c r="C114" t="s">
+      <c r="C114" t="s" s="0">
         <v>325</v>
       </c>
-      <c r="D114" t="s">
+      <c r="D114" t="s" s="0">
         <v>72</v>
       </c>
     </row>
@@ -3502,13 +3518,13 @@
       <c r="A115" s="2" t="s">
         <v>339</v>
       </c>
-      <c r="B115" t="s">
+      <c r="B115" t="s" s="0">
         <v>327</v>
       </c>
-      <c r="C115" t="s">
+      <c r="C115" t="s" s="0">
         <v>325</v>
       </c>
-      <c r="D115" t="s">
+      <c r="D115" t="s" s="0">
         <v>72</v>
       </c>
     </row>
@@ -3516,16 +3532,16 @@
       <c r="A116" s="2" t="s">
         <v>340</v>
       </c>
-      <c r="B116" t="s">
+      <c r="B116" t="s" s="0">
         <v>328</v>
       </c>
-      <c r="C116" t="s">
+      <c r="C116" t="s" s="0">
         <v>325</v>
       </c>
-      <c r="D116" t="s">
+      <c r="D116" t="s" s="0">
         <v>72</v>
       </c>
-      <c r="E116" t="s">
+      <c r="E116" t="s" s="0">
         <v>386</v>
       </c>
     </row>
@@ -3533,13 +3549,13 @@
       <c r="A117" s="2" t="s">
         <v>341</v>
       </c>
-      <c r="B117" t="s">
+      <c r="B117" t="s" s="0">
         <v>329</v>
       </c>
-      <c r="C117" t="s">
+      <c r="C117" t="s" s="0">
         <v>325</v>
       </c>
-      <c r="D117" t="s">
+      <c r="D117" t="s" s="0">
         <v>72</v>
       </c>
     </row>
@@ -3547,13 +3563,13 @@
       <c r="A118" s="2" t="s">
         <v>342</v>
       </c>
-      <c r="B118" t="s">
+      <c r="B118" t="s" s="0">
         <v>330</v>
       </c>
-      <c r="C118" t="s">
+      <c r="C118" t="s" s="0">
         <v>325</v>
       </c>
-      <c r="D118" t="s">
+      <c r="D118" t="s" s="0">
         <v>72</v>
       </c>
     </row>
@@ -3561,13 +3577,13 @@
       <c r="A119" s="2" t="s">
         <v>343</v>
       </c>
-      <c r="B119" t="s">
+      <c r="B119" t="s" s="0">
         <v>331</v>
       </c>
-      <c r="C119" t="s">
+      <c r="C119" t="s" s="0">
         <v>325</v>
       </c>
-      <c r="D119" t="s">
+      <c r="D119" t="s" s="0">
         <v>72</v>
       </c>
     </row>
@@ -3575,13 +3591,13 @@
       <c r="A120" s="2" t="s">
         <v>344</v>
       </c>
-      <c r="B120" t="s">
+      <c r="B120" t="s" s="0">
         <v>332</v>
       </c>
-      <c r="C120" t="s">
+      <c r="C120" t="s" s="0">
         <v>325</v>
       </c>
-      <c r="D120" t="s">
+      <c r="D120" t="s" s="0">
         <v>72</v>
       </c>
     </row>
@@ -3589,13 +3605,13 @@
       <c r="A121" s="2" t="s">
         <v>345</v>
       </c>
-      <c r="B121" t="s">
+      <c r="B121" t="s" s="0">
         <v>333</v>
       </c>
-      <c r="C121" t="s">
+      <c r="C121" t="s" s="0">
         <v>325</v>
       </c>
-      <c r="D121" t="s">
+      <c r="D121" t="s" s="0">
         <v>72</v>
       </c>
     </row>
@@ -3603,13 +3619,13 @@
       <c r="A122" s="2" t="s">
         <v>346</v>
       </c>
-      <c r="B122" t="s">
+      <c r="B122" t="s" s="0">
         <v>335</v>
       </c>
-      <c r="C122" t="s">
+      <c r="C122" t="s" s="0">
         <v>325</v>
       </c>
-      <c r="D122" t="s">
+      <c r="D122" t="s" s="0">
         <v>72</v>
       </c>
     </row>
@@ -3630,21 +3646,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.28515625" customWidth="1"/>
-    <col min="3" max="3" width="27.42578125" customWidth="1"/>
-    <col min="4" max="4" width="25.85546875" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" customWidth="1"/>
-    <col min="7" max="7" width="15" customWidth="1"/>
-    <col min="8" max="8" width="16.5703125" customWidth="1"/>
-    <col min="9" max="9" width="17.85546875" customWidth="1"/>
-    <col min="10" max="10" width="19.28515625" customWidth="1"/>
-    <col min="11" max="11" width="17.85546875" customWidth="1"/>
-    <col min="12" max="12" width="16.85546875" customWidth="1"/>
-    <col min="13" max="13" width="17" customWidth="1"/>
-    <col min="14" max="14" width="15.140625" customWidth="1"/>
-    <col min="15" max="15" width="17.7109375" customWidth="1"/>
-    <col min="16" max="16" width="15.5703125" customWidth="1"/>
+    <col min="2" max="2" customWidth="true" width="12.28515625"/>
+    <col min="3" max="3" customWidth="true" width="27.42578125"/>
+    <col min="4" max="4" customWidth="true" width="25.85546875"/>
+    <col min="5" max="5" customWidth="true" width="10.7109375"/>
+    <col min="6" max="6" customWidth="true" width="11.85546875"/>
+    <col min="7" max="7" customWidth="true" width="15.0"/>
+    <col min="8" max="8" customWidth="true" width="16.5703125"/>
+    <col min="9" max="9" customWidth="true" width="17.85546875"/>
+    <col min="10" max="10" customWidth="true" width="19.28515625"/>
+    <col min="11" max="11" customWidth="true" width="17.85546875"/>
+    <col min="12" max="12" customWidth="true" width="16.85546875"/>
+    <col min="13" max="13" customWidth="true" width="17.0"/>
+    <col min="14" max="14" customWidth="true" width="15.140625"/>
+    <col min="15" max="15" customWidth="true" width="17.7109375"/>
+    <col min="16" max="16" customWidth="true" width="15.5703125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="17" customFormat="1" x14ac:dyDescent="0.25">
@@ -3701,37 +3717,37 @@
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>217</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>15</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="0">
         <v>16</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" t="s" s="0">
         <v>17</v>
       </c>
-      <c r="F2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="F2" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="G2" t="s" s="0">
         <v>375</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" t="s" s="0">
         <v>376</v>
       </c>
       <c r="I2" s="18" t="s">
         <v>380</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" t="s" s="0">
         <v>377</v>
       </c>
       <c r="K2" s="18" t="s">
         <v>379</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L2" t="s" s="0">
         <v>378</v>
       </c>
       <c r="M2" s="18" t="s">
@@ -3742,37 +3758,37 @@
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>218</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>15</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" t="s" s="0">
         <v>16</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" t="s" s="0">
         <v>17</v>
       </c>
-      <c r="F3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" t="s">
+      <c r="F3" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="G3" t="s" s="0">
         <v>98</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" t="s" s="0">
         <v>377</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>423</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" t="s" s="0">
         <v>376</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>432</v>
       </c>
-      <c r="L3" t="s">
+      <c r="L3" t="s" s="0">
         <v>377</v>
       </c>
       <c r="M3" s="2" t="s">
@@ -3783,37 +3799,37 @@
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>219</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" t="s" s="0">
         <v>15</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" t="s" s="0">
         <v>16</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" t="s" s="0">
         <v>17</v>
       </c>
-      <c r="F4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G4" t="s">
+      <c r="F4" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="G4" t="s" s="0">
         <v>415</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" t="s" s="0">
         <v>378</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>424</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" t="s" s="0">
         <v>378</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>423</v>
       </c>
-      <c r="L4" t="s">
+      <c r="L4" t="s" s="0">
         <v>376</v>
       </c>
       <c r="M4" s="2" t="s">
@@ -3824,37 +3840,37 @@
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" t="s" s="0">
         <v>220</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" t="s" s="0">
         <v>15</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" t="s" s="0">
         <v>16</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" t="s" s="0">
         <v>17</v>
       </c>
-      <c r="F5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G5" t="s">
+      <c r="F5" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="G5" t="s" s="0">
         <v>416</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" t="s" s="0">
         <v>378</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>425</v>
       </c>
-      <c r="J5" t="s">
+      <c r="J5" t="s" s="0">
         <v>378</v>
       </c>
       <c r="K5" s="2" t="s">
         <v>433</v>
       </c>
-      <c r="L5" t="s">
+      <c r="L5" t="s" s="0">
         <v>376</v>
       </c>
       <c r="M5" s="2" t="s">
@@ -3865,37 +3881,37 @@
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" t="s" s="0">
         <v>221</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" t="s" s="0">
         <v>15</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" t="s" s="0">
         <v>16</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" t="s" s="0">
         <v>17</v>
       </c>
-      <c r="F6" t="s">
-        <v>18</v>
-      </c>
-      <c r="G6" t="s">
+      <c r="F6" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="G6" t="s" s="0">
         <v>417</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" t="s" s="0">
         <v>377</v>
       </c>
       <c r="I6" s="2" t="s">
         <v>426</v>
       </c>
-      <c r="J6" t="s">
+      <c r="J6" t="s" s="0">
         <v>377</v>
       </c>
       <c r="K6" s="2" t="s">
         <v>434</v>
       </c>
-      <c r="L6" t="s">
+      <c r="L6" t="s" s="0">
         <v>376</v>
       </c>
       <c r="M6" s="2" t="s">
@@ -3906,37 +3922,37 @@
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" t="s" s="0">
         <v>222</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" t="s" s="0">
         <v>15</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" t="s" s="0">
         <v>16</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" t="s" s="0">
         <v>17</v>
       </c>
-      <c r="F7" t="s">
-        <v>18</v>
-      </c>
-      <c r="G7" t="s">
+      <c r="F7" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="G7" t="s" s="0">
         <v>418</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H7" t="s" s="0">
         <v>376</v>
       </c>
       <c r="I7" s="2" t="s">
         <v>427</v>
       </c>
-      <c r="J7" t="s">
+      <c r="J7" t="s" s="0">
         <v>376</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>435</v>
       </c>
-      <c r="L7" t="s">
+      <c r="L7" t="s" s="0">
         <v>377</v>
       </c>
       <c r="M7" s="2" t="s">
@@ -3947,37 +3963,37 @@
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" t="s" s="0">
         <v>223</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" t="s" s="0">
         <v>15</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" t="s" s="0">
         <v>16</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" t="s" s="0">
         <v>17</v>
       </c>
-      <c r="F8" t="s">
-        <v>18</v>
-      </c>
-      <c r="G8" t="s">
+      <c r="F8" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="G8" t="s" s="0">
         <v>419</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H8" t="s" s="0">
         <v>376</v>
       </c>
       <c r="I8" s="2" t="s">
         <v>428</v>
       </c>
-      <c r="J8" t="s">
+      <c r="J8" t="s" s="0">
         <v>377</v>
       </c>
       <c r="K8" s="2" t="s">
         <v>436</v>
       </c>
-      <c r="L8" t="s">
+      <c r="L8" t="s" s="0">
         <v>378</v>
       </c>
       <c r="M8" s="2" t="s">
@@ -3988,37 +4004,37 @@
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" t="s" s="0">
         <v>224</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" t="s" s="0">
         <v>15</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" t="s" s="0">
         <v>16</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" t="s" s="0">
         <v>17</v>
       </c>
-      <c r="F9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G9" t="s">
+      <c r="F9" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="G9" t="s" s="0">
         <v>420</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H9" t="s" s="0">
         <v>377</v>
       </c>
       <c r="I9" s="2" t="s">
         <v>429</v>
       </c>
-      <c r="J9" t="s">
+      <c r="J9" t="s" s="0">
         <v>378</v>
       </c>
       <c r="K9" s="2" t="s">
         <v>437</v>
       </c>
-      <c r="L9" t="s">
+      <c r="L9" t="s" s="0">
         <v>378</v>
       </c>
       <c r="M9" s="2" t="s">
@@ -4029,37 +4045,37 @@
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" t="s" s="0">
         <v>225</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" t="s" s="0">
         <v>15</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" t="s" s="0">
         <v>16</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" t="s" s="0">
         <v>17</v>
       </c>
-      <c r="F10" t="s">
-        <v>18</v>
-      </c>
-      <c r="G10" t="s">
+      <c r="F10" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="G10" t="s" s="0">
         <v>421</v>
       </c>
-      <c r="H10" t="s">
+      <c r="H10" t="s" s="0">
         <v>378</v>
       </c>
       <c r="I10" s="2" t="s">
         <v>430</v>
       </c>
-      <c r="J10" t="s">
+      <c r="J10" t="s" s="0">
         <v>377</v>
       </c>
       <c r="K10" s="2" t="s">
         <v>438</v>
       </c>
-      <c r="L10" t="s">
+      <c r="L10" t="s" s="0">
         <v>376</v>
       </c>
       <c r="M10" s="2" t="s">
@@ -4070,37 +4086,37 @@
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" t="s" s="0">
         <v>226</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" t="s" s="0">
         <v>15</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" t="s" s="0">
         <v>16</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" t="s" s="0">
         <v>17</v>
       </c>
-      <c r="F11" t="s">
-        <v>18</v>
-      </c>
-      <c r="G11" t="s">
+      <c r="F11" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="G11" t="s" s="0">
         <v>422</v>
       </c>
-      <c r="H11" t="s">
+      <c r="H11" t="s" s="0">
         <v>378</v>
       </c>
       <c r="I11" s="2" t="s">
         <v>431</v>
       </c>
-      <c r="J11" t="s">
+      <c r="J11" t="s" s="0">
         <v>376</v>
       </c>
       <c r="K11" s="2" t="s">
         <v>439</v>
       </c>
-      <c r="L11" t="s">
+      <c r="L11" t="s" s="0">
         <v>376</v>
       </c>
       <c r="M11" s="2" t="s">
@@ -4122,16 +4138,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.42578125" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="40.28515625" customWidth="1"/>
-    <col min="5" max="5" width="22.7109375" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" customWidth="1"/>
-    <col min="7" max="7" width="21.42578125" customWidth="1"/>
-    <col min="8" max="8" width="21.28515625" customWidth="1"/>
-    <col min="9" max="9" width="18.28515625" customWidth="1"/>
-    <col min="10" max="10" width="9.28515625" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="6.42578125"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.7109375"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="34.5703125"/>
+    <col min="4" max="4" customWidth="true" width="40.28515625"/>
+    <col min="5" max="5" customWidth="true" width="22.7109375"/>
+    <col min="6" max="6" customWidth="true" width="12.42578125"/>
+    <col min="7" max="7" customWidth="true" width="21.42578125"/>
+    <col min="8" max="8" customWidth="true" width="21.28515625"/>
+    <col min="9" max="9" customWidth="true" width="18.28515625"/>
+    <col min="10" max="10" customWidth="true" width="9.28515625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -4171,10 +4187,10 @@
       <c r="B2" s="2" t="s">
         <v>326</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>325</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="0">
         <v>72</v>
       </c>
       <c r="E2" s="3" t="s">
@@ -4183,7 +4199,7 @@
       <c r="F2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" t="s" s="0">
         <v>74</v>
       </c>
       <c r="H2" s="2" t="s">
@@ -4199,10 +4215,10 @@
       <c r="B3" s="2" t="s">
         <v>334</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>325</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" t="s" s="0">
         <v>72</v>
       </c>
       <c r="E3" s="3" t="s">
@@ -4211,7 +4227,7 @@
       <c r="F3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" t="s" s="0">
         <v>74</v>
       </c>
       <c r="H3" s="2"/>
@@ -4225,10 +4241,10 @@
       <c r="B4" s="2" t="s">
         <v>327</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" t="s" s="0">
         <v>325</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" t="s" s="0">
         <v>72</v>
       </c>
       <c r="E4" s="3" t="s">
@@ -4237,7 +4253,7 @@
       <c r="F4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" t="s" s="0">
         <v>74</v>
       </c>
       <c r="H4" s="2"/>
@@ -4251,10 +4267,10 @@
       <c r="B5" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" t="s" s="0">
         <v>325</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" t="s" s="0">
         <v>72</v>
       </c>
       <c r="E5" s="3" t="s">
@@ -4263,7 +4279,7 @@
       <c r="F5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" t="s" s="0">
         <v>74</v>
       </c>
       <c r="H5" s="2"/>
@@ -4277,10 +4293,10 @@
       <c r="B6" s="2" t="s">
         <v>329</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" t="s" s="0">
         <v>325</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" t="s" s="0">
         <v>72</v>
       </c>
       <c r="E6" s="3" t="s">
@@ -4289,7 +4305,7 @@
       <c r="F6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" t="s" s="0">
         <v>74</v>
       </c>
       <c r="H6" s="2"/>
@@ -4303,10 +4319,10 @@
       <c r="B7" s="2" t="s">
         <v>330</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" t="s" s="0">
         <v>325</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" t="s" s="0">
         <v>72</v>
       </c>
       <c r="E7" s="3" t="s">
@@ -4315,7 +4331,7 @@
       <c r="F7" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" t="s" s="0">
         <v>74</v>
       </c>
       <c r="H7" s="2"/>
@@ -4329,10 +4345,10 @@
       <c r="B8" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" t="s" s="0">
         <v>325</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" t="s" s="0">
         <v>72</v>
       </c>
       <c r="E8" s="3" t="s">
@@ -4341,7 +4357,7 @@
       <c r="F8" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8" t="s" s="0">
         <v>74</v>
       </c>
       <c r="H8" s="2"/>
@@ -4355,10 +4371,10 @@
       <c r="B9" s="2" t="s">
         <v>332</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" t="s" s="0">
         <v>325</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" t="s" s="0">
         <v>72</v>
       </c>
       <c r="E9" s="3" t="s">
@@ -4367,7 +4383,7 @@
       <c r="F9" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G9" t="s" s="0">
         <v>74</v>
       </c>
       <c r="H9" s="2"/>
@@ -4381,10 +4397,10 @@
       <c r="B10" s="2" t="s">
         <v>333</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" t="s" s="0">
         <v>325</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" t="s" s="0">
         <v>72</v>
       </c>
       <c r="E10" s="3" t="s">
@@ -4393,7 +4409,7 @@
       <c r="F10" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G10" t="s" s="0">
         <v>74</v>
       </c>
       <c r="H10" s="2"/>
@@ -4407,10 +4423,10 @@
       <c r="B11" s="2" t="s">
         <v>335</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" t="s" s="0">
         <v>325</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" t="s" s="0">
         <v>72</v>
       </c>
       <c r="E11" s="3" t="s">
@@ -4419,7 +4435,7 @@
       <c r="F11" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G11" t="s" s="0">
         <v>74</v>
       </c>
       <c r="H11" s="2"/>
@@ -4457,11 +4473,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26" customWidth="1"/>
-    <col min="4" max="4" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.7109375"/>
+    <col min="3" max="3" customWidth="true" width="26.0"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="24.42578125"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="10.7109375"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="11.28515625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -4488,16 +4504,16 @@
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>104</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>15</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="0">
         <v>16</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" t="s" s="0">
         <v>17</v>
       </c>
       <c r="F2" s="3" t="s">
@@ -4508,16 +4524,16 @@
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>105</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>15</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" t="s" s="0">
         <v>16</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" t="s" s="0">
         <v>19</v>
       </c>
       <c r="F3" s="3" t="s">
@@ -4528,16 +4544,16 @@
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>106</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" t="s" s="0">
         <v>15</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" t="s" s="0">
         <v>16</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" t="s" s="0">
         <v>20</v>
       </c>
       <c r="F4" s="3" t="s">
@@ -4548,16 +4564,16 @@
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" t="s" s="0">
         <v>107</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" t="s" s="0">
         <v>15</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" t="s" s="0">
         <v>16</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" t="s" s="0">
         <v>21</v>
       </c>
       <c r="F5" s="3" t="s">
@@ -4568,16 +4584,16 @@
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" t="s" s="0">
         <v>108</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" t="s" s="0">
         <v>15</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" t="s" s="0">
         <v>16</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" t="s" s="0">
         <v>22</v>
       </c>
       <c r="F6" s="3" t="s">
@@ -4588,16 +4604,16 @@
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" t="s" s="0">
         <v>109</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" t="s" s="0">
         <v>15</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" t="s" s="0">
         <v>16</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" t="s" s="0">
         <v>23</v>
       </c>
       <c r="F7" s="3" t="s">
@@ -4608,16 +4624,16 @@
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" t="s" s="0">
         <v>110</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" t="s" s="0">
         <v>15</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" t="s" s="0">
         <v>16</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" t="s" s="0">
         <v>24</v>
       </c>
       <c r="F8" s="3" t="s">
@@ -4628,16 +4644,16 @@
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" t="s" s="0">
         <v>111</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" t="s" s="0">
         <v>15</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" t="s" s="0">
         <v>16</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" t="s" s="0">
         <v>25</v>
       </c>
       <c r="F9" s="3" t="s">
@@ -4648,16 +4664,16 @@
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" t="s" s="0">
         <v>112</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" t="s" s="0">
         <v>15</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" t="s" s="0">
         <v>16</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" t="s" s="0">
         <v>26</v>
       </c>
       <c r="F10" s="3" t="s">
@@ -4668,16 +4684,16 @@
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" t="s" s="0">
         <v>113</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" t="s" s="0">
         <v>15</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" t="s" s="0">
         <v>16</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" t="s" s="0">
         <v>27</v>
       </c>
       <c r="F11" s="3" t="s">
@@ -4704,18 +4720,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.7109375"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="30.0"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="38.0"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="10.28515625"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="11.28515625"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="9.7109375"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="9.42578125"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="25.42578125"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="13.0"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="10.7109375"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="16.7109375"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="11.28515625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
@@ -4772,41 +4788,44 @@
       <c r="B2" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="0">
         <v>38</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" t="s" s="0">
         <v>17</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" t="s" s="0">
         <v>39</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" t="s" s="0">
         <v>40</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" t="s" s="0">
         <v>58</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" t="s" s="0">
         <v>41</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" t="s" s="0">
         <v>42</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L2" t="s" s="0">
         <v>43</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="N2" t="s">
+      <c r="N2" t="s" s="0">
         <v>52</v>
+      </c>
+      <c r="O2" t="s" s="0">
+        <v>447</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -4816,34 +4835,34 @@
       <c r="B3" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" t="s" s="0">
         <v>38</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" t="s" s="0">
         <v>17</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" t="s" s="0">
         <v>56</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" t="s" s="0">
         <v>46</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K3" t="s" s="0">
         <v>48</v>
       </c>
-      <c r="L3" t="s">
+      <c r="L3" t="s" s="0">
         <v>44</v>
       </c>
       <c r="M3" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="N3" t="s">
+      <c r="N3" t="s" s="0">
         <v>53</v>
       </c>
     </row>
@@ -4854,25 +4873,25 @@
       <c r="B4" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" t="s" s="0">
         <v>38</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" t="s" s="0">
         <v>17</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" t="s" s="0">
         <v>57</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" t="s" s="0">
         <v>47</v>
       </c>
-      <c r="K4" t="s">
+      <c r="K4" t="s" s="0">
         <v>49</v>
       </c>
       <c r="L4" s="2" t="s">
@@ -4881,7 +4900,7 @@
       <c r="M4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="N4" t="s">
+      <c r="N4" t="s" s="0">
         <v>54</v>
       </c>
     </row>
@@ -4892,31 +4911,31 @@
       <c r="B5" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" t="s" s="0">
         <v>38</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" t="s" s="0">
         <v>17</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I5" t="s" s="0">
         <v>59</v>
       </c>
-      <c r="J5" t="s">
+      <c r="J5" t="s" s="0">
         <v>41</v>
       </c>
-      <c r="K5" t="s">
+      <c r="K5" t="s" s="0">
         <v>48</v>
       </c>
       <c r="L5" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="N5" t="s">
+      <c r="N5" t="s" s="0">
         <v>55</v>
       </c>
     </row>
@@ -4927,40 +4946,40 @@
       <c r="B6" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" t="s" s="0">
         <v>38</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" t="s" s="0">
         <v>17</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" t="s" s="0">
         <v>160</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" t="s" s="0">
         <v>161</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I6" t="s" s="0">
         <v>58</v>
       </c>
-      <c r="J6" t="s">
+      <c r="J6" t="s" s="0">
         <v>41</v>
       </c>
-      <c r="K6" t="s">
+      <c r="K6" t="s" s="0">
         <v>42</v>
       </c>
-      <c r="L6" t="s">
+      <c r="L6" t="s" s="0">
         <v>43</v>
       </c>
       <c r="M6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="N6" t="s">
+      <c r="N6" t="s" s="0">
         <v>53</v>
       </c>
     </row>
@@ -4971,25 +4990,25 @@
       <c r="B7" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" t="s" s="0">
         <v>38</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" t="s" s="0">
         <v>17</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="J7" t="s">
+      <c r="J7" t="s" s="0">
         <v>46</v>
       </c>
-      <c r="K7" t="s">
+      <c r="K7" t="s" s="0">
         <v>42</v>
       </c>
-      <c r="N7" t="s">
+      <c r="N7" t="s" s="0">
         <v>52</v>
       </c>
     </row>
@@ -5000,19 +5019,19 @@
       <c r="B8" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" t="s" s="0">
         <v>38</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" t="s" s="0">
         <v>17</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="N8" t="s">
+      <c r="N8" t="s" s="0">
         <v>54</v>
       </c>
     </row>
@@ -5023,13 +5042,13 @@
       <c r="B9" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" t="s" s="0">
         <v>38</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" t="s" s="0">
         <v>17</v>
       </c>
       <c r="F9" s="3" t="s">
@@ -5043,13 +5062,13 @@
       <c r="B10" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" t="s" s="0">
         <v>38</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" t="s" s="0">
         <v>17</v>
       </c>
       <c r="F10" s="3" t="s">
@@ -5063,13 +5082,13 @@
       <c r="B11" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" t="s" s="0">
         <v>38</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" t="s" s="0">
         <v>17</v>
       </c>
       <c r="F11" s="3" t="s">
@@ -5104,15 +5123,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.7109375"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="25.140625"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="22.42578125"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="10.28515625"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="11.28515625"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="14.7109375"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="18.7109375"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="11.28515625"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="16.28515625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -5154,23 +5173,23 @@
       <c r="B2" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>96</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="0">
         <v>97</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" t="s" s="0">
         <v>17</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" t="s" s="0">
         <v>98</v>
       </c>
-      <c r="H2" t="s">
-        <v>99</v>
+      <c r="H2" t="s" s="0">
+        <v>448</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>18</v>
@@ -5186,22 +5205,22 @@
       <c r="B3" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>96</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" t="s" s="0">
         <v>97</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" t="s" s="0">
         <v>17</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" t="s" s="0">
         <v>348</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" t="s" s="0">
         <v>349</v>
       </c>
       <c r="I3" s="3" t="s">
@@ -5218,22 +5237,22 @@
       <c r="B4" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" t="s" s="0">
         <v>96</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" t="s" s="0">
         <v>97</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" t="s" s="0">
         <v>17</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" t="s" s="0">
         <v>350</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" t="s" s="0">
         <v>351</v>
       </c>
       <c r="I4" s="3" t="s">
@@ -5250,22 +5269,22 @@
       <c r="B5" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" t="s" s="0">
         <v>96</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" t="s" s="0">
         <v>97</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" t="s" s="0">
         <v>17</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" t="s" s="0">
         <v>158</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" t="s" s="0">
         <v>159</v>
       </c>
       <c r="I5" s="3" t="s">
@@ -5282,22 +5301,22 @@
       <c r="B6" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" t="s" s="0">
         <v>96</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" t="s" s="0">
         <v>97</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" t="s" s="0">
         <v>17</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" t="s" s="0">
         <v>352</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" t="s" s="0">
         <v>353</v>
       </c>
       <c r="I6" s="3" t="s">
@@ -5314,22 +5333,22 @@
       <c r="B7" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" t="s" s="0">
         <v>96</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" t="s" s="0">
         <v>97</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" t="s" s="0">
         <v>17</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" t="s" s="0">
         <v>354</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H7" t="s" s="0">
         <v>355</v>
       </c>
       <c r="I7" s="3" t="s">
@@ -5346,22 +5365,22 @@
       <c r="B8" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" t="s" s="0">
         <v>96</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" t="s" s="0">
         <v>97</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" t="s" s="0">
         <v>17</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8" t="s" s="0">
         <v>356</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H8" t="s" s="0">
         <v>357</v>
       </c>
       <c r="I8" s="3" t="s">
@@ -5378,22 +5397,22 @@
       <c r="B9" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" t="s" s="0">
         <v>96</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" t="s" s="0">
         <v>97</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" t="s" s="0">
         <v>17</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G9" t="s" s="0">
         <v>361</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H9" t="s" s="0">
         <v>362</v>
       </c>
       <c r="I9" s="3" t="s">
@@ -5410,22 +5429,22 @@
       <c r="B10" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" t="s" s="0">
         <v>96</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" t="s" s="0">
         <v>97</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" t="s" s="0">
         <v>17</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G10" t="s" s="0">
         <v>347</v>
       </c>
-      <c r="H10" t="s">
+      <c r="H10" t="s" s="0">
         <v>360</v>
       </c>
       <c r="I10" s="3" t="s">
@@ -5442,22 +5461,22 @@
       <c r="B11" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" t="s" s="0">
         <v>96</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" t="s" s="0">
         <v>97</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" t="s" s="0">
         <v>17</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G11" t="s" s="0">
         <v>358</v>
       </c>
-      <c r="H11" t="s">
+      <c r="H11" t="s" s="0">
         <v>359</v>
       </c>
       <c r="I11" s="3" t="s">
@@ -5507,19 +5526,19 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" style="8"/>
-    <col min="2" max="2" width="15.85546875" style="8" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="39.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15" style="8" customWidth="1"/>
-    <col min="10" max="10" width="17" style="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.7109375" style="8" customWidth="1"/>
-    <col min="13" max="16384" width="9.28515625" style="8"/>
+    <col min="1" max="1" style="8" width="9.28515625"/>
+    <col min="2" max="2" customWidth="true" style="8" width="15.85546875"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="8" width="30.7109375"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="8" width="39.28515625"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="8" width="10.42578125"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="8" width="11.7109375"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="8" width="10.28515625"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="8" width="12.5703125"/>
+    <col min="9" max="9" customWidth="true" style="8" width="15.0"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" style="8" width="17.0"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="8" width="20.7109375"/>
+    <col min="12" max="12" customWidth="true" style="8" width="15.7109375"/>
+    <col min="13" max="16384" style="8" width="9.28515625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="45" x14ac:dyDescent="0.25">
@@ -5972,14 +5991,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.7109375"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="33.85546875"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="30.140625"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="22.28515625"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="11.28515625"/>
+    <col min="7" max="8" bestFit="true" customWidth="true" width="9.85546875"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="14.140625"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="11.28515625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
@@ -6039,10 +6058,10 @@
       <c r="B2" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>239</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="0">
         <v>240</v>
       </c>
       <c r="E2" s="3" t="s">
@@ -6059,10 +6078,10 @@
       <c r="B3" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>239</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" t="s" s="0">
         <v>240</v>
       </c>
       <c r="E3" s="3" t="s">
@@ -6079,10 +6098,10 @@
       <c r="B4" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" t="s" s="0">
         <v>239</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" t="s" s="0">
         <v>240</v>
       </c>
       <c r="E4" s="3" t="s">
@@ -6099,10 +6118,10 @@
       <c r="B5" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" t="s" s="0">
         <v>239</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" t="s" s="0">
         <v>240</v>
       </c>
       <c r="E5" s="3" t="s">
@@ -6119,10 +6138,10 @@
       <c r="B6" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" t="s" s="0">
         <v>239</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" t="s" s="0">
         <v>240</v>
       </c>
       <c r="E6" s="3" t="s">
@@ -6139,10 +6158,10 @@
       <c r="B7" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" t="s" s="0">
         <v>239</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" t="s" s="0">
         <v>240</v>
       </c>
       <c r="E7" s="3" t="s">
@@ -6159,10 +6178,10 @@
       <c r="B8" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" t="s" s="0">
         <v>239</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" t="s" s="0">
         <v>240</v>
       </c>
       <c r="E8" s="3" t="s">
@@ -6179,10 +6198,10 @@
       <c r="B9" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" t="s" s="0">
         <v>239</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" t="s" s="0">
         <v>240</v>
       </c>
       <c r="E9" s="3" t="s">
@@ -6199,10 +6218,10 @@
       <c r="B10" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" t="s" s="0">
         <v>239</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" t="s" s="0">
         <v>240</v>
       </c>
       <c r="E10" s="3" t="s">
@@ -6219,10 +6238,10 @@
       <c r="B11" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" t="s" s="0">
         <v>239</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" t="s" s="0">
         <v>240</v>
       </c>
       <c r="E11" s="3" t="s">
@@ -6270,12 +6289,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34" customWidth="1"/>
-    <col min="5" max="5" width="23" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" customWidth="1"/>
-    <col min="7" max="7" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.7109375"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="28.0"/>
+    <col min="4" max="4" customWidth="true" width="34.0"/>
+    <col min="5" max="5" customWidth="true" width="23.0"/>
+    <col min="6" max="6" customWidth="true" width="11.28515625"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="21.28515625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -6308,10 +6327,10 @@
       <c r="B2" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>259</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="0">
         <v>64</v>
       </c>
       <c r="E2" s="3" t="s">
@@ -6320,7 +6339,7 @@
       <c r="F2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" t="s" s="0">
         <v>68</v>
       </c>
     </row>
@@ -6331,10 +6350,10 @@
       <c r="B3" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>259</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" t="s" s="0">
         <v>64</v>
       </c>
       <c r="E3" s="3" t="s">
@@ -6351,10 +6370,10 @@
       <c r="B4" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" t="s" s="0">
         <v>259</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" t="s" s="0">
         <v>64</v>
       </c>
       <c r="E4" s="3" t="s">
@@ -6371,10 +6390,10 @@
       <c r="B5" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" t="s" s="0">
         <v>259</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" t="s" s="0">
         <v>64</v>
       </c>
       <c r="E5" s="3" t="s">
@@ -6391,10 +6410,10 @@
       <c r="B6" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" t="s" s="0">
         <v>259</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" t="s" s="0">
         <v>64</v>
       </c>
       <c r="E6" s="3" t="s">
@@ -6411,10 +6430,10 @@
       <c r="B7" s="2" t="s">
         <v>276</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" t="s" s="0">
         <v>259</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" t="s" s="0">
         <v>64</v>
       </c>
       <c r="E7" s="3" t="s">
@@ -6431,10 +6450,10 @@
       <c r="B8" s="2" t="s">
         <v>277</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" t="s" s="0">
         <v>259</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" t="s" s="0">
         <v>64</v>
       </c>
       <c r="E8" s="3" t="s">
@@ -6451,10 +6470,10 @@
       <c r="B9" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" t="s" s="0">
         <v>259</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" t="s" s="0">
         <v>64</v>
       </c>
       <c r="E9" s="3" t="s">
@@ -6463,7 +6482,7 @@
       <c r="F9" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G9" t="s" s="0">
         <v>363</v>
       </c>
     </row>
@@ -6474,10 +6493,10 @@
       <c r="B10" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" t="s" s="0">
         <v>259</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" t="s" s="0">
         <v>64</v>
       </c>
       <c r="E10" s="3" t="s">
@@ -6494,10 +6513,10 @@
       <c r="B11" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" t="s" s="0">
         <v>259</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" t="s" s="0">
         <v>64</v>
       </c>
       <c r="E11" s="3" t="s">
@@ -6538,13 +6557,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="41.28515625" customWidth="1"/>
-    <col min="4" max="4" width="40" customWidth="1"/>
-    <col min="5" max="5" width="24.42578125" customWidth="1"/>
-    <col min="6" max="6" width="19.5703125" customWidth="1"/>
-    <col min="7" max="7" width="22.7109375" customWidth="1"/>
-    <col min="8" max="8" width="20.28515625" customWidth="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.7109375"/>
+    <col min="3" max="3" customWidth="true" width="41.28515625"/>
+    <col min="4" max="4" customWidth="true" width="40.0"/>
+    <col min="5" max="5" customWidth="true" width="24.42578125"/>
+    <col min="6" max="6" customWidth="true" width="19.5703125"/>
+    <col min="7" max="7" customWidth="true" width="22.7109375"/>
+    <col min="8" max="8" customWidth="true" width="20.28515625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -6580,10 +6599,10 @@
       <c r="B2" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>292</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="0">
         <v>66</v>
       </c>
       <c r="E2" s="3" t="s">
@@ -6592,10 +6611,10 @@
       <c r="F2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" t="s" s="0">
         <v>69</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" t="s" s="0">
         <v>71</v>
       </c>
     </row>
@@ -6606,10 +6625,10 @@
       <c r="B3" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>292</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" t="s" s="0">
         <v>66</v>
       </c>
       <c r="E3" s="3" t="s">
@@ -6626,10 +6645,10 @@
       <c r="B4" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" t="s" s="0">
         <v>292</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" t="s" s="0">
         <v>66</v>
       </c>
       <c r="E4" s="3" t="s">
@@ -6646,10 +6665,10 @@
       <c r="B5" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" t="s" s="0">
         <v>292</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" t="s" s="0">
         <v>66</v>
       </c>
       <c r="E5" s="3" t="s">
@@ -6666,10 +6685,10 @@
       <c r="B6" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" t="s" s="0">
         <v>292</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" t="s" s="0">
         <v>66</v>
       </c>
       <c r="E6" s="3" t="s">
@@ -6686,10 +6705,10 @@
       <c r="B7" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" t="s" s="0">
         <v>292</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" t="s" s="0">
         <v>66</v>
       </c>
       <c r="E7" s="3" t="s">
@@ -6706,10 +6725,10 @@
       <c r="B8" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" t="s" s="0">
         <v>292</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" t="s" s="0">
         <v>66</v>
       </c>
       <c r="E8" s="3" t="s">
@@ -6726,10 +6745,10 @@
       <c r="B9" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" t="s" s="0">
         <v>292</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" t="s" s="0">
         <v>66</v>
       </c>
       <c r="E9" s="3" t="s">
@@ -6746,10 +6765,10 @@
       <c r="B10" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" t="s" s="0">
         <v>292</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" t="s" s="0">
         <v>66</v>
       </c>
       <c r="E10" s="3" t="s">
@@ -6766,10 +6785,10 @@
       <c r="B11" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" t="s" s="0">
         <v>292</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" t="s" s="0">
         <v>66</v>
       </c>
       <c r="E11" s="3" t="s">
@@ -6810,14 +6829,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="41.7109375" customWidth="1"/>
-    <col min="4" max="4" width="34.28515625" customWidth="1"/>
-    <col min="5" max="5" width="22.5703125" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" customWidth="1"/>
-    <col min="7" max="7" width="23" customWidth="1"/>
-    <col min="8" max="8" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.7109375" customWidth="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.7109375"/>
+    <col min="3" max="3" customWidth="true" width="41.7109375"/>
+    <col min="4" max="4" customWidth="true" width="34.28515625"/>
+    <col min="5" max="5" customWidth="true" width="22.5703125"/>
+    <col min="6" max="6" customWidth="true" width="11.28515625"/>
+    <col min="7" max="7" customWidth="true" width="23.0"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="15.7109375"/>
+    <col min="9" max="9" customWidth="true" width="21.7109375"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -6856,10 +6875,10 @@
       <c r="B2" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>303</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="0">
         <v>91</v>
       </c>
       <c r="E2" s="13" t="s">
@@ -6874,7 +6893,7 @@
       <c r="H2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" t="s" s="0">
         <v>367</v>
       </c>
     </row>
@@ -6885,10 +6904,10 @@
       <c r="B3" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>303</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" t="s" s="0">
         <v>91</v>
       </c>
       <c r="E3" s="13" t="s">
@@ -6911,10 +6930,10 @@
       <c r="B4" s="2" t="s">
         <v>305</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" t="s" s="0">
         <v>303</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" t="s" s="0">
         <v>91</v>
       </c>
       <c r="E4" s="13" t="s">
@@ -6937,10 +6956,10 @@
       <c r="B5" s="2" t="s">
         <v>306</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" t="s" s="0">
         <v>303</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" t="s" s="0">
         <v>91</v>
       </c>
       <c r="E5" s="13" t="s">
@@ -6963,10 +6982,10 @@
       <c r="B6" s="2" t="s">
         <v>307</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" t="s" s="0">
         <v>303</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" t="s" s="0">
         <v>91</v>
       </c>
       <c r="E6" s="13" t="s">
@@ -6989,10 +7008,10 @@
       <c r="B7" s="2" t="s">
         <v>308</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" t="s" s="0">
         <v>303</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" t="s" s="0">
         <v>91</v>
       </c>
       <c r="E7" s="13" t="s">
@@ -7015,10 +7034,10 @@
       <c r="B8" s="2" t="s">
         <v>309</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" t="s" s="0">
         <v>303</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" t="s" s="0">
         <v>91</v>
       </c>
       <c r="E8" s="13" t="s">
@@ -7041,10 +7060,10 @@
       <c r="B9" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" t="s" s="0">
         <v>303</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" t="s" s="0">
         <v>91</v>
       </c>
       <c r="E9" s="13" t="s">
@@ -7067,10 +7086,10 @@
       <c r="B10" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" t="s" s="0">
         <v>303</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" t="s" s="0">
         <v>91</v>
       </c>
       <c r="E10" s="13" t="s">
@@ -7093,10 +7112,10 @@
       <c r="B11" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" t="s" s="0">
         <v>303</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" t="s" s="0">
         <v>91</v>
       </c>
       <c r="E11" s="13" t="s">

</xml_diff>

<commit_message>
Implementation of Cucumber feature files and stepDefinitions are in progress
</commit_message>
<xml_diff>
--- a/src/main/resources/AutomationCatalogue_Batch41_TestData.xlsx
+++ b/src/main/resources/AutomationCatalogue_Batch41_TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AutomationCatalogue\Projects\TestAutomationCatalogue_Batch41\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA66B111-5B72-4818-AC03-32CD15FC2DFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57FF25A8-2277-44F9-BD41-E395C4307687}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="944" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="30195" yWindow="1395" windowWidth="21600" windowHeight="11235" tabRatio="944" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="10" r:id="rId1"/>
@@ -5277,8 +5277,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:O11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L29" sqref="L29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -5680,8 +5680,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N19" sqref="N19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>

</xml_diff>

<commit_message>
Created code for Demo WebShop "Create Address feature", "Demo Web shop StepDefinition" and "DemoWebshop_CreateAddress excel data"
</commit_message>
<xml_diff>
--- a/src/main/resources/AutomationCatalogue_Batch41_TestData.xlsx
+++ b/src/main/resources/AutomationCatalogue_Batch41_TestData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AutomationCatalogue\Projects\TestAutomationCatalogue_Batch41\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Automation Catalogue\Projects\TestAutomationCatalogue_Batch41\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57FF25A8-2277-44F9-BD41-E395C4307687}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71D90257-F4BC-4D83-9B83-95C1F9FA027A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="30195" yWindow="1395" windowWidth="21600" windowHeight="11235" tabRatio="944" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" tabRatio="944" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="10" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1619" uniqueCount="521">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1704" uniqueCount="603">
   <si>
     <t>S. No</t>
   </si>
@@ -1565,9 +1565,6 @@
     <t>Lake Shaun</t>
   </si>
   <si>
-    <t>4041</t>
-  </si>
-  <si>
     <t>8199 Elke Forges</t>
   </si>
   <si>
@@ -1599,6 +1596,255 @@
   </si>
   <si>
     <t>Brody Naidu</t>
+  </si>
+  <si>
+    <t>Alfreds</t>
+  </si>
+  <si>
+    <t>Maria </t>
+  </si>
+  <si>
+    <t>Maria@test.org</t>
+  </si>
+  <si>
+    <t>Maria org</t>
+  </si>
+  <si>
+    <t>Berlin</t>
+  </si>
+  <si>
+    <t>MN</t>
+  </si>
+  <si>
+    <t>1-457-082-1220</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trujillo </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Moreno </t>
+  </si>
+  <si>
+    <t>Moreno@test.org</t>
+  </si>
+  <si>
+    <t>Moreno org</t>
+  </si>
+  <si>
+    <t>MSP</t>
+  </si>
+  <si>
+    <t>1-457-089-1120</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Berglunds </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Christina </t>
+  </si>
+  <si>
+    <t>Christina@test.org</t>
+  </si>
+  <si>
+    <t>Christina org</t>
+  </si>
+  <si>
+    <t>Strasbourg</t>
+  </si>
+  <si>
+    <t>S-958 22</t>
+  </si>
+  <si>
+    <t>NY</t>
+  </si>
+  <si>
+    <t>1-457-082-8909</t>
+  </si>
+  <si>
+    <t>Handel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Roland </t>
+  </si>
+  <si>
+    <t>Roland@test.org</t>
+  </si>
+  <si>
+    <t>Nantes</t>
+  </si>
+  <si>
+    <t>WX3 6FW</t>
+  </si>
+  <si>
+    <t>NJ</t>
+  </si>
+  <si>
+    <t>1-457-564-8909</t>
+  </si>
+  <si>
+    <t>Carnes</t>
+  </si>
+  <si>
+    <t>Pontes</t>
+  </si>
+  <si>
+    <t>Pontes@test.org</t>
+  </si>
+  <si>
+    <t>Graz</t>
+  </si>
+  <si>
+    <t>Hauptstr. 29</t>
+  </si>
+  <si>
+    <t>Av. dos Lusíadas, 23</t>
+  </si>
+  <si>
+    <t>CT</t>
+  </si>
+  <si>
+    <t>1-457-192-2345</t>
+  </si>
+  <si>
+    <t xml:space="preserve">05432-043	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lonesome </t>
+  </si>
+  <si>
+    <t>Wilson</t>
+  </si>
+  <si>
+    <t>Wilson@test.org</t>
+  </si>
+  <si>
+    <t>Pontes Inc</t>
+  </si>
+  <si>
+    <t>Wilson Inc</t>
+  </si>
+  <si>
+    <t>Eugene</t>
+  </si>
+  <si>
+    <t>Cerrito 333</t>
+  </si>
+  <si>
+    <t>CA</t>
+  </si>
+  <si>
+    <t>1-620-192-6794</t>
+  </si>
+  <si>
+    <t>05454-876</t>
+  </si>
+  <si>
+    <t>Delicateses</t>
+  </si>
+  <si>
+    <t>Izquierdo</t>
+  </si>
+  <si>
+    <t>Izquierdo@test.org</t>
+  </si>
+  <si>
+    <t>Izquierdo Inc</t>
+  </si>
+  <si>
+    <t>Madrid</t>
+  </si>
+  <si>
+    <t>Fauntleroy Circus</t>
+  </si>
+  <si>
+    <t>C/ Araquil, 67</t>
+  </si>
+  <si>
+    <t>TX</t>
+  </si>
+  <si>
+    <t>1-967-152-2742</t>
+  </si>
+  <si>
+    <t>05442-030</t>
+  </si>
+  <si>
+    <t>Vinhoss</t>
+  </si>
+  <si>
+    <t>Pipps</t>
+  </si>
+  <si>
+    <t>Pipps@test.org</t>
+  </si>
+  <si>
+    <t>Pipps Ltd</t>
+  </si>
+  <si>
+    <t>Buenos Aires</t>
+  </si>
+  <si>
+    <t>12, rue des Bouchers</t>
+  </si>
+  <si>
+    <t>24, place Kléber</t>
+  </si>
+  <si>
+    <t>IA</t>
+  </si>
+  <si>
+    <t>1-489-492-6512</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Queen </t>
+  </si>
+  <si>
+    <t>Cozinha</t>
+  </si>
+  <si>
+    <t>Cozinha@test.org</t>
+  </si>
+  <si>
+    <t>Cozinha Pvt</t>
+  </si>
+  <si>
+    <t>Boise</t>
+  </si>
+  <si>
+    <t>Obere Str. 57</t>
+  </si>
+  <si>
+    <t>120 Hanover Sq.</t>
+  </si>
+  <si>
+    <t>Forsterstr. 57</t>
+  </si>
+  <si>
+    <t>2, rue des Bouchers</t>
+  </si>
+  <si>
+    <t>23 Tsawassen Blvd.</t>
+  </si>
+  <si>
+    <t>35 King George</t>
+  </si>
+  <si>
+    <t>Åkergatan 24</t>
+  </si>
+  <si>
+    <t>54, rue Royale</t>
+  </si>
+  <si>
+    <t>OW</t>
+  </si>
+  <si>
+    <t>1-967-567-2953</t>
+  </si>
+  <si>
+    <t>Roland org</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2743 Bering St.	</t>
   </si>
 </sst>
 </file>
@@ -2078,14 +2324,14 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.6"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.69140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="39" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="38" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.4609375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.3046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -3879,16 +4125,16 @@
       <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.6"/>
   <cols>
-    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="41.6640625" customWidth="1"/>
-    <col min="4" max="4" width="34.33203125" customWidth="1"/>
-    <col min="5" max="5" width="22.5546875" customWidth="1"/>
-    <col min="6" max="6" width="11.33203125" customWidth="1"/>
+    <col min="2" max="2" width="10.69140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.69140625" customWidth="1"/>
+    <col min="4" max="4" width="34.3046875" customWidth="1"/>
+    <col min="5" max="5" width="22.53515625" customWidth="1"/>
+    <col min="6" max="6" width="11.3046875" customWidth="1"/>
     <col min="7" max="7" width="23" customWidth="1"/>
-    <col min="8" max="8" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.6640625" customWidth="1"/>
+    <col min="8" max="8" width="15.69140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.69140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -3946,7 +4192,7 @@
         <v>6</v>
       </c>
       <c r="I2" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -4198,23 +4444,23 @@
       <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.6"/>
   <cols>
-    <col min="2" max="2" width="12.33203125" customWidth="1"/>
-    <col min="3" max="3" width="27.44140625" customWidth="1"/>
-    <col min="4" max="4" width="25.88671875" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" customWidth="1"/>
-    <col min="6" max="6" width="11.88671875" customWidth="1"/>
+    <col min="2" max="2" width="12.3046875" customWidth="1"/>
+    <col min="3" max="3" width="27.4609375" customWidth="1"/>
+    <col min="4" max="4" width="25.84375" customWidth="1"/>
+    <col min="5" max="5" width="10.69140625" customWidth="1"/>
+    <col min="6" max="6" width="11.84375" customWidth="1"/>
     <col min="7" max="7" width="15" customWidth="1"/>
-    <col min="8" max="8" width="16.5546875" customWidth="1"/>
-    <col min="9" max="9" width="17.88671875" customWidth="1"/>
-    <col min="10" max="10" width="19.33203125" customWidth="1"/>
-    <col min="11" max="11" width="17.88671875" customWidth="1"/>
-    <col min="12" max="12" width="16.88671875" customWidth="1"/>
+    <col min="8" max="8" width="16.53515625" customWidth="1"/>
+    <col min="9" max="9" width="17.84375" customWidth="1"/>
+    <col min="10" max="10" width="19.3046875" customWidth="1"/>
+    <col min="11" max="11" width="17.84375" customWidth="1"/>
+    <col min="12" max="12" width="16.84375" customWidth="1"/>
     <col min="13" max="13" width="17" customWidth="1"/>
-    <col min="14" max="14" width="15.109375" customWidth="1"/>
-    <col min="15" max="15" width="17.6640625" customWidth="1"/>
-    <col min="16" max="16" width="15.5546875" customWidth="1"/>
+    <col min="14" max="14" width="15.07421875" customWidth="1"/>
+    <col min="15" max="15" width="17.69140625" customWidth="1"/>
+    <col min="16" max="16" width="15.53515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="17" customFormat="1">
@@ -4699,18 +4945,18 @@
       <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.6"/>
   <cols>
-    <col min="1" max="1" width="6.44140625" customWidth="1"/>
-    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="40.33203125" customWidth="1"/>
-    <col min="5" max="5" width="22.6640625" customWidth="1"/>
-    <col min="6" max="6" width="12.44140625" customWidth="1"/>
-    <col min="7" max="7" width="21.44140625" customWidth="1"/>
-    <col min="8" max="8" width="21.33203125" customWidth="1"/>
-    <col min="9" max="9" width="18.33203125" customWidth="1"/>
-    <col min="10" max="10" width="9.33203125" customWidth="1"/>
+    <col min="1" max="1" width="6.4609375" customWidth="1"/>
+    <col min="2" max="2" width="10.69140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.53515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.3046875" customWidth="1"/>
+    <col min="5" max="5" width="22.69140625" customWidth="1"/>
+    <col min="6" max="6" width="12.4609375" customWidth="1"/>
+    <col min="7" max="7" width="21.4609375" customWidth="1"/>
+    <col min="8" max="8" width="21.3046875" customWidth="1"/>
+    <col min="9" max="9" width="18.3046875" customWidth="1"/>
+    <col min="10" max="10" width="9.3046875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -4766,7 +5012,7 @@
         <v>71</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
@@ -5034,13 +5280,13 @@
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.6"/>
   <cols>
-    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.69140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26" customWidth="1"/>
-    <col min="4" max="4" width="24.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.4609375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.69140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.3046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -5277,24 +5523,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:O11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.6"/>
   <cols>
-    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.69140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="38" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.3046875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.3046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.69140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.4609375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.4609375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.69140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.69140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.3046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
@@ -5684,17 +5930,17 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.6"/>
   <cols>
-    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.69140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.07421875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.4609375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.3046875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.3046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.69140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.69140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.3046875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.3046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -5926,7 +6172,7 @@
         <v>18</v>
       </c>
       <c r="G8" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="I8" s="3" t="s">
         <v>18</v>
@@ -6013,7 +6259,7 @@
         <v>18</v>
       </c>
       <c r="G11" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="I11" s="3" t="s">
         <v>18</v>
@@ -6060,24 +6306,24 @@
       <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9.3046875" defaultRowHeight="14.6"/>
   <cols>
-    <col min="1" max="1" width="9.33203125" style="8"/>
-    <col min="2" max="2" width="15.88671875" style="8" customWidth="1"/>
-    <col min="3" max="3" width="30.6640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="39.33203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.44140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.6640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.33203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.3046875" style="8"/>
+    <col min="2" max="2" width="15.84375" style="8" customWidth="1"/>
+    <col min="3" max="3" width="30.69140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.3046875" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.4609375" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.69140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.3046875" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.53515625" style="8" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15" style="8" customWidth="1"/>
     <col min="10" max="10" width="17" style="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.6640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.6640625" style="8" customWidth="1"/>
-    <col min="13" max="16384" width="9.33203125" style="8"/>
+    <col min="11" max="11" width="20.69140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.69140625" style="8" customWidth="1"/>
+    <col min="13" max="16384" width="9.3046875" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="28.8">
+    <row r="1" spans="1:12" ht="29.15">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -6115,7 +6361,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="28.8">
+    <row r="2" spans="1:12" ht="29.15">
       <c r="A2" s="9" t="s">
         <v>5</v>
       </c>
@@ -6153,7 +6399,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="28.8">
+    <row r="3" spans="1:12" ht="29.15">
       <c r="A3" s="9" t="s">
         <v>6</v>
       </c>
@@ -6191,7 +6437,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="28.8">
+    <row r="4" spans="1:12" ht="29.15">
       <c r="A4" s="9" t="s">
         <v>7</v>
       </c>
@@ -6229,7 +6475,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="28.8">
+    <row r="5" spans="1:12" ht="29.15">
       <c r="A5" s="9" t="s">
         <v>8</v>
       </c>
@@ -6267,7 +6513,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="28.8">
+    <row r="6" spans="1:12" ht="29.15">
       <c r="A6" s="9" t="s">
         <v>9</v>
       </c>
@@ -6305,7 +6551,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="28.8">
+    <row r="7" spans="1:12" ht="29.15">
       <c r="A7" s="9" t="s">
         <v>10</v>
       </c>
@@ -6343,7 +6589,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="28.8">
+    <row r="8" spans="1:12" ht="29.15">
       <c r="A8" s="9" t="s">
         <v>11</v>
       </c>
@@ -6381,7 +6627,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="28.8">
+    <row r="9" spans="1:12" ht="29.15">
       <c r="A9" s="9" t="s">
         <v>12</v>
       </c>
@@ -6419,7 +6665,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="28.8">
+    <row r="10" spans="1:12" ht="29.15">
       <c r="A10" s="9" t="s">
         <v>13</v>
       </c>
@@ -6457,7 +6703,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="28.8">
+    <row r="11" spans="1:12" ht="29.15">
       <c r="A11" s="9" t="s">
         <v>14</v>
       </c>
@@ -6521,20 +6767,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:P11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.6"/>
   <cols>
-    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.69140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.84375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.07421875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.3046875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.3046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="9.84375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.69140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.765625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.07421875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.15234375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.23046875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.765625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16">
@@ -6622,19 +6874,19 @@
         <v>508</v>
       </c>
       <c r="L2" t="s">
+        <v>602</v>
+      </c>
+      <c r="M2" t="s">
         <v>509</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>510</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>511</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>512</v>
-      </c>
-      <c r="P2" t="s">
-        <v>513</v>
       </c>
     </row>
     <row r="3" spans="1:16">
@@ -6656,6 +6908,36 @@
       <c r="F3" s="3" t="s">
         <v>18</v>
       </c>
+      <c r="G3" t="s">
+        <v>520</v>
+      </c>
+      <c r="H3" t="s">
+        <v>521</v>
+      </c>
+      <c r="I3" t="s">
+        <v>522</v>
+      </c>
+      <c r="J3" t="s">
+        <v>523</v>
+      </c>
+      <c r="K3" t="s">
+        <v>524</v>
+      </c>
+      <c r="L3" t="s">
+        <v>592</v>
+      </c>
+      <c r="M3" t="s">
+        <v>596</v>
+      </c>
+      <c r="N3" t="s">
+        <v>525</v>
+      </c>
+      <c r="O3" t="s">
+        <v>526</v>
+      </c>
+      <c r="P3">
+        <v>780001</v>
+      </c>
     </row>
     <row r="4" spans="1:16">
       <c r="A4" s="2" t="s">
@@ -6676,6 +6958,36 @@
       <c r="F4" s="3" t="s">
         <v>18</v>
       </c>
+      <c r="G4" t="s">
+        <v>527</v>
+      </c>
+      <c r="H4" t="s">
+        <v>528</v>
+      </c>
+      <c r="I4" t="s">
+        <v>529</v>
+      </c>
+      <c r="J4" t="s">
+        <v>530</v>
+      </c>
+      <c r="K4" t="s">
+        <v>435</v>
+      </c>
+      <c r="L4" t="s">
+        <v>593</v>
+      </c>
+      <c r="M4" t="s">
+        <v>597</v>
+      </c>
+      <c r="N4" t="s">
+        <v>531</v>
+      </c>
+      <c r="O4" t="s">
+        <v>532</v>
+      </c>
+      <c r="P4">
+        <v>7800078</v>
+      </c>
     </row>
     <row r="5" spans="1:16">
       <c r="A5" s="2" t="s">
@@ -6696,6 +7008,36 @@
       <c r="F5" s="3" t="s">
         <v>18</v>
       </c>
+      <c r="G5" t="s">
+        <v>533</v>
+      </c>
+      <c r="H5" t="s">
+        <v>534</v>
+      </c>
+      <c r="I5" t="s">
+        <v>535</v>
+      </c>
+      <c r="J5" t="s">
+        <v>536</v>
+      </c>
+      <c r="K5" t="s">
+        <v>537</v>
+      </c>
+      <c r="L5" t="s">
+        <v>594</v>
+      </c>
+      <c r="M5" t="s">
+        <v>538</v>
+      </c>
+      <c r="N5" t="s">
+        <v>539</v>
+      </c>
+      <c r="O5" t="s">
+        <v>540</v>
+      </c>
+      <c r="P5">
+        <v>5022</v>
+      </c>
     </row>
     <row r="6" spans="1:16">
       <c r="A6" s="2" t="s">
@@ -6716,6 +7058,36 @@
       <c r="F6" s="3" t="s">
         <v>18</v>
       </c>
+      <c r="G6" t="s">
+        <v>541</v>
+      </c>
+      <c r="H6" t="s">
+        <v>542</v>
+      </c>
+      <c r="I6" t="s">
+        <v>543</v>
+      </c>
+      <c r="J6" t="s">
+        <v>601</v>
+      </c>
+      <c r="K6" t="s">
+        <v>544</v>
+      </c>
+      <c r="L6" t="s">
+        <v>595</v>
+      </c>
+      <c r="M6" t="s">
+        <v>545</v>
+      </c>
+      <c r="N6" t="s">
+        <v>546</v>
+      </c>
+      <c r="O6" t="s">
+        <v>547</v>
+      </c>
+      <c r="P6">
+        <v>94117</v>
+      </c>
     </row>
     <row r="7" spans="1:16">
       <c r="A7" s="2" t="s">
@@ -6736,6 +7108,36 @@
       <c r="F7" s="3" t="s">
         <v>18</v>
       </c>
+      <c r="G7" t="s">
+        <v>548</v>
+      </c>
+      <c r="H7" t="s">
+        <v>549</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>550</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>560</v>
+      </c>
+      <c r="K7" t="s">
+        <v>551</v>
+      </c>
+      <c r="L7" t="s">
+        <v>552</v>
+      </c>
+      <c r="M7" t="s">
+        <v>553</v>
+      </c>
+      <c r="N7" t="s">
+        <v>554</v>
+      </c>
+      <c r="O7" t="s">
+        <v>555</v>
+      </c>
+      <c r="P7" t="s">
+        <v>556</v>
+      </c>
     </row>
     <row r="8" spans="1:16">
       <c r="A8" s="2" t="s">
@@ -6756,6 +7158,36 @@
       <c r="F8" s="3" t="s">
         <v>18</v>
       </c>
+      <c r="G8" t="s">
+        <v>557</v>
+      </c>
+      <c r="H8" t="s">
+        <v>558</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>559</v>
+      </c>
+      <c r="J8" t="s">
+        <v>561</v>
+      </c>
+      <c r="K8" t="s">
+        <v>562</v>
+      </c>
+      <c r="L8" t="s">
+        <v>563</v>
+      </c>
+      <c r="M8" t="s">
+        <v>552</v>
+      </c>
+      <c r="N8" t="s">
+        <v>564</v>
+      </c>
+      <c r="O8" t="s">
+        <v>565</v>
+      </c>
+      <c r="P8" t="s">
+        <v>566</v>
+      </c>
     </row>
     <row r="9" spans="1:16">
       <c r="A9" s="2" t="s">
@@ -6776,6 +7208,36 @@
       <c r="F9" s="3" t="s">
         <v>18</v>
       </c>
+      <c r="G9" t="s">
+        <v>567</v>
+      </c>
+      <c r="H9" t="s">
+        <v>568</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>569</v>
+      </c>
+      <c r="J9" t="s">
+        <v>570</v>
+      </c>
+      <c r="K9" t="s">
+        <v>571</v>
+      </c>
+      <c r="L9" t="s">
+        <v>572</v>
+      </c>
+      <c r="M9" t="s">
+        <v>573</v>
+      </c>
+      <c r="N9" t="s">
+        <v>574</v>
+      </c>
+      <c r="O9" t="s">
+        <v>575</v>
+      </c>
+      <c r="P9" t="s">
+        <v>576</v>
+      </c>
     </row>
     <row r="10" spans="1:16">
       <c r="A10" s="2" t="s">
@@ -6796,6 +7258,36 @@
       <c r="F10" s="3" t="s">
         <v>18</v>
       </c>
+      <c r="G10" t="s">
+        <v>577</v>
+      </c>
+      <c r="H10" t="s">
+        <v>578</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>579</v>
+      </c>
+      <c r="J10" t="s">
+        <v>580</v>
+      </c>
+      <c r="K10" t="s">
+        <v>581</v>
+      </c>
+      <c r="L10" t="s">
+        <v>582</v>
+      </c>
+      <c r="M10" t="s">
+        <v>583</v>
+      </c>
+      <c r="N10" t="s">
+        <v>584</v>
+      </c>
+      <c r="O10" t="s">
+        <v>585</v>
+      </c>
+      <c r="P10" t="s">
+        <v>566</v>
+      </c>
     </row>
     <row r="11" spans="1:16">
       <c r="A11" s="2" t="s">
@@ -6815,6 +7307,36 @@
       </c>
       <c r="F11" s="3" t="s">
         <v>18</v>
+      </c>
+      <c r="G11" t="s">
+        <v>586</v>
+      </c>
+      <c r="H11" t="s">
+        <v>587</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>588</v>
+      </c>
+      <c r="J11" t="s">
+        <v>589</v>
+      </c>
+      <c r="K11" t="s">
+        <v>590</v>
+      </c>
+      <c r="L11" t="s">
+        <v>591</v>
+      </c>
+      <c r="M11" t="s">
+        <v>598</v>
+      </c>
+      <c r="N11" t="s">
+        <v>599</v>
+      </c>
+      <c r="O11" t="s">
+        <v>600</v>
+      </c>
+      <c r="P11">
+        <v>99362</v>
       </c>
     </row>
   </sheetData>
@@ -6840,8 +7362,20 @@
     <hyperlink ref="F9" r:id="rId18" xr:uid="{00000000-0004-0000-0500-000011000000}"/>
     <hyperlink ref="F10" r:id="rId19" xr:uid="{00000000-0004-0000-0500-000012000000}"/>
     <hyperlink ref="F11" r:id="rId20" xr:uid="{00000000-0004-0000-0500-000013000000}"/>
+    <hyperlink ref="I3" r:id="rId21" xr:uid="{C81A3971-6034-4FA6-AD62-602659446BEA}"/>
+    <hyperlink ref="I4" r:id="rId22" xr:uid="{50D524F0-DAA2-4AFC-9FD2-5F1256FF0E23}"/>
+    <hyperlink ref="I5" r:id="rId23" xr:uid="{0DC85489-444B-47B8-92A0-845D4B4627BE}"/>
+    <hyperlink ref="I6" r:id="rId24" xr:uid="{79F23829-991F-42A6-B569-17DAD72BCA52}"/>
+    <hyperlink ref="J6" r:id="rId25" display="Roland@test.org" xr:uid="{F833B56F-A773-41B2-8C5A-4F16C9F1E6DA}"/>
+    <hyperlink ref="I7" r:id="rId26" xr:uid="{A9242B6A-3D43-472B-9E0C-E3FA9A74F3B3}"/>
+    <hyperlink ref="J7" r:id="rId27" display="Pontes@test.org" xr:uid="{0845BDEB-BF3B-405B-B45C-D6BBF8B66543}"/>
+    <hyperlink ref="I8" r:id="rId28" xr:uid="{BF376FC5-5CAD-44FA-A34D-2BEF6E7CF391}"/>
+    <hyperlink ref="I9" r:id="rId29" xr:uid="{6984E062-BA00-4CB1-BA56-5B7A334891FB}"/>
+    <hyperlink ref="I10" r:id="rId30" xr:uid="{CB379D73-899C-4760-842D-38F41CCF882A}"/>
+    <hyperlink ref="I11" r:id="rId31" xr:uid="{77D1F26A-2C1D-4A88-AE76-6C57C6317DD5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId32"/>
 </worksheet>
 </file>
 
@@ -6853,14 +7387,14 @@
       <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.6"/>
   <cols>
-    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.69140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="28" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="34" customWidth="1"/>
     <col min="5" max="5" width="23" customWidth="1"/>
-    <col min="6" max="6" width="11.33203125" customWidth="1"/>
-    <col min="7" max="7" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.3046875" customWidth="1"/>
+    <col min="7" max="7" width="21.3046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -6906,7 +7440,7 @@
         <v>18</v>
       </c>
       <c r="G2" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -7121,15 +7655,15 @@
       <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.6"/>
   <cols>
-    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="41.33203125" customWidth="1"/>
+    <col min="2" max="2" width="10.69140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.3046875" customWidth="1"/>
     <col min="4" max="4" width="40" customWidth="1"/>
-    <col min="5" max="5" width="24.44140625" customWidth="1"/>
-    <col min="6" max="6" width="19.5546875" customWidth="1"/>
-    <col min="7" max="7" width="22.6640625" customWidth="1"/>
-    <col min="8" max="8" width="20.33203125" customWidth="1"/>
+    <col min="5" max="5" width="24.4609375" customWidth="1"/>
+    <col min="6" max="6" width="19.53515625" customWidth="1"/>
+    <col min="7" max="7" width="22.69140625" customWidth="1"/>
+    <col min="8" max="8" width="20.3046875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -7178,10 +7712,10 @@
         <v>18</v>
       </c>
       <c r="G2" t="s">
+        <v>514</v>
+      </c>
+      <c r="H2" t="s">
         <v>515</v>
-      </c>
-      <c r="H2" t="s">
-        <v>516</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -7393,27 +7927,27 @@
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.6"/>
   <cols>
-    <col min="1" max="1" width="5.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.4609375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.53515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.4609375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.765625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.84375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.3046875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="25" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21.21875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="26.109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.53515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.84375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.84375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.23046875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="26.07421875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.84375" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="9" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.5546875" customWidth="1"/>
+    <col min="16" max="16" width="20.07421875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.3046875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.53515625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.53515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18">

</xml_diff>

<commit_message>
Latest Changes in TDD testcases in Progress
</commit_message>
<xml_diff>
--- a/src/main/resources/AutomationCatalogue_Batch41_TestData.xlsx
+++ b/src/main/resources/AutomationCatalogue_Batch41_TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AutomationCatalogue\Projects\TestAutomationCatalogue_Batch41\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9D587A2-0F91-4636-8E14-604514B6E2FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D7AFF44-C4A5-4CEA-825B-6D54F201AE59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="944" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="944" firstSheet="6" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="10" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1711" uniqueCount="604">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1708" uniqueCount="605">
   <si>
     <t>S. No</t>
   </si>
@@ -1848,6 +1848,9 @@
   </si>
   <si>
     <t>FAILED</t>
+  </si>
+  <si>
+    <t>QWRtaW5AMTIz</t>
   </si>
 </sst>
 </file>
@@ -1855,7 +1858,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1895,12 +1898,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1966,7 +1963,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -1988,13 +1985,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -2324,7 +2318,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G122"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
@@ -2362,15 +2356,15 @@
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="13" t="s">
         <v>109</v>
       </c>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="2" t="s">
@@ -2519,15 +2513,15 @@
       </c>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="15" t="s">
+      <c r="A13" s="14" t="s">
         <v>110</v>
       </c>
-      <c r="B13" s="15"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="15"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="2" t="s">
@@ -2676,15 +2670,15 @@
       </c>
     </row>
     <row r="24" spans="1:7">
-      <c r="A24" s="15" t="s">
+      <c r="A24" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="B24" s="15"/>
-      <c r="C24" s="15"/>
-      <c r="D24" s="15"/>
-      <c r="E24" s="15"/>
-      <c r="F24" s="15"/>
-      <c r="G24" s="15"/>
+      <c r="B24" s="14"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="14"/>
+      <c r="G24" s="14"/>
     </row>
     <row r="25" spans="1:7">
       <c r="A25" s="2" t="s">
@@ -2842,15 +2836,15 @@
       </c>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" s="15" t="s">
+      <c r="A35" s="14" t="s">
         <v>152</v>
       </c>
-      <c r="B35" s="15"/>
-      <c r="C35" s="15"/>
-      <c r="D35" s="15"/>
-      <c r="E35" s="15"/>
-      <c r="F35" s="15"/>
-      <c r="G35" s="15"/>
+      <c r="B35" s="14"/>
+      <c r="C35" s="14"/>
+      <c r="D35" s="14"/>
+      <c r="E35" s="14"/>
+      <c r="F35" s="14"/>
+      <c r="G35" s="14"/>
     </row>
     <row r="36" spans="1:7">
       <c r="A36" s="2" t="s">
@@ -3010,15 +3004,15 @@
       <c r="E45" s="2"/>
     </row>
     <row r="46" spans="1:7">
-      <c r="A46" s="15" t="s">
+      <c r="A46" s="14" t="s">
         <v>176</v>
       </c>
-      <c r="B46" s="15"/>
-      <c r="C46" s="15"/>
-      <c r="D46" s="15"/>
-      <c r="E46" s="15"/>
-      <c r="F46" s="15"/>
-      <c r="G46" s="15"/>
+      <c r="B46" s="14"/>
+      <c r="C46" s="14"/>
+      <c r="D46" s="14"/>
+      <c r="E46" s="14"/>
+      <c r="F46" s="14"/>
+      <c r="G46" s="14"/>
     </row>
     <row r="47" spans="1:7">
       <c r="A47" s="2" t="s">
@@ -3170,15 +3164,15 @@
       </c>
     </row>
     <row r="57" spans="1:7">
-      <c r="A57" s="15" t="s">
+      <c r="A57" s="14" t="s">
         <v>199</v>
       </c>
-      <c r="B57" s="15"/>
-      <c r="C57" s="15"/>
-      <c r="D57" s="15"/>
-      <c r="E57" s="15"/>
-      <c r="F57" s="15"/>
-      <c r="G57" s="15"/>
+      <c r="B57" s="14"/>
+      <c r="C57" s="14"/>
+      <c r="D57" s="14"/>
+      <c r="E57" s="14"/>
+      <c r="F57" s="14"/>
+      <c r="G57" s="14"/>
     </row>
     <row r="58" spans="1:7">
       <c r="A58" s="2" t="s">
@@ -3327,15 +3321,15 @@
       </c>
     </row>
     <row r="68" spans="1:7">
-      <c r="A68" s="15" t="s">
+      <c r="A68" s="14" t="s">
         <v>221</v>
       </c>
-      <c r="B68" s="15"/>
-      <c r="C68" s="15"/>
-      <c r="D68" s="15"/>
-      <c r="E68" s="15"/>
-      <c r="F68" s="15"/>
-      <c r="G68" s="15"/>
+      <c r="B68" s="14"/>
+      <c r="C68" s="14"/>
+      <c r="D68" s="14"/>
+      <c r="E68" s="14"/>
+      <c r="F68" s="14"/>
+      <c r="G68" s="14"/>
     </row>
     <row r="69" spans="1:7">
       <c r="A69" s="2" t="s">
@@ -3484,15 +3478,15 @@
       </c>
     </row>
     <row r="79" spans="1:7">
-      <c r="A79" s="15" t="s">
+      <c r="A79" s="14" t="s">
         <v>253</v>
       </c>
-      <c r="B79" s="15"/>
-      <c r="C79" s="15"/>
-      <c r="D79" s="15"/>
-      <c r="E79" s="15"/>
-      <c r="F79" s="15"/>
-      <c r="G79" s="15"/>
+      <c r="B79" s="14"/>
+      <c r="C79" s="14"/>
+      <c r="D79" s="14"/>
+      <c r="E79" s="14"/>
+      <c r="F79" s="14"/>
+      <c r="G79" s="14"/>
     </row>
     <row r="80" spans="1:7">
       <c r="A80" s="2" t="s">
@@ -3644,15 +3638,15 @@
       </c>
     </row>
     <row r="90" spans="1:7">
-      <c r="A90" s="15" t="s">
+      <c r="A90" s="14" t="s">
         <v>274</v>
       </c>
-      <c r="B90" s="15"/>
-      <c r="C90" s="15"/>
-      <c r="D90" s="15"/>
-      <c r="E90" s="15"/>
-      <c r="F90" s="15"/>
-      <c r="G90" s="15"/>
+      <c r="B90" s="14"/>
+      <c r="C90" s="14"/>
+      <c r="D90" s="14"/>
+      <c r="E90" s="14"/>
+      <c r="F90" s="14"/>
+      <c r="G90" s="14"/>
     </row>
     <row r="91" spans="1:7">
       <c r="A91" s="2" t="s">
@@ -3801,15 +3795,15 @@
       </c>
     </row>
     <row r="101" spans="1:7">
-      <c r="A101" s="15" t="s">
+      <c r="A101" s="14" t="s">
         <v>307</v>
       </c>
-      <c r="B101" s="15"/>
-      <c r="C101" s="15"/>
-      <c r="D101" s="15"/>
-      <c r="E101" s="15"/>
-      <c r="F101" s="15"/>
-      <c r="G101" s="15"/>
+      <c r="B101" s="14"/>
+      <c r="C101" s="14"/>
+      <c r="D101" s="14"/>
+      <c r="E101" s="14"/>
+      <c r="F101" s="14"/>
+      <c r="G101" s="14"/>
     </row>
     <row r="102" spans="1:7">
       <c r="A102" s="2" t="s">
@@ -3958,15 +3952,15 @@
       </c>
     </row>
     <row r="112" spans="1:7">
-      <c r="A112" s="15" t="s">
+      <c r="A112" s="14" t="s">
         <v>329</v>
       </c>
-      <c r="B112" s="15"/>
-      <c r="C112" s="15"/>
-      <c r="D112" s="15"/>
-      <c r="E112" s="15"/>
-      <c r="F112" s="15"/>
-      <c r="G112" s="15"/>
+      <c r="B112" s="14"/>
+      <c r="C112" s="14"/>
+      <c r="D112" s="14"/>
+      <c r="E112" s="14"/>
+      <c r="F112" s="14"/>
+      <c r="G112" s="14"/>
     </row>
     <row r="113" spans="1:6">
       <c r="A113" s="2" t="s">
@@ -4125,8 +4119,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -4135,7 +4129,7 @@
     <col min="3" max="3" customWidth="true" width="41.6640625"/>
     <col min="4" max="4" customWidth="true" width="34.33203125"/>
     <col min="5" max="5" customWidth="true" width="22.5546875"/>
-    <col min="6" max="6" customWidth="true" width="11.33203125"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="15.109375"/>
     <col min="7" max="7" customWidth="true" width="23.0"/>
     <col min="8" max="8" bestFit="true" customWidth="true" width="15.6640625"/>
     <col min="9" max="9" customWidth="true" width="21.6640625"/>
@@ -4183,11 +4177,11 @@
       <c r="D2" t="s" s="0">
         <v>87</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="F2" s="13" t="s">
-        <v>18</v>
+      <c r="F2" s="3" t="s">
+        <v>604</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>14</v>
@@ -4212,11 +4206,11 @@
       <c r="D3" t="s" s="0">
         <v>87</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="E3" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="F3" s="13" t="s">
-        <v>18</v>
+      <c r="F3" s="3" t="s">
+        <v>604</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>112</v>
@@ -4238,11 +4232,11 @@
       <c r="D4" t="s" s="0">
         <v>87</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="E4" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="F4" s="13" t="s">
-        <v>18</v>
+      <c r="F4" s="3" t="s">
+        <v>604</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>14</v>
@@ -4264,11 +4258,11 @@
       <c r="D5" t="s" s="0">
         <v>87</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="E5" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="F5" s="13" t="s">
-        <v>18</v>
+      <c r="F5" s="3" t="s">
+        <v>604</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>111</v>
@@ -4290,11 +4284,11 @@
       <c r="D6" t="s" s="0">
         <v>87</v>
       </c>
-      <c r="E6" s="13" t="s">
+      <c r="E6" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="F6" s="13" t="s">
-        <v>18</v>
+      <c r="F6" s="3" t="s">
+        <v>604</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>115</v>
@@ -4316,11 +4310,11 @@
       <c r="D7" t="s" s="0">
         <v>87</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="E7" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="F7" s="13" t="s">
-        <v>18</v>
+      <c r="F7" s="3" t="s">
+        <v>604</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>120</v>
@@ -4342,11 +4336,11 @@
       <c r="D8" t="s" s="0">
         <v>87</v>
       </c>
-      <c r="E8" s="13" t="s">
+      <c r="E8" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="F8" s="13" t="s">
-        <v>18</v>
+      <c r="F8" s="3" t="s">
+        <v>604</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>118</v>
@@ -4368,11 +4362,11 @@
       <c r="D9" t="s" s="0">
         <v>87</v>
       </c>
-      <c r="E9" s="13" t="s">
+      <c r="E9" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="F9" s="13" t="s">
-        <v>18</v>
+      <c r="F9" s="3" t="s">
+        <v>604</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>116</v>
@@ -4394,11 +4388,11 @@
       <c r="D10" t="s" s="0">
         <v>87</v>
       </c>
-      <c r="E10" s="13" t="s">
+      <c r="E10" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="F10" s="13" t="s">
-        <v>18</v>
+      <c r="F10" s="3" t="s">
+        <v>604</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>132</v>
@@ -4420,11 +4414,11 @@
       <c r="D11" t="s" s="0">
         <v>87</v>
       </c>
-      <c r="E11" s="13" t="s">
+      <c r="E11" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="F11" s="13" t="s">
-        <v>18</v>
+      <c r="F11" s="3" t="s">
+        <v>604</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>14</v>
@@ -4445,7 +4439,7 @@
   <dimension ref="A1:P11"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -4454,7 +4448,7 @@
     <col min="3" max="3" customWidth="true" width="27.44140625"/>
     <col min="4" max="4" customWidth="true" width="25.88671875"/>
     <col min="5" max="5" customWidth="true" width="10.6640625"/>
-    <col min="6" max="6" customWidth="true" width="11.88671875"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="15.109375"/>
     <col min="7" max="7" customWidth="true" width="15.0"/>
     <col min="8" max="8" customWidth="true" width="16.5546875"/>
     <col min="9" max="9" customWidth="true" width="17.88671875"/>
@@ -4467,53 +4461,53 @@
     <col min="16" max="16" customWidth="true" width="15.5546875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="17" customFormat="1">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:16" s="16" customFormat="1">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="F1" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="17" t="s">
+      <c r="G1" s="16" t="s">
         <v>343</v>
       </c>
-      <c r="H1" s="17" t="s">
+      <c r="H1" s="16" t="s">
         <v>344</v>
       </c>
-      <c r="I1" s="17" t="s">
+      <c r="I1" s="16" t="s">
         <v>345</v>
       </c>
-      <c r="J1" s="17" t="s">
+      <c r="J1" s="16" t="s">
         <v>346</v>
       </c>
-      <c r="K1" s="17" t="s">
+      <c r="K1" s="16" t="s">
         <v>347</v>
       </c>
-      <c r="L1" s="17" t="s">
+      <c r="L1" s="16" t="s">
         <v>348</v>
       </c>
-      <c r="M1" s="17" t="s">
+      <c r="M1" s="16" t="s">
         <v>349</v>
       </c>
-      <c r="N1" s="17" t="s">
+      <c r="N1" s="16" t="s">
         <v>357</v>
       </c>
-      <c r="O1" s="17" t="s">
+      <c r="O1" s="16" t="s">
         <v>358</v>
       </c>
-      <c r="P1" s="17" t="s">
+      <c r="P1" s="16" t="s">
         <v>359</v>
       </c>
     </row>
@@ -4533,8 +4527,8 @@
       <c r="E2" t="s" s="0">
         <v>17</v>
       </c>
-      <c r="F2" t="s" s="0">
-        <v>18</v>
+      <c r="F2" s="3" t="s">
+        <v>604</v>
       </c>
       <c r="G2" t="s" s="0">
         <v>350</v>
@@ -4542,19 +4536,19 @@
       <c r="H2" t="s" s="0">
         <v>351</v>
       </c>
-      <c r="I2" s="18" t="s">
+      <c r="I2" s="17" t="s">
         <v>355</v>
       </c>
       <c r="J2" t="s" s="0">
         <v>352</v>
       </c>
-      <c r="K2" s="18" t="s">
+      <c r="K2" s="17" t="s">
         <v>354</v>
       </c>
       <c r="L2" t="s" s="0">
         <v>353</v>
       </c>
-      <c r="M2" s="18" t="s">
+      <c r="M2" s="17" t="s">
         <v>356</v>
       </c>
       <c r="N2" t="s" s="0">
@@ -4583,8 +4577,8 @@
       <c r="E3" t="s" s="0">
         <v>17</v>
       </c>
-      <c r="F3" t="s" s="0">
-        <v>18</v>
+      <c r="F3" s="3" t="s">
+        <v>604</v>
       </c>
       <c r="G3" t="s" s="0">
         <v>94</v>
@@ -4624,8 +4618,8 @@
       <c r="E4" t="s" s="0">
         <v>17</v>
       </c>
-      <c r="F4" t="s" s="0">
-        <v>18</v>
+      <c r="F4" s="3" t="s">
+        <v>604</v>
       </c>
       <c r="G4" t="s" s="0">
         <v>390</v>
@@ -4665,8 +4659,8 @@
       <c r="E5" t="s" s="0">
         <v>17</v>
       </c>
-      <c r="F5" t="s" s="0">
-        <v>18</v>
+      <c r="F5" s="3" t="s">
+        <v>604</v>
       </c>
       <c r="G5" t="s" s="0">
         <v>391</v>
@@ -4706,8 +4700,8 @@
       <c r="E6" t="s" s="0">
         <v>17</v>
       </c>
-      <c r="F6" t="s" s="0">
-        <v>18</v>
+      <c r="F6" s="3" t="s">
+        <v>604</v>
       </c>
       <c r="G6" t="s" s="0">
         <v>392</v>
@@ -4747,8 +4741,8 @@
       <c r="E7" t="s" s="0">
         <v>17</v>
       </c>
-      <c r="F7" t="s" s="0">
-        <v>18</v>
+      <c r="F7" s="3" t="s">
+        <v>604</v>
       </c>
       <c r="G7" t="s" s="0">
         <v>393</v>
@@ -4788,8 +4782,8 @@
       <c r="E8" t="s" s="0">
         <v>17</v>
       </c>
-      <c r="F8" t="s" s="0">
-        <v>18</v>
+      <c r="F8" s="3" t="s">
+        <v>604</v>
       </c>
       <c r="G8" t="s" s="0">
         <v>394</v>
@@ -4829,8 +4823,8 @@
       <c r="E9" t="s" s="0">
         <v>17</v>
       </c>
-      <c r="F9" t="s" s="0">
-        <v>18</v>
+      <c r="F9" s="3" t="s">
+        <v>604</v>
       </c>
       <c r="G9" t="s" s="0">
         <v>395</v>
@@ -4870,8 +4864,8 @@
       <c r="E10" t="s" s="0">
         <v>17</v>
       </c>
-      <c r="F10" t="s" s="0">
-        <v>18</v>
+      <c r="F10" s="3" t="s">
+        <v>604</v>
       </c>
       <c r="G10" t="s" s="0">
         <v>396</v>
@@ -4911,8 +4905,8 @@
       <c r="E11" t="s" s="0">
         <v>17</v>
       </c>
-      <c r="F11" t="s" s="0">
-        <v>18</v>
+      <c r="F11" s="3" t="s">
+        <v>604</v>
       </c>
       <c r="G11" t="s" s="0">
         <v>397</v>
@@ -4945,8 +4939,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -4956,7 +4950,7 @@
     <col min="3" max="3" bestFit="true" customWidth="true" width="34.5546875"/>
     <col min="4" max="4" customWidth="true" width="40.33203125"/>
     <col min="5" max="5" customWidth="true" width="22.6640625"/>
-    <col min="6" max="6" customWidth="true" width="12.44140625"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="15.109375"/>
     <col min="7" max="7" customWidth="true" width="21.44140625"/>
     <col min="8" max="8" customWidth="true" width="21.33203125"/>
     <col min="9" max="9" customWidth="true" width="18.33203125"/>
@@ -5010,7 +5004,7 @@
         <v>65</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>18</v>
+        <v>604</v>
       </c>
       <c r="G2" t="s" s="0">
         <v>71</v>
@@ -5038,7 +5032,7 @@
         <v>65</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>18</v>
+        <v>604</v>
       </c>
       <c r="G3" t="s" s="0">
         <v>71</v>
@@ -5064,7 +5058,7 @@
         <v>65</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>18</v>
+        <v>604</v>
       </c>
       <c r="G4" t="s" s="0">
         <v>71</v>
@@ -5090,7 +5084,7 @@
         <v>65</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>18</v>
+        <v>604</v>
       </c>
       <c r="G5" t="s" s="0">
         <v>71</v>
@@ -5116,7 +5110,7 @@
         <v>65</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>18</v>
+        <v>604</v>
       </c>
       <c r="G6" t="s" s="0">
         <v>71</v>
@@ -5142,7 +5136,7 @@
         <v>65</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>18</v>
+        <v>604</v>
       </c>
       <c r="G7" t="s" s="0">
         <v>71</v>
@@ -5168,7 +5162,7 @@
         <v>65</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>18</v>
+        <v>604</v>
       </c>
       <c r="G8" t="s" s="0">
         <v>71</v>
@@ -5194,7 +5188,7 @@
         <v>65</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>18</v>
+        <v>604</v>
       </c>
       <c r="G9" t="s" s="0">
         <v>71</v>
@@ -5220,7 +5214,7 @@
         <v>65</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>18</v>
+        <v>604</v>
       </c>
       <c r="G10" t="s" s="0">
         <v>71</v>
@@ -5246,7 +5240,7 @@
         <v>65</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>18</v>
+        <v>604</v>
       </c>
       <c r="G11" t="s" s="0">
         <v>71</v>
@@ -5260,16 +5254,6 @@
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0A00-000000000000}"/>
     <hyperlink ref="E3:E11" r:id="rId2" display="aarosagarch@gmail.com" xr:uid="{00000000-0004-0000-0A00-000001000000}"/>
-    <hyperlink ref="F2" r:id="rId3" xr:uid="{00000000-0004-0000-0A00-000002000000}"/>
-    <hyperlink ref="F3" r:id="rId4" xr:uid="{00000000-0004-0000-0A00-000003000000}"/>
-    <hyperlink ref="F4" r:id="rId5" xr:uid="{00000000-0004-0000-0A00-000004000000}"/>
-    <hyperlink ref="F5" r:id="rId6" xr:uid="{00000000-0004-0000-0A00-000005000000}"/>
-    <hyperlink ref="F6" r:id="rId7" xr:uid="{00000000-0004-0000-0A00-000006000000}"/>
-    <hyperlink ref="F7" r:id="rId8" xr:uid="{00000000-0004-0000-0A00-000007000000}"/>
-    <hyperlink ref="F8" r:id="rId9" xr:uid="{00000000-0004-0000-0A00-000008000000}"/>
-    <hyperlink ref="F9" r:id="rId10" xr:uid="{00000000-0004-0000-0A00-000009000000}"/>
-    <hyperlink ref="F10" r:id="rId11" xr:uid="{00000000-0004-0000-0A00-00000A000000}"/>
-    <hyperlink ref="F11" r:id="rId12" xr:uid="{00000000-0004-0000-0A00-00000B000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -5281,7 +5265,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -5290,7 +5274,7 @@
     <col min="3" max="3" customWidth="true" width="26.0"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="24.44140625"/>
     <col min="5" max="5" bestFit="true" customWidth="true" width="10.6640625"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="11.33203125"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="15.109375"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -5330,7 +5314,7 @@
         <v>17</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>18</v>
+        <v>604</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -5350,7 +5334,7 @@
         <v>19</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>18</v>
+        <v>604</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -5370,7 +5354,7 @@
         <v>20</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>18</v>
+        <v>604</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -5390,7 +5374,7 @@
         <v>21</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>18</v>
+        <v>604</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -5410,7 +5394,7 @@
         <v>22</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>18</v>
+        <v>604</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -5430,7 +5414,7 @@
         <v>23</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>18</v>
+        <v>604</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -5450,7 +5434,7 @@
         <v>24</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>18</v>
+        <v>604</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -5470,7 +5454,7 @@
         <v>25</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>18</v>
+        <v>604</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -5490,7 +5474,7 @@
         <v>26</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>18</v>
+        <v>604</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -5510,15 +5494,11 @@
         <v>27</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>18</v>
+        <v>604</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="F3:F11" r:id="rId2" display="Admin@123" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -5528,7 +5508,7 @@
   <dimension ref="A1:O11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -5537,7 +5517,7 @@
     <col min="3" max="3" bestFit="true" customWidth="true" width="30.0"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="38.0"/>
     <col min="5" max="5" bestFit="true" customWidth="true" width="10.33203125"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="11.33203125"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="15.109375"/>
     <col min="7" max="7" bestFit="true" customWidth="true" width="9.6640625"/>
     <col min="8" max="8" bestFit="true" customWidth="true" width="9.44140625"/>
     <col min="9" max="9" bestFit="true" customWidth="true" width="25.44140625"/>
@@ -5611,7 +5591,7 @@
         <v>17</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>18</v>
+        <v>604</v>
       </c>
       <c r="G2" t="s" s="0">
         <v>39</v>
@@ -5658,7 +5638,7 @@
         <v>17</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>18</v>
+        <v>604</v>
       </c>
       <c r="I3" t="s" s="0">
         <v>56</v>
@@ -5696,7 +5676,7 @@
         <v>17</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>18</v>
+        <v>604</v>
       </c>
       <c r="I4" t="s" s="0">
         <v>57</v>
@@ -5734,7 +5714,7 @@
         <v>17</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>18</v>
+        <v>604</v>
       </c>
       <c r="I5" t="s" s="0">
         <v>59</v>
@@ -5769,7 +5749,7 @@
         <v>17</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>18</v>
+        <v>604</v>
       </c>
       <c r="G6" t="s" s="0">
         <v>153</v>
@@ -5813,7 +5793,7 @@
         <v>17</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>18</v>
+        <v>604</v>
       </c>
       <c r="J7" t="s" s="0">
         <v>46</v>
@@ -5842,7 +5822,7 @@
         <v>17</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>18</v>
+        <v>604</v>
       </c>
       <c r="N8" t="s" s="0">
         <v>54</v>
@@ -5865,7 +5845,7 @@
         <v>17</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>18</v>
+        <v>604</v>
       </c>
     </row>
     <row r="10" spans="1:15">
@@ -5885,7 +5865,7 @@
         <v>17</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>18</v>
+        <v>604</v>
       </c>
     </row>
     <row r="11" spans="1:15">
@@ -5905,23 +5885,11 @@
         <v>17</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>18</v>
+        <v>604</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
-    <hyperlink ref="F3" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
-    <hyperlink ref="F4" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
-    <hyperlink ref="F5" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
-    <hyperlink ref="F6" r:id="rId5" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
-    <hyperlink ref="F7" r:id="rId6" xr:uid="{00000000-0004-0000-0200-000005000000}"/>
-    <hyperlink ref="F8" r:id="rId7" xr:uid="{00000000-0004-0000-0200-000006000000}"/>
-    <hyperlink ref="F9" r:id="rId8" xr:uid="{00000000-0004-0000-0200-000007000000}"/>
-    <hyperlink ref="F10" r:id="rId9" xr:uid="{00000000-0004-0000-0200-000008000000}"/>
-    <hyperlink ref="F11" r:id="rId10" xr:uid="{00000000-0004-0000-0200-000009000000}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -5931,7 +5899,7 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -5940,7 +5908,7 @@
     <col min="3" max="3" bestFit="true" customWidth="true" width="25.109375"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="22.44140625"/>
     <col min="5" max="5" bestFit="true" customWidth="true" width="10.33203125"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="11.33203125"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="15.109375"/>
     <col min="7" max="7" bestFit="true" customWidth="true" width="14.6640625"/>
     <col min="8" max="8" bestFit="true" customWidth="true" width="18.6640625"/>
     <col min="9" max="9" bestFit="true" customWidth="true" width="11.33203125"/>
@@ -5996,7 +5964,7 @@
         <v>17</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>18</v>
+        <v>604</v>
       </c>
       <c r="G2" t="s" s="0">
         <v>94</v>
@@ -6008,7 +5976,7 @@
         <v>18</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>18</v>
+        <v>604</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -6028,7 +5996,7 @@
         <v>17</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>18</v>
+        <v>604</v>
       </c>
       <c r="G3" t="s" s="0">
         <v>391</v>
@@ -6037,7 +6005,7 @@
         <v>18</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>18</v>
+        <v>604</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -6057,7 +6025,7 @@
         <v>17</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>18</v>
+        <v>604</v>
       </c>
       <c r="G4" t="s" s="0">
         <v>394</v>
@@ -6066,7 +6034,7 @@
         <v>18</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>18</v>
+        <v>604</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -6086,7 +6054,7 @@
         <v>17</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>18</v>
+        <v>604</v>
       </c>
       <c r="G5" t="s" s="0">
         <v>393</v>
@@ -6095,7 +6063,7 @@
         <v>18</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>18</v>
+        <v>604</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -6115,7 +6083,7 @@
         <v>17</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>18</v>
+        <v>604</v>
       </c>
       <c r="G6" t="s" s="0">
         <v>392</v>
@@ -6124,7 +6092,7 @@
         <v>18</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>18</v>
+        <v>604</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -6144,7 +6112,7 @@
         <v>17</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>18</v>
+        <v>604</v>
       </c>
       <c r="G7" t="s" s="0">
         <v>393</v>
@@ -6153,7 +6121,7 @@
         <v>18</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>18</v>
+        <v>604</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -6173,7 +6141,7 @@
         <v>17</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>18</v>
+        <v>604</v>
       </c>
       <c r="G8" t="s" s="0">
         <v>518</v>
@@ -6182,7 +6150,7 @@
         <v>18</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>18</v>
+        <v>604</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -6202,7 +6170,7 @@
         <v>17</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>18</v>
+        <v>604</v>
       </c>
       <c r="G9" t="s" s="0">
         <v>395</v>
@@ -6211,7 +6179,7 @@
         <v>18</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>18</v>
+        <v>604</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -6231,7 +6199,7 @@
         <v>17</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>18</v>
+        <v>604</v>
       </c>
       <c r="G10" t="s" s="0">
         <v>395</v>
@@ -6240,7 +6208,7 @@
         <v>18</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>18</v>
+        <v>604</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -6260,7 +6228,7 @@
         <v>17</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>18</v>
+        <v>604</v>
       </c>
       <c r="G11" t="s" s="0">
         <v>519</v>
@@ -6269,34 +6237,22 @@
         <v>18</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>18</v>
+        <v>604</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
-    <hyperlink ref="I2" r:id="rId2" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
-    <hyperlink ref="J2" r:id="rId3" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
-    <hyperlink ref="F3:F11" r:id="rId4" display="Admin@123" xr:uid="{00000000-0004-0000-0300-000003000000}"/>
-    <hyperlink ref="I5" r:id="rId5" xr:uid="{00000000-0004-0000-0300-000004000000}"/>
-    <hyperlink ref="J5" r:id="rId6" xr:uid="{00000000-0004-0000-0300-000005000000}"/>
-    <hyperlink ref="I10" r:id="rId7" xr:uid="{00000000-0004-0000-0300-000006000000}"/>
-    <hyperlink ref="J10" r:id="rId8" xr:uid="{00000000-0004-0000-0300-000007000000}"/>
-    <hyperlink ref="I3" r:id="rId9" xr:uid="{00000000-0004-0000-0300-000008000000}"/>
-    <hyperlink ref="J3" r:id="rId10" xr:uid="{00000000-0004-0000-0300-000009000000}"/>
-    <hyperlink ref="I4" r:id="rId11" xr:uid="{00000000-0004-0000-0300-00000A000000}"/>
-    <hyperlink ref="J4" r:id="rId12" xr:uid="{00000000-0004-0000-0300-00000B000000}"/>
-    <hyperlink ref="I6" r:id="rId13" xr:uid="{00000000-0004-0000-0300-00000C000000}"/>
-    <hyperlink ref="J6" r:id="rId14" xr:uid="{00000000-0004-0000-0300-00000D000000}"/>
-    <hyperlink ref="I7" r:id="rId15" xr:uid="{00000000-0004-0000-0300-00000E000000}"/>
-    <hyperlink ref="J7" r:id="rId16" xr:uid="{00000000-0004-0000-0300-00000F000000}"/>
-    <hyperlink ref="I8" r:id="rId17" xr:uid="{00000000-0004-0000-0300-000010000000}"/>
-    <hyperlink ref="J8" r:id="rId18" xr:uid="{00000000-0004-0000-0300-000011000000}"/>
-    <hyperlink ref="I9" r:id="rId19" xr:uid="{00000000-0004-0000-0300-000012000000}"/>
-    <hyperlink ref="J9" r:id="rId20" xr:uid="{00000000-0004-0000-0300-000013000000}"/>
-    <hyperlink ref="I11" r:id="rId21" xr:uid="{00000000-0004-0000-0300-000014000000}"/>
-    <hyperlink ref="J11" r:id="rId22" xr:uid="{00000000-0004-0000-0300-000015000000}"/>
+    <hyperlink ref="I2" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
+    <hyperlink ref="I5" r:id="rId2" xr:uid="{00000000-0004-0000-0300-000004000000}"/>
+    <hyperlink ref="I10" r:id="rId3" xr:uid="{00000000-0004-0000-0300-000006000000}"/>
+    <hyperlink ref="I3" r:id="rId4" xr:uid="{00000000-0004-0000-0300-000008000000}"/>
+    <hyperlink ref="I4" r:id="rId5" xr:uid="{00000000-0004-0000-0300-00000A000000}"/>
+    <hyperlink ref="I6" r:id="rId6" xr:uid="{00000000-0004-0000-0300-00000C000000}"/>
+    <hyperlink ref="I7" r:id="rId7" xr:uid="{00000000-0004-0000-0300-00000E000000}"/>
+    <hyperlink ref="I8" r:id="rId8" xr:uid="{00000000-0004-0000-0300-000010000000}"/>
+    <hyperlink ref="I9" r:id="rId9" xr:uid="{00000000-0004-0000-0300-000012000000}"/>
+    <hyperlink ref="I11" r:id="rId10" xr:uid="{00000000-0004-0000-0300-000014000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6306,8 +6262,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:L17"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="14.4"/>
@@ -6317,7 +6273,7 @@
     <col min="3" max="3" bestFit="true" customWidth="true" style="8" width="30.6640625"/>
     <col min="4" max="4" bestFit="true" customWidth="true" style="8" width="39.33203125"/>
     <col min="5" max="5" bestFit="true" customWidth="true" style="8" width="10.44140625"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="8" width="11.6640625"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="8" width="15.109375"/>
     <col min="7" max="7" bestFit="true" customWidth="true" style="8" width="10.33203125"/>
     <col min="8" max="8" bestFit="true" customWidth="true" style="8" width="12.5546875"/>
     <col min="9" max="9" customWidth="true" style="8" width="15.0"/>
@@ -6327,7 +6283,7 @@
     <col min="13" max="16384" style="8" width="9.33203125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="28.8">
+    <row r="1" spans="1:12" ht="12.45" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -6365,7 +6321,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="28.8">
+    <row r="2" spans="1:12" ht="12.45" customHeight="1">
       <c r="A2" s="9" t="s">
         <v>5</v>
       </c>
@@ -6381,13 +6337,13 @@
       <c r="E2" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="11" t="s">
-        <v>18</v>
+      <c r="F2" s="3" t="s">
+        <v>604</v>
       </c>
       <c r="G2" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="H2" s="11" t="s">
         <v>82</v>
       </c>
       <c r="I2" s="10" t="s">
@@ -6403,7 +6359,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="28.8">
+    <row r="3" spans="1:12" ht="12.45" customHeight="1">
       <c r="A3" s="9" t="s">
         <v>6</v>
       </c>
@@ -6419,8 +6375,8 @@
       <c r="E3" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="11" t="s">
-        <v>18</v>
+      <c r="F3" s="3" t="s">
+        <v>604</v>
       </c>
       <c r="G3" s="10" t="s">
         <v>363</v>
@@ -6441,7 +6397,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="28.8">
+    <row r="4" spans="1:12" ht="12.45" customHeight="1">
       <c r="A4" s="9" t="s">
         <v>7</v>
       </c>
@@ -6457,13 +6413,13 @@
       <c r="E4" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="11" t="s">
-        <v>18</v>
+      <c r="F4" s="3" t="s">
+        <v>604</v>
       </c>
       <c r="G4" s="10" t="s">
         <v>364</v>
       </c>
-      <c r="H4" s="19" t="s">
+      <c r="H4" s="18" t="s">
         <v>373</v>
       </c>
       <c r="I4" s="10" t="s">
@@ -6479,7 +6435,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="28.8">
+    <row r="5" spans="1:12" ht="12.45" customHeight="1">
       <c r="A5" s="9" t="s">
         <v>8</v>
       </c>
@@ -6495,8 +6451,8 @@
       <c r="E5" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="11" t="s">
-        <v>18</v>
+      <c r="F5" s="3" t="s">
+        <v>604</v>
       </c>
       <c r="G5" s="10" t="s">
         <v>365</v>
@@ -6517,7 +6473,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="28.8">
+    <row r="6" spans="1:12" ht="12.45" customHeight="1">
       <c r="A6" s="9" t="s">
         <v>9</v>
       </c>
@@ -6533,8 +6489,8 @@
       <c r="E6" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="11" t="s">
-        <v>18</v>
+      <c r="F6" s="3" t="s">
+        <v>604</v>
       </c>
       <c r="G6" s="10" t="s">
         <v>366</v>
@@ -6555,7 +6511,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="28.8">
+    <row r="7" spans="1:12" ht="12.45" customHeight="1">
       <c r="A7" s="9" t="s">
         <v>10</v>
       </c>
@@ -6571,8 +6527,8 @@
       <c r="E7" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="F7" s="11" t="s">
-        <v>18</v>
+      <c r="F7" s="3" t="s">
+        <v>604</v>
       </c>
       <c r="G7" s="10" t="s">
         <v>367</v>
@@ -6593,7 +6549,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="28.8">
+    <row r="8" spans="1:12" ht="12.45" customHeight="1">
       <c r="A8" s="9" t="s">
         <v>11</v>
       </c>
@@ -6609,8 +6565,8 @@
       <c r="E8" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="F8" s="11" t="s">
-        <v>18</v>
+      <c r="F8" s="3" t="s">
+        <v>604</v>
       </c>
       <c r="G8" s="10" t="s">
         <v>368</v>
@@ -6631,7 +6587,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="28.8">
+    <row r="9" spans="1:12" ht="12.45" customHeight="1">
       <c r="A9" s="9" t="s">
         <v>12</v>
       </c>
@@ -6647,8 +6603,8 @@
       <c r="E9" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="F9" s="11" t="s">
-        <v>18</v>
+      <c r="F9" s="3" t="s">
+        <v>604</v>
       </c>
       <c r="G9" s="10" t="s">
         <v>369</v>
@@ -6669,7 +6625,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="28.8">
+    <row r="10" spans="1:12" ht="12.45" customHeight="1">
       <c r="A10" s="9" t="s">
         <v>13</v>
       </c>
@@ -6685,8 +6641,8 @@
       <c r="E10" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="F10" s="11" t="s">
-        <v>18</v>
+      <c r="F10" s="3" t="s">
+        <v>604</v>
       </c>
       <c r="G10" s="10" t="s">
         <v>370</v>
@@ -6707,7 +6663,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="28.8">
+    <row r="11" spans="1:12" ht="12.45" customHeight="1">
       <c r="A11" s="9" t="s">
         <v>14</v>
       </c>
@@ -6723,8 +6679,8 @@
       <c r="E11" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="F11" s="11" t="s">
-        <v>18</v>
+      <c r="F11" s="3" t="s">
+        <v>604</v>
       </c>
       <c r="G11" s="10" t="s">
         <v>371</v>
@@ -6746,24 +6702,12 @@
       </c>
     </row>
     <row r="17" spans="7:7">
-      <c r="G17" s="16"/>
+      <c r="G17" s="15"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="F11" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
-    <hyperlink ref="F10" r:id="rId2" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
-    <hyperlink ref="F9" r:id="rId3" xr:uid="{00000000-0004-0000-0400-000002000000}"/>
-    <hyperlink ref="F8" r:id="rId4" xr:uid="{00000000-0004-0000-0400-000003000000}"/>
-    <hyperlink ref="F7" r:id="rId5" xr:uid="{00000000-0004-0000-0400-000004000000}"/>
-    <hyperlink ref="F6" r:id="rId6" xr:uid="{00000000-0004-0000-0400-000005000000}"/>
-    <hyperlink ref="F5" r:id="rId7" xr:uid="{00000000-0004-0000-0400-000006000000}"/>
-    <hyperlink ref="F4" r:id="rId8" xr:uid="{00000000-0004-0000-0400-000007000000}"/>
-    <hyperlink ref="F3" r:id="rId9" xr:uid="{00000000-0004-0000-0400-000008000000}"/>
-    <hyperlink ref="F2" r:id="rId10" xr:uid="{00000000-0004-0000-0400-000009000000}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId11"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -6772,7 +6716,7 @@
   <dimension ref="A1:P11"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -6781,7 +6725,7 @@
     <col min="3" max="3" bestFit="true" customWidth="true" width="33.88671875"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="30.109375"/>
     <col min="5" max="5" bestFit="true" customWidth="true" width="22.33203125"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="11.33203125"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="15.109375"/>
     <col min="7" max="8" bestFit="true" customWidth="true" width="9.88671875"/>
     <col min="9" max="9" bestFit="true" customWidth="true" width="17.6640625"/>
     <col min="10" max="10" bestFit="true" customWidth="true" width="20.77734375"/>
@@ -6860,7 +6804,7 @@
         <v>65</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>18</v>
+        <v>604</v>
       </c>
       <c r="G2" t="s" s="0">
         <v>504</v>
@@ -6910,7 +6854,7 @@
         <v>65</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>18</v>
+        <v>604</v>
       </c>
       <c r="G3" t="s" s="0">
         <v>520</v>
@@ -6960,7 +6904,7 @@
         <v>65</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>18</v>
+        <v>604</v>
       </c>
       <c r="G4" t="s" s="0">
         <v>527</v>
@@ -7010,7 +6954,7 @@
         <v>65</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>18</v>
+        <v>604</v>
       </c>
       <c r="G5" t="s" s="0">
         <v>533</v>
@@ -7060,7 +7004,7 @@
         <v>65</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>18</v>
+        <v>604</v>
       </c>
       <c r="G6" t="s" s="0">
         <v>541</v>
@@ -7110,7 +7054,7 @@
         <v>65</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>18</v>
+        <v>604</v>
       </c>
       <c r="G7" t="s" s="0">
         <v>548</v>
@@ -7160,7 +7104,7 @@
         <v>65</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>18</v>
+        <v>604</v>
       </c>
       <c r="G8" t="s" s="0">
         <v>557</v>
@@ -7210,7 +7154,7 @@
         <v>65</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>18</v>
+        <v>604</v>
       </c>
       <c r="G9" t="s" s="0">
         <v>567</v>
@@ -7260,7 +7204,7 @@
         <v>65</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>18</v>
+        <v>604</v>
       </c>
       <c r="G10" t="s" s="0">
         <v>577</v>
@@ -7310,7 +7254,7 @@
         <v>65</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>18</v>
+        <v>604</v>
       </c>
       <c r="G11" t="s" s="0">
         <v>586</v>
@@ -7347,39 +7291,29 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
-    <hyperlink ref="F2" r:id="rId2" xr:uid="{00000000-0004-0000-0500-000001000000}"/>
-    <hyperlink ref="E3" r:id="rId3" xr:uid="{00000000-0004-0000-0500-000002000000}"/>
-    <hyperlink ref="E4" r:id="rId4" xr:uid="{00000000-0004-0000-0500-000003000000}"/>
-    <hyperlink ref="E5" r:id="rId5" xr:uid="{00000000-0004-0000-0500-000004000000}"/>
-    <hyperlink ref="E6" r:id="rId6" xr:uid="{00000000-0004-0000-0500-000005000000}"/>
-    <hyperlink ref="E7" r:id="rId7" xr:uid="{00000000-0004-0000-0500-000006000000}"/>
-    <hyperlink ref="E8" r:id="rId8" xr:uid="{00000000-0004-0000-0500-000007000000}"/>
-    <hyperlink ref="E9" r:id="rId9" xr:uid="{00000000-0004-0000-0500-000008000000}"/>
-    <hyperlink ref="E10" r:id="rId10" xr:uid="{00000000-0004-0000-0500-000009000000}"/>
-    <hyperlink ref="E11" r:id="rId11" xr:uid="{00000000-0004-0000-0500-00000A000000}"/>
-    <hyperlink ref="F3" r:id="rId12" xr:uid="{00000000-0004-0000-0500-00000B000000}"/>
-    <hyperlink ref="F4" r:id="rId13" xr:uid="{00000000-0004-0000-0500-00000C000000}"/>
-    <hyperlink ref="F5" r:id="rId14" xr:uid="{00000000-0004-0000-0500-00000D000000}"/>
-    <hyperlink ref="F6" r:id="rId15" xr:uid="{00000000-0004-0000-0500-00000E000000}"/>
-    <hyperlink ref="F7" r:id="rId16" xr:uid="{00000000-0004-0000-0500-00000F000000}"/>
-    <hyperlink ref="F8" r:id="rId17" xr:uid="{00000000-0004-0000-0500-000010000000}"/>
-    <hyperlink ref="F9" r:id="rId18" xr:uid="{00000000-0004-0000-0500-000011000000}"/>
-    <hyperlink ref="F10" r:id="rId19" xr:uid="{00000000-0004-0000-0500-000012000000}"/>
-    <hyperlink ref="F11" r:id="rId20" xr:uid="{00000000-0004-0000-0500-000013000000}"/>
-    <hyperlink ref="I3" r:id="rId21" xr:uid="{C81A3971-6034-4FA6-AD62-602659446BEA}"/>
-    <hyperlink ref="I4" r:id="rId22" xr:uid="{50D524F0-DAA2-4AFC-9FD2-5F1256FF0E23}"/>
-    <hyperlink ref="I5" r:id="rId23" xr:uid="{0DC85489-444B-47B8-92A0-845D4B4627BE}"/>
-    <hyperlink ref="I6" r:id="rId24" xr:uid="{79F23829-991F-42A6-B569-17DAD72BCA52}"/>
-    <hyperlink ref="J6" r:id="rId25" display="Roland@test.org" xr:uid="{F833B56F-A773-41B2-8C5A-4F16C9F1E6DA}"/>
-    <hyperlink ref="I7" r:id="rId26" xr:uid="{A9242B6A-3D43-472B-9E0C-E3FA9A74F3B3}"/>
-    <hyperlink ref="J7" r:id="rId27" display="Pontes@test.org" xr:uid="{0845BDEB-BF3B-405B-B45C-D6BBF8B66543}"/>
-    <hyperlink ref="I8" r:id="rId28" xr:uid="{BF376FC5-5CAD-44FA-A34D-2BEF6E7CF391}"/>
-    <hyperlink ref="I9" r:id="rId29" xr:uid="{6984E062-BA00-4CB1-BA56-5B7A334891FB}"/>
-    <hyperlink ref="I10" r:id="rId30" xr:uid="{CB379D73-899C-4760-842D-38F41CCF882A}"/>
-    <hyperlink ref="I11" r:id="rId31" xr:uid="{77D1F26A-2C1D-4A88-AE76-6C57C6317DD5}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{00000000-0004-0000-0500-000002000000}"/>
+    <hyperlink ref="E4" r:id="rId3" xr:uid="{00000000-0004-0000-0500-000003000000}"/>
+    <hyperlink ref="E5" r:id="rId4" xr:uid="{00000000-0004-0000-0500-000004000000}"/>
+    <hyperlink ref="E6" r:id="rId5" xr:uid="{00000000-0004-0000-0500-000005000000}"/>
+    <hyperlink ref="E7" r:id="rId6" xr:uid="{00000000-0004-0000-0500-000006000000}"/>
+    <hyperlink ref="E8" r:id="rId7" xr:uid="{00000000-0004-0000-0500-000007000000}"/>
+    <hyperlink ref="E9" r:id="rId8" xr:uid="{00000000-0004-0000-0500-000008000000}"/>
+    <hyperlink ref="E10" r:id="rId9" xr:uid="{00000000-0004-0000-0500-000009000000}"/>
+    <hyperlink ref="E11" r:id="rId10" xr:uid="{00000000-0004-0000-0500-00000A000000}"/>
+    <hyperlink ref="I3" r:id="rId11" xr:uid="{C81A3971-6034-4FA6-AD62-602659446BEA}"/>
+    <hyperlink ref="I4" r:id="rId12" xr:uid="{50D524F0-DAA2-4AFC-9FD2-5F1256FF0E23}"/>
+    <hyperlink ref="I5" r:id="rId13" xr:uid="{0DC85489-444B-47B8-92A0-845D4B4627BE}"/>
+    <hyperlink ref="I6" r:id="rId14" xr:uid="{79F23829-991F-42A6-B569-17DAD72BCA52}"/>
+    <hyperlink ref="J6" r:id="rId15" display="Roland@test.org" xr:uid="{F833B56F-A773-41B2-8C5A-4F16C9F1E6DA}"/>
+    <hyperlink ref="I7" r:id="rId16" xr:uid="{A9242B6A-3D43-472B-9E0C-E3FA9A74F3B3}"/>
+    <hyperlink ref="J7" r:id="rId17" display="Pontes@test.org" xr:uid="{0845BDEB-BF3B-405B-B45C-D6BBF8B66543}"/>
+    <hyperlink ref="I8" r:id="rId18" xr:uid="{BF376FC5-5CAD-44FA-A34D-2BEF6E7CF391}"/>
+    <hyperlink ref="I9" r:id="rId19" xr:uid="{6984E062-BA00-4CB1-BA56-5B7A334891FB}"/>
+    <hyperlink ref="I10" r:id="rId20" xr:uid="{CB379D73-899C-4760-842D-38F41CCF882A}"/>
+    <hyperlink ref="I11" r:id="rId21" xr:uid="{77D1F26A-2C1D-4A88-AE76-6C57C6317DD5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId32"/>
+  <pageSetup orientation="portrait" r:id="rId22"/>
 </worksheet>
 </file>
 
@@ -7388,7 +7322,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="F3" sqref="F3:F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -7397,7 +7331,7 @@
     <col min="3" max="3" bestFit="true" customWidth="true" width="28.0"/>
     <col min="4" max="4" customWidth="true" width="34.0"/>
     <col min="5" max="5" customWidth="true" width="23.0"/>
-    <col min="6" max="6" customWidth="true" width="11.33203125"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="15.109375"/>
     <col min="7" max="7" bestFit="true" customWidth="true" width="21.33203125"/>
   </cols>
   <sheetData>
@@ -7441,7 +7375,7 @@
         <v>65</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>18</v>
+        <v>604</v>
       </c>
       <c r="G2" t="s" s="0">
         <v>513</v>
@@ -7464,7 +7398,7 @@
         <v>65</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>18</v>
+        <v>604</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -7484,7 +7418,7 @@
         <v>65</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>18</v>
+        <v>604</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -7504,7 +7438,7 @@
         <v>65</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>18</v>
+        <v>604</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -7524,7 +7458,7 @@
         <v>65</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>18</v>
+        <v>604</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -7544,7 +7478,7 @@
         <v>65</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>18</v>
+        <v>604</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -7564,7 +7498,7 @@
         <v>65</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>18</v>
+        <v>604</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -7584,7 +7518,7 @@
         <v>65</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>18</v>
+        <v>604</v>
       </c>
       <c r="G9" t="s" s="0">
         <v>340</v>
@@ -7607,7 +7541,7 @@
         <v>65</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>18</v>
+        <v>604</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -7627,7 +7561,7 @@
         <v>65</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>18</v>
+        <v>604</v>
       </c>
     </row>
   </sheetData>
@@ -7635,19 +7569,9 @@
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
     <hyperlink ref="E3:E11" r:id="rId2" display="aarosagarch@gmail.com" xr:uid="{00000000-0004-0000-0600-000001000000}"/>
-    <hyperlink ref="F2" r:id="rId3" xr:uid="{00000000-0004-0000-0600-000002000000}"/>
-    <hyperlink ref="F3" r:id="rId4" xr:uid="{00000000-0004-0000-0600-000003000000}"/>
-    <hyperlink ref="F4" r:id="rId5" xr:uid="{00000000-0004-0000-0600-000004000000}"/>
-    <hyperlink ref="F5" r:id="rId6" xr:uid="{00000000-0004-0000-0600-000005000000}"/>
-    <hyperlink ref="F6" r:id="rId7" xr:uid="{00000000-0004-0000-0600-000006000000}"/>
-    <hyperlink ref="F7" r:id="rId8" xr:uid="{00000000-0004-0000-0600-000007000000}"/>
-    <hyperlink ref="F8" r:id="rId9" xr:uid="{00000000-0004-0000-0600-000008000000}"/>
-    <hyperlink ref="F9" r:id="rId10" xr:uid="{00000000-0004-0000-0600-000009000000}"/>
-    <hyperlink ref="F10" r:id="rId11" xr:uid="{00000000-0004-0000-0600-00000A000000}"/>
-    <hyperlink ref="F11" r:id="rId12" xr:uid="{00000000-0004-0000-0600-00000B000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId13"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -7656,7 +7580,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -7713,7 +7637,7 @@
         <v>65</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>18</v>
+        <v>604</v>
       </c>
       <c r="G2" t="s" s="0">
         <v>514</v>
@@ -7739,7 +7663,7 @@
         <v>65</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>18</v>
+        <v>604</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -7759,7 +7683,7 @@
         <v>65</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>18</v>
+        <v>604</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -7779,7 +7703,7 @@
         <v>65</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>18</v>
+        <v>604</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -7799,7 +7723,7 @@
         <v>65</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>18</v>
+        <v>604</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -7819,7 +7743,7 @@
         <v>65</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>18</v>
+        <v>604</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -7839,7 +7763,7 @@
         <v>65</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>18</v>
+        <v>604</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -7859,7 +7783,7 @@
         <v>65</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>18</v>
+        <v>604</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -7879,7 +7803,7 @@
         <v>65</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>18</v>
+        <v>604</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -7899,7 +7823,7 @@
         <v>65</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>18</v>
+        <v>604</v>
       </c>
     </row>
   </sheetData>
@@ -7907,19 +7831,9 @@
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0700-000000000000}"/>
     <hyperlink ref="E3:E11" r:id="rId2" display="aarosagarch@gmail.com" xr:uid="{00000000-0004-0000-0700-000001000000}"/>
-    <hyperlink ref="F2" r:id="rId3" xr:uid="{00000000-0004-0000-0700-000002000000}"/>
-    <hyperlink ref="F3" r:id="rId4" xr:uid="{00000000-0004-0000-0700-000003000000}"/>
-    <hyperlink ref="F4" r:id="rId5" xr:uid="{00000000-0004-0000-0700-000004000000}"/>
-    <hyperlink ref="F5" r:id="rId6" xr:uid="{00000000-0004-0000-0700-000005000000}"/>
-    <hyperlink ref="F6" r:id="rId7" xr:uid="{00000000-0004-0000-0700-000006000000}"/>
-    <hyperlink ref="F7" r:id="rId8" xr:uid="{00000000-0004-0000-0700-000007000000}"/>
-    <hyperlink ref="F8" r:id="rId9" xr:uid="{00000000-0004-0000-0700-000008000000}"/>
-    <hyperlink ref="F9" r:id="rId10" xr:uid="{00000000-0004-0000-0700-000009000000}"/>
-    <hyperlink ref="F10" r:id="rId11" xr:uid="{00000000-0004-0000-0700-00000A000000}"/>
-    <hyperlink ref="F11" r:id="rId12" xr:uid="{00000000-0004-0000-0700-00000B000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId13"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -7928,7 +7842,7 @@
   <dimension ref="A1:R11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -7938,8 +7852,7 @@
     <col min="3" max="3" bestFit="true" customWidth="true" width="28.5546875"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="35.44140625"/>
     <col min="5" max="5" bestFit="true" customWidth="true" width="9.77734375"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="10.88671875"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="13.33203125"/>
+    <col min="6" max="7" bestFit="true" customWidth="true" width="15.109375"/>
     <col min="8" max="8" bestFit="true" customWidth="true" width="25.0"/>
     <col min="9" max="9" bestFit="true" customWidth="true" width="10.5546875"/>
     <col min="10" max="10" bestFit="true" customWidth="true" width="10.88671875"/>
@@ -8027,10 +7940,10 @@
         <v>17</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>18</v>
+        <v>604</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>18</v>
+        <v>604</v>
       </c>
       <c r="H2" t="s" s="0">
         <v>434</v>
@@ -8077,10 +7990,10 @@
         <v>17</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>18</v>
+        <v>604</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>18</v>
+        <v>604</v>
       </c>
       <c r="H3" t="s" s="0">
         <v>440</v>
@@ -8127,10 +8040,10 @@
         <v>17</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>18</v>
+        <v>604</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>18</v>
+        <v>604</v>
       </c>
       <c r="H4" t="s" s="0">
         <v>448</v>
@@ -8177,10 +8090,10 @@
         <v>17</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>18</v>
+        <v>604</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>18</v>
+        <v>604</v>
       </c>
       <c r="H5" t="s" s="0">
         <v>455</v>
@@ -8227,10 +8140,10 @@
         <v>17</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>18</v>
+        <v>604</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>18</v>
+        <v>604</v>
       </c>
       <c r="H6" t="s" s="0">
         <v>461</v>
@@ -8277,10 +8190,10 @@
         <v>17</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>18</v>
+        <v>604</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>18</v>
+        <v>604</v>
       </c>
       <c r="H7" t="s" s="0">
         <v>468</v>
@@ -8327,10 +8240,10 @@
         <v>17</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>18</v>
+        <v>604</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>18</v>
+        <v>604</v>
       </c>
       <c r="H8" t="s" s="0">
         <v>475</v>
@@ -8377,10 +8290,10 @@
         <v>17</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>18</v>
+        <v>604</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>18</v>
+        <v>604</v>
       </c>
       <c r="H9" t="s" s="0">
         <v>481</v>
@@ -8427,10 +8340,10 @@
         <v>17</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>18</v>
+        <v>604</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>18</v>
+        <v>604</v>
       </c>
       <c r="H10" t="s" s="0">
         <v>487</v>
@@ -8477,10 +8390,10 @@
         <v>17</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>18</v>
+        <v>604</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>18</v>
+        <v>604</v>
       </c>
       <c r="H11" t="s" s="0">
         <v>493</v>
@@ -8511,28 +8424,6 @@
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{78E85523-8B8A-4FF8-B6DF-6ABCE4E261E9}"/>
-    <hyperlink ref="F3" r:id="rId2" xr:uid="{E48B2A5D-D234-49F1-A02D-AE64AB904F50}"/>
-    <hyperlink ref="F4" r:id="rId3" xr:uid="{2C39E39E-299F-4027-940A-542CFC54072F}"/>
-    <hyperlink ref="F5" r:id="rId4" xr:uid="{AAE88B86-3045-4C48-95D9-F2329F8D3B01}"/>
-    <hyperlink ref="F6" r:id="rId5" xr:uid="{F4540133-98D1-4054-BF38-A1AF32ED8764}"/>
-    <hyperlink ref="F7" r:id="rId6" xr:uid="{F3A59499-D0FD-41AD-9ABE-9E5FC3A2FD44}"/>
-    <hyperlink ref="F8" r:id="rId7" xr:uid="{1FDEBF05-2230-4EE4-83EE-0221B604CB87}"/>
-    <hyperlink ref="F9" r:id="rId8" xr:uid="{5E6FD6C0-5956-4587-9EB2-D47ADDFD745E}"/>
-    <hyperlink ref="F10" r:id="rId9" xr:uid="{52A939E6-D591-4FEF-A54E-07F3CDA3A09E}"/>
-    <hyperlink ref="F11" r:id="rId10" xr:uid="{0B2AE72D-1EF9-4476-AFF0-336AE0308108}"/>
-    <hyperlink ref="G2" r:id="rId11" xr:uid="{BD8B8265-F352-47AE-9076-6B44DA2677DF}"/>
-    <hyperlink ref="G3" r:id="rId12" xr:uid="{04378621-8AE5-41AB-8CF2-4EF376DE5F0C}"/>
-    <hyperlink ref="G4" r:id="rId13" xr:uid="{7564CCDB-C77B-413C-8836-0F1AC55A8223}"/>
-    <hyperlink ref="G5" r:id="rId14" xr:uid="{E9581CF5-C3A9-499D-8AD4-A3BD3113469A}"/>
-    <hyperlink ref="G6" r:id="rId15" xr:uid="{17E6F055-AE50-4BED-A201-FDA4A1D69947}"/>
-    <hyperlink ref="G7" r:id="rId16" xr:uid="{EA7D1214-B1B4-4111-AD55-94599FEB2DD2}"/>
-    <hyperlink ref="G8" r:id="rId17" xr:uid="{3A107175-E3E7-4550-B5B7-93E7156C1578}"/>
-    <hyperlink ref="G9" r:id="rId18" xr:uid="{C3AABCB5-54F3-4DF3-8EFB-CD61E89E2AD1}"/>
-    <hyperlink ref="G10" r:id="rId19" xr:uid="{8192347F-20CC-446E-BDE5-C45304623151}"/>
-    <hyperlink ref="G11" r:id="rId20" xr:uid="{3F4D9A79-3837-46A0-BB79-B25F57D926A7}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Code Refactoring of TDD testcases is completed
</commit_message>
<xml_diff>
--- a/src/main/resources/AutomationCatalogue_Batch41_TestData.xlsx
+++ b/src/main/resources/AutomationCatalogue_Batch41_TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AutomationCatalogue\Projects\TestAutomationCatalogue_Batch41\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{791E0DA8-C841-4E61-AB82-F7AA4F2D5FE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A45A4F84-7729-4CE1-A10F-EC725EBED5B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="944" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="944" firstSheet="4" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="10" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="819" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="849" uniqueCount="325">
   <si>
     <t>S. No</t>
   </si>
@@ -220,12 +220,6 @@
     <t xml:space="preserve"> DemoWebshop Application TotalOrders</t>
   </si>
   <si>
-    <t>TotalNumberOfOrders</t>
-  </si>
-  <si>
-    <t>SumOfAllOrders</t>
-  </si>
-  <si>
     <t xml:space="preserve"> DemoWebshop Application ApplyDisscount</t>
   </si>
   <si>
@@ -745,18 +739,12 @@
     <t>On Hold</t>
   </si>
   <si>
-    <t>Order number: 1505346</t>
-  </si>
-  <si>
     <t>415</t>
   </si>
   <si>
     <t>60416.195</t>
   </si>
   <si>
-    <t>Order number: 1505347</t>
-  </si>
-  <si>
     <t>Order number: 1505349</t>
   </si>
   <si>
@@ -808,160 +796,220 @@
     <t>Approved All these goals as they are relevant</t>
   </si>
   <si>
+    <t>QWRtaW5AMTIz</t>
+  </si>
+  <si>
+    <t>OrangeHRM Create and Verify Goal Status</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Christoper  Cooper </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dominic  Chase </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ralph  Edwards </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aaron  Hamilton </t>
+  </si>
+  <si>
+    <t>TC07-01</t>
+  </si>
+  <si>
+    <t>TC07-02</t>
+  </si>
+  <si>
+    <t>TC07-03</t>
+  </si>
+  <si>
+    <t>TC07-04</t>
+  </si>
+  <si>
+    <t>TC07-05</t>
+  </si>
+  <si>
+    <t>TC08-01</t>
+  </si>
+  <si>
+    <t>TC08-02</t>
+  </si>
+  <si>
+    <t>TC08-03</t>
+  </si>
+  <si>
+    <t>TC08-04</t>
+  </si>
+  <si>
+    <t>TC08-05</t>
+  </si>
+  <si>
+    <t>TC09-01</t>
+  </si>
+  <si>
+    <t>TC09-02</t>
+  </si>
+  <si>
+    <t>TC09-03</t>
+  </si>
+  <si>
+    <t>TC09-04</t>
+  </si>
+  <si>
+    <t>TC09-05</t>
+  </si>
+  <si>
+    <t>TC05_OrangeHRM_Goals</t>
+  </si>
+  <si>
+    <t>TC06_DemoWebShop_CreateAddress</t>
+  </si>
+  <si>
+    <t>TC07_DemoWebshop_ReOrder</t>
+  </si>
+  <si>
+    <t>TC08_DemoWebshop_TotalOrders</t>
+  </si>
+  <si>
+    <t>TC09_DemoWebshop_UpdateShoppingCart</t>
+  </si>
+  <si>
+    <t>TC10_DemoWebshop_ApplyDiscount</t>
+  </si>
+  <si>
+    <t>Title is not matched</t>
+  </si>
+  <si>
+    <t>Mobile Number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alice  Duval </t>
+  </si>
+  <si>
+    <t>0140</t>
+  </si>
+  <si>
+    <t>florene.rice</t>
+  </si>
+  <si>
+    <t>4104528605</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>Vince</t>
+  </si>
+  <si>
+    <t>Bednar</t>
+  </si>
+  <si>
+    <t>OOvwNdyn@test.org</t>
+  </si>
+  <si>
+    <t>Lesch LLC</t>
+  </si>
+  <si>
+    <t>Zambia</t>
+  </si>
+  <si>
+    <t>Other (Non US)</t>
+  </si>
+  <si>
+    <t>Port Lyndiaton</t>
+  </si>
+  <si>
+    <t>92436</t>
+  </si>
+  <si>
+    <t>10602 Jenni Harbors</t>
+  </si>
+  <si>
+    <t>AW</t>
+  </si>
+  <si>
+    <t>368-996-5809</t>
+  </si>
+  <si>
+    <t>12410249</t>
+  </si>
+  <si>
+    <t>Order number: 1546333</t>
+  </si>
+  <si>
+    <t>538</t>
+  </si>
+  <si>
+    <t>180447.7</t>
+  </si>
+  <si>
+    <t>Order number: 1547636</t>
+  </si>
+  <si>
+    <t>Order number: 1547643</t>
+  </si>
+  <si>
+    <t>0141</t>
+  </si>
+  <si>
     <t>FAILED</t>
   </si>
   <si>
-    <t>QWRtaW5AMTIz</t>
-  </si>
-  <si>
-    <t>OrangeHRM Create and Verify Goal Status</t>
-  </si>
-  <si>
-    <t>Comments</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Christoper  Cooper </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dominic  Chase </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ralph  Edwards </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aaron  Hamilton </t>
-  </si>
-  <si>
-    <t>TC07-01</t>
-  </si>
-  <si>
-    <t>TC07-02</t>
-  </si>
-  <si>
-    <t>TC07-03</t>
-  </si>
-  <si>
-    <t>TC07-04</t>
-  </si>
-  <si>
-    <t>TC07-05</t>
-  </si>
-  <si>
-    <t>TC08-01</t>
-  </si>
-  <si>
-    <t>TC08-02</t>
-  </si>
-  <si>
-    <t>TC08-03</t>
-  </si>
-  <si>
-    <t>TC08-04</t>
-  </si>
-  <si>
-    <t>TC08-05</t>
-  </si>
-  <si>
-    <t>TC09-01</t>
-  </si>
-  <si>
-    <t>TC09-02</t>
-  </si>
-  <si>
-    <t>TC09-03</t>
-  </si>
-  <si>
-    <t>TC09-04</t>
-  </si>
-  <si>
-    <t>TC09-05</t>
-  </si>
-  <si>
-    <t>TC05_OrangeHRM_Goals</t>
-  </si>
-  <si>
-    <t>TC06_DemoWebShop_CreateAddress</t>
-  </si>
-  <si>
-    <t>TC07_DemoWebshop_ReOrder</t>
-  </si>
-  <si>
-    <t>TC08_DemoWebshop_TotalOrders</t>
-  </si>
-  <si>
-    <t>TC09_DemoWebshop_UpdateShoppingCart</t>
-  </si>
-  <si>
-    <t>TC10_DemoWebshop_ApplyDiscount</t>
-  </si>
-  <si>
-    <t>Title is not matched</t>
-  </si>
-  <si>
-    <t>Mobile Number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alice  Duval </t>
-  </si>
-  <si>
-    <t>0140</t>
-  </si>
-  <si>
-    <t>florene.rice</t>
-  </si>
-  <si>
-    <t>4104528605</t>
-  </si>
-  <si>
-    <t>Country</t>
-  </si>
-  <si>
-    <t>State</t>
-  </si>
-  <si>
-    <t>Vince</t>
-  </si>
-  <si>
-    <t>Bednar</t>
-  </si>
-  <si>
-    <t>OOvwNdyn@test.org</t>
-  </si>
-  <si>
-    <t>Lesch LLC</t>
-  </si>
-  <si>
-    <t>Zambia</t>
-  </si>
-  <si>
-    <t>Other (Non US)</t>
-  </si>
-  <si>
-    <t>Port Lyndiaton</t>
-  </si>
-  <si>
-    <t>92436</t>
-  </si>
-  <si>
-    <t>10602 Jenni Harbors</t>
-  </si>
-  <si>
-    <t>AW</t>
-  </si>
-  <si>
-    <t>368-996-5809</t>
-  </si>
-  <si>
-    <t>12410249</t>
-  </si>
-  <si>
-    <t>Order number: 1546333</t>
-  </si>
-  <si>
-    <t>538</t>
-  </si>
-  <si>
-    <t>180447.7</t>
+    <t>2426454497</t>
+  </si>
+  <si>
+    <t>Abraham</t>
+  </si>
+  <si>
+    <t>Greenholt</t>
+  </si>
+  <si>
+    <t>uhDFkejK@test.org</t>
+  </si>
+  <si>
+    <t>Dietrich LLC</t>
+  </si>
+  <si>
+    <t>Hungary</t>
+  </si>
+  <si>
+    <t>Ricebury</t>
+  </si>
+  <si>
+    <t>519</t>
+  </si>
+  <si>
+    <t>2409 Florinda Alley</t>
+  </si>
+  <si>
+    <t>BD</t>
+  </si>
+  <si>
+    <t>103.731.0786</t>
+  </si>
+  <si>
+    <t>02603218</t>
+  </si>
+  <si>
+    <t>Order number: 1547646</t>
+  </si>
+  <si>
+    <t>550</t>
+  </si>
+  <si>
+    <t>184332.7</t>
+  </si>
+  <si>
+    <t>Order number: 1547649</t>
+  </si>
+  <si>
+    <t>Order number: 1547650</t>
   </si>
 </sst>
 </file>
@@ -1406,30 +1454,30 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>257</v>
+        <v>186</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="7" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
@@ -1443,7 +1491,7 @@
         <v>5</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C3" t="s" s="0">
         <v>15</v>
@@ -1452,7 +1500,7 @@
         <v>16</v>
       </c>
       <c r="F3" t="s" s="0">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -1460,7 +1508,7 @@
         <v>6</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C4" t="s" s="0">
         <v>15</v>
@@ -1474,7 +1522,7 @@
         <v>7</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C5" t="s" s="0">
         <v>15</v>
@@ -1483,7 +1531,7 @@
         <v>16</v>
       </c>
       <c r="E5" t="s" s="0">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -1491,7 +1539,7 @@
         <v>8</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C6" t="s" s="0">
         <v>15</v>
@@ -1505,7 +1553,7 @@
         <v>9</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C7" t="s" s="0">
         <v>15</v>
@@ -1516,7 +1564,7 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
@@ -1530,7 +1578,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C9" t="s" s="0">
         <v>31</v>
@@ -1539,7 +1587,7 @@
         <v>32</v>
       </c>
       <c r="F9" t="s" s="0">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -1547,7 +1595,7 @@
         <v>11</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C10" t="s" s="0">
         <v>31</v>
@@ -1561,7 +1609,7 @@
         <v>12</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C11" t="s" s="0">
         <v>31</v>
@@ -1575,7 +1623,7 @@
         <v>13</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C12" t="s" s="0">
         <v>31</v>
@@ -1589,7 +1637,7 @@
         <v>14</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C13" t="s" s="0">
         <v>31</v>
@@ -1600,7 +1648,7 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="8" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
@@ -1611,86 +1659,89 @@
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C15" t="s" s="0">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D15" t="s" s="0">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F15" t="s" s="0">
-        <v>188</v>
+        <v>307</v>
+      </c>
+      <c r="G15" t="s" s="0">
+        <v>281</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C16" t="s" s="0">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D16" t="s" s="0">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C17" t="s" s="0">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D17" t="s" s="0">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C18" t="s" s="0">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D18" t="s" s="0">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E18" t="s" s="0">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C19" t="s" s="0">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D19" t="s" s="0">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E19" t="s" s="0">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="8" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B20" s="8"/>
       <c r="C20" s="8"/>
@@ -1701,90 +1752,90 @@
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C21" t="s" s="0">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E21" s="2"/>
       <c r="F21" t="s" s="0">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G21" t="s" s="0">
-        <v>286</v>
+        <v>281</v>
       </c>
     </row>
     <row r="22" spans="1:7">
       <c r="A22" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C22" t="s" s="0">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E22" s="2"/>
     </row>
     <row r="23" spans="1:7">
       <c r="A23" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C23" t="s" s="0">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E23" s="2"/>
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C24" t="s" s="0">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E24" s="2"/>
     </row>
     <row r="25" spans="1:7">
       <c r="A25" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C25" t="s" s="0">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="26" spans="1:7">
       <c r="A26" s="8" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B26" s="8"/>
       <c r="C26" s="8"/>
@@ -1795,80 +1846,83 @@
     </row>
     <row r="27" spans="1:7">
       <c r="A27" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C27" t="s" s="0">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="D27" t="s" s="0">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F27" t="s" s="0">
-        <v>188</v>
+        <v>307</v>
+      </c>
+      <c r="G27" t="s" s="0">
+        <v>281</v>
       </c>
     </row>
     <row r="28" spans="1:7">
       <c r="A28" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C28" t="s" s="0">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="D28" t="s" s="0">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="29" spans="1:7">
       <c r="A29" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B29" t="s" s="0">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C29" t="s" s="0">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="D29" t="s" s="0">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="30" spans="1:7">
       <c r="A30" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B30" t="s" s="0">
+        <v>158</v>
+      </c>
+      <c r="C30" t="s" s="0">
+        <v>275</v>
+      </c>
+      <c r="D30" t="s" s="0">
         <v>160</v>
-      </c>
-      <c r="C30" t="s" s="0">
-        <v>280</v>
-      </c>
-      <c r="D30" t="s" s="0">
-        <v>162</v>
       </c>
     </row>
     <row r="31" spans="1:7">
       <c r="A31" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B31" t="s" s="0">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C31" t="s" s="0">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="D31" t="s" s="0">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="32" spans="1:7">
       <c r="A32" s="8" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B32" s="8"/>
       <c r="C32" s="8"/>
@@ -1879,83 +1933,83 @@
     </row>
     <row r="33" spans="1:7">
       <c r="A33" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C33" t="s" s="0">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="D33" t="s" s="0">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="F33" t="s" s="0">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="34" spans="1:7">
       <c r="A34" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C34" t="s" s="0">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="D34" t="s" s="0">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="35" spans="1:7">
       <c r="A35" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C35" t="s" s="0">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="D35" t="s" s="0">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="36" spans="1:7">
       <c r="A36" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C36" t="s" s="0">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="D36" t="s" s="0">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E36" t="s" s="0">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="37" spans="1:7">
       <c r="A37" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C37" t="s" s="0">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="D37" t="s" s="0">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="38" spans="1:7">
       <c r="A38" s="8" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B38" s="8"/>
       <c r="C38" s="8"/>
@@ -1966,30 +2020,30 @@
     </row>
     <row r="39" spans="1:7">
       <c r="A39" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B39" t="s" s="0">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="C39" t="s" s="0">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="D39" t="s" s="0">
         <v>58</v>
       </c>
       <c r="F39" t="s" s="0">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="40" spans="1:7">
       <c r="A40" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B40" t="s" s="0">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="C40" t="s" s="0">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="D40" t="s" s="0">
         <v>58</v>
@@ -1997,30 +2051,30 @@
     </row>
     <row r="41" spans="1:7">
       <c r="A41" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B41" t="s" s="0">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="C41" t="s" s="0">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="D41" t="s" s="0">
         <v>58</v>
       </c>
       <c r="E41" t="s" s="0">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="42" spans="1:7">
       <c r="A42" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B42" t="s" s="0">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="C42" t="s" s="0">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="D42" t="s" s="0">
         <v>58</v>
@@ -2028,13 +2082,13 @@
     </row>
     <row r="43" spans="1:7">
       <c r="A43" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B43" t="s" s="0">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="C43" t="s" s="0">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="D43" t="s" s="0">
         <v>58</v>
@@ -2042,7 +2096,7 @@
     </row>
     <row r="44" spans="1:7">
       <c r="A44" s="8" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B44" s="8"/>
       <c r="C44" s="8"/>
@@ -2053,30 +2107,30 @@
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="C45" t="s" s="0">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="D45" t="s" s="0">
         <v>60</v>
       </c>
       <c r="F45" t="s" s="0">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="46" spans="1:7">
       <c r="A46" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="C46" t="s" s="0">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="D46" t="s" s="0">
         <v>60</v>
@@ -2084,13 +2138,13 @@
     </row>
     <row r="47" spans="1:7">
       <c r="A47" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="C47" t="s" s="0">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="D47" t="s" s="0">
         <v>60</v>
@@ -2098,13 +2152,13 @@
     </row>
     <row r="48" spans="1:7">
       <c r="A48" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="C48" t="s" s="0">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="D48" t="s" s="0">
         <v>60</v>
@@ -2112,13 +2166,13 @@
     </row>
     <row r="49" spans="1:7">
       <c r="A49" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="C49" t="s" s="0">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="D49" t="s" s="0">
         <v>60</v>
@@ -2126,7 +2180,7 @@
     </row>
     <row r="50" spans="1:7">
       <c r="A50" s="8" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B50" s="8"/>
       <c r="C50" s="8"/>
@@ -2137,80 +2191,80 @@
     </row>
     <row r="51" spans="1:7">
       <c r="A51" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="C51" t="s" s="0">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="D51" t="s" s="0">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F51" t="s" s="0">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="52" spans="1:7">
       <c r="A52" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="C52" t="s" s="0">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="D52" t="s" s="0">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="53" spans="1:7">
       <c r="A53" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="C53" t="s" s="0">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="D53" t="s" s="0">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="54" spans="1:7">
       <c r="A54" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="C54" t="s" s="0">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="D54" t="s" s="0">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="55" spans="1:7">
       <c r="A55" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B55" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="C55" t="s" s="0">
         <v>279</v>
       </c>
-      <c r="C55" t="s" s="0">
-        <v>284</v>
-      </c>
       <c r="D55" t="s" s="0">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="56" spans="1:7">
       <c r="A56" s="8" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B56" s="8"/>
       <c r="C56" s="8"/>
@@ -2221,78 +2275,78 @@
     </row>
     <row r="57" spans="1:7">
       <c r="A57" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B57" t="s" s="0">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C57" t="s" s="0">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="D57" t="s" s="0">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F57" t="s" s="0">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="58" spans="1:7">
       <c r="A58" s="2" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B58" t="s" s="0">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C58" t="s" s="0">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="D58" t="s" s="0">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="59" spans="1:7">
       <c r="A59" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B59" t="s" s="0">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C59" t="s" s="0">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="D59" t="s" s="0">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="60" spans="1:7">
       <c r="A60" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B60" t="s" s="0">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C60" t="s" s="0">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="D60" t="s" s="0">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E60" t="s" s="0">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="61" spans="1:7">
       <c r="A61" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B61" t="s" s="0">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C61" t="s" s="0">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="D61" t="s" s="0">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -2324,31 +2378,31 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>79</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>81</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -2356,19 +2410,19 @@
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>59</v>
       </c>
       <c r="F2" t="s" s="0">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>14</v>
@@ -2377,7 +2431,7 @@
         <v>6</v>
       </c>
       <c r="I2" t="s" s="0">
-        <v>239</v>
+        <v>323</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -2385,22 +2439,22 @@
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="D3" t="s" s="0">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>59</v>
       </c>
       <c r="F3" t="s" s="0">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>7</v>
@@ -2411,19 +2465,19 @@
         <v>7</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="C4" t="s" s="0">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="D4" t="s" s="0">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>59</v>
       </c>
       <c r="F4" t="s" s="0">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>14</v>
@@ -2437,22 +2491,22 @@
         <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="C5" t="s" s="0">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="D5" t="s" s="0">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>59</v>
       </c>
       <c r="F5" t="s" s="0">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>6</v>
@@ -2463,22 +2517,22 @@
         <v>9</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="C6" t="s" s="0">
         <v>279</v>
       </c>
-      <c r="C6" t="s" s="0">
-        <v>284</v>
-      </c>
       <c r="D6" t="s" s="0">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>59</v>
       </c>
       <c r="F6" t="s" s="0">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>6</v>
@@ -2495,8 +2549,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2516,7 +2570,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -2531,7 +2585,7 @@
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H1" s="4" t="s">
         <v>57</v>
@@ -2542,25 +2596,25 @@
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>59</v>
       </c>
       <c r="F2" t="s" s="0">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="G2" t="s" s="0">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>240</v>
+        <v>324</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -2568,22 +2622,22 @@
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="D3" t="s" s="0">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>59</v>
       </c>
       <c r="F3" t="s" s="0">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="G3" t="s" s="0">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H3" s="2"/>
     </row>
@@ -2592,22 +2646,22 @@
         <v>7</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C4" t="s" s="0">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="D4" t="s" s="0">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>59</v>
       </c>
       <c r="F4" t="s" s="0">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="G4" t="s" s="0">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H4" s="2"/>
     </row>
@@ -2616,22 +2670,22 @@
         <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C5" t="s" s="0">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="D5" t="s" s="0">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>59</v>
       </c>
       <c r="F5" t="s" s="0">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="G5" t="s" s="0">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H5" s="2"/>
     </row>
@@ -2640,22 +2694,22 @@
         <v>9</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C6" t="s" s="0">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="D6" t="s" s="0">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>59</v>
       </c>
       <c r="F6" t="s" s="0">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="G6" t="s" s="0">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H6" s="2"/>
     </row>
@@ -2692,7 +2746,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -2712,7 +2766,7 @@
         <v>5</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C2" t="s" s="0">
         <v>15</v>
@@ -2724,7 +2778,7 @@
         <v>17</v>
       </c>
       <c r="F2" t="s" s="0">
-        <v>258</v>
+        <v>253</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -2732,7 +2786,7 @@
         <v>6</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C3" t="s" s="0">
         <v>15</v>
@@ -2744,7 +2798,7 @@
         <v>18</v>
       </c>
       <c r="F3" t="s" s="0">
-        <v>258</v>
+        <v>253</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -2752,7 +2806,7 @@
         <v>7</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C4" t="s" s="0">
         <v>15</v>
@@ -2764,7 +2818,7 @@
         <v>19</v>
       </c>
       <c r="F4" t="s" s="0">
-        <v>258</v>
+        <v>253</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -2772,7 +2826,7 @@
         <v>8</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C5" t="s" s="0">
         <v>15</v>
@@ -2784,7 +2838,7 @@
         <v>20</v>
       </c>
       <c r="F5" t="s" s="0">
-        <v>258</v>
+        <v>253</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -2792,7 +2846,7 @@
         <v>9</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C6" t="s" s="0">
         <v>15</v>
@@ -2804,7 +2858,7 @@
         <v>21</v>
       </c>
       <c r="F6" t="s" s="0">
-        <v>258</v>
+        <v>253</v>
       </c>
     </row>
   </sheetData>
@@ -2842,7 +2896,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -2889,7 +2943,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C2" t="s" s="0">
         <v>31</v>
@@ -2901,7 +2955,7 @@
         <v>17</v>
       </c>
       <c r="F2" t="s" s="0">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="G2" t="s" s="0">
         <v>33</v>
@@ -2928,7 +2982,7 @@
         <v>46</v>
       </c>
       <c r="O2" t="s" s="0">
-        <v>289</v>
+        <v>306</v>
       </c>
     </row>
     <row r="3" spans="1:15">
@@ -2936,7 +2990,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C3" t="s" s="0">
         <v>31</v>
@@ -2948,7 +3002,7 @@
         <v>17</v>
       </c>
       <c r="F3" t="s" s="0">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="I3" t="s" s="0">
         <v>50</v>
@@ -2974,7 +3028,7 @@
         <v>7</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C4" t="s" s="0">
         <v>31</v>
@@ -2986,7 +3040,7 @@
         <v>17</v>
       </c>
       <c r="F4" t="s" s="0">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="I4" t="s" s="0">
         <v>51</v>
@@ -3012,7 +3066,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C5" t="s" s="0">
         <v>31</v>
@@ -3024,7 +3078,7 @@
         <v>17</v>
       </c>
       <c r="F5" t="s" s="0">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="I5" t="s" s="0">
         <v>53</v>
@@ -3047,7 +3101,7 @@
         <v>9</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C6" t="s" s="0">
         <v>31</v>
@@ -3059,13 +3113,13 @@
         <v>17</v>
       </c>
       <c r="F6" t="s" s="0">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="G6" t="s" s="0">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="H6" t="s" s="0">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="I6" t="s" s="0">
         <v>52</v>
@@ -3118,7 +3172,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -3150,31 +3204,31 @@
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E2" t="s" s="0">
         <v>17</v>
       </c>
       <c r="F2" t="s" s="0">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="G2" t="s" s="0">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="H2" t="s" s="0">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="I2" t="s" s="0">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="J2" t="s" s="0">
-        <v>258</v>
+        <v>253</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -3182,28 +3236,28 @@
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D3" t="s" s="0">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E3" t="s" s="0">
         <v>17</v>
       </c>
       <c r="F3" t="s" s="0">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="G3" t="s" s="0">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="I3" t="s" s="0">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="J3" t="s" s="0">
-        <v>258</v>
+        <v>253</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -3211,28 +3265,28 @@
         <v>7</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C4" t="s" s="0">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D4" t="s" s="0">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E4" t="s" s="0">
         <v>17</v>
       </c>
       <c r="F4" t="s" s="0">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="G4" t="s" s="0">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="I4" t="s" s="0">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="J4" t="s" s="0">
-        <v>258</v>
+        <v>253</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -3240,28 +3294,28 @@
         <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C5" t="s" s="0">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D5" t="s" s="0">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E5" t="s" s="0">
         <v>17</v>
       </c>
       <c r="F5" t="s" s="0">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="G5" t="s" s="0">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="I5" t="s" s="0">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="J5" t="s" s="0">
-        <v>258</v>
+        <v>253</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -3269,28 +3323,28 @@
         <v>9</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C6" t="s" s="0">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D6" t="s" s="0">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E6" t="s" s="0">
         <v>17</v>
       </c>
       <c r="F6" t="s" s="0">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="G6" t="s" s="0">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="I6" t="s" s="0">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="J6" t="s" s="0">
-        <v>258</v>
+        <v>253</v>
       </c>
     </row>
   </sheetData>
@@ -3329,7 +3383,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -3344,25 +3398,25 @@
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="M1" s="13" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
     </row>
     <row r="2" spans="1:13" customFormat="1">
@@ -3370,40 +3424,40 @@
         <v>5</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E2" s="11" t="s">
         <v>17</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="G2" s="11" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="H2" s="11" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="I2" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="J2" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="K2" s="11" t="s">
+        <v>206</v>
+      </c>
+      <c r="L2" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="J2" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="K2" s="11" t="s">
-        <v>208</v>
-      </c>
-      <c r="L2" s="11" t="s">
-        <v>74</v>
-      </c>
       <c r="M2" s="5" t="s">
-        <v>291</v>
+        <v>308</v>
       </c>
     </row>
     <row r="3" spans="1:13" customFormat="1">
@@ -3411,37 +3465,37 @@
         <v>6</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E3" s="12" t="s">
         <v>17</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="H3" s="12" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="I3" s="12" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="J3" s="12" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="K3" s="12" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="L3" s="12" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="4" spans="1:13" customFormat="1">
@@ -3449,37 +3503,37 @@
         <v>7</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E4" s="11" t="s">
         <v>17</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="H4" s="11" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="I4" s="11" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="J4" s="11" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="K4" s="11" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="L4" s="11" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="5" spans="1:13" customFormat="1">
@@ -3487,37 +3541,37 @@
         <v>8</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E5" s="11" t="s">
         <v>17</v>
       </c>
       <c r="F5" s="11" t="s">
+        <v>253</v>
+      </c>
+      <c r="G5" s="11" t="s">
         <v>258</v>
       </c>
-      <c r="G5" s="11" t="s">
-        <v>263</v>
-      </c>
       <c r="H5" s="11" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="I5" s="11" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="J5" s="11" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="K5" s="11" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="L5" s="11" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="6" spans="1:13" customFormat="1">
@@ -3525,37 +3579,37 @@
         <v>9</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E6" s="11" t="s">
         <v>17</v>
       </c>
       <c r="F6" s="11" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="H6" s="11" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="I6" s="11" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="J6" s="11" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="K6" s="11" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="L6" s="11" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:13">
@@ -3616,7 +3670,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C1" s="9" t="s">
         <v>1</v>
@@ -3631,61 +3685,61 @@
         <v>4</v>
       </c>
       <c r="G1" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1" s="9" t="s">
         <v>189</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="J1" s="9" t="s">
+        <v>237</v>
+      </c>
+      <c r="K1" s="9" t="s">
+        <v>238</v>
+      </c>
+      <c r="L1" s="9" t="s">
         <v>190</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="M1" s="9" t="s">
         <v>191</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="N1" s="9" t="s">
+        <v>239</v>
+      </c>
+      <c r="O1" s="9" t="s">
+        <v>240</v>
+      </c>
+      <c r="P1" s="9" t="s">
+        <v>192</v>
+      </c>
+      <c r="Q1" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="R1" s="9" t="s">
         <v>241</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="S1" s="9" t="s">
         <v>242</v>
       </c>
-      <c r="L1" s="9" t="s">
-        <v>192</v>
-      </c>
-      <c r="M1" s="9" t="s">
-        <v>193</v>
-      </c>
-      <c r="N1" s="9" t="s">
+      <c r="T1" s="9" t="s">
         <v>243</v>
       </c>
-      <c r="O1" s="9" t="s">
+      <c r="U1" s="9" t="s">
         <v>244</v>
       </c>
-      <c r="P1" s="9" t="s">
-        <v>194</v>
-      </c>
-      <c r="Q1" s="9" t="s">
-        <v>195</v>
-      </c>
-      <c r="R1" s="9" t="s">
+      <c r="V1" s="9" t="s">
         <v>245</v>
       </c>
-      <c r="S1" s="9" t="s">
-        <v>246</v>
-      </c>
-      <c r="T1" s="9" t="s">
-        <v>247</v>
-      </c>
-      <c r="U1" s="9" t="s">
-        <v>248</v>
-      </c>
-      <c r="V1" s="9" t="s">
-        <v>249</v>
-      </c>
       <c r="W1" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="X1" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="Y1" s="9" t="s">
         <v>203</v>
-      </c>
-      <c r="X1" s="9" t="s">
-        <v>204</v>
-      </c>
-      <c r="Y1" s="9" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="2" spans="1:25">
@@ -3693,76 +3747,76 @@
         <v>5</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="E2" t="s" s="0">
         <v>17</v>
       </c>
       <c r="F2" t="s" s="0">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="G2" t="s" s="0">
+        <v>194</v>
+      </c>
+      <c r="H2" t="s" s="0">
+        <v>195</v>
+      </c>
+      <c r="I2" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="J2" s="10" t="s">
+        <v>246</v>
+      </c>
+      <c r="K2" s="10" t="s">
+        <v>247</v>
+      </c>
+      <c r="L2" t="s" s="0">
         <v>196</v>
       </c>
-      <c r="H2" t="s" s="0">
+      <c r="M2" s="10" t="s">
+        <v>198</v>
+      </c>
+      <c r="N2" s="10" t="s">
+        <v>248</v>
+      </c>
+      <c r="O2" s="10" t="s">
+        <v>249</v>
+      </c>
+      <c r="P2" t="s" s="0">
         <v>197</v>
       </c>
-      <c r="I2" s="10" t="s">
-        <v>201</v>
-      </c>
-      <c r="J2" s="10" t="s">
+      <c r="Q2" s="10" t="s">
+        <v>200</v>
+      </c>
+      <c r="R2" s="10" t="s">
         <v>250</v>
       </c>
-      <c r="K2" s="10" t="s">
+      <c r="S2" s="10" t="s">
         <v>251</v>
       </c>
-      <c r="L2" t="s" s="0">
-        <v>198</v>
-      </c>
-      <c r="M2" s="10" t="s">
-        <v>200</v>
-      </c>
-      <c r="N2" s="10" t="s">
+      <c r="T2" s="10" t="s">
         <v>252</v>
       </c>
-      <c r="O2" s="10" t="s">
-        <v>253</v>
-      </c>
-      <c r="P2" t="s" s="0">
-        <v>199</v>
-      </c>
-      <c r="Q2" s="10" t="s">
-        <v>202</v>
-      </c>
-      <c r="R2" s="10" t="s">
-        <v>254</v>
-      </c>
-      <c r="S2" s="10" t="s">
-        <v>255</v>
-      </c>
-      <c r="T2" s="10" t="s">
-        <v>256</v>
-      </c>
       <c r="U2" s="10" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="V2" s="10" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="W2" t="s" s="0">
+        <v>231</v>
+      </c>
+      <c r="X2" t="s" s="0">
+        <v>232</v>
+      </c>
+      <c r="Y2" t="s" s="0">
         <v>233</v>
-      </c>
-      <c r="X2" t="s" s="0">
-        <v>234</v>
-      </c>
-      <c r="Y2" t="s" s="0">
-        <v>235</v>
       </c>
     </row>
     <row r="3" spans="1:25">
@@ -3770,44 +3824,44 @@
         <v>6</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="D3" t="s" s="0">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="E3" t="s" s="0">
         <v>17</v>
       </c>
       <c r="F3" t="s" s="0">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="G3" t="s" s="0">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="H3" t="s" s="0">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
       <c r="L3" t="s" s="0">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
       <c r="P3" t="s" s="0">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="R3" s="2"/>
       <c r="S3" s="2"/>
@@ -3820,44 +3874,44 @@
         <v>7</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C4" t="s" s="0">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="D4" t="s" s="0">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="E4" t="s" s="0">
         <v>17</v>
       </c>
       <c r="F4" t="s" s="0">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="G4" t="s" s="0">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="H4" t="s" s="0">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
       <c r="L4" t="s" s="0">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
       <c r="P4" t="s" s="0">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="R4" s="2"/>
       <c r="S4" s="2"/>
@@ -3870,44 +3924,44 @@
         <v>8</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C5" t="s" s="0">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="D5" t="s" s="0">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="E5" t="s" s="0">
         <v>17</v>
       </c>
       <c r="F5" t="s" s="0">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="G5" t="s" s="0">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="H5" t="s" s="0">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
       <c r="L5" t="s" s="0">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
       <c r="P5" t="s" s="0">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="R5" s="2"/>
       <c r="S5" s="2"/>
@@ -3920,44 +3974,44 @@
         <v>9</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C6" t="s" s="0">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="D6" t="s" s="0">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="E6" t="s" s="0">
         <v>17</v>
       </c>
       <c r="F6" t="s" s="0">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="G6" t="s" s="0">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="H6" t="s" s="0">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
       <c r="L6" t="s" s="0">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
       <c r="P6" t="s" s="0">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="Q6" s="2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="R6" s="2"/>
       <c r="S6" s="2"/>
@@ -3975,7 +4029,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:R6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
@@ -4004,7 +4058,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -4022,37 +4076,37 @@
         <v>22</v>
       </c>
       <c r="H1" s="13" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I1" s="13" t="s">
+        <v>173</v>
+      </c>
+      <c r="J1" s="13" t="s">
+        <v>174</v>
+      </c>
+      <c r="K1" s="13" t="s">
+        <v>287</v>
+      </c>
+      <c r="L1" s="13" t="s">
+        <v>288</v>
+      </c>
+      <c r="M1" s="13" t="s">
         <v>175</v>
       </c>
-      <c r="J1" s="13" t="s">
+      <c r="N1" s="13" t="s">
         <v>176</v>
       </c>
-      <c r="K1" s="13" t="s">
-        <v>292</v>
-      </c>
-      <c r="L1" s="13" t="s">
-        <v>293</v>
-      </c>
-      <c r="M1" s="13" t="s">
+      <c r="O1" s="13" t="s">
         <v>177</v>
       </c>
-      <c r="N1" s="13" t="s">
+      <c r="P1" s="13" t="s">
         <v>178</v>
       </c>
-      <c r="O1" s="13" t="s">
+      <c r="Q1" s="13" t="s">
         <v>179</v>
       </c>
-      <c r="P1" s="13" t="s">
+      <c r="R1" s="13" t="s">
         <v>180</v>
-      </c>
-      <c r="Q1" s="13" t="s">
-        <v>181</v>
-      </c>
-      <c r="R1" s="13" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="2" spans="1:18">
@@ -4060,55 +4114,55 @@
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>59</v>
       </c>
       <c r="F2" t="s" s="0">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="G2" t="s" s="0">
+        <v>309</v>
+      </c>
+      <c r="H2" t="s" s="0">
+        <v>310</v>
+      </c>
+      <c r="I2" t="s" s="0">
+        <v>311</v>
+      </c>
+      <c r="J2" t="s" s="0">
+        <v>312</v>
+      </c>
+      <c r="K2" t="s" s="0">
+        <v>313</v>
+      </c>
+      <c r="L2" t="s" s="0">
         <v>294</v>
       </c>
-      <c r="H2" t="s" s="0">
-        <v>295</v>
-      </c>
-      <c r="I2" t="s" s="0">
-        <v>296</v>
-      </c>
-      <c r="J2" t="s" s="0">
-        <v>297</v>
-      </c>
-      <c r="K2" t="s" s="0">
-        <v>298</v>
-      </c>
-      <c r="L2" t="s" s="0">
-        <v>299</v>
-      </c>
       <c r="M2" t="s" s="0">
-        <v>300</v>
+        <v>314</v>
       </c>
       <c r="N2" t="s" s="0">
-        <v>301</v>
+        <v>315</v>
       </c>
       <c r="O2" t="s" s="0">
-        <v>302</v>
+        <v>316</v>
       </c>
       <c r="P2" t="s" s="0">
-        <v>303</v>
+        <v>317</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>304</v>
+        <v>318</v>
       </c>
       <c r="R2" t="s" s="0">
-        <v>305</v>
+        <v>319</v>
       </c>
     </row>
     <row r="3" spans="1:18">
@@ -4116,19 +4170,19 @@
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="D3" t="s" s="0">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>59</v>
       </c>
       <c r="F3" t="s" s="0">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="Q3" s="2"/>
       <c r="R3" s="2"/>
@@ -4138,19 +4192,19 @@
         <v>7</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C4" t="s" s="0">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="D4" t="s" s="0">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>59</v>
       </c>
       <c r="F4" t="s" s="0">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="R4" s="2"/>
     </row>
@@ -4159,19 +4213,19 @@
         <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C5" t="s" s="0">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="D5" t="s" s="0">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>59</v>
       </c>
       <c r="F5" t="s" s="0">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="R5" s="2"/>
     </row>
@@ -4180,19 +4234,19 @@
         <v>9</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C6" t="s" s="0">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="D6" t="s" s="0">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>59</v>
       </c>
       <c r="F6" t="s" s="0">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="R6" s="2"/>
     </row>
@@ -4233,7 +4287,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -4256,10 +4310,10 @@
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="D2" t="s" s="0">
         <v>58</v>
@@ -4268,10 +4322,10 @@
         <v>59</v>
       </c>
       <c r="F2" t="s" s="0">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="G2" t="s" s="0">
-        <v>306</v>
+        <v>320</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -4279,10 +4333,10 @@
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="D3" t="s" s="0">
         <v>58</v>
@@ -4291,7 +4345,7 @@
         <v>59</v>
       </c>
       <c r="F3" t="s" s="0">
-        <v>258</v>
+        <v>253</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -4299,10 +4353,10 @@
         <v>7</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="C4" t="s" s="0">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="D4" t="s" s="0">
         <v>58</v>
@@ -4311,7 +4365,7 @@
         <v>59</v>
       </c>
       <c r="F4" t="s" s="0">
-        <v>258</v>
+        <v>253</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -4319,10 +4373,10 @@
         <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="C5" t="s" s="0">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="D5" t="s" s="0">
         <v>58</v>
@@ -4331,7 +4385,7 @@
         <v>59</v>
       </c>
       <c r="F5" t="s" s="0">
-        <v>258</v>
+        <v>253</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -4339,10 +4393,10 @@
         <v>9</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="C6" t="s" s="0">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="D6" t="s" s="0">
         <v>58</v>
@@ -4351,7 +4405,7 @@
         <v>59</v>
       </c>
       <c r="F6" t="s" s="0">
-        <v>258</v>
+        <v>253</v>
       </c>
     </row>
   </sheetData>
@@ -4389,7 +4443,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -4404,10 +4458,10 @@
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>307</v>
+        <v>321</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>308</v>
+        <v>322</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -4415,10 +4469,10 @@
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="D2" t="s" s="0">
         <v>60</v>
@@ -4427,13 +4481,13 @@
         <v>59</v>
       </c>
       <c r="F2" t="s" s="0">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="G2" t="s" s="0">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="H2" t="s" s="0">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -4441,10 +4495,10 @@
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="D3" t="s" s="0">
         <v>60</v>
@@ -4453,7 +4507,7 @@
         <v>59</v>
       </c>
       <c r="F3" t="s" s="0">
-        <v>258</v>
+        <v>253</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -4461,10 +4515,10 @@
         <v>7</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="C4" t="s" s="0">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="D4" t="s" s="0">
         <v>60</v>
@@ -4473,7 +4527,7 @@
         <v>59</v>
       </c>
       <c r="F4" t="s" s="0">
-        <v>258</v>
+        <v>253</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -4481,10 +4535,10 @@
         <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="C5" t="s" s="0">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="D5" t="s" s="0">
         <v>60</v>
@@ -4493,7 +4547,7 @@
         <v>59</v>
       </c>
       <c r="F5" t="s" s="0">
-        <v>258</v>
+        <v>253</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -4501,10 +4555,10 @@
         <v>9</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="C6" t="s" s="0">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="D6" t="s" s="0">
         <v>60</v>
@@ -4513,7 +4567,7 @@
         <v>59</v>
       </c>
       <c r="F6" t="s" s="0">
-        <v>258</v>
+        <v>253</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Code Refactoring of BDD testcases is in progress
</commit_message>
<xml_diff>
--- a/src/main/resources/AutomationCatalogue_Batch41_TestData.xlsx
+++ b/src/main/resources/AutomationCatalogue_Batch41_TestData.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AutomationCatalogue\Projects\TestAutomationCatalogue_Batch41\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A45A4F84-7729-4CE1-A10F-EC725EBED5B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80E0FF46-3884-4EF9-9A2A-61D122EACA64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="944" firstSheet="4" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="944" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="10" r:id="rId1"/>
@@ -27,7 +27,7 @@
   </sheets>
   <calcPr calcId="124519"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="849" uniqueCount="325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="826" uniqueCount="314">
   <si>
     <t>S. No</t>
   </si>
@@ -745,9 +745,6 @@
     <t>60416.195</t>
   </si>
   <si>
-    <t>Order number: 1505349</t>
-  </si>
-  <si>
     <t>First Goal Name</t>
   </si>
   <si>
@@ -889,72 +886,18 @@
     <t xml:space="preserve">Alice  Duval </t>
   </si>
   <si>
-    <t>0140</t>
-  </si>
-  <si>
     <t>florene.rice</t>
   </si>
   <si>
-    <t>4104528605</t>
-  </si>
-  <si>
     <t>Country</t>
   </si>
   <si>
     <t>State</t>
   </si>
   <si>
-    <t>Vince</t>
-  </si>
-  <si>
-    <t>Bednar</t>
-  </si>
-  <si>
-    <t>OOvwNdyn@test.org</t>
-  </si>
-  <si>
-    <t>Lesch LLC</t>
-  </si>
-  <si>
-    <t>Zambia</t>
-  </si>
-  <si>
     <t>Other (Non US)</t>
   </si>
   <si>
-    <t>Port Lyndiaton</t>
-  </si>
-  <si>
-    <t>92436</t>
-  </si>
-  <si>
-    <t>10602 Jenni Harbors</t>
-  </si>
-  <si>
-    <t>AW</t>
-  </si>
-  <si>
-    <t>368-996-5809</t>
-  </si>
-  <si>
-    <t>12410249</t>
-  </si>
-  <si>
-    <t>Order number: 1546333</t>
-  </si>
-  <si>
-    <t>538</t>
-  </si>
-  <si>
-    <t>180447.7</t>
-  </si>
-  <si>
-    <t>Order number: 1547636</t>
-  </si>
-  <si>
-    <t>Order number: 1547643</t>
-  </si>
-  <si>
     <t>0141</t>
   </si>
   <si>
@@ -1010,13 +953,36 @@
   </si>
   <si>
     <t>Order number: 1547650</t>
+  </si>
+  <si>
+    <t>David</t>
+  </si>
+  <si>
+    <t>Jessy</t>
+  </si>
+  <si>
+    <t>Srinath</t>
+  </si>
+  <si>
+    <t>Goutham</t>
+  </si>
+  <si>
+    <t>Raja</t>
+  </si>
+  <si>
+    <t>Srinivas</t>
+  </si>
+  <si>
+    <t>0143</t>
+  </si>
+  <si>
+    <t>lisbeth.medhurst</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="5">
     <font>
       <sz val="11"/>
@@ -1444,12 +1410,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="5.0"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="10.6640625"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="39.0"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="39.6640625"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="9.44140625"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="18.33203125"/>
+    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -1472,7 +1438,7 @@
         <v>186</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -1490,16 +1456,16 @@
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s" s="0">
+      <c r="B3" t="s">
         <v>88</v>
       </c>
-      <c r="C3" t="s" s="0">
+      <c r="C3" t="s">
         <v>15</v>
       </c>
-      <c r="D3" t="s" s="0">
+      <c r="D3" t="s">
         <v>16</v>
       </c>
-      <c r="F3" t="s" s="0">
+      <c r="F3" t="s">
         <v>186</v>
       </c>
     </row>
@@ -1507,13 +1473,13 @@
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s" s="0">
+      <c r="B4" t="s">
         <v>89</v>
       </c>
-      <c r="C4" t="s" s="0">
+      <c r="C4" t="s">
         <v>15</v>
       </c>
-      <c r="D4" t="s" s="0">
+      <c r="D4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1521,16 +1487,16 @@
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B5" t="s" s="0">
+      <c r="B5" t="s">
         <v>90</v>
       </c>
-      <c r="C5" t="s" s="0">
+      <c r="C5" t="s">
         <v>15</v>
       </c>
-      <c r="D5" t="s" s="0">
+      <c r="D5" t="s">
         <v>16</v>
       </c>
-      <c r="E5" t="s" s="0">
+      <c r="E5" t="s">
         <v>205</v>
       </c>
     </row>
@@ -1538,13 +1504,13 @@
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B6" t="s" s="0">
+      <c r="B6" t="s">
         <v>91</v>
       </c>
-      <c r="C6" t="s" s="0">
+      <c r="C6" t="s">
         <v>15</v>
       </c>
-      <c r="D6" t="s" s="0">
+      <c r="D6" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1552,13 +1518,13 @@
       <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B7" t="s" s="0">
+      <c r="B7" t="s">
         <v>92</v>
       </c>
-      <c r="C7" t="s" s="0">
+      <c r="C7" t="s">
         <v>15</v>
       </c>
-      <c r="D7" t="s" s="0">
+      <c r="D7" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1580,13 +1546,13 @@
       <c r="B9" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="C9" t="s" s="0">
+      <c r="C9" t="s">
         <v>31</v>
       </c>
-      <c r="D9" t="s" s="0">
+      <c r="D9" t="s">
         <v>32</v>
       </c>
-      <c r="F9" t="s" s="0">
+      <c r="F9" t="s">
         <v>186</v>
       </c>
     </row>
@@ -1597,10 +1563,10 @@
       <c r="B10" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="C10" t="s" s="0">
+      <c r="C10" t="s">
         <v>31</v>
       </c>
-      <c r="D10" t="s" s="0">
+      <c r="D10" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1611,11 +1577,14 @@
       <c r="B11" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="C11" t="s" s="0">
+      <c r="C11" t="s">
         <v>31</v>
       </c>
-      <c r="D11" t="s" s="0">
+      <c r="D11" t="s">
         <v>32</v>
+      </c>
+      <c r="F11" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -1625,10 +1594,10 @@
       <c r="B12" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="C12" t="s" s="0">
+      <c r="C12" t="s">
         <v>31</v>
       </c>
-      <c r="D12" t="s" s="0">
+      <c r="D12" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1639,10 +1608,10 @@
       <c r="B13" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="C13" t="s" s="0">
+      <c r="C13" t="s">
         <v>31</v>
       </c>
-      <c r="D13" t="s" s="0">
+      <c r="D13" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1664,17 +1633,17 @@
       <c r="B15" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="C15" t="s" s="0">
+      <c r="C15" t="s">
         <v>83</v>
       </c>
-      <c r="D15" t="s" s="0">
+      <c r="D15" t="s">
         <v>84</v>
       </c>
-      <c r="F15" t="s" s="0">
-        <v>307</v>
-      </c>
-      <c r="G15" t="s" s="0">
-        <v>281</v>
+      <c r="F15" t="s">
+        <v>288</v>
+      </c>
+      <c r="G15" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -1684,10 +1653,10 @@
       <c r="B16" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="C16" t="s" s="0">
+      <c r="C16" t="s">
         <v>83</v>
       </c>
-      <c r="D16" t="s" s="0">
+      <c r="D16" t="s">
         <v>84</v>
       </c>
     </row>
@@ -1698,10 +1667,10 @@
       <c r="B17" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="C17" t="s" s="0">
+      <c r="C17" t="s">
         <v>83</v>
       </c>
-      <c r="D17" t="s" s="0">
+      <c r="D17" t="s">
         <v>84</v>
       </c>
     </row>
@@ -1712,13 +1681,13 @@
       <c r="B18" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="C18" t="s" s="0">
+      <c r="C18" t="s">
         <v>83</v>
       </c>
-      <c r="D18" t="s" s="0">
+      <c r="D18" t="s">
         <v>84</v>
       </c>
-      <c r="E18" t="s" s="0">
+      <c r="E18" t="s">
         <v>205</v>
       </c>
     </row>
@@ -1729,14 +1698,17 @@
       <c r="B19" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="C19" t="s" s="0">
+      <c r="C19" t="s">
         <v>83</v>
       </c>
-      <c r="D19" t="s" s="0">
+      <c r="D19" t="s">
         <v>84</v>
       </c>
-      <c r="E19" t="s" s="0">
+      <c r="E19" t="s">
         <v>205</v>
+      </c>
+      <c r="F19" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -1754,31 +1726,31 @@
       <c r="A21" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B21" t="s" s="0">
+      <c r="B21" t="s">
         <v>140</v>
       </c>
-      <c r="C21" t="s" s="0">
+      <c r="C21" t="s">
         <v>139</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>74</v>
       </c>
       <c r="E21" s="2"/>
-      <c r="F21" t="s" s="0">
+      <c r="F21" t="s">
         <v>186</v>
       </c>
-      <c r="G21" t="s" s="0">
-        <v>281</v>
+      <c r="G21" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="22" spans="1:7">
       <c r="A22" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="B22" t="s" s="0">
+      <c r="B22" t="s">
         <v>144</v>
       </c>
-      <c r="C22" t="s" s="0">
+      <c r="C22" t="s">
         <v>139</v>
       </c>
       <c r="D22" s="2" t="s">
@@ -1790,10 +1762,10 @@
       <c r="A23" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="B23" t="s" s="0">
+      <c r="B23" t="s">
         <v>141</v>
       </c>
-      <c r="C23" t="s" s="0">
+      <c r="C23" t="s">
         <v>139</v>
       </c>
       <c r="D23" s="2" t="s">
@@ -1805,10 +1777,10 @@
       <c r="A24" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="B24" t="s" s="0">
+      <c r="B24" t="s">
         <v>142</v>
       </c>
-      <c r="C24" t="s" s="0">
+      <c r="C24" t="s">
         <v>139</v>
       </c>
       <c r="D24" s="2" t="s">
@@ -1820,10 +1792,10 @@
       <c r="A25" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="B25" t="s" s="0">
+      <c r="B25" t="s">
         <v>143</v>
       </c>
-      <c r="C25" t="s" s="0">
+      <c r="C25" t="s">
         <v>139</v>
       </c>
       <c r="D25" s="2" t="s">
@@ -1848,33 +1820,33 @@
       <c r="A27" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="B27" t="s" s="0">
+      <c r="B27" t="s">
         <v>155</v>
       </c>
-      <c r="C27" t="s" s="0">
-        <v>275</v>
-      </c>
-      <c r="D27" t="s" s="0">
+      <c r="C27" t="s">
+        <v>274</v>
+      </c>
+      <c r="D27" t="s">
         <v>160</v>
       </c>
-      <c r="F27" t="s" s="0">
-        <v>307</v>
-      </c>
-      <c r="G27" t="s" s="0">
-        <v>281</v>
+      <c r="F27" t="s">
+        <v>288</v>
+      </c>
+      <c r="G27" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="28" spans="1:7">
       <c r="A28" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="B28" t="s" s="0">
+      <c r="B28" t="s">
         <v>156</v>
       </c>
-      <c r="C28" t="s" s="0">
-        <v>275</v>
-      </c>
-      <c r="D28" t="s" s="0">
+      <c r="C28" t="s">
+        <v>274</v>
+      </c>
+      <c r="D28" t="s">
         <v>160</v>
       </c>
     </row>
@@ -1882,13 +1854,13 @@
       <c r="A29" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="B29" t="s" s="0">
+      <c r="B29" t="s">
         <v>157</v>
       </c>
-      <c r="C29" t="s" s="0">
-        <v>275</v>
-      </c>
-      <c r="D29" t="s" s="0">
+      <c r="C29" t="s">
+        <v>274</v>
+      </c>
+      <c r="D29" t="s">
         <v>160</v>
       </c>
     </row>
@@ -1896,13 +1868,13 @@
       <c r="A30" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="B30" t="s" s="0">
+      <c r="B30" t="s">
         <v>158</v>
       </c>
-      <c r="C30" t="s" s="0">
-        <v>275</v>
-      </c>
-      <c r="D30" t="s" s="0">
+      <c r="C30" t="s">
+        <v>274</v>
+      </c>
+      <c r="D30" t="s">
         <v>160</v>
       </c>
     </row>
@@ -1910,13 +1882,13 @@
       <c r="A31" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="B31" t="s" s="0">
+      <c r="B31" t="s">
         <v>159</v>
       </c>
-      <c r="C31" t="s" s="0">
-        <v>275</v>
-      </c>
-      <c r="D31" t="s" s="0">
+      <c r="C31" t="s">
+        <v>274</v>
+      </c>
+      <c r="D31" t="s">
         <v>160</v>
       </c>
     </row>
@@ -1938,13 +1910,13 @@
       <c r="B33" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="C33" t="s" s="0">
-        <v>276</v>
-      </c>
-      <c r="D33" t="s" s="0">
+      <c r="C33" t="s">
+        <v>275</v>
+      </c>
+      <c r="D33" t="s">
         <v>172</v>
       </c>
-      <c r="F33" t="s" s="0">
+      <c r="F33" t="s">
         <v>186</v>
       </c>
     </row>
@@ -1955,10 +1927,10 @@
       <c r="B34" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="C34" t="s" s="0">
-        <v>276</v>
-      </c>
-      <c r="D34" t="s" s="0">
+      <c r="C34" t="s">
+        <v>275</v>
+      </c>
+      <c r="D34" t="s">
         <v>172</v>
       </c>
     </row>
@@ -1969,10 +1941,10 @@
       <c r="B35" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="C35" t="s" s="0">
-        <v>276</v>
-      </c>
-      <c r="D35" t="s" s="0">
+      <c r="C35" t="s">
+        <v>275</v>
+      </c>
+      <c r="D35" t="s">
         <v>172</v>
       </c>
     </row>
@@ -1983,13 +1955,13 @@
       <c r="B36" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="C36" t="s" s="0">
-        <v>276</v>
-      </c>
-      <c r="D36" t="s" s="0">
+      <c r="C36" t="s">
+        <v>275</v>
+      </c>
+      <c r="D36" t="s">
         <v>172</v>
       </c>
-      <c r="E36" t="s" s="0">
+      <c r="E36" t="s">
         <v>205</v>
       </c>
     </row>
@@ -2000,10 +1972,10 @@
       <c r="B37" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="C37" t="s" s="0">
-        <v>276</v>
-      </c>
-      <c r="D37" t="s" s="0">
+      <c r="C37" t="s">
+        <v>275</v>
+      </c>
+      <c r="D37" t="s">
         <v>172</v>
       </c>
     </row>
@@ -2022,16 +1994,16 @@
       <c r="A39" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="B39" t="s" s="0">
-        <v>260</v>
-      </c>
-      <c r="C39" t="s" s="0">
-        <v>277</v>
-      </c>
-      <c r="D39" t="s" s="0">
+      <c r="B39" t="s">
+        <v>259</v>
+      </c>
+      <c r="C39" t="s">
+        <v>276</v>
+      </c>
+      <c r="D39" t="s">
         <v>58</v>
       </c>
-      <c r="F39" t="s" s="0">
+      <c r="F39" t="s">
         <v>186</v>
       </c>
     </row>
@@ -2039,13 +2011,13 @@
       <c r="A40" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="B40" t="s" s="0">
-        <v>261</v>
-      </c>
-      <c r="C40" t="s" s="0">
-        <v>277</v>
-      </c>
-      <c r="D40" t="s" s="0">
+      <c r="B40" t="s">
+        <v>260</v>
+      </c>
+      <c r="C40" t="s">
+        <v>276</v>
+      </c>
+      <c r="D40" t="s">
         <v>58</v>
       </c>
     </row>
@@ -2053,16 +2025,16 @@
       <c r="A41" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="B41" t="s" s="0">
-        <v>262</v>
-      </c>
-      <c r="C41" t="s" s="0">
-        <v>277</v>
-      </c>
-      <c r="D41" t="s" s="0">
+      <c r="B41" t="s">
+        <v>261</v>
+      </c>
+      <c r="C41" t="s">
+        <v>276</v>
+      </c>
+      <c r="D41" t="s">
         <v>58</v>
       </c>
-      <c r="E41" t="s" s="0">
+      <c r="E41" t="s">
         <v>205</v>
       </c>
     </row>
@@ -2070,13 +2042,13 @@
       <c r="A42" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="B42" t="s" s="0">
-        <v>263</v>
-      </c>
-      <c r="C42" t="s" s="0">
-        <v>277</v>
-      </c>
-      <c r="D42" t="s" s="0">
+      <c r="B42" t="s">
+        <v>262</v>
+      </c>
+      <c r="C42" t="s">
+        <v>276</v>
+      </c>
+      <c r="D42" t="s">
         <v>58</v>
       </c>
     </row>
@@ -2084,13 +2056,13 @@
       <c r="A43" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="B43" t="s" s="0">
-        <v>264</v>
-      </c>
-      <c r="C43" t="s" s="0">
-        <v>277</v>
-      </c>
-      <c r="D43" t="s" s="0">
+      <c r="B43" t="s">
+        <v>263</v>
+      </c>
+      <c r="C43" t="s">
+        <v>276</v>
+      </c>
+      <c r="D43" t="s">
         <v>58</v>
       </c>
     </row>
@@ -2110,15 +2082,15 @@
         <v>134</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>265</v>
-      </c>
-      <c r="C45" t="s" s="0">
-        <v>278</v>
-      </c>
-      <c r="D45" t="s" s="0">
+        <v>264</v>
+      </c>
+      <c r="C45" t="s">
+        <v>277</v>
+      </c>
+      <c r="D45" t="s">
         <v>60</v>
       </c>
-      <c r="F45" t="s" s="0">
+      <c r="F45" t="s">
         <v>186</v>
       </c>
     </row>
@@ -2127,12 +2099,12 @@
         <v>135</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>266</v>
-      </c>
-      <c r="C46" t="s" s="0">
-        <v>278</v>
-      </c>
-      <c r="D46" t="s" s="0">
+        <v>265</v>
+      </c>
+      <c r="C46" t="s">
+        <v>277</v>
+      </c>
+      <c r="D46" t="s">
         <v>60</v>
       </c>
     </row>
@@ -2141,12 +2113,12 @@
         <v>136</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>267</v>
-      </c>
-      <c r="C47" t="s" s="0">
-        <v>278</v>
-      </c>
-      <c r="D47" t="s" s="0">
+        <v>266</v>
+      </c>
+      <c r="C47" t="s">
+        <v>277</v>
+      </c>
+      <c r="D47" t="s">
         <v>60</v>
       </c>
     </row>
@@ -2155,12 +2127,12 @@
         <v>137</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>268</v>
-      </c>
-      <c r="C48" t="s" s="0">
-        <v>278</v>
-      </c>
-      <c r="D48" t="s" s="0">
+        <v>267</v>
+      </c>
+      <c r="C48" t="s">
+        <v>277</v>
+      </c>
+      <c r="D48" t="s">
         <v>60</v>
       </c>
     </row>
@@ -2169,12 +2141,12 @@
         <v>138</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>269</v>
-      </c>
-      <c r="C49" t="s" s="0">
-        <v>278</v>
-      </c>
-      <c r="D49" t="s" s="0">
+        <v>268</v>
+      </c>
+      <c r="C49" t="s">
+        <v>277</v>
+      </c>
+      <c r="D49" t="s">
         <v>60</v>
       </c>
     </row>
@@ -2194,15 +2166,15 @@
         <v>145</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>270</v>
-      </c>
-      <c r="C51" t="s" s="0">
-        <v>279</v>
-      </c>
-      <c r="D51" t="s" s="0">
+        <v>269</v>
+      </c>
+      <c r="C51" t="s">
+        <v>278</v>
+      </c>
+      <c r="D51" t="s">
         <v>78</v>
       </c>
-      <c r="F51" t="s" s="0">
+      <c r="F51" t="s">
         <v>186</v>
       </c>
     </row>
@@ -2211,12 +2183,12 @@
         <v>146</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>271</v>
-      </c>
-      <c r="C52" t="s" s="0">
-        <v>279</v>
-      </c>
-      <c r="D52" t="s" s="0">
+        <v>270</v>
+      </c>
+      <c r="C52" t="s">
+        <v>278</v>
+      </c>
+      <c r="D52" t="s">
         <v>78</v>
       </c>
     </row>
@@ -2225,12 +2197,12 @@
         <v>147</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>272</v>
-      </c>
-      <c r="C53" t="s" s="0">
-        <v>279</v>
-      </c>
-      <c r="D53" t="s" s="0">
+        <v>271</v>
+      </c>
+      <c r="C53" t="s">
+        <v>278</v>
+      </c>
+      <c r="D53" t="s">
         <v>78</v>
       </c>
     </row>
@@ -2239,12 +2211,12 @@
         <v>148</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>273</v>
-      </c>
-      <c r="C54" t="s" s="0">
-        <v>279</v>
-      </c>
-      <c r="D54" t="s" s="0">
+        <v>272</v>
+      </c>
+      <c r="C54" t="s">
+        <v>278</v>
+      </c>
+      <c r="D54" t="s">
         <v>78</v>
       </c>
     </row>
@@ -2253,12 +2225,12 @@
         <v>149</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>274</v>
-      </c>
-      <c r="C55" t="s" s="0">
-        <v>279</v>
-      </c>
-      <c r="D55" t="s" s="0">
+        <v>273</v>
+      </c>
+      <c r="C55" t="s">
+        <v>278</v>
+      </c>
+      <c r="D55" t="s">
         <v>78</v>
       </c>
     </row>
@@ -2277,16 +2249,16 @@
       <c r="A57" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="B57" t="s" s="0">
+      <c r="B57" t="s">
         <v>167</v>
       </c>
-      <c r="C57" t="s" s="0">
-        <v>280</v>
-      </c>
-      <c r="D57" t="s" s="0">
+      <c r="C57" t="s">
+        <v>279</v>
+      </c>
+      <c r="D57" t="s">
         <v>61</v>
       </c>
-      <c r="F57" t="s" s="0">
+      <c r="F57" t="s">
         <v>186</v>
       </c>
     </row>
@@ -2294,13 +2266,13 @@
       <c r="A58" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="B58" t="s" s="0">
+      <c r="B58" t="s">
         <v>168</v>
       </c>
-      <c r="C58" t="s" s="0">
-        <v>280</v>
-      </c>
-      <c r="D58" t="s" s="0">
+      <c r="C58" t="s">
+        <v>279</v>
+      </c>
+      <c r="D58" t="s">
         <v>61</v>
       </c>
     </row>
@@ -2308,13 +2280,13 @@
       <c r="A59" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="B59" t="s" s="0">
+      <c r="B59" t="s">
         <v>169</v>
       </c>
-      <c r="C59" t="s" s="0">
-        <v>280</v>
-      </c>
-      <c r="D59" t="s" s="0">
+      <c r="C59" t="s">
+        <v>279</v>
+      </c>
+      <c r="D59" t="s">
         <v>61</v>
       </c>
     </row>
@@ -2322,16 +2294,16 @@
       <c r="A60" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="B60" t="s" s="0">
+      <c r="B60" t="s">
         <v>170</v>
       </c>
-      <c r="C60" t="s" s="0">
-        <v>280</v>
-      </c>
-      <c r="D60" t="s" s="0">
+      <c r="C60" t="s">
+        <v>279</v>
+      </c>
+      <c r="D60" t="s">
         <v>61</v>
       </c>
-      <c r="E60" t="s" s="0">
+      <c r="E60" t="s">
         <v>205</v>
       </c>
     </row>
@@ -2339,13 +2311,13 @@
       <c r="A61" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="B61" t="s" s="0">
+      <c r="B61" t="s">
         <v>171</v>
       </c>
-      <c r="C61" t="s" s="0">
-        <v>280</v>
-      </c>
-      <c r="D61" t="s" s="0">
+      <c r="C61" t="s">
+        <v>279</v>
+      </c>
+      <c r="D61" t="s">
         <v>61</v>
       </c>
     </row>
@@ -2366,14 +2338,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="10.6640625"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="39.0"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="21.109375"/>
-    <col min="5" max="5" customWidth="true" width="22.5546875"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="15.109375"/>
-    <col min="7" max="7" customWidth="true" width="23.0"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="15.6640625"/>
-    <col min="9" max="9" customWidth="true" width="21.6640625"/>
+    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.5546875" customWidth="1"/>
+    <col min="6" max="6" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23" customWidth="1"/>
+    <col min="8" max="8" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -2410,19 +2382,19 @@
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>270</v>
-      </c>
-      <c r="C2" t="s" s="0">
-        <v>279</v>
-      </c>
-      <c r="D2" t="s" s="0">
+        <v>269</v>
+      </c>
+      <c r="C2" t="s">
+        <v>278</v>
+      </c>
+      <c r="D2" t="s">
         <v>78</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="F2" t="s" s="0">
-        <v>253</v>
+      <c r="F2" t="s">
+        <v>252</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>14</v>
@@ -2430,8 +2402,8 @@
       <c r="H2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I2" t="s" s="0">
-        <v>323</v>
+      <c r="I2" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -2439,19 +2411,19 @@
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>271</v>
-      </c>
-      <c r="C3" t="s" s="0">
-        <v>279</v>
-      </c>
-      <c r="D3" t="s" s="0">
+        <v>270</v>
+      </c>
+      <c r="C3" t="s">
+        <v>278</v>
+      </c>
+      <c r="D3" t="s">
         <v>78</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="F3" t="s" s="0">
-        <v>253</v>
+      <c r="F3" t="s">
+        <v>252</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>96</v>
@@ -2465,19 +2437,19 @@
         <v>7</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>272</v>
-      </c>
-      <c r="C4" t="s" s="0">
-        <v>279</v>
-      </c>
-      <c r="D4" t="s" s="0">
+        <v>271</v>
+      </c>
+      <c r="C4" t="s">
+        <v>278</v>
+      </c>
+      <c r="D4" t="s">
         <v>78</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="F4" t="s" s="0">
-        <v>253</v>
+      <c r="F4" t="s">
+        <v>252</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>14</v>
@@ -2491,19 +2463,19 @@
         <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>273</v>
-      </c>
-      <c r="C5" t="s" s="0">
-        <v>279</v>
-      </c>
-      <c r="D5" t="s" s="0">
+        <v>272</v>
+      </c>
+      <c r="C5" t="s">
+        <v>278</v>
+      </c>
+      <c r="D5" t="s">
         <v>78</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="F5" t="s" s="0">
-        <v>253</v>
+      <c r="F5" t="s">
+        <v>252</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>95</v>
@@ -2517,19 +2489,19 @@
         <v>9</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>274</v>
-      </c>
-      <c r="C6" t="s" s="0">
-        <v>279</v>
-      </c>
-      <c r="D6" t="s" s="0">
+        <v>273</v>
+      </c>
+      <c r="C6" t="s">
+        <v>278</v>
+      </c>
+      <c r="D6" t="s">
         <v>78</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="F6" t="s" s="0">
-        <v>253</v>
+      <c r="F6" t="s">
+        <v>252</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>99</v>
@@ -2549,20 +2521,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="6.44140625"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="10.6640625"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="34.5546875"/>
-    <col min="4" max="4" customWidth="true" width="40.33203125"/>
-    <col min="5" max="5" customWidth="true" width="22.6640625"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="15.109375"/>
-    <col min="7" max="7" customWidth="true" width="21.44140625"/>
-    <col min="8" max="8" customWidth="true" width="21.33203125"/>
+    <col min="1" max="1" width="6.44140625" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.33203125" customWidth="1"/>
+    <col min="5" max="5" width="22.6640625" customWidth="1"/>
+    <col min="6" max="6" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.44140625" customWidth="1"/>
+    <col min="8" max="8" width="21.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -2598,23 +2570,23 @@
       <c r="B2" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="C2" t="s" s="0">
-        <v>280</v>
-      </c>
-      <c r="D2" t="s" s="0">
+      <c r="C2" t="s">
+        <v>279</v>
+      </c>
+      <c r="D2" t="s">
         <v>61</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="F2" t="s" s="0">
-        <v>253</v>
-      </c>
-      <c r="G2" t="s" s="0">
+      <c r="F2" t="s">
+        <v>252</v>
+      </c>
+      <c r="G2" t="s">
         <v>63</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>324</v>
+        <v>305</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -2624,19 +2596,19 @@
       <c r="B3" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="C3" t="s" s="0">
-        <v>280</v>
-      </c>
-      <c r="D3" t="s" s="0">
+      <c r="C3" t="s">
+        <v>279</v>
+      </c>
+      <c r="D3" t="s">
         <v>61</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="F3" t="s" s="0">
-        <v>253</v>
-      </c>
-      <c r="G3" t="s" s="0">
+      <c r="F3" t="s">
+        <v>252</v>
+      </c>
+      <c r="G3" t="s">
         <v>63</v>
       </c>
       <c r="H3" s="2"/>
@@ -2648,19 +2620,19 @@
       <c r="B4" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="C4" t="s" s="0">
-        <v>280</v>
-      </c>
-      <c r="D4" t="s" s="0">
+      <c r="C4" t="s">
+        <v>279</v>
+      </c>
+      <c r="D4" t="s">
         <v>61</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="F4" t="s" s="0">
-        <v>253</v>
-      </c>
-      <c r="G4" t="s" s="0">
+      <c r="F4" t="s">
+        <v>252</v>
+      </c>
+      <c r="G4" t="s">
         <v>63</v>
       </c>
       <c r="H4" s="2"/>
@@ -2672,19 +2644,19 @@
       <c r="B5" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="C5" t="s" s="0">
-        <v>280</v>
-      </c>
-      <c r="D5" t="s" s="0">
+      <c r="C5" t="s">
+        <v>279</v>
+      </c>
+      <c r="D5" t="s">
         <v>61</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="F5" t="s" s="0">
-        <v>253</v>
-      </c>
-      <c r="G5" t="s" s="0">
+      <c r="F5" t="s">
+        <v>252</v>
+      </c>
+      <c r="G5" t="s">
         <v>63</v>
       </c>
       <c r="H5" s="2"/>
@@ -2696,19 +2668,19 @@
       <c r="B6" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="C6" t="s" s="0">
-        <v>280</v>
-      </c>
-      <c r="D6" t="s" s="0">
+      <c r="C6" t="s">
+        <v>279</v>
+      </c>
+      <c r="D6" t="s">
         <v>61</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="F6" t="s" s="0">
-        <v>253</v>
-      </c>
-      <c r="G6" t="s" s="0">
+      <c r="F6" t="s">
+        <v>252</v>
+      </c>
+      <c r="G6" t="s">
         <v>63</v>
       </c>
       <c r="H6" s="2"/>
@@ -2729,16 +2701,16 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="E3" sqref="E3:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="10.6640625"/>
-    <col min="3" max="3" customWidth="true" width="26.0"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="24.44140625"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="10.6640625"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="15.109375"/>
+    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26" customWidth="1"/>
+    <col min="4" max="4" width="24.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -2765,105 +2737,106 @@
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s" s="0">
+      <c r="B2" t="s">
         <v>88</v>
       </c>
-      <c r="C2" t="s" s="0">
+      <c r="C2" t="s">
         <v>15</v>
       </c>
-      <c r="D2" t="s" s="0">
+      <c r="D2" t="s">
         <v>16</v>
       </c>
-      <c r="E2" t="s" s="0">
+      <c r="E2" t="s">
         <v>17</v>
       </c>
-      <c r="F2" t="s" s="0">
-        <v>253</v>
+      <c r="F2" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s" s="0">
+      <c r="B3" t="s">
         <v>89</v>
       </c>
-      <c r="C3" t="s" s="0">
+      <c r="C3" t="s">
         <v>15</v>
       </c>
-      <c r="D3" t="s" s="0">
+      <c r="D3" t="s">
         <v>16</v>
       </c>
-      <c r="E3" t="s" s="0">
+      <c r="E3" t="s">
         <v>18</v>
       </c>
-      <c r="F3" t="s" s="0">
-        <v>253</v>
+      <c r="F3" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B4" t="s" s="0">
+      <c r="B4" t="s">
         <v>90</v>
       </c>
-      <c r="C4" t="s" s="0">
+      <c r="C4" t="s">
         <v>15</v>
       </c>
-      <c r="D4" t="s" s="0">
+      <c r="D4" t="s">
         <v>16</v>
       </c>
-      <c r="E4" t="s" s="0">
+      <c r="E4" t="s">
         <v>19</v>
       </c>
-      <c r="F4" t="s" s="0">
-        <v>253</v>
+      <c r="F4" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B5" t="s" s="0">
+      <c r="B5" t="s">
         <v>91</v>
       </c>
-      <c r="C5" t="s" s="0">
+      <c r="C5" t="s">
         <v>15</v>
       </c>
-      <c r="D5" t="s" s="0">
+      <c r="D5" t="s">
         <v>16</v>
       </c>
-      <c r="E5" t="s" s="0">
+      <c r="E5" t="s">
         <v>20</v>
       </c>
-      <c r="F5" t="s" s="0">
-        <v>253</v>
+      <c r="F5" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B6" t="s" s="0">
+      <c r="B6" t="s">
         <v>92</v>
       </c>
-      <c r="C6" t="s" s="0">
+      <c r="C6" t="s">
         <v>15</v>
       </c>
-      <c r="D6" t="s" s="0">
+      <c r="D6" t="s">
         <v>16</v>
       </c>
-      <c r="E6" t="s" s="0">
+      <c r="E6" t="s">
         <v>21</v>
       </c>
-      <c r="F6" t="s" s="0">
-        <v>253</v>
+      <c r="F6" t="s">
+        <v>252</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2872,23 +2845,23 @@
   <dimension ref="A1:O6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="10.6640625"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="30.0"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="38.0"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="10.33203125"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="15.109375"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="9.6640625"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="9.44140625"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="25.44140625"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="13.0"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="10.6640625"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="16.6640625"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="11.33203125"/>
+    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
@@ -2945,44 +2918,44 @@
       <c r="B2" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="C2" t="s" s="0">
+      <c r="C2" t="s">
         <v>31</v>
       </c>
-      <c r="D2" t="s" s="0">
+      <c r="D2" t="s">
         <v>32</v>
       </c>
-      <c r="E2" t="s" s="0">
+      <c r="E2" t="s">
         <v>17</v>
       </c>
-      <c r="F2" t="s" s="0">
-        <v>253</v>
-      </c>
-      <c r="G2" t="s" s="0">
+      <c r="F2" t="s">
+        <v>252</v>
+      </c>
+      <c r="G2" t="s">
         <v>33</v>
       </c>
-      <c r="H2" t="s" s="0">
+      <c r="H2" t="s">
         <v>34</v>
       </c>
-      <c r="I2" t="s" s="0">
+      <c r="I2" t="s">
         <v>52</v>
       </c>
-      <c r="J2" t="s" s="0">
+      <c r="J2" t="s">
         <v>35</v>
       </c>
-      <c r="K2" t="s" s="0">
+      <c r="K2" t="s">
         <v>36</v>
       </c>
-      <c r="L2" t="s" s="0">
+      <c r="L2" t="s">
         <v>37</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="N2" t="s" s="0">
+      <c r="N2" t="s">
         <v>46</v>
       </c>
-      <c r="O2" t="s" s="0">
-        <v>306</v>
+      <c r="O2" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="3" spans="1:15">
@@ -2992,34 +2965,40 @@
       <c r="B3" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="C3" t="s" s="0">
+      <c r="C3" t="s">
         <v>31</v>
       </c>
-      <c r="D3" t="s" s="0">
+      <c r="D3" t="s">
         <v>32</v>
       </c>
-      <c r="E3" t="s" s="0">
+      <c r="E3" t="s">
         <v>17</v>
       </c>
-      <c r="F3" t="s" s="0">
-        <v>253</v>
-      </c>
-      <c r="I3" t="s" s="0">
+      <c r="F3" t="s">
+        <v>252</v>
+      </c>
+      <c r="G3" t="s">
+        <v>306</v>
+      </c>
+      <c r="H3" t="s">
+        <v>307</v>
+      </c>
+      <c r="I3" t="s">
         <v>50</v>
       </c>
-      <c r="J3" t="s" s="0">
+      <c r="J3" t="s">
         <v>40</v>
       </c>
-      <c r="K3" t="s" s="0">
+      <c r="K3" t="s">
         <v>42</v>
       </c>
-      <c r="L3" t="s" s="0">
+      <c r="L3" t="s">
         <v>38</v>
       </c>
       <c r="M3" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="N3" t="s" s="0">
+      <c r="N3" t="s">
         <v>47</v>
       </c>
     </row>
@@ -3030,25 +3009,31 @@
       <c r="B4" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="C4" t="s" s="0">
+      <c r="C4" t="s">
         <v>31</v>
       </c>
-      <c r="D4" t="s" s="0">
+      <c r="D4" t="s">
         <v>32</v>
       </c>
-      <c r="E4" t="s" s="0">
+      <c r="E4" t="s">
         <v>17</v>
       </c>
-      <c r="F4" t="s" s="0">
-        <v>253</v>
-      </c>
-      <c r="I4" t="s" s="0">
+      <c r="F4" t="s">
+        <v>252</v>
+      </c>
+      <c r="G4" t="s">
+        <v>308</v>
+      </c>
+      <c r="H4" t="s">
+        <v>309</v>
+      </c>
+      <c r="I4" t="s">
         <v>51</v>
       </c>
-      <c r="J4" t="s" s="0">
+      <c r="J4" t="s">
         <v>41</v>
       </c>
-      <c r="K4" t="s" s="0">
+      <c r="K4" t="s">
         <v>43</v>
       </c>
       <c r="L4" s="2" t="s">
@@ -3057,8 +3042,11 @@
       <c r="M4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="N4" t="s" s="0">
+      <c r="N4" t="s">
         <v>48</v>
+      </c>
+      <c r="O4" t="s">
+        <v>312</v>
       </c>
     </row>
     <row r="5" spans="1:15">
@@ -3068,31 +3056,37 @@
       <c r="B5" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="C5" t="s" s="0">
+      <c r="C5" t="s">
         <v>31</v>
       </c>
-      <c r="D5" t="s" s="0">
+      <c r="D5" t="s">
         <v>32</v>
       </c>
-      <c r="E5" t="s" s="0">
+      <c r="E5" t="s">
         <v>17</v>
       </c>
-      <c r="F5" t="s" s="0">
-        <v>253</v>
-      </c>
-      <c r="I5" t="s" s="0">
+      <c r="F5" t="s">
+        <v>252</v>
+      </c>
+      <c r="G5" t="s">
+        <v>310</v>
+      </c>
+      <c r="H5" t="s">
+        <v>311</v>
+      </c>
+      <c r="I5" t="s">
         <v>53</v>
       </c>
-      <c r="J5" t="s" s="0">
+      <c r="J5" t="s">
         <v>35</v>
       </c>
-      <c r="K5" t="s" s="0">
+      <c r="K5" t="s">
         <v>42</v>
       </c>
       <c r="L5" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="N5" t="s" s="0">
+      <c r="N5" t="s">
         <v>49</v>
       </c>
     </row>
@@ -3103,40 +3097,40 @@
       <c r="B6" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="C6" t="s" s="0">
+      <c r="C6" t="s">
         <v>31</v>
       </c>
-      <c r="D6" t="s" s="0">
+      <c r="D6" t="s">
         <v>32</v>
       </c>
-      <c r="E6" t="s" s="0">
+      <c r="E6" t="s">
         <v>17</v>
       </c>
-      <c r="F6" t="s" s="0">
-        <v>253</v>
-      </c>
-      <c r="G6" t="s" s="0">
+      <c r="F6" t="s">
+        <v>252</v>
+      </c>
+      <c r="G6" t="s">
         <v>127</v>
       </c>
-      <c r="H6" t="s" s="0">
+      <c r="H6" t="s">
         <v>128</v>
       </c>
-      <c r="I6" t="s" s="0">
+      <c r="I6" t="s">
         <v>52</v>
       </c>
-      <c r="J6" t="s" s="0">
+      <c r="J6" t="s">
         <v>35</v>
       </c>
-      <c r="K6" t="s" s="0">
+      <c r="K6" t="s">
         <v>36</v>
       </c>
-      <c r="L6" t="s" s="0">
+      <c r="L6" t="s">
         <v>37</v>
       </c>
       <c r="M6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="N6" t="s" s="0">
+      <c r="N6" t="s">
         <v>47</v>
       </c>
     </row>
@@ -3150,21 +3144,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="10.6640625"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="25.109375"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="22.44140625"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="10.33203125"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="15.109375"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="14.6640625"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="18.6640625"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="15.109375"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="16.21875"/>
+    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -3189,7 +3183,7 @@
       <c r="G1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="13" t="s">
         <v>55</v>
       </c>
       <c r="I1" s="1" t="s">
@@ -3206,29 +3200,29 @@
       <c r="B2" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="C2" t="s" s="0">
+      <c r="C2" t="s">
         <v>83</v>
       </c>
-      <c r="D2" t="s" s="0">
+      <c r="D2" t="s">
         <v>84</v>
       </c>
-      <c r="E2" t="s" s="0">
+      <c r="E2" t="s">
         <v>17</v>
       </c>
-      <c r="F2" t="s" s="0">
-        <v>253</v>
-      </c>
-      <c r="G2" t="s" s="0">
+      <c r="F2" t="s">
+        <v>252</v>
+      </c>
+      <c r="G2" t="s">
         <v>85</v>
       </c>
-      <c r="H2" t="s" s="0">
-        <v>285</v>
-      </c>
-      <c r="I2" t="s" s="0">
-        <v>253</v>
-      </c>
-      <c r="J2" t="s" s="0">
-        <v>253</v>
+      <c r="H2" t="s">
+        <v>283</v>
+      </c>
+      <c r="I2" t="s">
+        <v>252</v>
+      </c>
+      <c r="J2" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -3238,26 +3232,26 @@
       <c r="B3" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="C3" t="s" s="0">
+      <c r="C3" t="s">
         <v>83</v>
       </c>
-      <c r="D3" t="s" s="0">
+      <c r="D3" t="s">
         <v>84</v>
       </c>
-      <c r="E3" t="s" s="0">
+      <c r="E3" t="s">
         <v>17</v>
       </c>
-      <c r="F3" t="s" s="0">
-        <v>253</v>
-      </c>
-      <c r="G3" t="s" s="0">
+      <c r="F3" t="s">
+        <v>252</v>
+      </c>
+      <c r="G3" t="s">
         <v>216</v>
       </c>
-      <c r="I3" t="s" s="0">
-        <v>253</v>
-      </c>
-      <c r="J3" t="s" s="0">
-        <v>253</v>
+      <c r="I3" t="s">
+        <v>252</v>
+      </c>
+      <c r="J3" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -3267,26 +3261,26 @@
       <c r="B4" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="C4" t="s" s="0">
+      <c r="C4" t="s">
         <v>83</v>
       </c>
-      <c r="D4" t="s" s="0">
+      <c r="D4" t="s">
         <v>84</v>
       </c>
-      <c r="E4" t="s" s="0">
+      <c r="E4" t="s">
         <v>17</v>
       </c>
-      <c r="F4" t="s" s="0">
-        <v>253</v>
-      </c>
-      <c r="G4" t="s" s="0">
+      <c r="F4" t="s">
+        <v>252</v>
+      </c>
+      <c r="G4" t="s">
         <v>219</v>
       </c>
-      <c r="I4" t="s" s="0">
-        <v>253</v>
-      </c>
-      <c r="J4" t="s" s="0">
-        <v>253</v>
+      <c r="I4" t="s">
+        <v>252</v>
+      </c>
+      <c r="J4" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -3296,26 +3290,26 @@
       <c r="B5" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="C5" t="s" s="0">
+      <c r="C5" t="s">
         <v>83</v>
       </c>
-      <c r="D5" t="s" s="0">
+      <c r="D5" t="s">
         <v>84</v>
       </c>
-      <c r="E5" t="s" s="0">
+      <c r="E5" t="s">
         <v>17</v>
       </c>
-      <c r="F5" t="s" s="0">
-        <v>253</v>
-      </c>
-      <c r="G5" t="s" s="0">
+      <c r="F5" t="s">
+        <v>252</v>
+      </c>
+      <c r="G5" t="s">
         <v>218</v>
       </c>
-      <c r="I5" t="s" s="0">
-        <v>253</v>
-      </c>
-      <c r="J5" t="s" s="0">
-        <v>253</v>
+      <c r="I5" t="s">
+        <v>252</v>
+      </c>
+      <c r="J5" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -3325,26 +3319,29 @@
       <c r="B6" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="C6" t="s" s="0">
+      <c r="C6" t="s">
         <v>83</v>
       </c>
-      <c r="D6" t="s" s="0">
+      <c r="D6" t="s">
         <v>84</v>
       </c>
-      <c r="E6" t="s" s="0">
+      <c r="E6" t="s">
         <v>17</v>
       </c>
-      <c r="F6" t="s" s="0">
-        <v>253</v>
-      </c>
-      <c r="G6" t="s" s="0">
+      <c r="F6" t="s">
+        <v>252</v>
+      </c>
+      <c r="G6" t="s">
         <v>217</v>
       </c>
-      <c r="I6" t="s" s="0">
-        <v>253</v>
-      </c>
-      <c r="J6" t="s" s="0">
-        <v>253</v>
+      <c r="H6" t="s">
+        <v>313</v>
+      </c>
+      <c r="I6" t="s">
+        <v>252</v>
+      </c>
+      <c r="J6" t="s">
+        <v>252</v>
       </c>
     </row>
   </sheetData>
@@ -3358,24 +3355,24 @@
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" style="5" width="9.33203125"/>
-    <col min="2" max="2" customWidth="true" style="5" width="15.88671875"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="5" width="30.6640625"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="5" width="39.33203125"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="5" width="10.44140625"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="5" width="15.109375"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="5" width="17.77734375"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="5" width="17.109375"/>
-    <col min="9" max="9" customWidth="true" style="5" width="15.0"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" style="5" width="17.0"/>
-    <col min="11" max="12" bestFit="true" customWidth="true" style="5" width="22.6640625"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" style="5" width="14.88671875"/>
-    <col min="14" max="16384" style="5" width="9.33203125"/>
+    <col min="1" max="1" width="9.33203125" style="5"/>
+    <col min="2" max="2" width="15.88671875" style="5" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.77734375" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15" style="5" customWidth="1"/>
+    <col min="10" max="10" width="17" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="22.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.88671875" style="5" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.33203125" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" customFormat="1">
@@ -3416,7 +3413,7 @@
         <v>69</v>
       </c>
       <c r="M1" s="13" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="2" spans="1:13" customFormat="1">
@@ -3436,10 +3433,10 @@
         <v>17</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="G2" s="11" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="H2" s="11" t="s">
         <v>73</v>
@@ -3457,7 +3454,7 @@
         <v>72</v>
       </c>
       <c r="M2" s="5" t="s">
-        <v>308</v>
+        <v>289</v>
       </c>
     </row>
     <row r="3" spans="1:13" customFormat="1">
@@ -3477,10 +3474,10 @@
         <v>17</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H3" s="12" t="s">
         <v>207</v>
@@ -3515,10 +3512,10 @@
         <v>17</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="H4" s="11" t="s">
         <v>208</v>
@@ -3553,10 +3550,10 @@
         <v>17</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="H5" s="11" t="s">
         <v>209</v>
@@ -3591,10 +3588,10 @@
         <v>17</v>
       </c>
       <c r="F6" s="11" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="H6" s="11" t="s">
         <v>210</v>
@@ -3641,28 +3638,28 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="12.33203125"/>
-    <col min="3" max="3" customWidth="true" width="27.44140625"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="37.6640625"/>
-    <col min="5" max="5" customWidth="true" width="10.6640625"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="15.109375"/>
-    <col min="7" max="7" customWidth="true" width="15.0"/>
-    <col min="8" max="8" customWidth="true" width="16.5546875"/>
-    <col min="9" max="10" customWidth="true" width="17.88671875"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="19.5546875"/>
-    <col min="12" max="12" customWidth="true" width="19.33203125"/>
-    <col min="13" max="13" customWidth="true" width="17.88671875"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="17.33203125"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="22.21875"/>
-    <col min="16" max="16" customWidth="true" width="16.88671875"/>
-    <col min="17" max="18" customWidth="true" width="17.0"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="22.21875"/>
-    <col min="20" max="20" customWidth="true" width="22.21875"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="27.109375"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="29.0"/>
-    <col min="23" max="23" customWidth="true" width="15.109375"/>
-    <col min="24" max="24" customWidth="true" width="17.6640625"/>
-    <col min="25" max="25" customWidth="true" width="15.5546875"/>
+    <col min="2" max="2" width="12.33203125" customWidth="1"/>
+    <col min="3" max="3" width="27.44140625" customWidth="1"/>
+    <col min="4" max="4" width="37.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" customWidth="1"/>
+    <col min="6" max="6" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15" customWidth="1"/>
+    <col min="8" max="8" width="16.5546875" customWidth="1"/>
+    <col min="9" max="10" width="17.88671875" customWidth="1"/>
+    <col min="11" max="11" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.33203125" customWidth="1"/>
+    <col min="13" max="13" width="17.88671875" customWidth="1"/>
+    <col min="14" max="14" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="22.21875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.88671875" customWidth="1"/>
+    <col min="17" max="18" width="17" customWidth="1"/>
+    <col min="19" max="19" width="22.21875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="22.21875" customWidth="1"/>
+    <col min="21" max="21" width="27.109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="29" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="15.109375" customWidth="1"/>
+    <col min="24" max="24" width="17.6640625" customWidth="1"/>
+    <col min="25" max="25" width="15.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" s="9" customFormat="1">
@@ -3694,10 +3691,10 @@
         <v>189</v>
       </c>
       <c r="J1" s="9" t="s">
+        <v>236</v>
+      </c>
+      <c r="K1" s="9" t="s">
         <v>237</v>
-      </c>
-      <c r="K1" s="9" t="s">
-        <v>238</v>
       </c>
       <c r="L1" s="9" t="s">
         <v>190</v>
@@ -3706,10 +3703,10 @@
         <v>191</v>
       </c>
       <c r="N1" s="9" t="s">
+        <v>238</v>
+      </c>
+      <c r="O1" s="9" t="s">
         <v>239</v>
-      </c>
-      <c r="O1" s="9" t="s">
-        <v>240</v>
       </c>
       <c r="P1" s="9" t="s">
         <v>192</v>
@@ -3718,19 +3715,19 @@
         <v>193</v>
       </c>
       <c r="R1" s="9" t="s">
+        <v>240</v>
+      </c>
+      <c r="S1" s="9" t="s">
         <v>241</v>
       </c>
-      <c r="S1" s="9" t="s">
+      <c r="T1" s="9" t="s">
         <v>242</v>
       </c>
-      <c r="T1" s="9" t="s">
+      <c r="U1" s="9" t="s">
         <v>243</v>
       </c>
-      <c r="U1" s="9" t="s">
+      <c r="V1" s="9" t="s">
         <v>244</v>
-      </c>
-      <c r="V1" s="9" t="s">
-        <v>245</v>
       </c>
       <c r="W1" s="9" t="s">
         <v>201</v>
@@ -3746,62 +3743,62 @@
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s" s="0">
+      <c r="B2" t="s">
         <v>155</v>
       </c>
-      <c r="C2" t="s" s="0">
-        <v>275</v>
-      </c>
-      <c r="D2" t="s" s="0">
-        <v>254</v>
-      </c>
-      <c r="E2" t="s" s="0">
+      <c r="C2" t="s">
+        <v>274</v>
+      </c>
+      <c r="D2" t="s">
+        <v>253</v>
+      </c>
+      <c r="E2" t="s">
         <v>17</v>
       </c>
-      <c r="F2" t="s" s="0">
-        <v>253</v>
-      </c>
-      <c r="G2" t="s" s="0">
+      <c r="F2" t="s">
+        <v>252</v>
+      </c>
+      <c r="G2" t="s">
         <v>194</v>
       </c>
-      <c r="H2" t="s" s="0">
+      <c r="H2" t="s">
         <v>195</v>
       </c>
       <c r="I2" s="10" t="s">
         <v>199</v>
       </c>
       <c r="J2" s="10" t="s">
+        <v>245</v>
+      </c>
+      <c r="K2" s="10" t="s">
         <v>246</v>
       </c>
-      <c r="K2" s="10" t="s">
-        <v>247</v>
-      </c>
-      <c r="L2" t="s" s="0">
+      <c r="L2" t="s">
         <v>196</v>
       </c>
       <c r="M2" s="10" t="s">
         <v>198</v>
       </c>
       <c r="N2" s="10" t="s">
+        <v>247</v>
+      </c>
+      <c r="O2" s="10" t="s">
         <v>248</v>
       </c>
-      <c r="O2" s="10" t="s">
-        <v>249</v>
-      </c>
-      <c r="P2" t="s" s="0">
+      <c r="P2" t="s">
         <v>197</v>
       </c>
       <c r="Q2" s="10" t="s">
         <v>200</v>
       </c>
       <c r="R2" s="10" t="s">
+        <v>249</v>
+      </c>
+      <c r="S2" s="10" t="s">
         <v>250</v>
       </c>
-      <c r="S2" s="10" t="s">
+      <c r="T2" s="10" t="s">
         <v>251</v>
-      </c>
-      <c r="T2" s="10" t="s">
-        <v>252</v>
       </c>
       <c r="U2" s="10" t="s">
         <v>115</v>
@@ -3809,13 +3806,13 @@
       <c r="V2" s="10" t="s">
         <v>184</v>
       </c>
-      <c r="W2" t="s" s="0">
+      <c r="W2" t="s">
         <v>231</v>
       </c>
-      <c r="X2" t="s" s="0">
+      <c r="X2" t="s">
         <v>232</v>
       </c>
-      <c r="Y2" t="s" s="0">
+      <c r="Y2" t="s">
         <v>233</v>
       </c>
     </row>
@@ -3823,25 +3820,25 @@
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s" s="0">
+      <c r="B3" t="s">
         <v>156</v>
       </c>
-      <c r="C3" t="s" s="0">
-        <v>275</v>
-      </c>
-      <c r="D3" t="s" s="0">
-        <v>254</v>
-      </c>
-      <c r="E3" t="s" s="0">
+      <c r="C3" t="s">
+        <v>274</v>
+      </c>
+      <c r="D3" t="s">
+        <v>253</v>
+      </c>
+      <c r="E3" t="s">
         <v>17</v>
       </c>
-      <c r="F3" t="s" s="0">
-        <v>253</v>
-      </c>
-      <c r="G3" t="s" s="0">
+      <c r="F3" t="s">
+        <v>252</v>
+      </c>
+      <c r="G3" t="s">
         <v>85</v>
       </c>
-      <c r="H3" t="s" s="0">
+      <c r="H3" t="s">
         <v>196</v>
       </c>
       <c r="I3" s="2" t="s">
@@ -3849,7 +3846,7 @@
       </c>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
-      <c r="L3" t="s" s="0">
+      <c r="L3" t="s">
         <v>195</v>
       </c>
       <c r="M3" s="2" t="s">
@@ -3857,7 +3854,7 @@
       </c>
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
-      <c r="P3" t="s" s="0">
+      <c r="P3" t="s">
         <v>196</v>
       </c>
       <c r="Q3" s="2" t="s">
@@ -3873,25 +3870,25 @@
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B4" t="s" s="0">
+      <c r="B4" t="s">
         <v>157</v>
       </c>
-      <c r="C4" t="s" s="0">
-        <v>275</v>
-      </c>
-      <c r="D4" t="s" s="0">
-        <v>254</v>
-      </c>
-      <c r="E4" t="s" s="0">
+      <c r="C4" t="s">
+        <v>274</v>
+      </c>
+      <c r="D4" t="s">
+        <v>253</v>
+      </c>
+      <c r="E4" t="s">
         <v>17</v>
       </c>
-      <c r="F4" t="s" s="0">
-        <v>253</v>
-      </c>
-      <c r="G4" t="s" s="0">
+      <c r="F4" t="s">
+        <v>252</v>
+      </c>
+      <c r="G4" t="s">
         <v>215</v>
       </c>
-      <c r="H4" t="s" s="0">
+      <c r="H4" t="s">
         <v>197</v>
       </c>
       <c r="I4" s="2" t="s">
@@ -3899,7 +3896,7 @@
       </c>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
-      <c r="L4" t="s" s="0">
+      <c r="L4" t="s">
         <v>197</v>
       </c>
       <c r="M4" s="2" t="s">
@@ -3907,7 +3904,7 @@
       </c>
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
-      <c r="P4" t="s" s="0">
+      <c r="P4" t="s">
         <v>195</v>
       </c>
       <c r="Q4" s="2" t="s">
@@ -3923,25 +3920,25 @@
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B5" t="s" s="0">
+      <c r="B5" t="s">
         <v>158</v>
       </c>
-      <c r="C5" t="s" s="0">
-        <v>275</v>
-      </c>
-      <c r="D5" t="s" s="0">
-        <v>254</v>
-      </c>
-      <c r="E5" t="s" s="0">
+      <c r="C5" t="s">
+        <v>274</v>
+      </c>
+      <c r="D5" t="s">
+        <v>253</v>
+      </c>
+      <c r="E5" t="s">
         <v>17</v>
       </c>
-      <c r="F5" t="s" s="0">
-        <v>253</v>
-      </c>
-      <c r="G5" t="s" s="0">
+      <c r="F5" t="s">
+        <v>252</v>
+      </c>
+      <c r="G5" t="s">
         <v>216</v>
       </c>
-      <c r="H5" t="s" s="0">
+      <c r="H5" t="s">
         <v>197</v>
       </c>
       <c r="I5" s="2" t="s">
@@ -3949,7 +3946,7 @@
       </c>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
-      <c r="L5" t="s" s="0">
+      <c r="L5" t="s">
         <v>197</v>
       </c>
       <c r="M5" s="2" t="s">
@@ -3957,7 +3954,7 @@
       </c>
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
-      <c r="P5" t="s" s="0">
+      <c r="P5" t="s">
         <v>195</v>
       </c>
       <c r="Q5" s="2" t="s">
@@ -3973,25 +3970,25 @@
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B6" t="s" s="0">
+      <c r="B6" t="s">
         <v>159</v>
       </c>
-      <c r="C6" t="s" s="0">
-        <v>275</v>
-      </c>
-      <c r="D6" t="s" s="0">
-        <v>254</v>
-      </c>
-      <c r="E6" t="s" s="0">
+      <c r="C6" t="s">
+        <v>274</v>
+      </c>
+      <c r="D6" t="s">
+        <v>253</v>
+      </c>
+      <c r="E6" t="s">
         <v>17</v>
       </c>
-      <c r="F6" t="s" s="0">
-        <v>253</v>
-      </c>
-      <c r="G6" t="s" s="0">
+      <c r="F6" t="s">
+        <v>252</v>
+      </c>
+      <c r="G6" t="s">
         <v>217</v>
       </c>
-      <c r="H6" t="s" s="0">
+      <c r="H6" t="s">
         <v>196</v>
       </c>
       <c r="I6" s="2" t="s">
@@ -3999,7 +3996,7 @@
       </c>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
-      <c r="L6" t="s" s="0">
+      <c r="L6" t="s">
         <v>196</v>
       </c>
       <c r="M6" s="2" t="s">
@@ -4007,7 +4004,7 @@
       </c>
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
-      <c r="P6" t="s" s="0">
+      <c r="P6" t="s">
         <v>195</v>
       </c>
       <c r="Q6" s="2" t="s">
@@ -4035,22 +4032,22 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="10.6640625"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="33.88671875"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="30.109375"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="22.33203125"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="15.109375"/>
-    <col min="7" max="8" bestFit="true" customWidth="true" width="9.88671875"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="19.5546875"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="9.109375"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="7.77734375"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="14.109375"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="13.5546875"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="8.88671875"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="18.21875"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="8.0"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="13.77734375"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="10.88671875"/>
+    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.77734375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18">
@@ -4085,10 +4082,10 @@
         <v>174</v>
       </c>
       <c r="K1" s="13" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="L1" s="13" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="M1" s="13" t="s">
         <v>175</v>
@@ -4116,53 +4113,53 @@
       <c r="B2" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="C2" t="s" s="0">
-        <v>276</v>
-      </c>
-      <c r="D2" t="s" s="0">
+      <c r="C2" t="s">
+        <v>275</v>
+      </c>
+      <c r="D2" t="s">
         <v>172</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="F2" t="s" s="0">
-        <v>253</v>
-      </c>
-      <c r="G2" t="s" s="0">
-        <v>309</v>
-      </c>
-      <c r="H2" t="s" s="0">
-        <v>310</v>
-      </c>
-      <c r="I2" t="s" s="0">
-        <v>311</v>
-      </c>
-      <c r="J2" t="s" s="0">
-        <v>312</v>
-      </c>
-      <c r="K2" t="s" s="0">
-        <v>313</v>
-      </c>
-      <c r="L2" t="s" s="0">
+      <c r="F2" t="s">
+        <v>252</v>
+      </c>
+      <c r="G2" t="s">
+        <v>290</v>
+      </c>
+      <c r="H2" t="s">
+        <v>291</v>
+      </c>
+      <c r="I2" t="s">
+        <v>292</v>
+      </c>
+      <c r="J2" t="s">
+        <v>293</v>
+      </c>
+      <c r="K2" t="s">
         <v>294</v>
       </c>
-      <c r="M2" t="s" s="0">
-        <v>314</v>
-      </c>
-      <c r="N2" t="s" s="0">
-        <v>315</v>
-      </c>
-      <c r="O2" t="s" s="0">
-        <v>316</v>
-      </c>
-      <c r="P2" t="s" s="0">
-        <v>317</v>
+      <c r="L2" t="s">
+        <v>286</v>
+      </c>
+      <c r="M2" t="s">
+        <v>295</v>
+      </c>
+      <c r="N2" t="s">
+        <v>296</v>
+      </c>
+      <c r="O2" t="s">
+        <v>297</v>
+      </c>
+      <c r="P2" t="s">
+        <v>298</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>318</v>
-      </c>
-      <c r="R2" t="s" s="0">
-        <v>319</v>
+        <v>299</v>
+      </c>
+      <c r="R2" t="s">
+        <v>300</v>
       </c>
     </row>
     <row r="3" spans="1:18">
@@ -4172,17 +4169,17 @@
       <c r="B3" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="C3" t="s" s="0">
-        <v>276</v>
-      </c>
-      <c r="D3" t="s" s="0">
+      <c r="C3" t="s">
+        <v>275</v>
+      </c>
+      <c r="D3" t="s">
         <v>172</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="F3" t="s" s="0">
-        <v>253</v>
+      <c r="F3" t="s">
+        <v>252</v>
       </c>
       <c r="Q3" s="2"/>
       <c r="R3" s="2"/>
@@ -4194,17 +4191,17 @@
       <c r="B4" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="C4" t="s" s="0">
-        <v>276</v>
-      </c>
-      <c r="D4" t="s" s="0">
+      <c r="C4" t="s">
+        <v>275</v>
+      </c>
+      <c r="D4" t="s">
         <v>172</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="F4" t="s" s="0">
-        <v>253</v>
+      <c r="F4" t="s">
+        <v>252</v>
       </c>
       <c r="R4" s="2"/>
     </row>
@@ -4215,17 +4212,17 @@
       <c r="B5" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="C5" t="s" s="0">
-        <v>276</v>
-      </c>
-      <c r="D5" t="s" s="0">
+      <c r="C5" t="s">
+        <v>275</v>
+      </c>
+      <c r="D5" t="s">
         <v>172</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="F5" t="s" s="0">
-        <v>253</v>
+      <c r="F5" t="s">
+        <v>252</v>
       </c>
       <c r="R5" s="2"/>
     </row>
@@ -4236,17 +4233,17 @@
       <c r="B6" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="C6" t="s" s="0">
-        <v>276</v>
-      </c>
-      <c r="D6" t="s" s="0">
+      <c r="C6" t="s">
+        <v>275</v>
+      </c>
+      <c r="D6" t="s">
         <v>172</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="F6" t="s" s="0">
-        <v>253</v>
+      <c r="F6" t="s">
+        <v>252</v>
       </c>
       <c r="R6" s="2"/>
     </row>
@@ -4274,12 +4271,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="10.6640625"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="28.0"/>
-    <col min="4" max="4" customWidth="true" width="34.0"/>
-    <col min="5" max="5" customWidth="true" width="23.0"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="15.109375"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="21.33203125"/>
+    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34" customWidth="1"/>
+    <col min="5" max="5" width="23" customWidth="1"/>
+    <col min="6" max="6" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -4310,22 +4307,22 @@
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>260</v>
-      </c>
-      <c r="C2" t="s" s="0">
-        <v>277</v>
-      </c>
-      <c r="D2" t="s" s="0">
+        <v>259</v>
+      </c>
+      <c r="C2" t="s">
+        <v>276</v>
+      </c>
+      <c r="D2" t="s">
         <v>58</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="F2" t="s" s="0">
-        <v>253</v>
-      </c>
-      <c r="G2" t="s" s="0">
-        <v>320</v>
+      <c r="F2" t="s">
+        <v>252</v>
+      </c>
+      <c r="G2" t="s">
+        <v>301</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -4333,19 +4330,19 @@
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>261</v>
-      </c>
-      <c r="C3" t="s" s="0">
-        <v>277</v>
-      </c>
-      <c r="D3" t="s" s="0">
+        <v>260</v>
+      </c>
+      <c r="C3" t="s">
+        <v>276</v>
+      </c>
+      <c r="D3" t="s">
         <v>58</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="F3" t="s" s="0">
-        <v>253</v>
+      <c r="F3" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -4353,19 +4350,19 @@
         <v>7</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="C4" t="s" s="0">
-        <v>277</v>
-      </c>
-      <c r="D4" t="s" s="0">
+        <v>261</v>
+      </c>
+      <c r="C4" t="s">
+        <v>276</v>
+      </c>
+      <c r="D4" t="s">
         <v>58</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="F4" t="s" s="0">
-        <v>253</v>
+      <c r="F4" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -4373,19 +4370,19 @@
         <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>263</v>
-      </c>
-      <c r="C5" t="s" s="0">
-        <v>277</v>
-      </c>
-      <c r="D5" t="s" s="0">
+        <v>262</v>
+      </c>
+      <c r="C5" t="s">
+        <v>276</v>
+      </c>
+      <c r="D5" t="s">
         <v>58</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="F5" t="s" s="0">
-        <v>253</v>
+      <c r="F5" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -4393,19 +4390,19 @@
         <v>9</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>264</v>
-      </c>
-      <c r="C6" t="s" s="0">
-        <v>277</v>
-      </c>
-      <c r="D6" t="s" s="0">
+        <v>263</v>
+      </c>
+      <c r="C6" t="s">
+        <v>276</v>
+      </c>
+      <c r="D6" t="s">
         <v>58</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="F6" t="s" s="0">
-        <v>253</v>
+      <c r="F6" t="s">
+        <v>252</v>
       </c>
     </row>
   </sheetData>
@@ -4429,13 +4426,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="10.6640625"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="31.109375"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="36.33203125"/>
-    <col min="5" max="5" customWidth="true" width="24.44140625"/>
-    <col min="6" max="6" customWidth="true" width="19.5546875"/>
-    <col min="7" max="7" customWidth="true" width="22.6640625"/>
-    <col min="8" max="8" customWidth="true" width="20.33203125"/>
+    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.44140625" customWidth="1"/>
+    <col min="6" max="6" width="19.5546875" customWidth="1"/>
+    <col min="7" max="7" width="22.6640625" customWidth="1"/>
+    <col min="8" max="8" width="20.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -4458,10 +4455,10 @@
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>321</v>
+        <v>302</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>322</v>
+        <v>303</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -4469,24 +4466,24 @@
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>265</v>
-      </c>
-      <c r="C2" t="s" s="0">
-        <v>278</v>
-      </c>
-      <c r="D2" t="s" s="0">
+        <v>264</v>
+      </c>
+      <c r="C2" t="s">
+        <v>277</v>
+      </c>
+      <c r="D2" t="s">
         <v>60</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="F2" t="s" s="0">
-        <v>253</v>
-      </c>
-      <c r="G2" t="s" s="0">
+      <c r="F2" t="s">
+        <v>252</v>
+      </c>
+      <c r="G2" t="s">
         <v>234</v>
       </c>
-      <c r="H2" t="s" s="0">
+      <c r="H2" t="s">
         <v>235</v>
       </c>
     </row>
@@ -4495,19 +4492,19 @@
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>266</v>
-      </c>
-      <c r="C3" t="s" s="0">
-        <v>278</v>
-      </c>
-      <c r="D3" t="s" s="0">
+        <v>265</v>
+      </c>
+      <c r="C3" t="s">
+        <v>277</v>
+      </c>
+      <c r="D3" t="s">
         <v>60</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="F3" t="s" s="0">
-        <v>253</v>
+      <c r="F3" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -4515,19 +4512,19 @@
         <v>7</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>267</v>
-      </c>
-      <c r="C4" t="s" s="0">
-        <v>278</v>
-      </c>
-      <c r="D4" t="s" s="0">
+        <v>266</v>
+      </c>
+      <c r="C4" t="s">
+        <v>277</v>
+      </c>
+      <c r="D4" t="s">
         <v>60</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="F4" t="s" s="0">
-        <v>253</v>
+      <c r="F4" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -4535,19 +4532,19 @@
         <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>268</v>
-      </c>
-      <c r="C5" t="s" s="0">
-        <v>278</v>
-      </c>
-      <c r="D5" t="s" s="0">
+        <v>267</v>
+      </c>
+      <c r="C5" t="s">
+        <v>277</v>
+      </c>
+      <c r="D5" t="s">
         <v>60</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="F5" t="s" s="0">
-        <v>253</v>
+      <c r="F5" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -4555,19 +4552,19 @@
         <v>9</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>269</v>
-      </c>
-      <c r="C6" t="s" s="0">
-        <v>278</v>
-      </c>
-      <c r="D6" t="s" s="0">
+        <v>268</v>
+      </c>
+      <c r="C6" t="s">
+        <v>277</v>
+      </c>
+      <c r="D6" t="s">
         <v>60</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="F6" t="s" s="0">
-        <v>253</v>
+      <c r="F6" t="s">
+        <v>252</v>
       </c>
     </row>
   </sheetData>

</xml_diff>